<commit_message>
Woodcamps, improvements to resource calculations and data displaying
Implemented woodcamp mechanic (buying WC, wood gain/loss per second)
Started implementing the Research section
Fixed resource bar slider not applying changes
Changed how wood (per click, per second, storage, etc.) values get calculated and displayed
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B3DC0C-17E0-4A4F-99EF-D5CB748B5429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DB08C7-F40B-44C7-9B9B-28333E9030A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="503">
   <si>
     <t xml:space="preserve">Tier </t>
   </si>
@@ -1305,9 +1305,6 @@
     <t>Oak storage +10</t>
   </si>
   <si>
-    <t>double storage</t>
-  </si>
-  <si>
     <t>ROUND((1.14^(M35)+M35^3)+148, 0)</t>
   </si>
   <si>
@@ -1428,9 +1425,6 @@
     <t>faster research 1%</t>
   </si>
   <si>
-    <t>better storage upgarade +10</t>
-  </si>
-  <si>
     <t>lower woodcamp production costs 1%</t>
   </si>
   <si>
@@ -1519,6 +1513,39 @@
   </si>
   <si>
     <t>Increase Oak per click 3%</t>
+  </si>
+  <si>
+    <t>multiply storage</t>
+  </si>
+  <si>
+    <t>better storage upgarade +40</t>
+  </si>
+  <si>
+    <t>Keep all research</t>
+  </si>
+  <si>
+    <t>Double all storage</t>
+  </si>
+  <si>
+    <t>Research 2 at a time</t>
+  </si>
+  <si>
+    <t>Research all Button</t>
+  </si>
+  <si>
+    <t>Buy Max Woodcamps</t>
+  </si>
+  <si>
+    <t>Build an Apple woodcamps</t>
+  </si>
+  <si>
+    <t>Unlock Production slider</t>
+  </si>
+  <si>
+    <t>Buy Max Levels</t>
+  </si>
+  <si>
+    <t>5000 Oak, 1000 Apple</t>
   </si>
 </sst>
 </file>
@@ -1975,6 +2002,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1982,7 +2010,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2565,7 +2592,7 @@
         <v>18</v>
       </c>
       <c r="I32" s="40" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J32" s="35" t="s">
         <v>8</v>
@@ -2633,7 +2660,7 @@
         <v>16</v>
       </c>
       <c r="I36" s="40" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J36" s="35" t="s">
         <v>25</v>
@@ -2650,7 +2677,7 @@
         <v>26</v>
       </c>
       <c r="I37" s="40" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J37" s="35" t="s">
         <v>11</v>
@@ -2684,7 +2711,7 @@
         <v>31</v>
       </c>
       <c r="I39" s="40" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J39" s="35" t="s">
         <v>20</v>
@@ -2701,7 +2728,7 @@
         <v>33</v>
       </c>
       <c r="I40" s="40" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J40" s="35" t="s">
         <v>11</v>
@@ -2718,7 +2745,7 @@
         <v>37</v>
       </c>
       <c r="I41" s="40" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J41" s="35" t="s">
         <v>25</v>
@@ -2752,7 +2779,7 @@
         <v>41</v>
       </c>
       <c r="I43" s="40" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J43" s="35" t="s">
         <v>20</v>
@@ -2769,7 +2796,7 @@
         <v>45</v>
       </c>
       <c r="I44" s="40" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J44" s="35" t="s">
         <v>34</v>
@@ -2821,7 +2848,7 @@
   </sheetPr>
   <dimension ref="A2:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -3117,7 +3144,7 @@
       <c r="F11" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="55"/>
+      <c r="G11" s="52"/>
       <c r="H11" s="1">
         <v>100</v>
       </c>
@@ -3689,8 +3716,8 @@
   </sheetPr>
   <dimension ref="A2:Y275"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3741,30 +3768,30 @@
         <v>76</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I5" t="s">
         <v>419</v>
       </c>
       <c r="J5" s="45" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K5" s="45" t="s">
-        <v>456</v>
-      </c>
-      <c r="M5" s="52" t="s">
+        <v>455</v>
+      </c>
+      <c r="M5" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52"/>
-      <c r="R5" s="52"/>
-      <c r="S5" s="52"/>
-      <c r="T5" s="52"/>
-      <c r="U5" s="52"/>
-      <c r="V5" s="52"/>
-      <c r="W5" s="52"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="53"/>
+      <c r="U5" s="53"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="53"/>
     </row>
     <row r="6" spans="1:23" ht="13.5" thickBot="1">
       <c r="A6" s="35" t="s">
@@ -3783,20 +3810,20 @@
         <v>416</v>
       </c>
       <c r="G6" s="45" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H6">
         <f>ROUND(1.28^M35 + 1.3 * M35^2.8, 0)+7</f>
         <v>10</v>
       </c>
       <c r="I6" s="45" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J6" s="45" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K6" s="45" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="M6" s="36" t="s">
         <v>79</v>
@@ -3849,23 +3876,23 @@
         <v>421</v>
       </c>
       <c r="G7" s="45" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H7">
         <f>ROUND(1.29^M35 + 1.3 * M35^1.8, 0)+22</f>
         <v>25</v>
       </c>
       <c r="I7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J7" s="45" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K7" s="45" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="L7" s="45" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="M7" s="26" t="s">
         <v>89</v>
@@ -3915,25 +3942,25 @@
         <v>3</v>
       </c>
       <c r="F8" s="45" t="s">
-        <v>422</v>
+        <v>492</v>
       </c>
       <c r="G8" s="45" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H8">
         <v>120</v>
       </c>
       <c r="I8" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J8" s="45" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K8" s="45" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="L8" s="45" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="M8" s="27" t="s">
         <v>99</v>
@@ -3983,22 +4010,22 @@
         <v>4</v>
       </c>
       <c r="F9" s="45" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G9" s="45" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="H9">
         <v>150</v>
       </c>
       <c r="I9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="J9" s="45" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K9" s="45" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="M9" s="27" t="s">
         <v>106</v>
@@ -4048,10 +4075,10 @@
         <v>5</v>
       </c>
       <c r="F10" s="45" t="s">
+        <v>453</v>
+      </c>
+      <c r="G10" s="45" t="s">
         <v>454</v>
-      </c>
-      <c r="G10" s="45" t="s">
-        <v>455</v>
       </c>
       <c r="H10">
         <v>500</v>
@@ -4100,19 +4127,19 @@
         <v>6</v>
       </c>
       <c r="F11" s="45" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H11">
         <v>750</v>
       </c>
       <c r="I11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J11" s="45" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="L11" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="M11" s="27" t="s">
         <v>117</v>
@@ -4156,16 +4183,16 @@
         <v>7</v>
       </c>
       <c r="F12" s="45" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H12">
         <v>1400</v>
       </c>
       <c r="I12" s="45" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J12" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M12" s="27" t="s">
         <v>120</v>
@@ -4207,7 +4234,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="46" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H13" s="1">
         <v>10000</v>
@@ -4343,6 +4370,10 @@
       <c r="E17" s="1">
         <v>12</v>
       </c>
+      <c r="G17" t="e">
+        <f>log</f>
+        <v>#NAME?</v>
+      </c>
       <c r="M17" s="40"/>
       <c r="N17" s="40" t="s">
         <v>407</v>
@@ -4427,7 +4458,7 @@
         <v>15</v>
       </c>
       <c r="F20" s="45" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="M20" s="35"/>
       <c r="N20" s="40"/>
@@ -4511,7 +4542,7 @@
         <v>4.11E+17</v>
       </c>
       <c r="I23" s="50" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>127</v>
@@ -4542,13 +4573,13 @@
         <v>1</v>
       </c>
       <c r="F24" s="45" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H24">
         <v>20</v>
       </c>
       <c r="I24" s="50" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>128</v>
@@ -4579,13 +4610,13 @@
         <v>2</v>
       </c>
       <c r="F25" s="45" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H25">
         <v>30</v>
       </c>
       <c r="I25" s="50" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>129</v>
@@ -4615,13 +4646,13 @@
         <v>3</v>
       </c>
       <c r="F26" s="45" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="H26">
         <v>150</v>
       </c>
       <c r="I26" s="50" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>131</v>
@@ -4651,13 +4682,13 @@
         <v>4</v>
       </c>
       <c r="F27" s="45" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H27">
         <v>300</v>
       </c>
       <c r="I27" s="50" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>132</v>
@@ -4687,13 +4718,13 @@
         <v>5</v>
       </c>
       <c r="F28" s="45" t="s">
-        <v>463</v>
+        <v>493</v>
       </c>
       <c r="H28">
         <v>400</v>
       </c>
       <c r="I28" s="50" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="M28" s="40"/>
       <c r="N28" s="40"/>
@@ -4748,13 +4779,13 @@
         <v>7</v>
       </c>
       <c r="F30" s="45" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H30">
         <v>1200</v>
       </c>
       <c r="I30" s="50" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="M30" s="40"/>
       <c r="N30" s="40"/>
@@ -4779,13 +4810,13 @@
         <v>8</v>
       </c>
       <c r="F31" s="45" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H31">
         <v>2000</v>
       </c>
       <c r="I31" s="50" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="12.75">
@@ -4799,16 +4830,16 @@
         <v>9</v>
       </c>
       <c r="F32" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="H32">
         <v>2200</v>
       </c>
       <c r="I32" s="50" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="33" spans="3:25" ht="12.75">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" ht="12.75">
       <c r="C33" s="1">
         <v>28</v>
       </c>
@@ -4819,7 +4850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="3:25" ht="12.75">
+    <row r="34" spans="1:25" ht="12.75">
       <c r="C34" s="1">
         <v>29</v>
       </c>
@@ -4834,7 +4865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="3:25" ht="12.75">
+    <row r="35" spans="1:25" ht="12.75">
       <c r="C35" s="1">
         <v>30</v>
       </c>
@@ -4861,7 +4892,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="3:25" ht="12.75">
+    <row r="36" spans="1:25" ht="12.75">
       <c r="C36" s="1">
         <v>31</v>
       </c>
@@ -4886,7 +4917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="3:25" ht="12.75">
+    <row r="37" spans="1:25" ht="12.75">
       <c r="C37" s="1">
         <v>32</v>
       </c>
@@ -4915,7 +4946,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="38" spans="3:25" ht="12.75">
+    <row r="38" spans="1:25" ht="12.75">
       <c r="C38" s="1">
         <v>33</v>
       </c>
@@ -4940,7 +4971,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="3:25" ht="12.75">
+    <row r="39" spans="1:25" ht="12.75">
       <c r="C39" s="1">
         <v>34</v>
       </c>
@@ -4966,7 +4997,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="3:25" ht="12.75">
+    <row r="40" spans="1:25" ht="12.75">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <f>LOG(A40, 9)</f>
+        <v>0</v>
+      </c>
       <c r="C40" s="1">
         <v>35</v>
       </c>
@@ -4989,7 +5027,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="3:25" ht="12.75">
+    <row r="41" spans="1:25" ht="12.75">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <f t="shared" ref="B41:B62" si="2">LOG(A41, 9)</f>
+        <v>0.63092975357145742</v>
+      </c>
       <c r="C41" s="1">
         <v>36</v>
       </c>
@@ -5014,7 +5059,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="3:25" ht="12.75">
+    <row r="42" spans="1:25" ht="12.75">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="2"/>
+        <v>0.88562187458071107</v>
+      </c>
       <c r="C42" s="1">
         <v>37</v>
       </c>
@@ -5025,7 +5077,7 @@
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="45">
@@ -5043,7 +5095,14 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="3:25" ht="12.75">
+    <row r="43" spans="1:25" ht="12.75">
+      <c r="A43">
+        <v>10</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="2"/>
+        <v>1.0479516371446924</v>
+      </c>
       <c r="C43" s="1">
         <v>38</v>
       </c>
@@ -5069,7 +5128,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="3:25" ht="12.75">
+    <row r="44" spans="1:25" ht="12.75">
+      <c r="A44">
+        <v>13</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="2"/>
+        <v>1.1673587597363964</v>
+      </c>
       <c r="C44" s="1">
         <v>39</v>
       </c>
@@ -5092,7 +5158,14 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="3:25" ht="12.75">
+    <row r="45" spans="1:25" ht="12.75">
+      <c r="A45">
+        <v>16</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="2"/>
+        <v>1.2618595071429148</v>
+      </c>
       <c r="C45" s="1">
         <v>40</v>
       </c>
@@ -5115,7 +5188,14 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="3:25" ht="12.75">
+    <row r="46" spans="1:25" ht="12.75">
+      <c r="A46">
+        <v>19</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="2"/>
+        <v>1.3400719296231876</v>
+      </c>
       <c r="C46" s="1">
         <v>41</v>
       </c>
@@ -5138,7 +5218,14 @@
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="3:25" ht="12.75">
+    <row r="47" spans="1:25" ht="12.75">
+      <c r="A47">
+        <v>22</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="2"/>
+        <v>1.4067940461077977</v>
+      </c>
       <c r="C47" s="1">
         <v>42</v>
       </c>
@@ -5161,7 +5248,14 @@
         <v>181</v>
       </c>
     </row>
-    <row r="48" spans="3:25" ht="12.75">
+    <row r="48" spans="1:25" ht="12.75">
+      <c r="A48">
+        <v>25</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="2"/>
+        <v>1.4649735207179269</v>
+      </c>
       <c r="C48" s="1">
         <v>43</v>
       </c>
@@ -5184,7 +5278,14 @@
         <v>210</v>
       </c>
     </row>
-    <row r="49" spans="3:15" ht="12.75">
+    <row r="49" spans="1:15" ht="12.75">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="2"/>
+        <v>1.5165516281521685</v>
+      </c>
       <c r="C49" s="1">
         <v>44</v>
       </c>
@@ -5207,7 +5308,14 @@
         <v>241</v>
       </c>
     </row>
-    <row r="50" spans="3:15" ht="12.75">
+    <row r="50" spans="1:15" ht="12.75">
+      <c r="A50">
+        <v>31</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="2"/>
+        <v>1.5628749286285073</v>
+      </c>
       <c r="C50" s="1">
         <v>45</v>
       </c>
@@ -5230,7 +5338,14 @@
         <v>275</v>
       </c>
     </row>
-    <row r="51" spans="3:15" ht="12.75">
+    <row r="51" spans="1:15" ht="12.75">
+      <c r="A51">
+        <v>34</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="2"/>
+        <v>1.6049158383670117</v>
+      </c>
       <c r="C51" s="1">
         <v>46</v>
       </c>
@@ -5252,7 +5367,14 @@
         <v>311</v>
       </c>
     </row>
-    <row r="52" spans="3:15" ht="12.75">
+    <row r="52" spans="1:15" ht="12.75">
+      <c r="A52">
+        <v>37</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="2"/>
+        <v>1.6433995641091363</v>
+      </c>
       <c r="C52" s="1">
         <v>47</v>
       </c>
@@ -5289,7 +5411,14 @@
         <v>349</v>
       </c>
     </row>
-    <row r="53" spans="3:15" ht="12.75">
+    <row r="53" spans="1:15" ht="12.75">
+      <c r="A53">
+        <v>40</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="2"/>
+        <v>1.6788813907161495</v>
+      </c>
       <c r="C53" s="1">
         <v>48</v>
       </c>
@@ -5303,7 +5432,7 @@
         <v>6</v>
       </c>
       <c r="H53" s="45" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M53">
         <v>19</v>
@@ -5317,7 +5446,14 @@
         <v>390</v>
       </c>
     </row>
-    <row r="54" spans="3:15" ht="12.75">
+    <row r="54" spans="1:15" ht="12.75">
+      <c r="A54">
+        <v>43</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="2"/>
+        <v>1.7117959422488396</v>
+      </c>
       <c r="C54" s="1">
         <v>49</v>
       </c>
@@ -5345,7 +5481,14 @@
         <v>433</v>
       </c>
     </row>
-    <row r="55" spans="3:15" ht="12.75">
+    <row r="55" spans="1:15" ht="12.75">
+      <c r="A55">
+        <v>46</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="2"/>
+        <v>1.7424897918858642</v>
+      </c>
       <c r="C55" s="1">
         <v>50</v>
       </c>
@@ -5368,7 +5511,7 @@
         <v>500</v>
       </c>
       <c r="L55" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="M55">
         <v>21</v>
@@ -5382,7 +5525,14 @@
         <v>479</v>
       </c>
     </row>
-    <row r="56" spans="3:15" ht="12.75">
+    <row r="56" spans="1:15" ht="12.75">
+      <c r="A56">
+        <v>49</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="2"/>
+        <v>1.7712437491614221</v>
+      </c>
       <c r="C56" s="1">
         <v>51</v>
       </c>
@@ -5396,7 +5546,7 @@
         <v>6</v>
       </c>
       <c r="L56" s="45" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M56">
         <v>22</v>
@@ -5410,7 +5560,14 @@
         <v>528</v>
       </c>
     </row>
-    <row r="57" spans="3:15" ht="12.75">
+    <row r="57" spans="1:15" ht="12.75">
+      <c r="A57">
+        <v>52</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="2"/>
+        <v>1.7982885133078537</v>
+      </c>
       <c r="C57" s="1">
         <v>52</v>
       </c>
@@ -5435,7 +5592,14 @@
         <v>579</v>
       </c>
     </row>
-    <row r="58" spans="3:15" ht="12.75">
+    <row r="58" spans="1:15" ht="12.75">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="2"/>
+        <v>1.8238159296810326</v>
+      </c>
       <c r="C58" s="1">
         <v>53</v>
       </c>
@@ -5449,7 +5613,7 @@
         <v>6</v>
       </c>
       <c r="L58" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="M58">
         <v>24</v>
@@ -5463,7 +5627,14 @@
         <v>634</v>
       </c>
     </row>
-    <row r="59" spans="3:15" ht="12.75">
+    <row r="59" spans="1:15" ht="12.75">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="2"/>
+        <v>1.8479872528410597</v>
+      </c>
       <c r="C59" s="1">
         <v>54</v>
       </c>
@@ -5477,7 +5648,7 @@
         <v>9</v>
       </c>
       <c r="H59" s="45" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="M59">
         <v>25</v>
@@ -5491,7 +5662,14 @@
         <v>691</v>
       </c>
     </row>
-    <row r="60" spans="3:15" ht="12.75">
+    <row r="60" spans="1:15" ht="12.75">
+      <c r="A60">
+        <v>61</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="2"/>
+        <v>1.8709393234427967</v>
+      </c>
       <c r="C60" s="1">
         <v>55</v>
       </c>
@@ -5513,7 +5691,14 @@
         <v>752</v>
       </c>
     </row>
-    <row r="61" spans="3:15" ht="12.75">
+    <row r="61" spans="1:15" ht="12.75">
+      <c r="A61">
+        <v>64</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="2"/>
+        <v>1.8927892607143719</v>
+      </c>
       <c r="C61" s="1">
         <v>56</v>
       </c>
@@ -5535,7 +5720,14 @@
         <v>817</v>
       </c>
     </row>
-    <row r="62" spans="3:15" ht="12.75">
+    <row r="62" spans="1:15" ht="12.75">
+      <c r="A62">
+        <v>9887654321</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="2"/>
+        <v>10.474374360724788</v>
+      </c>
       <c r="C62" s="1">
         <v>57</v>
       </c>
@@ -5557,7 +5749,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="63" spans="3:15" ht="12.75">
+    <row r="63" spans="1:15" ht="12.75">
       <c r="C63" s="1">
         <v>58</v>
       </c>
@@ -5579,7 +5771,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="64" spans="3:15" ht="12.75">
+    <row r="64" spans="1:15" ht="12.75">
       <c r="C64" s="1">
         <v>59</v>
       </c>
@@ -6385,11 +6577,11 @@
         <v>66</v>
       </c>
       <c r="N100" s="45">
-        <f t="shared" ref="N100:N160" si="2">ROUND(1.28^M100 + 1.3 * M100^1.8, 0)</f>
+        <f t="shared" ref="N100:N160" si="3">ROUND(1.28^M100 + 1.3 * M100^1.8, 0)</f>
         <v>11910975</v>
       </c>
       <c r="O100">
-        <f t="shared" ref="O100:O163" si="3">ROUND(1.15^(M100+5)+M100^2,0)</f>
+        <f t="shared" ref="O100:O163" si="4">ROUND(1.15^(M100+5)+M100^2,0)</f>
         <v>24752</v>
       </c>
     </row>
@@ -6407,11 +6599,11 @@
         <v>67</v>
       </c>
       <c r="N101" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15245430</v>
       </c>
       <c r="O101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27944</v>
       </c>
     </row>
@@ -6429,11 +6621,11 @@
         <v>68</v>
       </c>
       <c r="N102" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19513513</v>
       </c>
       <c r="O102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>31598</v>
       </c>
     </row>
@@ -6451,11 +6643,11 @@
         <v>69</v>
       </c>
       <c r="N103" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24976642</v>
       </c>
       <c r="O103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35781</v>
       </c>
     </row>
@@ -6473,11 +6665,11 @@
         <v>70</v>
       </c>
       <c r="N104" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31969429</v>
       </c>
       <c r="O104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40573</v>
       </c>
     </row>
@@ -6495,11 +6687,11 @@
         <v>71</v>
       </c>
       <c r="N105" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40920176</v>
       </c>
       <c r="O105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>46065</v>
       </c>
     </row>
@@ -6517,11 +6709,11 @@
         <v>72</v>
       </c>
       <c r="N106" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>52377115</v>
       </c>
       <c r="O106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>52361</v>
       </c>
     </row>
@@ -6539,11 +6731,11 @@
         <v>73</v>
       </c>
       <c r="N107" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>67041977</v>
       </c>
       <c r="O107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>59583</v>
       </c>
     </row>
@@ -6561,11 +6753,11 @@
         <v>74</v>
       </c>
       <c r="N108" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85812981</v>
       </c>
       <c r="O108">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67868</v>
       </c>
     </row>
@@ -6583,11 +6775,11 @@
         <v>75</v>
       </c>
       <c r="N109" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>109839846</v>
       </c>
       <c r="O109">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>77376</v>
       </c>
     </row>
@@ -6605,11 +6797,11 @@
         <v>76</v>
       </c>
       <c r="N110" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140594214</v>
       </c>
       <c r="O110">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>88290</v>
       </c>
     </row>
@@ -6627,11 +6819,11 @@
         <v>77</v>
       </c>
       <c r="N111" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>179959785</v>
       </c>
       <c r="O111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100820</v>
       </c>
     </row>
@@ -6649,11 +6841,11 @@
         <v>78</v>
       </c>
       <c r="N112" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>230347695</v>
       </c>
       <c r="O112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>115208</v>
       </c>
     </row>
@@ -6671,11 +6863,11 @@
         <v>79</v>
       </c>
       <c r="N113" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>294844200</v>
       </c>
       <c r="O113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>131734</v>
       </c>
     </row>
@@ -6693,11 +6885,11 @@
         <v>80</v>
       </c>
       <c r="N114" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>377399706</v>
       </c>
       <c r="O114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150717</v>
       </c>
     </row>
@@ -6715,11 +6907,11 @@
         <v>81</v>
       </c>
       <c r="N115" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>483070732</v>
       </c>
       <c r="O115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>172525</v>
       </c>
     </row>
@@ -6737,11 +6929,11 @@
         <v>82</v>
       </c>
       <c r="N116" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>618329625</v>
       </c>
       <c r="O116">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>197583</v>
       </c>
     </row>
@@ -6759,11 +6951,11 @@
         <v>83</v>
       </c>
       <c r="N117" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>791460985</v>
       </c>
       <c r="O117">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>226377</v>
       </c>
     </row>
@@ -6781,11 +6973,11 @@
         <v>84</v>
       </c>
       <c r="N118" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1013069106</v>
       </c>
       <c r="O118">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>259467</v>
       </c>
     </row>
@@ -6803,11 +6995,11 @@
         <v>85</v>
       </c>
       <c r="N119" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1296727478</v>
       </c>
       <c r="O119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>297497</v>
       </c>
     </row>
@@ -6825,11 +7017,11 @@
         <v>86</v>
       </c>
       <c r="N120" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1659810172</v>
       </c>
       <c r="O120">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>341209</v>
       </c>
     </row>
@@ -6847,11 +7039,11 @@
         <v>87</v>
       </c>
       <c r="N121" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2124555999</v>
       </c>
       <c r="O121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>391454</v>
       </c>
     </row>
@@ -6869,11 +7061,11 @@
         <v>88</v>
       </c>
       <c r="N122" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2719430635</v>
       </c>
       <c r="O122">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>449212</v>
       </c>
     </row>
@@ -6891,11 +7083,11 @@
         <v>89</v>
       </c>
       <c r="N123" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3480870146</v>
       </c>
       <c r="O123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>515609</v>
       </c>
     </row>
@@ -6913,11 +7105,11 @@
         <v>90</v>
       </c>
       <c r="N124" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4455512697</v>
       </c>
       <c r="O124">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>591941</v>
       </c>
     </row>
@@ -6935,11 +7127,11 @@
         <v>91</v>
       </c>
       <c r="N125" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5703055139</v>
       </c>
       <c r="O125">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>679699</v>
       </c>
     </row>
@@ -6957,11 +7149,11 @@
         <v>92</v>
       </c>
       <c r="N126" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7299909442</v>
       </c>
       <c r="O126">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>780594</v>
       </c>
     </row>
@@ -6979,11 +7171,11 @@
         <v>93</v>
       </c>
       <c r="N127" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9343882927</v>
       </c>
       <c r="O127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>896599</v>
       </c>
     </row>
@@ -7001,11 +7193,11 @@
         <v>94</v>
       </c>
       <c r="N128" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11960168963</v>
       </c>
       <c r="O128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1029978</v>
       </c>
     </row>
@@ -7023,11 +7215,11 @@
         <v>95</v>
       </c>
       <c r="N129" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15309015065</v>
       </c>
       <c r="O129">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1183338</v>
       </c>
     </row>
@@ -7045,11 +7237,11 @@
         <v>96</v>
       </c>
       <c r="N130" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19595538051</v>
       </c>
       <c r="O130">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1359676</v>
       </c>
     </row>
@@ -7067,11 +7259,11 @@
         <v>97</v>
       </c>
       <c r="N131" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25082287450</v>
       </c>
       <c r="O131">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1562439</v>
       </c>
     </row>
@@ -7089,11 +7281,11 @@
         <v>98</v>
       </c>
       <c r="N132" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32105326655</v>
       </c>
       <c r="O132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1795588</v>
       </c>
     </row>
@@ -7111,11 +7303,11 @@
         <v>99</v>
       </c>
       <c r="N133" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41094816813</v>
       </c>
       <c r="O133">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2063683</v>
       </c>
     </row>
@@ -7133,11 +7325,11 @@
         <v>100</v>
       </c>
       <c r="N134" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>52601364191</v>
       </c>
       <c r="O134">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2371964</v>
       </c>
     </row>
@@ -7155,11 +7347,11 @@
         <v>101</v>
       </c>
       <c r="N135" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>67329744809</v>
       </c>
       <c r="O135">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2726459</v>
       </c>
     </row>
@@ -7177,11 +7369,11 @@
         <v>102</v>
       </c>
       <c r="N136" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>86182071974</v>
       </c>
       <c r="O136">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3134101</v>
       </c>
     </row>
@@ -7199,11 +7391,11 @@
         <v>103</v>
       </c>
       <c r="N137" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>110313050720</v>
       </c>
       <c r="O137">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3602861</v>
       </c>
     </row>
@@ -7221,11 +7413,11 @@
         <v>104</v>
       </c>
       <c r="N138" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>141200703489</v>
       </c>
       <c r="O138">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4141905</v>
       </c>
     </row>
@@ -7243,11 +7435,11 @@
         <v>105</v>
       </c>
       <c r="N139" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>180736899008</v>
       </c>
       <c r="O139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4761778</v>
       </c>
     </row>
@@ -7262,17 +7454,17 @@
         <v>9</v>
       </c>
       <c r="F140" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="M140">
         <v>106</v>
       </c>
       <c r="N140" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>231343229245</v>
       </c>
       <c r="O140">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5474602</v>
       </c>
     </row>
@@ -7290,11 +7482,11 @@
         <v>107</v>
       </c>
       <c r="N141" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>296119331922</v>
       </c>
       <c r="O141">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6294320</v>
       </c>
     </row>
@@ -7312,11 +7504,11 @@
         <v>108</v>
       </c>
       <c r="N142" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>379032743322</v>
       </c>
       <c r="O142">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7236965</v>
       </c>
     </row>
@@ -7334,11 +7526,11 @@
         <v>109</v>
       </c>
       <c r="N143" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>485161909888</v>
       </c>
       <c r="O143">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8320977</v>
       </c>
     </row>
@@ -7356,11 +7548,11 @@
         <v>110</v>
       </c>
       <c r="N144" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>621007243064</v>
       </c>
       <c r="O144">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9567561</v>
       </c>
     </row>
@@ -7378,11 +7570,11 @@
         <v>111</v>
       </c>
       <c r="N145" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>794889269503</v>
       </c>
       <c r="O145">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11001101</v>
       </c>
     </row>
@@ -7400,11 +7592,11 @@
         <v>112</v>
       </c>
       <c r="N146" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1017458263317</v>
       </c>
       <c r="O146">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12649641</v>
       </c>
     </row>
@@ -7422,11 +7614,11 @@
         <v>113</v>
       </c>
       <c r="N147" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1302346575371</v>
       </c>
       <c r="O147">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14545431</v>
       </c>
     </row>
@@ -7444,11 +7636,11 @@
         <v>114</v>
       </c>
       <c r="N148" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1667003614772</v>
       </c>
       <c r="O148">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16725557</v>
       </c>
     </row>
@@ -7466,11 +7658,11 @@
         <v>115</v>
       </c>
       <c r="N149" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2133764625177</v>
       </c>
       <c r="O149">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19232670</v>
       </c>
     </row>
@@ -7488,11 +7680,11 @@
         <v>116</v>
       </c>
       <c r="N150" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2731218718468</v>
       </c>
       <c r="O150">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22115818</v>
       </c>
     </row>
@@ -7510,11 +7702,11 @@
         <v>117</v>
       </c>
       <c r="N151" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3495959957851</v>
       </c>
       <c r="O151">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25431405</v>
       </c>
     </row>
@@ -7532,11 +7724,11 @@
         <v>118</v>
       </c>
       <c r="N152" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4474828744233</v>
       </c>
       <c r="O152">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>29244297</v>
       </c>
     </row>
@@ -7554,11 +7746,11 @@
         <v>119</v>
       </c>
       <c r="N153" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5727780790773</v>
       </c>
       <c r="O153">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33629090</v>
       </c>
     </row>
@@ -7576,11 +7768,11 @@
         <v>120</v>
       </c>
       <c r="N154" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7331559410315</v>
       </c>
       <c r="O154">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>38671569</v>
       </c>
     </row>
@@ -7598,11 +7790,11 @@
         <v>121</v>
       </c>
       <c r="N155" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9384396043300</v>
       </c>
       <c r="O155">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>44470385</v>
       </c>
     </row>
@@ -7620,11 +7812,11 @@
         <v>122</v>
       </c>
       <c r="N156" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12012026933490</v>
       </c>
       <c r="O156">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>51138990</v>
       </c>
     </row>
@@ -7642,11 +7834,11 @@
         <v>123</v>
       </c>
       <c r="N157" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15375394472904</v>
       </c>
       <c r="O157">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>58807851</v>
       </c>
     </row>
@@ -7664,11 +7856,11 @@
         <v>124</v>
       </c>
       <c r="N158" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19680504923324</v>
       </c>
       <c r="O158">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67627006</v>
       </c>
     </row>
@@ -7686,11 +7878,11 @@
         <v>125</v>
       </c>
       <c r="N159" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25191046299832</v>
       </c>
       <c r="O159">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>77768999</v>
       </c>
     </row>
@@ -7708,11 +7900,11 @@
         <v>126</v>
       </c>
       <c r="N160" s="45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32244539261731</v>
       </c>
       <c r="O160">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>89432257</v>
       </c>
     </row>
@@ -7734,7 +7926,7 @@
         <v>41273010252932</v>
       </c>
       <c r="O161">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>102844967</v>
       </c>
     </row>
@@ -7752,11 +7944,11 @@
         <v>128</v>
       </c>
       <c r="N162" s="45">
-        <f t="shared" ref="N162:N175" si="4">ROUND(1.28^M162 + 1.3 * M162^1.8, 0)</f>
+        <f t="shared" ref="N162:N175" si="5">ROUND(1.28^M162 + 1.3 * M162^1.8, 0)</f>
         <v>52829453121638</v>
       </c>
       <c r="O162">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>118269547</v>
       </c>
     </row>
@@ -7774,11 +7966,11 @@
         <v>129</v>
       </c>
       <c r="N163" s="45">
+        <f t="shared" si="5"/>
+        <v>67621699993550</v>
+      </c>
+      <c r="O163">
         <f t="shared" si="4"/>
-        <v>67621699993550</v>
-      </c>
-      <c r="O163">
-        <f t="shared" si="3"/>
         <v>136007779</v>
       </c>
     </row>
@@ -7796,11 +7988,11 @@
         <v>130</v>
       </c>
       <c r="N164" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>86555775989567</v>
       </c>
       <c r="O164">
-        <f t="shared" ref="O164:O184" si="5">ROUND(1.15^(M164+5)+M164^2,0)</f>
+        <f t="shared" ref="O164:O184" si="6">ROUND(1.15^(M164+5)+M164^2,0)</f>
         <v>156406708</v>
       </c>
     </row>
@@ -7818,11 +8010,11 @@
         <v>131</v>
       </c>
       <c r="N165" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>110791393264437</v>
       </c>
       <c r="O165">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>179865441</v>
       </c>
     </row>
@@ -7840,11 +8032,11 @@
         <v>132</v>
       </c>
       <c r="N166" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>141812983376239</v>
       </c>
       <c r="O166">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>206842946</v>
       </c>
     </row>
@@ -7862,11 +8054,11 @@
         <v>133</v>
       </c>
       <c r="N167" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>181520618719314</v>
       </c>
       <c r="O167">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>237867039</v>
       </c>
     </row>
@@ -7884,11 +8076,11 @@
         <v>134</v>
       </c>
       <c r="N168" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>232346391958418</v>
       </c>
       <c r="O168">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>273544708</v>
       </c>
     </row>
@@ -7906,11 +8098,11 @@
         <v>135</v>
       </c>
       <c r="N169" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>297403381704440</v>
       </c>
       <c r="O169">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>314573990</v>
       </c>
     </row>
@@ -7928,11 +8120,11 @@
         <v>136</v>
       </c>
       <c r="N170" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>380676328579314</v>
       </c>
       <c r="O170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>361757626</v>
       </c>
     </row>
@@ -7950,11 +8142,11 @@
         <v>137</v>
       </c>
       <c r="N171" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>487265700579121</v>
       </c>
       <c r="O171">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>416018769</v>
       </c>
     </row>
@@ -7972,11 +8164,11 @@
         <v>138</v>
       </c>
       <c r="N172" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>623700096738842</v>
       </c>
       <c r="O172">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>478419044</v>
       </c>
     </row>
@@ -7994,11 +8186,11 @@
         <v>139</v>
       </c>
       <c r="N173" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>798336123823251</v>
       </c>
       <c r="O173">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>550179320</v>
       </c>
     </row>
@@ -8016,11 +8208,11 @@
         <v>140</v>
       </c>
       <c r="N174" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1021870238491260</v>
       </c>
       <c r="O174">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>632703599</v>
       </c>
     </row>
@@ -8038,11 +8230,11 @@
         <v>141</v>
       </c>
       <c r="N175" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1307993905266280</v>
       </c>
       <c r="O175">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>727606480</v>
       </c>
     </row>
@@ -8064,7 +8256,7 @@
         <v>1674232198738270</v>
       </c>
       <c r="O176">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>836744753</v>
       </c>
     </row>
@@ -8082,11 +8274,11 @@
         <v>143</v>
       </c>
       <c r="N177" s="45">
-        <f t="shared" ref="N177:N184" si="6">ROUND(1.28^M177 + 1.3 * M177^1.8, 0)</f>
+        <f t="shared" ref="N177:N184" si="7">ROUND(1.28^M177 + 1.3 * M177^1.8, 0)</f>
         <v>2143017214382390</v>
       </c>
       <c r="O177">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>962253727</v>
       </c>
     </row>
@@ -8104,11 +8296,11 @@
         <v>144</v>
       </c>
       <c r="N178" s="45">
+        <f t="shared" si="7"/>
+        <v>2743062034406820</v>
+      </c>
+      <c r="O178">
         <f t="shared" si="6"/>
-        <v>2743062034406820</v>
-      </c>
-      <c r="O178">
-        <f t="shared" si="5"/>
         <v>1106589005</v>
       </c>
     </row>
@@ -8126,11 +8318,11 @@
         <v>145</v>
       </c>
       <c r="N179" s="45">
+        <f t="shared" si="7"/>
+        <v>3511119404038070</v>
+      </c>
+      <c r="O179">
         <f t="shared" si="6"/>
-        <v>3511119404038070</v>
-      </c>
-      <c r="O179">
-        <f t="shared" si="5"/>
         <v>1272574535</v>
       </c>
     </row>
@@ -8148,11 +8340,11 @@
         <v>146</v>
       </c>
       <c r="N180" s="45">
+        <f t="shared" si="7"/>
+        <v>4494232837166020</v>
+      </c>
+      <c r="O180">
         <f t="shared" si="6"/>
-        <v>4494232837166020</v>
-      </c>
-      <c r="O180">
-        <f t="shared" si="5"/>
         <v>1463457852</v>
       </c>
     </row>
@@ -8170,11 +8362,11 @@
         <v>147</v>
       </c>
       <c r="N181" s="45">
+        <f t="shared" si="7"/>
+        <v>5752618031569770</v>
+      </c>
+      <c r="O181">
         <f t="shared" si="6"/>
-        <v>5752618031569770</v>
-      </c>
-      <c r="O181">
-        <f t="shared" si="5"/>
         <v>1682973625</v>
       </c>
     </row>
@@ -8192,11 +8384,11 @@
         <v>148</v>
       </c>
       <c r="N182" s="45">
+        <f t="shared" si="7"/>
+        <v>7363351080406540</v>
+      </c>
+      <c r="O182">
         <f t="shared" si="6"/>
-        <v>7363351080406540</v>
-      </c>
-      <c r="O182">
-        <f t="shared" si="5"/>
         <v>1935416723</v>
       </c>
     </row>
@@ -8214,11 +8406,11 @@
         <v>149</v>
       </c>
       <c r="N183" s="45">
+        <f t="shared" si="7"/>
+        <v>9425089382917560</v>
+      </c>
+      <c r="O183">
         <f t="shared" si="6"/>
-        <v>9425089382917560</v>
-      </c>
-      <c r="O183">
-        <f t="shared" si="5"/>
         <v>2225726243</v>
       </c>
     </row>
@@ -8236,11 +8428,11 @@
         <v>150</v>
       </c>
       <c r="N184" s="45">
+        <f t="shared" si="7"/>
+        <v>1.20641144101316E+16</v>
+      </c>
+      <c r="O184">
         <f t="shared" si="6"/>
-        <v>1.20641144101316E+16</v>
-      </c>
-      <c r="O184">
-        <f t="shared" si="5"/>
         <v>2559582148</v>
       </c>
     </row>
@@ -8891,7 +9083,7 @@
         <v>3</v>
       </c>
       <c r="H242" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="243" spans="1:8" ht="15.75" customHeight="1">
@@ -8905,7 +9097,7 @@
         <v>4</v>
       </c>
       <c r="H243" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="244" spans="1:8" ht="15.75" customHeight="1">
@@ -8919,7 +9111,7 @@
         <v>5</v>
       </c>
       <c r="H244" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="245" spans="1:8" ht="15.75" customHeight="1">
@@ -8933,7 +9125,7 @@
         <v>6</v>
       </c>
       <c r="H245" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="246" spans="1:8" ht="15.75" customHeight="1">
@@ -8947,7 +9139,7 @@
         <v>7</v>
       </c>
       <c r="H246" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="247" spans="1:8" ht="15.75" customHeight="1">
@@ -8961,7 +9153,7 @@
         <v>8</v>
       </c>
       <c r="H247" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="248" spans="1:8" ht="15.75" customHeight="1">
@@ -8975,7 +9167,7 @@
         <v>9</v>
       </c>
       <c r="H248" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="249" spans="1:8" ht="15.75" customHeight="1">
@@ -8989,7 +9181,7 @@
         <v>10</v>
       </c>
       <c r="H249" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="250" spans="1:8" ht="15.75" customHeight="1">
@@ -9006,7 +9198,7 @@
         <v>11</v>
       </c>
       <c r="H250" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="251" spans="1:8" ht="15.75" customHeight="1">
@@ -9023,7 +9215,7 @@
         <v>12</v>
       </c>
       <c r="H251" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="252" spans="1:8" ht="15.75" customHeight="1">
@@ -9040,7 +9232,7 @@
         <v>13</v>
       </c>
       <c r="H252" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="253" spans="1:8" ht="15.75" customHeight="1">
@@ -9057,7 +9249,7 @@
         <v>14</v>
       </c>
       <c r="H253" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="254" spans="1:8" ht="15.75" customHeight="1">
@@ -9071,7 +9263,7 @@
         <v>15</v>
       </c>
       <c r="H254" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="255" spans="1:8" ht="15.75" customHeight="1">
@@ -9085,7 +9277,7 @@
         <v>16</v>
       </c>
       <c r="H255" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="256" spans="1:8" ht="15.75" customHeight="1">
@@ -9099,7 +9291,7 @@
         <v>17</v>
       </c>
       <c r="H256" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="257" spans="3:8" ht="15.75" customHeight="1">
@@ -9152,7 +9344,7 @@
         <v>3</v>
       </c>
       <c r="H260" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="261" spans="3:8" ht="15.75" customHeight="1">
@@ -9166,7 +9358,7 @@
         <v>4</v>
       </c>
       <c r="H261" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="262" spans="3:8" ht="15.75" customHeight="1">
@@ -9180,7 +9372,7 @@
         <v>5</v>
       </c>
       <c r="H262" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="263" spans="3:8" ht="15.75" customHeight="1">
@@ -9194,7 +9386,7 @@
         <v>6</v>
       </c>
       <c r="H263" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="264" spans="3:8" ht="15.75" customHeight="1">
@@ -9208,7 +9400,7 @@
         <v>7</v>
       </c>
       <c r="H264" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="265" spans="3:8" ht="15.75" customHeight="1">
@@ -9222,7 +9414,7 @@
         <v>8</v>
       </c>
       <c r="H265" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="266" spans="3:8" ht="15.75" customHeight="1">
@@ -9236,7 +9428,7 @@
         <v>9</v>
       </c>
       <c r="H266" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="267" spans="3:8" ht="15.75" customHeight="1">
@@ -9250,7 +9442,7 @@
         <v>10</v>
       </c>
       <c r="H267" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="268" spans="3:8" ht="15.75" customHeight="1">
@@ -9264,7 +9456,7 @@
         <v>11</v>
       </c>
       <c r="H268" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="269" spans="3:8" ht="15.75" customHeight="1">
@@ -9278,7 +9470,7 @@
         <v>12</v>
       </c>
       <c r="H269" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="270" spans="3:8" ht="15.75" customHeight="1">
@@ -9292,7 +9484,7 @@
         <v>13</v>
       </c>
       <c r="H270" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="271" spans="3:8" ht="15.75" customHeight="1">
@@ -9306,7 +9498,7 @@
         <v>14</v>
       </c>
       <c r="H271" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="272" spans="3:8" ht="15.75" customHeight="1">
@@ -9320,7 +9512,7 @@
         <v>15</v>
       </c>
       <c r="H272" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="273" spans="3:8" ht="15.75" customHeight="1">
@@ -9334,7 +9526,7 @@
         <v>16</v>
       </c>
       <c r="H273" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="274" spans="3:8" ht="15.75" customHeight="1">
@@ -9348,7 +9540,7 @@
         <v>17</v>
       </c>
       <c r="H274" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="275" spans="3:8" ht="15.75" customHeight="1">
@@ -9362,7 +9554,7 @@
         <v>18</v>
       </c>
       <c r="H275" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -9381,11 +9573,14 @@
   </sheetPr>
   <dimension ref="C2:J65"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="6" max="6" width="38.85546875" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:10">
@@ -9430,7 +9625,13 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>138</v>
+        <v>196</v>
+      </c>
+      <c r="I5" t="s">
+        <v>502</v>
+      </c>
+      <c r="J5" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="3:10">
@@ -9444,7 +9645,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="3:10">
@@ -9458,7 +9659,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="3:10">
@@ -9472,7 +9673,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="3:10">
@@ -9486,7 +9687,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="3:10">
@@ -9500,7 +9701,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="3:10">
@@ -9514,7 +9715,7 @@
         <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="3:10">
@@ -9528,7 +9729,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="3:10">
@@ -9542,7 +9743,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="3:10">
@@ -9556,7 +9757,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="3:10">
@@ -9570,7 +9771,7 @@
         <v>3</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="3:10">
@@ -9584,7 +9785,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -9598,7 +9799,7 @@
         <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="3:6">
@@ -9612,7 +9813,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="3:6">
@@ -9626,7 +9827,7 @@
         <v>7</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="3:6">
@@ -9640,7 +9841,7 @@
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="3:6">
@@ -9653,8 +9854,8 @@
       <c r="E21" s="1">
         <v>9</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>154</v>
+      <c r="F21" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="3:6">
@@ -9667,8 +9868,8 @@
       <c r="E22" s="1">
         <v>10</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>155</v>
+      <c r="F22" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="3:6">
@@ -9682,7 +9883,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="3:6">
@@ -9696,7 +9897,7 @@
         <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="3:6">
@@ -9710,7 +9911,7 @@
         <v>13</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="3:6">
@@ -9724,7 +9925,7 @@
         <v>14</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="3:6">
@@ -9738,7 +9939,7 @@
         <v>15</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="3:6">
@@ -9752,7 +9953,7 @@
         <v>16</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="3:6">
@@ -9766,7 +9967,7 @@
         <v>17</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="3:6">
@@ -9780,7 +9981,7 @@
         <v>18</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="3:6">
@@ -9794,7 +9995,7 @@
         <v>19</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="3:6">
@@ -9808,7 +10009,7 @@
         <v>20</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="3:6">
@@ -9822,7 +10023,7 @@
         <v>21</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="3:6">
@@ -9836,7 +10037,7 @@
         <v>22</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="3:6">
@@ -9850,7 +10051,7 @@
         <v>23</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="3:6">
@@ -9864,7 +10065,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="3:6">
@@ -9878,7 +10079,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="3:6">
@@ -9892,7 +10093,7 @@
         <v>2</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="3:6">
@@ -9906,7 +10107,7 @@
         <v>3</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="3:6">
@@ -9920,7 +10121,7 @@
         <v>4</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="3:6">
@@ -9934,7 +10135,7 @@
         <v>5</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="3:6">
@@ -9948,7 +10149,7 @@
         <v>6</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="3:6">
@@ -9962,7 +10163,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="3:6">
@@ -9976,7 +10177,7 @@
         <v>2</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="3:6">
@@ -9990,7 +10191,7 @@
         <v>3</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="3:6">
@@ -10004,7 +10205,7 @@
         <v>4</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="3:6">
@@ -10018,7 +10219,7 @@
         <v>5</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="3:6">
@@ -10032,7 +10233,7 @@
         <v>6</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="3:6">
@@ -10046,7 +10247,7 @@
         <v>7</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="3:6">
@@ -10060,7 +10261,7 @@
         <v>1</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="3:6">
@@ -10074,7 +10275,7 @@
         <v>2</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="3:6">
@@ -10088,7 +10289,7 @@
         <v>3</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="3:6">
@@ -10102,7 +10303,7 @@
         <v>4</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="3:6">
@@ -10116,7 +10317,7 @@
         <v>5</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="3:6">
@@ -10130,7 +10331,7 @@
         <v>6</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="56" spans="3:6">
@@ -10144,7 +10345,7 @@
         <v>7</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="3:6">
@@ -10158,7 +10359,7 @@
         <v>8</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="3:6">
@@ -10172,7 +10373,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="3:6">
@@ -10186,7 +10387,7 @@
         <v>2</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="60" spans="3:6">
@@ -10200,7 +10401,7 @@
         <v>3</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="61" spans="3:6">
@@ -10214,7 +10415,7 @@
         <v>4</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" spans="3:6">
@@ -10222,7 +10423,7 @@
         <v>58</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="63" spans="3:6">
@@ -10788,9 +10989,14 @@
   </sheetPr>
   <dimension ref="C4:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="4" spans="3:7">
       <c r="C4" s="1" t="s">
@@ -10858,6 +11064,9 @@
       <c r="C12" s="1">
         <v>6</v>
       </c>
+      <c r="D12" t="s">
+        <v>496</v>
+      </c>
       <c r="G12" s="1">
         <v>135</v>
       </c>
@@ -10882,6 +11091,9 @@
       <c r="C15" s="1">
         <v>9</v>
       </c>
+      <c r="D15" t="s">
+        <v>495</v>
+      </c>
       <c r="G15" s="1">
         <v>666</v>
       </c>
@@ -10953,6 +11165,9 @@
     <row r="24" spans="3:7">
       <c r="C24" s="1">
         <v>18</v>
+      </c>
+      <c r="D24" t="s">
+        <v>494</v>
       </c>
       <c r="G24" s="28" t="s">
         <v>234</v>
@@ -11136,11 +11351,14 @@
   </sheetPr>
   <dimension ref="C3:V105"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="26" customWidth="1"/>
   </cols>
@@ -11154,15 +11372,15 @@
       </c>
     </row>
     <row r="4" spans="3:22">
-      <c r="O4" s="53" t="s">
+      <c r="O4" s="54" t="s">
         <v>255</v>
       </c>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
+      <c r="P4" s="55"/>
+      <c r="Q4" s="55"/>
+      <c r="R4" s="55"/>
+      <c r="S4" s="55"/>
+      <c r="T4" s="55"/>
+      <c r="U4" s="55"/>
     </row>
     <row r="5" spans="3:22">
       <c r="C5" s="1" t="s">
@@ -11298,6 +11516,9 @@
       <c r="D10" s="1" t="s">
         <v>150</v>
       </c>
+      <c r="G10" t="s">
+        <v>497</v>
+      </c>
       <c r="L10" s="1">
         <v>5</v>
       </c>
@@ -11340,6 +11561,9 @@
       <c r="D13" s="1" t="s">
         <v>153</v>
       </c>
+      <c r="G13" t="s">
+        <v>498</v>
+      </c>
       <c r="L13" s="1">
         <v>8</v>
       </c>
@@ -11354,6 +11578,9 @@
       <c r="D14" s="2" t="s">
         <v>154</v>
       </c>
+      <c r="G14" t="s">
+        <v>501</v>
+      </c>
       <c r="L14" s="1">
         <v>9</v>
       </c>
@@ -11571,7 +11798,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="33" spans="3:4">
+    <row r="33" spans="3:7">
       <c r="C33" s="1">
         <v>28</v>
       </c>
@@ -11579,7 +11806,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="34" spans="3:4">
+    <row r="34" spans="3:7">
       <c r="C34" s="1">
         <v>29</v>
       </c>
@@ -11587,7 +11814,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="3:4">
+    <row r="35" spans="3:7">
       <c r="C35" s="1">
         <v>30</v>
       </c>
@@ -11595,7 +11822,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="36" spans="3:4">
+    <row r="36" spans="3:7">
       <c r="C36" s="1">
         <v>31</v>
       </c>
@@ -11603,7 +11830,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="37" spans="3:4">
+    <row r="37" spans="3:7">
       <c r="C37" s="1">
         <v>32</v>
       </c>
@@ -11611,7 +11838,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="38" spans="3:4">
+    <row r="38" spans="3:7">
       <c r="C38" s="1">
         <v>33</v>
       </c>
@@ -11619,52 +11846,58 @@
         <v>298</v>
       </c>
     </row>
-    <row r="39" spans="3:4">
+    <row r="39" spans="3:7">
       <c r="C39" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="3:4">
+      <c r="D39" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="G39" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7">
       <c r="C40" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="3:4">
+    <row r="41" spans="3:7">
       <c r="C41" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="3:4">
+    <row r="42" spans="3:7">
       <c r="C42" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="3:4">
+    <row r="43" spans="3:7">
       <c r="C43" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="3:4">
+    <row r="44" spans="3:7">
       <c r="C44" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="3:4">
+    <row r="45" spans="3:7">
       <c r="C45" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="3:4">
+    <row r="46" spans="3:7">
       <c r="C46" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="3:4">
+    <row r="47" spans="3:7">
       <c r="C47" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="3:4">
+    <row r="48" spans="3:7">
       <c r="C48" s="1">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Implementing upgrade effects, till Chestnut now
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FDF369-9951-497E-9319-4D7AE6795881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C65ED08-08F3-4A5A-9BA9-5D5853900B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,24 +24,11 @@
     <sheet name="Fishing" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="823">
   <si>
     <t xml:space="preserve">Tier </t>
   </si>
@@ -2513,6 +2500,12 @@
   </si>
   <si>
     <t>wood per second 2% increase per level</t>
+  </si>
+  <si>
+    <t>Better wood price +10</t>
+  </si>
+  <si>
+    <t>levels effects 3%</t>
   </si>
 </sst>
 </file>
@@ -2610,7 +2603,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="45">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2873,6 +2866,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3191,13 +3190,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="31" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="32" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3249,7 +3241,14 @@
     <xf numFmtId="0" fontId="2" fillId="44" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4956,8 +4955,8 @@
   </sheetPr>
   <dimension ref="A1:X276"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="B78" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5058,19 +5057,19 @@
       <c r="K5" s="45" t="s">
         <v>432</v>
       </c>
-      <c r="M5" s="61" t="s">
+      <c r="M5" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="N5" s="61"/>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="61"/>
-      <c r="R5" s="61"/>
-      <c r="S5" s="61"/>
-      <c r="T5" s="61"/>
-      <c r="U5" s="61"/>
-      <c r="V5" s="61"/>
-      <c r="W5" s="61"/>
+      <c r="N5" s="110"/>
+      <c r="O5" s="110"/>
+      <c r="P5" s="110"/>
+      <c r="Q5" s="110"/>
+      <c r="R5" s="110"/>
+      <c r="S5" s="110"/>
+      <c r="T5" s="110"/>
+      <c r="U5" s="110"/>
+      <c r="V5" s="110"/>
+      <c r="W5" s="110"/>
     </row>
     <row r="6" spans="1:23" ht="13.5" thickBot="1">
       <c r="A6" s="35" t="s">
@@ -5085,10 +5084,10 @@
       <c r="D6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E6" s="70">
+      <c r="E6" s="67">
         <v>1</v>
       </c>
-      <c r="F6" s="108" t="s">
+      <c r="F6" s="105" t="s">
         <v>817</v>
       </c>
       <c r="G6" s="45" t="s">
@@ -5154,10 +5153,10 @@
       <c r="D7">
         <v>1.3</v>
       </c>
-      <c r="E7" s="70">
+      <c r="E7" s="67">
         <v>2</v>
       </c>
-      <c r="F7" s="68" t="s">
+      <c r="F7" s="65" t="s">
         <v>400</v>
       </c>
       <c r="G7" s="45" t="s">
@@ -5226,10 +5225,10 @@
       <c r="D8">
         <v>3.16</v>
       </c>
-      <c r="E8" s="70">
+      <c r="E8" s="67">
         <v>3</v>
       </c>
-      <c r="F8" s="78" t="s">
+      <c r="F8" s="75" t="s">
         <v>537</v>
       </c>
       <c r="G8" s="45" t="s">
@@ -5297,10 +5296,10 @@
       <c r="D9">
         <v>1.1599999999999999</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="67">
         <v>4</v>
       </c>
-      <c r="F9" s="108" t="s">
+      <c r="F9" s="105" t="s">
         <v>818</v>
       </c>
       <c r="G9" s="45" t="s">
@@ -5365,10 +5364,10 @@
       <c r="D10">
         <v>4.2</v>
       </c>
-      <c r="E10" s="70">
+      <c r="E10" s="67">
         <v>5</v>
       </c>
-      <c r="F10" s="107" t="s">
+      <c r="F10" s="104" t="s">
         <v>430</v>
       </c>
       <c r="G10" s="45" t="s">
@@ -5420,10 +5419,10 @@
       <c r="D11">
         <v>2.1</v>
       </c>
-      <c r="E11" s="70">
+      <c r="E11" s="67">
         <v>6</v>
       </c>
-      <c r="F11" s="78" t="s">
+      <c r="F11" s="75" t="s">
         <v>819</v>
       </c>
       <c r="H11">
@@ -5479,10 +5478,10 @@
       <c r="D12">
         <v>2.16</v>
       </c>
-      <c r="E12" s="70">
+      <c r="E12" s="67">
         <v>7</v>
       </c>
-      <c r="F12" s="105" t="s">
+      <c r="F12" s="102" t="s">
         <v>662</v>
       </c>
       <c r="H12">
@@ -5533,10 +5532,10 @@
       <c r="D13">
         <v>7.4</v>
       </c>
-      <c r="E13" s="70">
+      <c r="E13" s="67">
         <v>8</v>
       </c>
-      <c r="F13" s="68" t="s">
+      <c r="F13" s="65" t="s">
         <v>747</v>
       </c>
       <c r="H13" s="1">
@@ -5577,10 +5576,10 @@
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="70">
+      <c r="E14" s="67">
         <v>9</v>
       </c>
-      <c r="F14" s="100" t="s">
+      <c r="F14" s="97" t="s">
         <v>715</v>
       </c>
       <c r="M14" s="27" t="s">
@@ -5611,10 +5610,10 @@
       <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="70">
+      <c r="E15" s="67">
         <v>10</v>
       </c>
-      <c r="F15" s="101" t="s">
+      <c r="F15" s="98" t="s">
         <v>761</v>
       </c>
       <c r="M15" s="40" t="s">
@@ -5645,10 +5644,10 @@
       <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="70">
+      <c r="E16" s="67">
         <v>11</v>
       </c>
-      <c r="F16" s="102" t="s">
+      <c r="F16" s="99" t="s">
         <v>743</v>
       </c>
       <c r="M16" s="40" t="s">
@@ -5679,10 +5678,10 @@
       <c r="C17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="70">
+      <c r="E17" s="67">
         <v>12</v>
       </c>
-      <c r="F17" s="100" t="s">
+      <c r="F17" s="97" t="s">
         <v>729</v>
       </c>
       <c r="G17" t="e">
@@ -5715,10 +5714,10 @@
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="70">
+      <c r="E18" s="67">
         <v>13</v>
       </c>
-      <c r="F18" s="78" t="s">
+      <c r="F18" s="75" t="s">
         <v>595</v>
       </c>
       <c r="M18" s="40"/>
@@ -5750,10 +5749,10 @@
       <c r="D19">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E19" s="70">
+      <c r="E19" s="67">
         <v>14</v>
       </c>
-      <c r="F19" s="77" t="s">
+      <c r="F19" s="74" t="s">
         <v>623</v>
       </c>
       <c r="M19" s="40"/>
@@ -5778,10 +5777,10 @@
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="70">
+      <c r="E20" s="67">
         <v>15</v>
       </c>
-      <c r="F20" s="108" t="s">
+      <c r="F20" s="105" t="s">
         <v>820</v>
       </c>
       <c r="M20" s="35"/>
@@ -5809,10 +5808,10 @@
       <c r="D21">
         <v>3.21</v>
       </c>
-      <c r="E21" s="70">
+      <c r="E21" s="67">
         <v>16</v>
       </c>
-      <c r="F21" s="68" t="s">
+      <c r="F21" s="65" t="s">
         <v>464</v>
       </c>
       <c r="M21" s="40"/>
@@ -5837,10 +5836,10 @@
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="70">
+      <c r="E22" s="67">
         <v>17</v>
       </c>
-      <c r="F22" s="77" t="s">
+      <c r="F22" s="74" t="s">
         <v>630</v>
       </c>
       <c r="M22" s="40"/>
@@ -5865,10 +5864,10 @@
       <c r="C23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="70">
+      <c r="E23" s="67">
         <v>18</v>
       </c>
-      <c r="F23" s="103" t="s">
+      <c r="F23" s="100" t="s">
         <v>682</v>
       </c>
       <c r="H23" s="44">
@@ -5896,19 +5895,19 @@
     </row>
     <row r="24" spans="1:23" ht="12.75">
       <c r="A24" s="1"/>
-      <c r="B24" s="109">
+      <c r="B24" s="106">
         <v>19</v>
       </c>
-      <c r="C24" s="110" t="s">
+      <c r="C24" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="111">
+      <c r="D24" s="108">
         <v>1.2</v>
       </c>
-      <c r="E24" s="109">
+      <c r="E24" s="106">
         <v>1</v>
       </c>
-      <c r="F24" s="108" t="s">
+      <c r="F24" s="105" t="s">
         <v>434</v>
       </c>
       <c r="H24">
@@ -5948,7 +5947,7 @@
       <c r="E25" s="1">
         <v>2</v>
       </c>
-      <c r="F25" s="68" t="s">
+      <c r="F25" s="65" t="s">
         <v>435</v>
       </c>
       <c r="H25">
@@ -5987,7 +5986,7 @@
       <c r="E26" s="1">
         <v>3</v>
       </c>
-      <c r="F26" s="78" t="s">
+      <c r="F26" s="75" t="s">
         <v>538</v>
       </c>
       <c r="H26">
@@ -6026,7 +6025,7 @@
       <c r="E27" s="1">
         <v>4</v>
       </c>
-      <c r="F27" s="68" t="s">
+      <c r="F27" s="65" t="s">
         <v>759</v>
       </c>
       <c r="H27">
@@ -6059,10 +6058,10 @@
       <c r="C28" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="113">
         <v>5</v>
       </c>
-      <c r="F28" s="108" t="s">
+      <c r="F28" s="105" t="s">
         <v>463</v>
       </c>
       <c r="H28">
@@ -6098,7 +6097,7 @@
       <c r="E29" s="1">
         <v>6</v>
       </c>
-      <c r="F29" s="107" t="s">
+      <c r="F29" s="104" t="s">
         <v>92</v>
       </c>
       <c r="H29">
@@ -6129,8 +6128,8 @@
       <c r="E30" s="1">
         <v>7</v>
       </c>
-      <c r="F30" s="108" t="s">
-        <v>429</v>
+      <c r="F30" s="105" t="s">
+        <v>818</v>
       </c>
       <c r="H30">
         <v>1200</v>
@@ -6160,7 +6159,7 @@
       <c r="E31" s="1">
         <v>8</v>
       </c>
-      <c r="F31" s="68" t="s">
+      <c r="F31" s="65" t="s">
         <v>464</v>
       </c>
       <c r="H31">
@@ -6186,7 +6185,7 @@
       <c r="E32" s="1">
         <v>9</v>
       </c>
-      <c r="F32" s="78" t="s">
+      <c r="F32" s="75" t="s">
         <v>600</v>
       </c>
       <c r="H32">
@@ -6206,10 +6205,10 @@
       <c r="E33" s="1">
         <v>10</v>
       </c>
-      <c r="F33" s="105" t="s">
+      <c r="F33" s="102" t="s">
         <v>658</v>
       </c>
-      <c r="O33" s="82" t="s">
+      <c r="O33" s="79" t="s">
         <v>756</v>
       </c>
     </row>
@@ -6223,7 +6222,7 @@
       <c r="E34" s="1">
         <v>11</v>
       </c>
-      <c r="F34" s="77" t="s">
+      <c r="F34" s="74" t="s">
         <v>624</v>
       </c>
       <c r="L34" s="40"/>
@@ -6251,7 +6250,7 @@
       <c r="E35" s="1">
         <v>12</v>
       </c>
-      <c r="F35" s="78" t="s">
+      <c r="F35" s="75" t="s">
         <v>757</v>
       </c>
       <c r="L35" s="46" t="s">
@@ -6304,7 +6303,7 @@
       <c r="E36" s="1">
         <v>13</v>
       </c>
-      <c r="F36" s="100" t="s">
+      <c r="F36" s="97" t="s">
         <v>718</v>
       </c>
       <c r="G36" s="1" t="s">
@@ -6314,40 +6313,40 @@
       <c r="L36" s="40">
         <v>1</v>
       </c>
-      <c r="M36" s="65" t="s">
+      <c r="M36" s="62" t="s">
         <v>395</v>
       </c>
-      <c r="N36" s="75" t="s">
+      <c r="N36" s="72" t="s">
         <v>537</v>
       </c>
-      <c r="O36" s="76" t="s">
+      <c r="O36" s="73" t="s">
         <v>552</v>
       </c>
-      <c r="P36" s="80" t="s">
+      <c r="P36" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="Q36" s="69" t="s">
+      <c r="Q36" s="66" t="s">
         <v>623</v>
       </c>
-      <c r="R36" s="85" t="s">
+      <c r="R36" s="82" t="s">
         <v>566</v>
       </c>
-      <c r="S36" s="88" t="s">
+      <c r="S36" s="85" t="s">
         <v>658</v>
       </c>
-      <c r="T36" s="94" t="s">
+      <c r="T36" s="91" t="s">
         <v>673</v>
       </c>
-      <c r="U36" s="99" t="s">
+      <c r="U36" s="96" t="s">
         <v>694</v>
       </c>
-      <c r="V36" s="98" t="s">
+      <c r="V36" s="95" t="s">
         <v>703</v>
       </c>
-      <c r="W36" s="96" t="s">
+      <c r="W36" s="93" t="s">
         <v>714</v>
       </c>
-      <c r="X36" s="93" t="s">
+      <c r="X36" s="90" t="s">
         <v>746</v>
       </c>
     </row>
@@ -6361,7 +6360,7 @@
       <c r="E37" s="1">
         <v>14</v>
       </c>
-      <c r="F37" s="77" t="s">
+      <c r="F37" s="74" t="s">
         <v>632</v>
       </c>
       <c r="G37" s="45" t="s">
@@ -6372,40 +6371,40 @@
       <c r="L37" s="40">
         <v>2</v>
       </c>
-      <c r="M37" s="71" t="s">
+      <c r="M37" s="68" t="s">
         <v>396</v>
       </c>
-      <c r="N37" s="66" t="s">
+      <c r="N37" s="63" t="s">
         <v>538</v>
       </c>
-      <c r="O37" s="67" t="s">
+      <c r="O37" s="64" t="s">
         <v>553</v>
       </c>
-      <c r="P37" s="81" t="s">
+      <c r="P37" s="78" t="s">
         <v>562</v>
       </c>
-      <c r="Q37" s="86" t="s">
+      <c r="Q37" s="83" t="s">
         <v>624</v>
       </c>
-      <c r="R37" s="87" t="s">
+      <c r="R37" s="84" t="s">
         <v>761</v>
       </c>
-      <c r="S37" s="79" t="s">
+      <c r="S37" s="76" t="s">
         <v>659</v>
       </c>
-      <c r="T37" s="89" t="s">
+      <c r="T37" s="86" t="s">
         <v>674</v>
       </c>
-      <c r="U37" s="90" t="s">
+      <c r="U37" s="87" t="s">
         <v>695</v>
       </c>
-      <c r="V37" s="91" t="s">
+      <c r="V37" s="88" t="s">
         <v>704</v>
       </c>
-      <c r="W37" s="92" t="s">
+      <c r="W37" s="89" t="s">
         <v>715</v>
       </c>
-      <c r="X37" s="93" t="s">
+      <c r="X37" s="90" t="s">
         <v>745</v>
       </c>
     </row>
@@ -6419,7 +6418,7 @@
       <c r="E38" s="1">
         <v>15</v>
       </c>
-      <c r="F38" s="103" t="s">
+      <c r="F38" s="100" t="s">
         <v>690</v>
       </c>
       <c r="G38" t="s">
@@ -6429,40 +6428,40 @@
       <c r="L38" s="40">
         <v>3</v>
       </c>
-      <c r="M38" s="71" t="s">
+      <c r="M38" s="68" t="s">
         <v>505</v>
       </c>
-      <c r="N38" s="66" t="s">
+      <c r="N38" s="63" t="s">
         <v>539</v>
       </c>
-      <c r="O38" s="67" t="s">
+      <c r="O38" s="64" t="s">
         <v>554</v>
       </c>
-      <c r="P38" s="81" t="s">
+      <c r="P38" s="78" t="s">
         <v>621</v>
       </c>
-      <c r="Q38" s="86" t="s">
+      <c r="Q38" s="83" t="s">
         <v>625</v>
       </c>
-      <c r="R38" s="87" t="s">
+      <c r="R38" s="84" t="s">
         <v>656</v>
       </c>
-      <c r="S38" s="79" t="s">
+      <c r="S38" s="76" t="s">
         <v>661</v>
       </c>
-      <c r="T38" s="95" t="s">
+      <c r="T38" s="92" t="s">
         <v>675</v>
       </c>
-      <c r="U38" s="90" t="s">
+      <c r="U38" s="87" t="s">
         <v>696</v>
       </c>
-      <c r="V38" s="91" t="s">
+      <c r="V38" s="88" t="s">
         <v>705</v>
       </c>
-      <c r="W38" s="92" t="s">
+      <c r="W38" s="89" t="s">
         <v>716</v>
       </c>
-      <c r="X38" s="93" t="s">
+      <c r="X38" s="90" t="s">
         <v>744</v>
       </c>
     </row>
@@ -6476,7 +6475,7 @@
       <c r="E39" s="1">
         <v>16</v>
       </c>
-      <c r="F39" s="104" t="s">
+      <c r="F39" s="101" t="s">
         <v>695</v>
       </c>
       <c r="G39" s="1" t="s">
@@ -6487,40 +6486,40 @@
       <c r="L39" s="40">
         <v>4</v>
       </c>
-      <c r="M39" s="71" t="s">
+      <c r="M39" s="68" t="s">
         <v>506</v>
       </c>
-      <c r="N39" s="66" t="s">
+      <c r="N39" s="63" t="s">
         <v>540</v>
       </c>
-      <c r="O39" s="67" t="s">
+      <c r="O39" s="64" t="s">
         <v>555</v>
       </c>
-      <c r="P39" s="81" t="s">
+      <c r="P39" s="78" t="s">
         <v>622</v>
       </c>
-      <c r="Q39" s="86" t="s">
+      <c r="Q39" s="83" t="s">
         <v>649</v>
       </c>
-      <c r="R39" s="87" t="s">
+      <c r="R39" s="84" t="s">
         <v>657</v>
       </c>
-      <c r="S39" s="79" t="s">
+      <c r="S39" s="76" t="s">
         <v>662</v>
       </c>
-      <c r="T39" s="89" t="s">
+      <c r="T39" s="86" t="s">
         <v>678</v>
       </c>
-      <c r="U39" s="90" t="s">
+      <c r="U39" s="87" t="s">
         <v>697</v>
       </c>
-      <c r="V39" s="91" t="s">
+      <c r="V39" s="88" t="s">
         <v>708</v>
       </c>
-      <c r="W39" s="92" t="s">
+      <c r="W39" s="89" t="s">
         <v>717</v>
       </c>
-      <c r="X39" s="97" t="s">
+      <c r="X39" s="94" t="s">
         <v>742</v>
       </c>
     </row>
@@ -6537,7 +6536,7 @@
       <c r="E40" s="1">
         <v>17</v>
       </c>
-      <c r="F40" s="103" t="s">
+      <c r="F40" s="100" t="s">
         <v>675</v>
       </c>
       <c r="G40" t="s">
@@ -6546,38 +6545,38 @@
       <c r="L40" s="40">
         <v>5</v>
       </c>
-      <c r="M40" s="72" t="s">
+      <c r="M40" s="69" t="s">
         <v>507</v>
       </c>
-      <c r="N40" s="66" t="s">
+      <c r="N40" s="63" t="s">
         <v>541</v>
       </c>
-      <c r="O40" s="67" t="s">
+      <c r="O40" s="64" t="s">
         <v>556</v>
       </c>
       <c r="P40" s="57" t="s">
         <v>119</v>
       </c>
-      <c r="Q40" s="86" t="s">
+      <c r="Q40" s="83" t="s">
         <v>650</v>
       </c>
       <c r="R40" s="57"/>
-      <c r="S40" s="79" t="s">
+      <c r="S40" s="76" t="s">
         <v>663</v>
       </c>
-      <c r="T40" s="89" t="s">
+      <c r="T40" s="86" t="s">
         <v>679</v>
       </c>
-      <c r="U40" s="90" t="s">
+      <c r="U40" s="87" t="s">
         <v>698</v>
       </c>
-      <c r="V40" s="91" t="s">
+      <c r="V40" s="88" t="s">
         <v>709</v>
       </c>
-      <c r="W40" s="92" t="s">
+      <c r="W40" s="89" t="s">
         <v>718</v>
       </c>
-      <c r="X40" s="97" t="s">
+      <c r="X40" s="94" t="s">
         <v>743</v>
       </c>
     </row>
@@ -6594,7 +6593,7 @@
       <c r="E41" s="1">
         <v>18</v>
       </c>
-      <c r="F41" s="100" t="s">
+      <c r="F41" s="97" t="s">
         <v>723</v>
       </c>
       <c r="G41" s="1"/>
@@ -6602,35 +6601,35 @@
       <c r="L41" s="40">
         <v>6</v>
       </c>
-      <c r="M41" s="71" t="s">
+      <c r="M41" s="68" t="s">
         <v>508</v>
       </c>
-      <c r="N41" s="66" t="s">
+      <c r="N41" s="63" t="s">
         <v>542</v>
       </c>
-      <c r="O41" s="67" t="s">
+      <c r="O41" s="64" t="s">
         <v>557</v>
       </c>
       <c r="P41" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="Q41" s="86" t="s">
+      <c r="Q41" s="83" t="s">
         <v>626</v>
       </c>
       <c r="R41" s="57"/>
-      <c r="S41" s="79" t="s">
+      <c r="S41" s="76" t="s">
         <v>660</v>
       </c>
-      <c r="T41" s="89" t="s">
+      <c r="T41" s="86" t="s">
         <v>680</v>
       </c>
-      <c r="U41" s="90" t="s">
+      <c r="U41" s="87" t="s">
         <v>699</v>
       </c>
-      <c r="V41" s="91" t="s">
+      <c r="V41" s="88" t="s">
         <v>710</v>
       </c>
-      <c r="W41" s="92" t="s">
+      <c r="W41" s="89" t="s">
         <v>719</v>
       </c>
       <c r="X41" s="55"/>
@@ -6639,17 +6638,17 @@
       <c r="A42">
         <v>7</v>
       </c>
-      <c r="B42" s="109">
+      <c r="B42" s="106">
         <v>37</v>
       </c>
-      <c r="C42" s="110" t="s">
+      <c r="C42" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="111"/>
-      <c r="E42" s="109">
+      <c r="D42" s="108"/>
+      <c r="E42" s="106">
         <v>1</v>
       </c>
-      <c r="F42" s="108" t="s">
+      <c r="F42" s="105" t="s">
         <v>505</v>
       </c>
       <c r="G42" s="1"/>
@@ -6659,35 +6658,35 @@
       <c r="L42" s="40">
         <v>7</v>
       </c>
-      <c r="M42" s="71" t="s">
+      <c r="M42" s="68" t="s">
         <v>509</v>
       </c>
-      <c r="N42" s="66" t="s">
+      <c r="N42" s="63" t="s">
         <v>543</v>
       </c>
-      <c r="O42" s="67" t="s">
+      <c r="O42" s="64" t="s">
         <v>558</v>
       </c>
       <c r="P42" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="Q42" s="86" t="s">
+      <c r="Q42" s="83" t="s">
         <v>627</v>
       </c>
       <c r="R42" s="57"/>
-      <c r="S42" s="79" t="s">
+      <c r="S42" s="76" t="s">
         <v>664</v>
       </c>
-      <c r="T42" s="89" t="s">
+      <c r="T42" s="86" t="s">
         <v>681</v>
       </c>
-      <c r="U42" s="90" t="s">
+      <c r="U42" s="87" t="s">
         <v>700</v>
       </c>
-      <c r="V42" s="91" t="s">
+      <c r="V42" s="88" t="s">
         <v>711</v>
       </c>
-      <c r="W42" s="92" t="s">
+      <c r="W42" s="89" t="s">
         <v>720</v>
       </c>
       <c r="X42" s="55"/>
@@ -6702,45 +6701,45 @@
       <c r="C43" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="70">
+      <c r="E43" s="67">
         <v>2</v>
       </c>
-      <c r="F43" s="68" t="s">
+      <c r="F43" s="65" t="s">
         <v>554</v>
       </c>
       <c r="G43" s="1"/>
       <c r="L43" s="40">
         <v>8</v>
       </c>
-      <c r="M43" s="71" t="s">
+      <c r="M43" s="68" t="s">
         <v>510</v>
       </c>
-      <c r="N43" s="66" t="s">
+      <c r="N43" s="63" t="s">
         <v>544</v>
       </c>
-      <c r="O43" s="67" t="s">
+      <c r="O43" s="64" t="s">
         <v>559</v>
       </c>
       <c r="P43" s="57" t="s">
         <v>359</v>
       </c>
-      <c r="Q43" s="86" t="s">
+      <c r="Q43" s="83" t="s">
         <v>628</v>
       </c>
       <c r="R43" s="57"/>
-      <c r="S43" s="79" t="s">
+      <c r="S43" s="76" t="s">
         <v>665</v>
       </c>
-      <c r="T43" s="89" t="s">
+      <c r="T43" s="86" t="s">
         <v>682</v>
       </c>
-      <c r="U43" s="90" t="s">
+      <c r="U43" s="87" t="s">
         <v>701</v>
       </c>
-      <c r="V43" s="91" t="s">
+      <c r="V43" s="88" t="s">
         <v>712</v>
       </c>
-      <c r="W43" s="92" t="s">
+      <c r="W43" s="89" t="s">
         <v>721</v>
       </c>
       <c r="X43" s="55"/>
@@ -6755,45 +6754,45 @@
       <c r="C44" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E44" s="70">
+      <c r="E44" s="67">
         <v>3</v>
       </c>
-      <c r="F44" s="78" t="s">
+      <c r="F44" s="75" t="s">
         <v>539</v>
       </c>
       <c r="G44" s="1"/>
       <c r="L44" s="40">
         <v>9</v>
       </c>
-      <c r="M44" s="72" t="s">
+      <c r="M44" s="69" t="s">
         <v>511</v>
       </c>
-      <c r="N44" s="66" t="s">
+      <c r="N44" s="63" t="s">
         <v>545</v>
       </c>
-      <c r="O44" s="67" t="s">
+      <c r="O44" s="64" t="s">
         <v>560</v>
       </c>
       <c r="P44" s="57" t="s">
         <v>360</v>
       </c>
-      <c r="Q44" s="86" t="s">
+      <c r="Q44" s="83" t="s">
         <v>651</v>
       </c>
       <c r="R44" s="57"/>
-      <c r="S44" s="79" t="s">
+      <c r="S44" s="76" t="s">
         <v>666</v>
       </c>
-      <c r="T44" s="95" t="s">
+      <c r="T44" s="92" t="s">
         <v>686</v>
       </c>
-      <c r="U44" s="90" t="s">
+      <c r="U44" s="87" t="s">
         <v>702</v>
       </c>
-      <c r="V44" s="91" t="s">
+      <c r="V44" s="88" t="s">
         <v>713</v>
       </c>
-      <c r="W44" s="92" t="s">
+      <c r="W44" s="89" t="s">
         <v>722</v>
       </c>
       <c r="X44" s="55"/>
@@ -6811,43 +6810,43 @@
       <c r="D45">
         <v>1.3</v>
       </c>
-      <c r="E45" s="70">
+      <c r="E45" s="67">
         <v>4</v>
       </c>
-      <c r="F45" s="78" t="s">
+      <c r="F45" s="75" t="s">
         <v>584</v>
       </c>
       <c r="G45" s="1"/>
       <c r="L45" s="40">
         <v>10</v>
       </c>
-      <c r="M45" s="71" t="s">
+      <c r="M45" s="68" t="s">
         <v>512</v>
       </c>
-      <c r="N45" s="66" t="s">
+      <c r="N45" s="63" t="s">
         <v>546</v>
       </c>
-      <c r="O45" s="67" t="s">
+      <c r="O45" s="64" t="s">
         <v>561</v>
       </c>
       <c r="P45" s="57" t="s">
         <v>366</v>
       </c>
-      <c r="Q45" s="86" t="s">
+      <c r="Q45" s="83" t="s">
         <v>654</v>
       </c>
       <c r="R45" s="57"/>
-      <c r="S45" s="79" t="s">
+      <c r="S45" s="76" t="s">
         <v>667</v>
       </c>
-      <c r="T45" s="89" t="s">
+      <c r="T45" s="86" t="s">
         <v>683</v>
       </c>
       <c r="U45" s="57"/>
-      <c r="V45" s="91" t="s">
+      <c r="V45" s="88" t="s">
         <v>706</v>
       </c>
-      <c r="W45" s="92" t="s">
+      <c r="W45" s="89" t="s">
         <v>723</v>
       </c>
       <c r="X45" s="59"/>
@@ -6862,43 +6861,43 @@
       <c r="C46" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="70">
+      <c r="E46" s="67">
         <v>5</v>
       </c>
-      <c r="F46" s="108" t="s">
+      <c r="F46" s="105" t="s">
         <v>576</v>
       </c>
       <c r="G46" s="1"/>
       <c r="L46" s="40">
         <v>11</v>
       </c>
-      <c r="M46" s="71" t="s">
+      <c r="M46" s="68" t="s">
         <v>513</v>
       </c>
-      <c r="N46" s="66" t="s">
+      <c r="N46" s="63" t="s">
         <v>547</v>
       </c>
-      <c r="O46" s="67" t="s">
+      <c r="O46" s="64" t="s">
         <v>750</v>
       </c>
       <c r="P46" s="55" t="s">
         <v>367</v>
       </c>
-      <c r="Q46" s="86" t="s">
+      <c r="Q46" s="83" t="s">
         <v>655</v>
       </c>
       <c r="R46" s="55"/>
-      <c r="S46" s="79" t="s">
+      <c r="S46" s="76" t="s">
         <v>672</v>
       </c>
-      <c r="T46" s="89" t="s">
+      <c r="T46" s="86" t="s">
         <v>684</v>
       </c>
       <c r="U46" s="55"/>
-      <c r="V46" s="91" t="s">
+      <c r="V46" s="88" t="s">
         <v>707</v>
       </c>
-      <c r="W46" s="92" t="s">
+      <c r="W46" s="89" t="s">
         <v>724</v>
       </c>
       <c r="X46" s="55"/>
@@ -6913,43 +6912,43 @@
       <c r="C47" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E47" s="70">
+      <c r="E47" s="67">
         <v>6</v>
       </c>
-      <c r="F47" s="68" t="s">
+      <c r="F47" s="65" t="s">
         <v>760</v>
       </c>
       <c r="G47" s="1"/>
       <c r="L47" s="40">
         <v>12</v>
       </c>
-      <c r="M47" s="71" t="s">
+      <c r="M47" s="68" t="s">
         <v>514</v>
       </c>
-      <c r="N47" s="66" t="s">
+      <c r="N47" s="63" t="s">
         <v>548</v>
       </c>
-      <c r="O47" s="67" t="s">
+      <c r="O47" s="64" t="s">
         <v>751</v>
       </c>
       <c r="P47" s="55" t="s">
         <v>368</v>
       </c>
-      <c r="Q47" s="86" t="s">
+      <c r="Q47" s="83" t="s">
         <v>629</v>
       </c>
       <c r="R47" s="55"/>
-      <c r="S47" s="79" t="s">
+      <c r="S47" s="76" t="s">
         <v>670</v>
       </c>
-      <c r="T47" s="89" t="s">
+      <c r="T47" s="86" t="s">
         <v>685</v>
       </c>
       <c r="U47" s="55"/>
-      <c r="V47" s="91" t="s">
+      <c r="V47" s="88" t="s">
         <v>763</v>
       </c>
-      <c r="W47" s="92" t="s">
+      <c r="W47" s="89" t="s">
         <v>725</v>
       </c>
       <c r="X47" s="55"/>
@@ -6964,41 +6963,41 @@
       <c r="C48" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E48" s="70">
+      <c r="E48" s="67">
         <v>7</v>
       </c>
-      <c r="F48" s="105" t="s">
+      <c r="F48" s="102" t="s">
         <v>667</v>
       </c>
       <c r="G48" s="1"/>
       <c r="L48" s="40">
         <v>13</v>
       </c>
-      <c r="M48" s="72" t="s">
+      <c r="M48" s="69" t="s">
         <v>515</v>
       </c>
-      <c r="N48" s="66" t="s">
+      <c r="N48" s="63" t="s">
         <v>549</v>
       </c>
-      <c r="O48" s="67" t="s">
+      <c r="O48" s="64" t="s">
         <v>752</v>
       </c>
       <c r="P48" s="57" t="s">
         <v>369</v>
       </c>
-      <c r="Q48" s="86" t="s">
+      <c r="Q48" s="83" t="s">
         <v>630</v>
       </c>
       <c r="R48" s="55"/>
-      <c r="S48" s="79" t="s">
+      <c r="S48" s="76" t="s">
         <v>669</v>
       </c>
-      <c r="T48" s="89" t="s">
+      <c r="T48" s="86" t="s">
         <v>687</v>
       </c>
       <c r="U48" s="55"/>
       <c r="V48" s="55"/>
-      <c r="W48" s="92" t="s">
+      <c r="W48" s="89" t="s">
         <v>726</v>
       </c>
       <c r="X48" s="55"/>
@@ -7013,41 +7012,41 @@
       <c r="C49" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="70">
+      <c r="E49" s="67">
         <v>8</v>
       </c>
-      <c r="F49" s="78" t="s">
+      <c r="F49" s="75" t="s">
         <v>608</v>
       </c>
       <c r="G49" s="1"/>
       <c r="L49" s="40">
         <v>14</v>
       </c>
-      <c r="M49" s="71" t="s">
+      <c r="M49" s="68" t="s">
         <v>516</v>
       </c>
-      <c r="N49" s="66" t="s">
+      <c r="N49" s="63" t="s">
         <v>550</v>
       </c>
-      <c r="O49" s="67" t="s">
+      <c r="O49" s="64" t="s">
         <v>753</v>
       </c>
       <c r="P49" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="Q49" s="86" t="s">
+      <c r="Q49" s="83" t="s">
         <v>644</v>
       </c>
       <c r="R49" s="55"/>
-      <c r="S49" s="79" t="s">
+      <c r="S49" s="76" t="s">
         <v>671</v>
       </c>
-      <c r="T49" s="89" t="s">
+      <c r="T49" s="86" t="s">
         <v>688</v>
       </c>
       <c r="U49" s="55"/>
       <c r="V49" s="55"/>
-      <c r="W49" s="92" t="s">
+      <c r="W49" s="89" t="s">
         <v>727</v>
       </c>
       <c r="X49" s="55"/>
@@ -7062,41 +7061,41 @@
       <c r="C50" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E50" s="70">
+      <c r="E50" s="67">
         <v>9</v>
       </c>
-      <c r="F50" s="100" t="s">
+      <c r="F50" s="97" t="s">
         <v>720</v>
       </c>
       <c r="G50" s="1"/>
       <c r="L50" s="40">
         <v>15</v>
       </c>
-      <c r="M50" s="71" t="s">
+      <c r="M50" s="68" t="s">
         <v>517</v>
       </c>
-      <c r="N50" s="66" t="s">
+      <c r="N50" s="63" t="s">
         <v>551</v>
       </c>
-      <c r="O50" s="67" t="s">
+      <c r="O50" s="64" t="s">
         <v>754</v>
       </c>
       <c r="P50" s="57" t="s">
         <v>371</v>
       </c>
-      <c r="Q50" s="86" t="s">
+      <c r="Q50" s="83" t="s">
         <v>645</v>
       </c>
       <c r="R50" s="55"/>
-      <c r="S50" s="79" t="s">
+      <c r="S50" s="76" t="s">
         <v>668</v>
       </c>
-      <c r="T50" s="89" t="s">
+      <c r="T50" s="86" t="s">
         <v>689</v>
       </c>
       <c r="U50" s="55"/>
       <c r="V50" s="55"/>
-      <c r="W50" s="92" t="s">
+      <c r="W50" s="89" t="s">
         <v>728</v>
       </c>
       <c r="X50" s="55"/>
@@ -7111,38 +7110,38 @@
       <c r="C51" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E51" s="70">
+      <c r="E51" s="67">
         <v>10</v>
       </c>
-      <c r="F51" s="102" t="s">
+      <c r="F51" s="99" t="s">
         <v>746</v>
       </c>
       <c r="L51" s="40">
         <v>16</v>
       </c>
-      <c r="M51" s="73" t="s">
+      <c r="M51" s="70" t="s">
         <v>429</v>
       </c>
-      <c r="N51" s="66" t="s">
+      <c r="N51" s="63" t="s">
         <v>403</v>
       </c>
-      <c r="O51" s="67" t="s">
+      <c r="O51" s="64" t="s">
         <v>464</v>
       </c>
       <c r="P51" s="57" t="s">
         <v>372</v>
       </c>
-      <c r="Q51" s="86" t="s">
+      <c r="Q51" s="83" t="s">
         <v>646</v>
       </c>
       <c r="R51" s="55"/>
       <c r="S51" s="55"/>
-      <c r="T51" s="89" t="s">
+      <c r="T51" s="86" t="s">
         <v>690</v>
       </c>
       <c r="U51" s="55"/>
       <c r="V51" s="55"/>
-      <c r="W51" s="92" t="s">
+      <c r="W51" s="89" t="s">
         <v>729</v>
       </c>
       <c r="X51" s="55"/>
@@ -7157,10 +7156,10 @@
       <c r="C52" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E52" s="70">
+      <c r="E52" s="67">
         <v>11</v>
       </c>
-      <c r="F52" s="77" t="s">
+      <c r="F52" s="74" t="s">
         <v>635</v>
       </c>
       <c r="G52" s="1" t="s">
@@ -7181,29 +7180,29 @@
       <c r="L52" s="40">
         <v>17</v>
       </c>
-      <c r="M52" s="73" t="s">
+      <c r="M52" s="70" t="s">
         <v>429</v>
       </c>
-      <c r="N52" s="66" t="s">
+      <c r="N52" s="63" t="s">
         <v>403</v>
       </c>
-      <c r="O52" s="67" t="s">
+      <c r="O52" s="64" t="s">
         <v>464</v>
       </c>
       <c r="P52" s="57" t="s">
         <v>373</v>
       </c>
-      <c r="Q52" s="86" t="s">
+      <c r="Q52" s="83" t="s">
         <v>631</v>
       </c>
       <c r="R52" s="55"/>
       <c r="S52" s="55"/>
-      <c r="T52" s="89" t="s">
+      <c r="T52" s="86" t="s">
         <v>691</v>
       </c>
       <c r="U52" s="55"/>
       <c r="V52" s="55"/>
-      <c r="W52" s="92" t="s">
+      <c r="W52" s="89" t="s">
         <v>730</v>
       </c>
       <c r="X52" s="55"/>
@@ -7218,10 +7217,10 @@
       <c r="C53" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="70">
+      <c r="E53" s="67">
         <v>12</v>
       </c>
-      <c r="F53" s="78" t="s">
+      <c r="F53" s="75" t="s">
         <v>592</v>
       </c>
       <c r="G53" s="1" t="s">
@@ -7233,29 +7232,29 @@
       <c r="L53" s="40">
         <v>18</v>
       </c>
-      <c r="M53" s="73" t="s">
+      <c r="M53" s="70" t="s">
         <v>429</v>
       </c>
-      <c r="N53" s="66" t="s">
+      <c r="N53" s="63" t="s">
         <v>584</v>
       </c>
-      <c r="O53" s="67" t="s">
+      <c r="O53" s="64" t="s">
         <v>464</v>
       </c>
       <c r="P53" s="57" t="s">
         <v>374</v>
       </c>
-      <c r="Q53" s="86" t="s">
+      <c r="Q53" s="83" t="s">
         <v>632</v>
       </c>
       <c r="R53" s="55"/>
       <c r="S53" s="55"/>
-      <c r="T53" s="89" t="s">
+      <c r="T53" s="86" t="s">
         <v>692</v>
       </c>
       <c r="U53" s="55"/>
       <c r="V53" s="55"/>
-      <c r="W53" s="92" t="s">
+      <c r="W53" s="89" t="s">
         <v>731</v>
       </c>
       <c r="X53" s="55"/>
@@ -7270,10 +7269,10 @@
       <c r="C54" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="70">
+      <c r="E54" s="67">
         <v>13</v>
       </c>
-      <c r="F54" s="103" t="s">
+      <c r="F54" s="100" t="s">
         <v>677</v>
       </c>
       <c r="G54" s="1" t="s">
@@ -7282,29 +7281,29 @@
       <c r="L54" s="40">
         <v>19</v>
       </c>
-      <c r="M54" s="73" t="s">
+      <c r="M54" s="70" t="s">
         <v>429</v>
       </c>
-      <c r="N54" s="66" t="s">
+      <c r="N54" s="63" t="s">
         <v>585</v>
       </c>
-      <c r="O54" s="67" t="s">
+      <c r="O54" s="64" t="s">
         <v>464</v>
       </c>
       <c r="P54" s="57" t="s">
         <v>375</v>
       </c>
-      <c r="Q54" s="86" t="s">
+      <c r="Q54" s="83" t="s">
         <v>633</v>
       </c>
       <c r="R54" s="55"/>
       <c r="S54" s="55"/>
-      <c r="T54" s="89" t="s">
+      <c r="T54" s="86" t="s">
         <v>693</v>
       </c>
       <c r="U54" s="55"/>
       <c r="V54" s="55"/>
-      <c r="W54" s="92" t="s">
+      <c r="W54" s="89" t="s">
         <v>732</v>
       </c>
       <c r="X54" s="55"/>
@@ -7319,10 +7318,10 @@
       <c r="C55" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="70">
+      <c r="E55" s="67">
         <v>14</v>
       </c>
-      <c r="F55" s="77" t="s">
+      <c r="F55" s="74" t="s">
         <v>628</v>
       </c>
       <c r="G55" s="1" t="s">
@@ -7340,29 +7339,29 @@
       <c r="L55" s="40">
         <v>20</v>
       </c>
-      <c r="M55" s="73" t="s">
+      <c r="M55" s="70" t="s">
         <v>429</v>
       </c>
-      <c r="N55" s="66" t="s">
+      <c r="N55" s="63" t="s">
         <v>586</v>
       </c>
-      <c r="O55" s="67" t="s">
+      <c r="O55" s="64" t="s">
         <v>755</v>
       </c>
       <c r="P55" s="57" t="s">
         <v>380</v>
       </c>
-      <c r="Q55" s="86" t="s">
+      <c r="Q55" s="83" t="s">
         <v>634</v>
       </c>
       <c r="R55" s="55"/>
       <c r="S55" s="55"/>
-      <c r="T55" s="89" t="s">
+      <c r="T55" s="86" t="s">
         <v>676</v>
       </c>
       <c r="U55" s="55"/>
       <c r="V55" s="55"/>
-      <c r="W55" s="92" t="s">
+      <c r="W55" s="89" t="s">
         <v>733</v>
       </c>
       <c r="X55" s="55"/>
@@ -7377,10 +7376,10 @@
       <c r="C56" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E56" s="70">
+      <c r="E56" s="67">
         <v>15</v>
       </c>
-      <c r="F56" s="100" t="s">
+      <c r="F56" s="97" t="s">
         <v>736</v>
       </c>
       <c r="G56" s="1" t="s">
@@ -7389,29 +7388,29 @@
       <c r="L56" s="40">
         <v>21</v>
       </c>
-      <c r="M56" s="73" t="s">
+      <c r="M56" s="70" t="s">
         <v>429</v>
       </c>
-      <c r="N56" s="66" t="s">
+      <c r="N56" s="63" t="s">
         <v>610</v>
       </c>
-      <c r="O56" s="67" t="s">
+      <c r="O56" s="64" t="s">
         <v>747</v>
       </c>
       <c r="P56" s="55" t="s">
         <v>392</v>
       </c>
-      <c r="Q56" s="86" t="s">
+      <c r="Q56" s="83" t="s">
         <v>635</v>
       </c>
       <c r="R56" s="55"/>
       <c r="S56" s="55"/>
-      <c r="T56" s="89" t="s">
+      <c r="T56" s="86" t="s">
         <v>677</v>
       </c>
       <c r="U56" s="55"/>
       <c r="V56" s="55"/>
-      <c r="W56" s="92" t="s">
+      <c r="W56" s="89" t="s">
         <v>734</v>
       </c>
       <c r="X56" s="55"/>
@@ -7429,10 +7428,10 @@
       <c r="D57">
         <v>1.18</v>
       </c>
-      <c r="E57" s="70">
+      <c r="E57" s="67">
         <v>16</v>
       </c>
-      <c r="F57" s="108" t="s">
+      <c r="F57" s="105" t="s">
         <v>429</v>
       </c>
       <c r="G57" s="1" t="s">
@@ -7441,29 +7440,29 @@
       <c r="L57" s="40">
         <v>22</v>
       </c>
-      <c r="M57" s="73" t="s">
+      <c r="M57" s="70" t="s">
         <v>429</v>
       </c>
-      <c r="N57" s="66" t="s">
+      <c r="N57" s="63" t="s">
         <v>611</v>
       </c>
-      <c r="O57" s="67" t="s">
+      <c r="O57" s="64" t="s">
         <v>748</v>
       </c>
       <c r="P57" s="55" t="s">
         <v>393</v>
       </c>
-      <c r="Q57" s="86" t="s">
+      <c r="Q57" s="83" t="s">
         <v>636</v>
       </c>
       <c r="R57" s="55"/>
       <c r="S57" s="55"/>
-      <c r="T57" s="95" t="s">
+      <c r="T57" s="92" t="s">
         <v>762</v>
       </c>
       <c r="U57" s="55"/>
       <c r="V57" s="55"/>
-      <c r="W57" s="92" t="s">
+      <c r="W57" s="89" t="s">
         <v>735</v>
       </c>
       <c r="X57" s="55"/>
@@ -7478,10 +7477,10 @@
       <c r="C58" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E58" s="70">
+      <c r="E58" s="67">
         <v>17</v>
       </c>
-      <c r="F58" s="68" t="s">
+      <c r="F58" s="65" t="s">
         <v>619</v>
       </c>
       <c r="G58" s="1" t="s">
@@ -7490,17 +7489,17 @@
       <c r="L58" s="40">
         <v>23</v>
       </c>
-      <c r="M58" s="73" t="s">
+      <c r="M58" s="70" t="s">
         <v>429</v>
       </c>
-      <c r="N58" s="66" t="s">
+      <c r="N58" s="63" t="s">
         <v>587</v>
       </c>
-      <c r="O58" s="67" t="s">
+      <c r="O58" s="64" t="s">
         <v>760</v>
       </c>
       <c r="P58" s="55"/>
-      <c r="Q58" s="86" t="s">
+      <c r="Q58" s="83" t="s">
         <v>637</v>
       </c>
       <c r="R58" s="55"/>
@@ -7508,7 +7507,7 @@
       <c r="T58" s="55"/>
       <c r="U58" s="55"/>
       <c r="V58" s="55"/>
-      <c r="W58" s="92" t="s">
+      <c r="W58" s="89" t="s">
         <v>736</v>
       </c>
       <c r="X58" s="55"/>
@@ -7523,10 +7522,10 @@
       <c r="C59" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="70">
+      <c r="E59" s="67">
         <v>18</v>
       </c>
-      <c r="F59" s="106" t="s">
+      <c r="F59" s="103" t="s">
         <v>763</v>
       </c>
       <c r="G59" s="1" t="s">
@@ -7538,17 +7537,17 @@
       <c r="L59" s="40">
         <v>24</v>
       </c>
-      <c r="M59" s="73" t="s">
+      <c r="M59" s="70" t="s">
         <v>429</v>
       </c>
-      <c r="N59" s="66" t="s">
+      <c r="N59" s="63" t="s">
         <v>588</v>
       </c>
-      <c r="O59" s="67" t="s">
+      <c r="O59" s="64" t="s">
         <v>759</v>
       </c>
       <c r="P59" s="55"/>
-      <c r="Q59" s="86" t="s">
+      <c r="Q59" s="83" t="s">
         <v>638</v>
       </c>
       <c r="R59" s="55"/>
@@ -7556,7 +7555,7 @@
       <c r="T59" s="55"/>
       <c r="U59" s="55"/>
       <c r="V59" s="55"/>
-      <c r="W59" s="92" t="s">
+      <c r="W59" s="89" t="s">
         <v>737</v>
       </c>
       <c r="X59" s="55"/>
@@ -7565,33 +7564,33 @@
       <c r="A60">
         <v>61</v>
       </c>
-      <c r="B60" s="109">
+      <c r="B60" s="106">
         <v>55</v>
       </c>
-      <c r="C60" s="110" t="s">
+      <c r="C60" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="D60" s="111"/>
-      <c r="E60" s="109">
+      <c r="D60" s="108"/>
+      <c r="E60" s="106">
         <v>1</v>
       </c>
-      <c r="F60" s="108" t="s">
+      <c r="F60" s="105" t="s">
         <v>506</v>
       </c>
       <c r="L60" s="40">
         <v>25</v>
       </c>
-      <c r="M60" s="73" t="s">
+      <c r="M60" s="70" t="s">
         <v>429</v>
       </c>
-      <c r="N60" s="66" t="s">
+      <c r="N60" s="63" t="s">
         <v>589</v>
       </c>
-      <c r="O60" s="67" t="s">
+      <c r="O60" s="64" t="s">
         <v>612</v>
       </c>
       <c r="P60" s="55"/>
-      <c r="Q60" s="86" t="s">
+      <c r="Q60" s="83" t="s">
         <v>639</v>
       </c>
       <c r="R60" s="55"/>
@@ -7599,7 +7598,7 @@
       <c r="T60" s="55"/>
       <c r="U60" s="55"/>
       <c r="V60" s="55"/>
-      <c r="W60" s="92" t="s">
+      <c r="W60" s="89" t="s">
         <v>738</v>
       </c>
       <c r="X60" s="55"/>
@@ -7617,7 +7616,7 @@
       <c r="E61" s="1">
         <v>2</v>
       </c>
-      <c r="F61" s="68" t="s">
+      <c r="F61" s="65" t="s">
         <v>555</v>
       </c>
       <c r="I61" s="45" t="s">
@@ -7626,17 +7625,17 @@
       <c r="L61" s="40">
         <v>26</v>
       </c>
-      <c r="M61" s="73" t="s">
+      <c r="M61" s="70" t="s">
         <v>429</v>
       </c>
-      <c r="N61" s="66" t="s">
+      <c r="N61" s="63" t="s">
         <v>590</v>
       </c>
-      <c r="O61" s="67" t="s">
+      <c r="O61" s="64" t="s">
         <v>613</v>
       </c>
       <c r="P61" s="55"/>
-      <c r="Q61" s="86" t="s">
+      <c r="Q61" s="83" t="s">
         <v>640</v>
       </c>
       <c r="R61" s="55"/>
@@ -7644,7 +7643,7 @@
       <c r="T61" s="55"/>
       <c r="U61" s="55"/>
       <c r="V61" s="55"/>
-      <c r="W61" s="92" t="s">
+      <c r="W61" s="89" t="s">
         <v>739</v>
       </c>
       <c r="X61" s="55"/>
@@ -7662,23 +7661,23 @@
       <c r="E62" s="1">
         <v>3</v>
       </c>
-      <c r="F62" s="78" t="s">
+      <c r="F62" s="75" t="s">
         <v>540</v>
       </c>
       <c r="L62" s="40">
         <v>27</v>
       </c>
-      <c r="M62" s="74" t="s">
+      <c r="M62" s="71" t="s">
         <v>574</v>
       </c>
-      <c r="N62" s="66" t="s">
+      <c r="N62" s="63" t="s">
         <v>591</v>
       </c>
-      <c r="O62" s="67" t="s">
+      <c r="O62" s="64" t="s">
         <v>614</v>
       </c>
       <c r="P62" s="55"/>
-      <c r="Q62" s="86" t="s">
+      <c r="Q62" s="83" t="s">
         <v>641</v>
       </c>
       <c r="R62" s="55"/>
@@ -7686,7 +7685,7 @@
       <c r="T62" s="55"/>
       <c r="U62" s="55"/>
       <c r="V62" s="55"/>
-      <c r="W62" s="92" t="s">
+      <c r="W62" s="89" t="s">
         <v>740</v>
       </c>
       <c r="X62" s="55"/>
@@ -7701,23 +7700,23 @@
       <c r="E63" s="1">
         <v>4</v>
       </c>
-      <c r="F63" s="68" t="s">
+      <c r="F63" s="65" t="s">
         <v>464</v>
       </c>
       <c r="L63" s="40">
         <v>28</v>
       </c>
-      <c r="M63" s="74" t="s">
+      <c r="M63" s="71" t="s">
         <v>575</v>
       </c>
-      <c r="N63" s="66" t="s">
+      <c r="N63" s="63" t="s">
         <v>592</v>
       </c>
-      <c r="O63" s="67" t="s">
+      <c r="O63" s="64" t="s">
         <v>615</v>
       </c>
       <c r="P63" s="55"/>
-      <c r="Q63" s="86" t="s">
+      <c r="Q63" s="83" t="s">
         <v>642</v>
       </c>
       <c r="R63" s="55"/>
@@ -7725,7 +7724,7 @@
       <c r="T63" s="55"/>
       <c r="U63" s="55"/>
       <c r="V63" s="55"/>
-      <c r="W63" s="92" t="s">
+      <c r="W63" s="89" t="s">
         <v>741</v>
       </c>
       <c r="X63" s="55"/>
@@ -7740,23 +7739,23 @@
       <c r="E64" s="1">
         <v>5</v>
       </c>
-      <c r="F64" s="105" t="s">
+      <c r="F64" s="102" t="s">
         <v>670</v>
       </c>
       <c r="L64" s="40">
         <v>29</v>
       </c>
-      <c r="M64" s="74" t="s">
+      <c r="M64" s="71" t="s">
         <v>463</v>
       </c>
-      <c r="N64" s="66" t="s">
+      <c r="N64" s="63" t="s">
         <v>593</v>
       </c>
-      <c r="O64" s="67" t="s">
+      <c r="O64" s="64" t="s">
         <v>616</v>
       </c>
       <c r="P64" s="55"/>
-      <c r="Q64" s="86" t="s">
+      <c r="Q64" s="83" t="s">
         <v>643</v>
       </c>
       <c r="R64" s="55"/>
@@ -7777,23 +7776,23 @@
       <c r="E65" s="1">
         <v>6</v>
       </c>
-      <c r="F65" s="100" t="s">
+      <c r="F65" s="97" t="s">
         <v>738</v>
       </c>
       <c r="L65" s="40">
         <v>30</v>
       </c>
-      <c r="M65" s="74" t="s">
+      <c r="M65" s="71" t="s">
         <v>571</v>
       </c>
-      <c r="N65" s="66" t="s">
+      <c r="N65" s="63" t="s">
         <v>594</v>
       </c>
-      <c r="O65" s="67" t="s">
+      <c r="O65" s="64" t="s">
         <v>617</v>
       </c>
       <c r="P65" s="55"/>
-      <c r="Q65" s="86" t="s">
+      <c r="Q65" s="83" t="s">
         <v>652</v>
       </c>
       <c r="R65" s="55"/>
@@ -7814,23 +7813,23 @@
       <c r="E66" s="1">
         <v>7</v>
       </c>
-      <c r="F66" s="108" t="s">
+      <c r="F66" s="105" t="s">
         <v>571</v>
       </c>
       <c r="L66" s="40">
         <v>31</v>
       </c>
-      <c r="M66" s="74" t="s">
+      <c r="M66" s="71" t="s">
         <v>572</v>
       </c>
-      <c r="N66" s="66" t="s">
+      <c r="N66" s="63" t="s">
         <v>388</v>
       </c>
-      <c r="O66" s="67" t="s">
+      <c r="O66" s="64" t="s">
         <v>618</v>
       </c>
       <c r="P66" s="55"/>
-      <c r="Q66" s="86" t="s">
+      <c r="Q66" s="83" t="s">
         <v>653</v>
       </c>
       <c r="R66" s="55"/>
@@ -7851,23 +7850,23 @@
       <c r="E67" s="1">
         <v>8</v>
       </c>
-      <c r="F67" s="106" t="s">
+      <c r="F67" s="103" t="s">
         <v>708</v>
       </c>
       <c r="L67" s="40">
         <v>32</v>
       </c>
-      <c r="M67" s="74" t="s">
+      <c r="M67" s="71" t="s">
         <v>573</v>
       </c>
-      <c r="N67" s="66" t="s">
+      <c r="N67" s="63" t="s">
         <v>388</v>
       </c>
-      <c r="O67" s="67" t="s">
+      <c r="O67" s="64" t="s">
         <v>619</v>
       </c>
       <c r="P67" s="55"/>
-      <c r="Q67" s="86" t="s">
+      <c r="Q67" s="83" t="s">
         <v>647</v>
       </c>
       <c r="R67" s="55"/>
@@ -7888,23 +7887,23 @@
       <c r="E68" s="1">
         <v>9</v>
       </c>
-      <c r="F68" s="78" t="s">
+      <c r="F68" s="75" t="s">
         <v>597</v>
       </c>
       <c r="L68" s="40">
         <v>33</v>
       </c>
-      <c r="M68" s="83" t="s">
+      <c r="M68" s="80" t="s">
         <v>579</v>
       </c>
-      <c r="N68" s="66" t="s">
+      <c r="N68" s="63" t="s">
         <v>387</v>
       </c>
-      <c r="O68" s="67" t="s">
+      <c r="O68" s="64" t="s">
         <v>619</v>
       </c>
       <c r="P68" s="55"/>
-      <c r="Q68" s="86" t="s">
+      <c r="Q68" s="83" t="s">
         <v>648</v>
       </c>
       <c r="R68" s="55"/>
@@ -7925,19 +7924,19 @@
       <c r="E69" s="1">
         <v>10</v>
       </c>
-      <c r="F69" s="103" t="s">
+      <c r="F69" s="100" t="s">
         <v>762</v>
       </c>
       <c r="L69" s="40">
         <v>34</v>
       </c>
-      <c r="M69" s="83" t="s">
+      <c r="M69" s="80" t="s">
         <v>388</v>
       </c>
-      <c r="N69" s="66" t="s">
+      <c r="N69" s="63" t="s">
         <v>387</v>
       </c>
-      <c r="O69" s="67" t="s">
+      <c r="O69" s="64" t="s">
         <v>619</v>
       </c>
       <c r="P69" s="55"/>
@@ -7963,19 +7962,19 @@
       <c r="E70" s="1">
         <v>11</v>
       </c>
-      <c r="F70" s="103" t="s">
+      <c r="F70" s="100" t="s">
         <v>685</v>
       </c>
       <c r="L70" s="40">
         <v>35</v>
       </c>
-      <c r="M70" s="83" t="s">
+      <c r="M70" s="80" t="s">
         <v>388</v>
       </c>
-      <c r="N70" s="66" t="s">
+      <c r="N70" s="63" t="s">
         <v>595</v>
       </c>
-      <c r="O70" s="67" t="s">
+      <c r="O70" s="64" t="s">
         <v>620</v>
       </c>
       <c r="P70" s="55"/>
@@ -7998,21 +7997,21 @@
       <c r="E71" s="1">
         <v>12</v>
       </c>
-      <c r="F71" s="100" t="s">
+      <c r="F71" s="97" t="s">
         <v>730</v>
       </c>
       <c r="L71" s="40">
         <v>36</v>
       </c>
-      <c r="M71" s="83" t="s">
+      <c r="M71" s="80" t="s">
         <v>387</v>
       </c>
-      <c r="N71" s="66" t="s">
+      <c r="N71" s="63" t="s">
         <v>595</v>
       </c>
       <c r="O71" s="55"/>
       <c r="P71" s="55"/>
-      <c r="Q71" s="64"/>
+      <c r="Q71" s="61"/>
       <c r="R71" s="55"/>
       <c r="S71" s="55"/>
       <c r="T71" s="55"/>
@@ -8031,16 +8030,16 @@
       <c r="E72" s="1">
         <v>13</v>
       </c>
-      <c r="F72" s="78" t="s">
+      <c r="F72" s="75" t="s">
         <v>609</v>
       </c>
       <c r="L72" s="40">
         <v>37</v>
       </c>
-      <c r="M72" s="83" t="s">
+      <c r="M72" s="80" t="s">
         <v>387</v>
       </c>
-      <c r="N72" s="66" t="s">
+      <c r="N72" s="63" t="s">
         <v>595</v>
       </c>
       <c r="O72" s="55"/>
@@ -8064,16 +8063,16 @@
       <c r="E73" s="1">
         <v>14</v>
       </c>
-      <c r="F73" s="77" t="s">
+      <c r="F73" s="74" t="s">
         <v>634</v>
       </c>
       <c r="L73" s="40">
         <v>38</v>
       </c>
-      <c r="M73" s="83" t="s">
+      <c r="M73" s="80" t="s">
         <v>387</v>
       </c>
-      <c r="N73" s="66" t="s">
+      <c r="N73" s="63" t="s">
         <v>596</v>
       </c>
       <c r="O73" s="55"/>
@@ -8097,16 +8096,16 @@
       <c r="E74" s="1">
         <v>15</v>
       </c>
-      <c r="F74" s="108" t="s">
+      <c r="F74" s="105" t="s">
         <v>387</v>
       </c>
       <c r="L74" s="40">
         <v>39</v>
       </c>
-      <c r="M74" s="74" t="s">
+      <c r="M74" s="71" t="s">
         <v>576</v>
       </c>
-      <c r="N74" s="66" t="s">
+      <c r="N74" s="63" t="s">
         <v>597</v>
       </c>
       <c r="O74" s="55"/>
@@ -8130,16 +8129,16 @@
       <c r="E75" s="1">
         <v>16</v>
       </c>
-      <c r="F75" s="77" t="s">
+      <c r="F75" s="74" t="s">
         <v>627</v>
       </c>
       <c r="L75" s="40">
         <v>40</v>
       </c>
-      <c r="M75" s="74" t="s">
+      <c r="M75" s="71" t="s">
         <v>577</v>
       </c>
-      <c r="N75" s="66" t="s">
+      <c r="N75" s="63" t="s">
         <v>598</v>
       </c>
       <c r="O75" s="55"/>
@@ -8163,16 +8162,16 @@
       <c r="E76" s="1">
         <v>17</v>
       </c>
-      <c r="F76" s="104" t="s">
+      <c r="F76" s="101" t="s">
         <v>702</v>
       </c>
       <c r="L76" s="40">
         <v>41</v>
       </c>
-      <c r="M76" s="74" t="s">
+      <c r="M76" s="71" t="s">
         <v>578</v>
       </c>
-      <c r="N76" s="66" t="s">
+      <c r="N76" s="63" t="s">
         <v>599</v>
       </c>
       <c r="O76" s="55"/>
@@ -8196,16 +8195,16 @@
       <c r="E77" s="1">
         <v>18</v>
       </c>
-      <c r="F77" s="77" t="s">
+      <c r="F77" s="74" t="s">
         <v>642</v>
       </c>
       <c r="L77" s="40">
         <v>42</v>
       </c>
-      <c r="M77" s="83" t="s">
+      <c r="M77" s="80" t="s">
         <v>580</v>
       </c>
-      <c r="N77" s="66" t="s">
+      <c r="N77" s="63" t="s">
         <v>601</v>
       </c>
       <c r="O77" s="55"/>
@@ -8220,26 +8219,26 @@
       <c r="X77" s="55"/>
     </row>
     <row r="78" spans="2:24" ht="12.75">
-      <c r="B78" s="109">
+      <c r="B78" s="106">
         <v>73</v>
       </c>
-      <c r="C78" s="110" t="s">
+      <c r="C78" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="D78" s="111"/>
-      <c r="E78" s="109">
+      <c r="D78" s="108"/>
+      <c r="E78" s="106">
         <v>1</v>
       </c>
-      <c r="F78" s="108" t="s">
+      <c r="F78" s="105" t="s">
         <v>507</v>
       </c>
       <c r="L78" s="40">
         <v>43</v>
       </c>
-      <c r="M78" s="83" t="s">
+      <c r="M78" s="80" t="s">
         <v>581</v>
       </c>
-      <c r="N78" s="66" t="s">
+      <c r="N78" s="63" t="s">
         <v>600</v>
       </c>
       <c r="O78" s="55"/>
@@ -8260,19 +8259,19 @@
       <c r="C79" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E79" s="70">
+      <c r="E79" s="67">
         <v>2</v>
       </c>
-      <c r="F79" s="68" t="s">
+      <c r="F79" s="65" t="s">
         <v>556</v>
       </c>
       <c r="L79" s="40">
         <v>44</v>
       </c>
-      <c r="M79" s="83" t="s">
+      <c r="M79" s="80" t="s">
         <v>582</v>
       </c>
-      <c r="N79" s="66" t="s">
+      <c r="N79" s="63" t="s">
         <v>602</v>
       </c>
       <c r="O79" s="55"/>
@@ -8293,19 +8292,19 @@
       <c r="C80" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E80" s="70">
+      <c r="E80" s="67">
         <v>3</v>
       </c>
-      <c r="F80" s="78" t="s">
+      <c r="F80" s="75" t="s">
         <v>541</v>
       </c>
       <c r="L80" s="40">
         <v>45</v>
       </c>
-      <c r="M80" s="83" t="s">
+      <c r="M80" s="80" t="s">
         <v>583</v>
       </c>
-      <c r="N80" s="66" t="s">
+      <c r="N80" s="63" t="s">
         <v>609</v>
       </c>
       <c r="O80" s="55"/>
@@ -8326,17 +8325,17 @@
       <c r="C81" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E81" s="70">
+      <c r="E81" s="67">
         <v>4</v>
       </c>
-      <c r="F81" s="108" t="s">
+      <c r="F81" s="105" t="s">
         <v>583</v>
       </c>
       <c r="L81" s="40">
         <v>46</v>
       </c>
       <c r="M81" s="55"/>
-      <c r="N81" s="66" t="s">
+      <c r="N81" s="63" t="s">
         <v>603</v>
       </c>
       <c r="O81" s="55"/>
@@ -8357,17 +8356,17 @@
       <c r="C82" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E82" s="70">
+      <c r="E82" s="67">
         <v>5</v>
       </c>
-      <c r="F82" s="78" t="s">
+      <c r="F82" s="75" t="s">
         <v>599</v>
       </c>
       <c r="L82" s="40">
         <v>47</v>
       </c>
       <c r="M82" s="55"/>
-      <c r="N82" s="66" t="s">
+      <c r="N82" s="63" t="s">
         <v>604</v>
       </c>
       <c r="O82" s="55"/>
@@ -8391,17 +8390,17 @@
       <c r="D83">
         <v>1.5</v>
       </c>
-      <c r="E83" s="70">
+      <c r="E83" s="67">
         <v>6</v>
       </c>
-      <c r="F83" s="105" t="s">
+      <c r="F83" s="102" t="s">
         <v>672</v>
       </c>
       <c r="L83" s="40">
         <v>48</v>
       </c>
       <c r="M83" s="55"/>
-      <c r="N83" s="66" t="s">
+      <c r="N83" s="63" t="s">
         <v>605</v>
       </c>
       <c r="O83" s="55"/>
@@ -8422,17 +8421,17 @@
       <c r="C84" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E84" s="70">
+      <c r="E84" s="67">
         <v>7</v>
       </c>
-      <c r="F84" s="101" t="s">
+      <c r="F84" s="98" t="s">
         <v>566</v>
       </c>
       <c r="L84" s="40">
         <v>49</v>
       </c>
       <c r="M84" s="55"/>
-      <c r="N84" s="84" t="s">
+      <c r="N84" s="81" t="s">
         <v>606</v>
       </c>
       <c r="O84" s="55"/>
@@ -8453,17 +8452,17 @@
       <c r="C85" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E85" s="70">
+      <c r="E85" s="67">
         <v>8</v>
       </c>
-      <c r="F85" s="100" t="s">
+      <c r="F85" s="97" t="s">
         <v>741</v>
       </c>
       <c r="L85" s="40">
         <v>50</v>
       </c>
       <c r="M85" s="55"/>
-      <c r="N85" s="84" t="s">
+      <c r="N85" s="81" t="s">
         <v>607</v>
       </c>
       <c r="O85" s="55"/>
@@ -8484,17 +8483,17 @@
       <c r="C86" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E86" s="70">
+      <c r="E86" s="67">
         <v>9</v>
       </c>
-      <c r="F86" s="77" t="s">
-        <v>625</v>
+      <c r="F86" s="74" t="s">
+        <v>821</v>
       </c>
       <c r="L86" s="40">
         <v>51</v>
       </c>
       <c r="M86" s="55"/>
-      <c r="N86" s="66" t="s">
+      <c r="N86" s="63" t="s">
         <v>608</v>
       </c>
       <c r="O86" s="55"/>
@@ -8515,10 +8514,10 @@
       <c r="C87" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E87" s="70">
+      <c r="E87" s="67">
         <v>10</v>
       </c>
-      <c r="F87" s="68" t="s">
+      <c r="F87" s="65" t="s">
         <v>764</v>
       </c>
       <c r="M87">
@@ -8565,10 +8564,10 @@
       <c r="C88" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E88" s="70">
+      <c r="E88" s="67">
         <v>11</v>
       </c>
-      <c r="F88" s="78" t="s">
+      <c r="F88" s="75" t="s">
         <v>589</v>
       </c>
       <c r="M88">
@@ -8597,10 +8596,10 @@
       <c r="C89" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E89" s="70">
+      <c r="E89" s="67">
         <v>12</v>
       </c>
-      <c r="F89" s="68" t="s">
+      <c r="F89" s="65" t="s">
         <v>619</v>
       </c>
       <c r="T89" t="s">
@@ -8614,11 +8613,11 @@
       <c r="C90" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E90" s="70">
+      <c r="E90" s="67">
         <v>13</v>
       </c>
-      <c r="F90" s="100" t="s">
-        <v>726</v>
+      <c r="F90" s="97" t="s">
+        <v>822</v>
       </c>
       <c r="T90" s="58" t="s">
         <v>519</v>
@@ -8644,10 +8643,10 @@
       <c r="C91" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E91" s="70">
+      <c r="E91" s="67">
         <v>14</v>
       </c>
-      <c r="F91" s="103" t="s">
+      <c r="F91" s="100" t="s">
         <v>676</v>
       </c>
       <c r="T91" s="58" t="s">
@@ -8674,10 +8673,10 @@
       <c r="C92" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E92" s="70">
+      <c r="E92" s="67">
         <v>15</v>
       </c>
-      <c r="F92" s="103" t="s">
+      <c r="F92" s="100" t="s">
         <v>679</v>
       </c>
       <c r="T92" s="58" t="s">
@@ -8704,10 +8703,10 @@
       <c r="C93" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E93" s="70">
+      <c r="E93" s="67">
         <v>16</v>
       </c>
-      <c r="F93" s="77" t="s">
+      <c r="F93" s="74" t="s">
         <v>633</v>
       </c>
       <c r="T93" s="58" t="s">
@@ -8737,11 +8736,11 @@
       <c r="D94">
         <v>1.19</v>
       </c>
-      <c r="E94" s="70">
+      <c r="E94" s="67">
         <v>17</v>
       </c>
-      <c r="F94" s="108" t="s">
-        <v>429</v>
+      <c r="F94" s="105" t="s">
+        <v>818</v>
       </c>
       <c r="T94" s="58" t="s">
         <v>522</v>
@@ -8767,10 +8766,10 @@
       <c r="C95" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E95" s="70">
+      <c r="E95" s="67">
         <v>18</v>
       </c>
-      <c r="F95" s="106" t="s">
+      <c r="F95" s="103" t="s">
         <v>712</v>
       </c>
       <c r="T95" s="58" t="s">
@@ -8791,17 +8790,17 @@
       </c>
     </row>
     <row r="96" spans="2:24" ht="12.75">
-      <c r="B96" s="109">
+      <c r="B96" s="106">
         <v>91</v>
       </c>
-      <c r="C96" s="110" t="s">
+      <c r="C96" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="D96" s="111"/>
-      <c r="E96" s="109">
+      <c r="D96" s="108"/>
+      <c r="E96" s="106">
         <v>1</v>
       </c>
-      <c r="F96" s="108" t="s">
+      <c r="F96" s="105" t="s">
         <v>508</v>
       </c>
       <c r="T96" s="58" t="s">
@@ -8831,7 +8830,7 @@
       <c r="E97" s="1">
         <v>2</v>
       </c>
-      <c r="F97" s="68" t="s">
+      <c r="F97" s="65" t="s">
         <v>557</v>
       </c>
       <c r="T97" s="58" t="s">
@@ -8861,7 +8860,7 @@
       <c r="E98" s="1">
         <v>3</v>
       </c>
-      <c r="F98" s="78" t="s">
+      <c r="F98" s="75" t="s">
         <v>542</v>
       </c>
       <c r="T98" s="58" t="s">
@@ -8891,7 +8890,7 @@
       <c r="E99" s="1">
         <v>4</v>
       </c>
-      <c r="F99" s="105" t="s">
+      <c r="F99" s="102" t="s">
         <v>665</v>
       </c>
       <c r="T99" s="58" t="s">
@@ -8921,7 +8920,7 @@
       <c r="E100" s="1">
         <v>5</v>
       </c>
-      <c r="F100" s="100" t="s">
+      <c r="F100" s="97" t="s">
         <v>739</v>
       </c>
       <c r="T100" s="58" t="s">
@@ -8951,7 +8950,7 @@
       <c r="E101" s="1">
         <v>6</v>
       </c>
-      <c r="F101" s="106" t="s">
+      <c r="F101" s="103" t="s">
         <v>710</v>
       </c>
       <c r="T101" s="58" t="s">
@@ -8981,7 +8980,7 @@
       <c r="E102" s="1">
         <v>7</v>
       </c>
-      <c r="F102" s="78" t="s">
+      <c r="F102" s="75" t="s">
         <v>591</v>
       </c>
       <c r="T102" s="45" t="s">
@@ -9011,7 +9010,7 @@
       <c r="E103" s="1">
         <v>8</v>
       </c>
-      <c r="F103" s="77" t="s">
+      <c r="F103" s="74" t="s">
         <v>651</v>
       </c>
       <c r="T103" s="45"/>
@@ -9026,7 +9025,7 @@
       <c r="E104" s="1">
         <v>9</v>
       </c>
-      <c r="F104" s="103" t="s">
+      <c r="F104" s="100" t="s">
         <v>766</v>
       </c>
     </row>
@@ -9040,7 +9039,7 @@
       <c r="E105" s="1">
         <v>10</v>
       </c>
-      <c r="F105" s="78" t="s">
+      <c r="F105" s="75" t="s">
         <v>603</v>
       </c>
     </row>
@@ -9054,7 +9053,7 @@
       <c r="E106" s="1">
         <v>11</v>
       </c>
-      <c r="F106" s="108" t="s">
+      <c r="F106" s="105" t="s">
         <v>387</v>
       </c>
     </row>
@@ -9068,7 +9067,7 @@
       <c r="E107" s="1">
         <v>12</v>
       </c>
-      <c r="F107" s="103" t="s">
+      <c r="F107" s="100" t="s">
         <v>680</v>
       </c>
     </row>
@@ -9085,7 +9084,7 @@
       <c r="E108" s="1">
         <v>13</v>
       </c>
-      <c r="F108" s="78" t="s">
+      <c r="F108" s="75" t="s">
         <v>590</v>
       </c>
     </row>
@@ -9099,7 +9098,7 @@
       <c r="E109" s="1">
         <v>14</v>
       </c>
-      <c r="F109" s="77" t="s">
+      <c r="F109" s="74" t="s">
         <v>640</v>
       </c>
       <c r="U109">
@@ -9125,7 +9124,7 @@
       <c r="E110" s="1">
         <v>15</v>
       </c>
-      <c r="F110" s="68" t="s">
+      <c r="F110" s="65" t="s">
         <v>612</v>
       </c>
     </row>
@@ -9139,7 +9138,7 @@
       <c r="E111" s="1">
         <v>16</v>
       </c>
-      <c r="F111" s="100" t="s">
+      <c r="F111" s="97" t="s">
         <v>734</v>
       </c>
     </row>
@@ -9153,7 +9152,7 @@
       <c r="E112" s="1">
         <v>17</v>
       </c>
-      <c r="F112" s="108" t="s">
+      <c r="F112" s="105" t="s">
         <v>582</v>
       </c>
       <c r="N112">
@@ -9174,7 +9173,7 @@
       <c r="E113" s="1">
         <v>18</v>
       </c>
-      <c r="F113" s="78" t="s">
+      <c r="F113" s="75" t="s">
         <v>598</v>
       </c>
       <c r="L113" s="45"/>
@@ -9211,17 +9210,17 @@
       </c>
     </row>
     <row r="114" spans="2:24" ht="12.75">
-      <c r="B114" s="109">
+      <c r="B114" s="106">
         <v>109</v>
       </c>
-      <c r="C114" s="112" t="s">
+      <c r="C114" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="D114" s="111"/>
-      <c r="E114" s="109">
+      <c r="D114" s="108"/>
+      <c r="E114" s="106">
         <v>1</v>
       </c>
-      <c r="F114" s="108" t="s">
+      <c r="F114" s="105" t="s">
         <v>509</v>
       </c>
       <c r="L114" s="45"/>
@@ -9260,10 +9259,10 @@
       <c r="C115" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E115" s="70">
+      <c r="E115" s="67">
         <v>2</v>
       </c>
-      <c r="F115" s="68" t="s">
+      <c r="F115" s="65" t="s">
         <v>558</v>
       </c>
       <c r="L115" s="45"/>
@@ -9302,10 +9301,10 @@
       <c r="C116" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E116" s="70">
+      <c r="E116" s="67">
         <v>3</v>
       </c>
-      <c r="F116" s="78" t="s">
+      <c r="F116" s="75" t="s">
         <v>543</v>
       </c>
       <c r="L116" s="45"/>
@@ -9344,10 +9343,10 @@
       <c r="C117" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E117" s="70">
+      <c r="E117" s="67">
         <v>4</v>
       </c>
-      <c r="F117" s="105" t="s">
+      <c r="F117" s="102" t="s">
         <v>659</v>
       </c>
       <c r="L117" s="45"/>
@@ -9377,10 +9376,10 @@
       <c r="C118" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E118" s="70">
+      <c r="E118" s="67">
         <v>5</v>
       </c>
-      <c r="F118" s="101" t="s">
+      <c r="F118" s="98" t="s">
         <v>656</v>
       </c>
       <c r="M118">
@@ -9409,10 +9408,10 @@
       <c r="C119" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E119" s="70">
+      <c r="E119" s="67">
         <v>6</v>
       </c>
-      <c r="F119" s="100" t="s">
+      <c r="F119" s="97" t="s">
         <v>716</v>
       </c>
       <c r="L119" s="45"/>
@@ -9443,10 +9442,10 @@
       <c r="C120" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E120" s="70">
+      <c r="E120" s="67">
         <v>7</v>
       </c>
-      <c r="F120" s="100" t="s">
+      <c r="F120" s="97" t="s">
         <v>767</v>
       </c>
       <c r="M120">
@@ -9468,10 +9467,10 @@
       <c r="C121" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E121" s="70">
+      <c r="E121" s="67">
         <v>8</v>
       </c>
-      <c r="F121" s="68" t="s">
+      <c r="F121" s="65" t="s">
         <v>616</v>
       </c>
       <c r="M121">
@@ -9493,10 +9492,10 @@
       <c r="C122" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E122" s="70">
+      <c r="E122" s="67">
         <v>9</v>
       </c>
-      <c r="F122" s="106" t="s">
+      <c r="F122" s="103" t="s">
         <v>709</v>
       </c>
       <c r="M122">
@@ -9518,10 +9517,10 @@
       <c r="C123" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E123" s="70">
+      <c r="E123" s="67">
         <v>10</v>
       </c>
-      <c r="F123" s="108" t="s">
+      <c r="F123" s="105" t="s">
         <v>577</v>
       </c>
       <c r="M123">
@@ -9543,10 +9542,10 @@
       <c r="C124" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E124" s="70">
+      <c r="E124" s="67">
         <v>11</v>
       </c>
-      <c r="F124" s="78" t="s">
+      <c r="F124" s="75" t="s">
         <v>606</v>
       </c>
       <c r="M124">
@@ -9568,10 +9567,10 @@
       <c r="C125" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E125" s="70">
+      <c r="E125" s="67">
         <v>12</v>
       </c>
-      <c r="F125" s="104" t="s">
+      <c r="F125" s="101" t="s">
         <v>698</v>
       </c>
       <c r="M125">
@@ -9593,10 +9592,10 @@
       <c r="C126" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E126" s="70">
+      <c r="E126" s="67">
         <v>13</v>
       </c>
-      <c r="F126" s="108" t="s">
+      <c r="F126" s="105" t="s">
         <v>388</v>
       </c>
       <c r="M126">
@@ -9618,10 +9617,10 @@
       <c r="C127" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E127" s="70">
+      <c r="E127" s="67">
         <v>14</v>
       </c>
-      <c r="F127" s="77" t="s">
+      <c r="F127" s="74" t="s">
         <v>649</v>
       </c>
       <c r="M127">
@@ -9643,10 +9642,10 @@
       <c r="C128" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E128" s="70">
+      <c r="E128" s="67">
         <v>15</v>
       </c>
-      <c r="F128" s="103" t="s">
+      <c r="F128" s="100" t="s">
         <v>683</v>
       </c>
       <c r="M128">
@@ -9671,10 +9670,10 @@
       <c r="D129">
         <v>1.7</v>
       </c>
-      <c r="E129" s="70">
+      <c r="E129" s="67">
         <v>16</v>
       </c>
-      <c r="F129" s="102" t="s">
+      <c r="F129" s="99" t="s">
         <v>744</v>
       </c>
       <c r="M129">
@@ -9696,10 +9695,10 @@
       <c r="C130" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E130" s="70">
+      <c r="E130" s="67">
         <v>17</v>
       </c>
-      <c r="F130" s="78" t="s">
+      <c r="F130" s="75" t="s">
         <v>587</v>
       </c>
       <c r="M130">
@@ -9721,10 +9720,10 @@
       <c r="C131" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E131" s="70">
+      <c r="E131" s="67">
         <v>18</v>
       </c>
-      <c r="F131" s="108" t="s">
+      <c r="F131" s="105" t="s">
         <v>768</v>
       </c>
       <c r="M131">
@@ -9740,17 +9739,17 @@
       </c>
     </row>
     <row r="132" spans="2:15" ht="12.75">
-      <c r="B132" s="109">
+      <c r="B132" s="106">
         <v>127</v>
       </c>
-      <c r="C132" s="110" t="s">
+      <c r="C132" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="D132" s="111"/>
-      <c r="E132" s="109">
+      <c r="D132" s="108"/>
+      <c r="E132" s="106">
         <v>1</v>
       </c>
-      <c r="F132" s="108" t="s">
+      <c r="F132" s="105" t="s">
         <v>510</v>
       </c>
       <c r="L132" s="45" t="s">
@@ -9778,7 +9777,7 @@
       <c r="E133" s="1">
         <v>2</v>
       </c>
-      <c r="F133" s="68" t="s">
+      <c r="F133" s="65" t="s">
         <v>559</v>
       </c>
       <c r="L133" t="s">
@@ -9806,7 +9805,7 @@
       <c r="E134" s="1">
         <v>3</v>
       </c>
-      <c r="F134" s="78" t="s">
+      <c r="F134" s="75" t="s">
         <v>544</v>
       </c>
       <c r="L134" s="45" t="s">
@@ -9834,7 +9833,7 @@
       <c r="E135" s="1">
         <v>4</v>
       </c>
-      <c r="F135" s="105" t="s">
+      <c r="F135" s="102" t="s">
         <v>660</v>
       </c>
       <c r="M135">
@@ -9859,7 +9858,7 @@
       <c r="E136" s="1">
         <v>5</v>
       </c>
-      <c r="F136" s="100" t="s">
+      <c r="F136" s="97" t="s">
         <v>722</v>
       </c>
       <c r="L136" t="s">
@@ -9887,7 +9886,7 @@
       <c r="E137" s="1">
         <v>6</v>
       </c>
-      <c r="F137" s="106" t="s">
+      <c r="F137" s="103" t="s">
         <v>713</v>
       </c>
       <c r="M137">
@@ -9912,7 +9911,7 @@
       <c r="E138" s="1">
         <v>7</v>
       </c>
-      <c r="F138" s="77" t="s">
+      <c r="F138" s="74" t="s">
         <v>629</v>
       </c>
       <c r="M138">
@@ -9937,7 +9936,7 @@
       <c r="E139" s="1">
         <v>8</v>
       </c>
-      <c r="F139" s="104" t="s">
+      <c r="F139" s="101" t="s">
         <v>696</v>
       </c>
       <c r="M139">
@@ -9962,7 +9961,7 @@
       <c r="E140" s="1">
         <v>9</v>
       </c>
-      <c r="F140" s="103" t="s">
+      <c r="F140" s="100" t="s">
         <v>686</v>
       </c>
       <c r="M140">
@@ -9987,7 +9986,7 @@
       <c r="E141" s="1">
         <v>10</v>
       </c>
-      <c r="F141" s="77" t="s">
+      <c r="F141" s="74" t="s">
         <v>637</v>
       </c>
       <c r="M141">
@@ -10012,7 +10011,7 @@
       <c r="E142" s="1">
         <v>11</v>
       </c>
-      <c r="F142" s="108" t="s">
+      <c r="F142" s="105" t="s">
         <v>581</v>
       </c>
       <c r="M142">
@@ -10037,7 +10036,7 @@
       <c r="E143" s="1">
         <v>12</v>
       </c>
-      <c r="F143" s="78" t="s">
+      <c r="F143" s="75" t="s">
         <v>595</v>
       </c>
       <c r="M143">
@@ -10062,7 +10061,7 @@
       <c r="E144" s="1">
         <v>13</v>
       </c>
-      <c r="F144" s="100" t="s">
+      <c r="F144" s="97" t="s">
         <v>740</v>
       </c>
       <c r="M144">
@@ -10087,7 +10086,7 @@
       <c r="E145" s="1">
         <v>14</v>
       </c>
-      <c r="F145" s="77" t="s">
+      <c r="F145" s="74" t="s">
         <v>648</v>
       </c>
       <c r="M145">
@@ -10112,7 +10111,7 @@
       <c r="E146" s="1">
         <v>15</v>
       </c>
-      <c r="F146" s="108" t="s">
+      <c r="F146" s="105" t="s">
         <v>579</v>
       </c>
       <c r="M146">
@@ -10137,7 +10136,7 @@
       <c r="E147" s="1">
         <v>16</v>
       </c>
-      <c r="F147" s="78" t="s">
+      <c r="F147" s="75" t="s">
         <v>602</v>
       </c>
       <c r="M147">
@@ -10162,7 +10161,7 @@
       <c r="E148" s="1">
         <v>17</v>
       </c>
-      <c r="F148" s="102" t="s">
+      <c r="F148" s="99" t="s">
         <v>769</v>
       </c>
       <c r="M148">
@@ -10190,7 +10189,7 @@
       <c r="E149" s="1">
         <v>18</v>
       </c>
-      <c r="F149" s="103" t="s">
+      <c r="F149" s="100" t="s">
         <v>688</v>
       </c>
       <c r="M149">
@@ -10206,17 +10205,17 @@
       </c>
     </row>
     <row r="150" spans="2:15" ht="12.75">
-      <c r="B150" s="109">
+      <c r="B150" s="106">
         <v>145</v>
       </c>
-      <c r="C150" s="110" t="s">
+      <c r="C150" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="D150" s="111"/>
-      <c r="E150" s="109">
+      <c r="D150" s="108"/>
+      <c r="E150" s="106">
         <v>1</v>
       </c>
-      <c r="F150" s="108" t="s">
+      <c r="F150" s="105" t="s">
         <v>511</v>
       </c>
       <c r="M150">
@@ -10238,10 +10237,10 @@
       <c r="C151" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E151" s="70">
+      <c r="E151" s="67">
         <v>2</v>
       </c>
-      <c r="F151" s="68" t="s">
+      <c r="F151" s="65" t="s">
         <v>560</v>
       </c>
       <c r="M151">
@@ -10263,10 +10262,10 @@
       <c r="C152" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E152" s="70">
+      <c r="E152" s="67">
         <v>3</v>
       </c>
-      <c r="F152" s="78" t="s">
+      <c r="F152" s="75" t="s">
         <v>545</v>
       </c>
       <c r="M152">
@@ -10291,10 +10290,10 @@
       <c r="D153">
         <v>1.9</v>
       </c>
-      <c r="E153" s="70">
+      <c r="E153" s="67">
         <v>4</v>
       </c>
-      <c r="F153" s="105" t="s">
+      <c r="F153" s="102" t="s">
         <v>669</v>
       </c>
       <c r="M153">
@@ -10316,10 +10315,10 @@
       <c r="C154" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E154" s="70">
+      <c r="E154" s="67">
         <v>5</v>
       </c>
-      <c r="F154" s="100" t="s">
+      <c r="F154" s="97" t="s">
         <v>727</v>
       </c>
       <c r="M154">
@@ -10344,10 +10343,10 @@
       <c r="D155">
         <v>1.2</v>
       </c>
-      <c r="E155" s="70">
+      <c r="E155" s="67">
         <v>6</v>
       </c>
-      <c r="F155" s="108" t="s">
+      <c r="F155" s="105" t="s">
         <v>429</v>
       </c>
       <c r="M155">
@@ -10369,10 +10368,10 @@
       <c r="C156" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E156" s="70">
+      <c r="E156" s="67">
         <v>7</v>
       </c>
-      <c r="F156" s="78" t="s">
+      <c r="F156" s="75" t="s">
         <v>601</v>
       </c>
       <c r="M156">
@@ -10394,10 +10393,10 @@
       <c r="C157" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E157" s="70">
+      <c r="E157" s="67">
         <v>8</v>
       </c>
-      <c r="F157" s="68" t="s">
+      <c r="F157" s="65" t="s">
         <v>613</v>
       </c>
       <c r="M157">
@@ -10419,10 +10418,10 @@
       <c r="C158" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E158" s="70">
+      <c r="E158" s="67">
         <v>9</v>
       </c>
-      <c r="F158" s="103" t="s">
+      <c r="F158" s="100" t="s">
         <v>692</v>
       </c>
       <c r="M158">
@@ -10444,10 +10443,10 @@
       <c r="C159" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E159" s="70">
+      <c r="E159" s="67">
         <v>10</v>
       </c>
-      <c r="F159" s="78" t="s">
+      <c r="F159" s="75" t="s">
         <v>388</v>
       </c>
       <c r="M159">
@@ -10469,10 +10468,10 @@
       <c r="C160" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E160" s="70">
+      <c r="E160" s="67">
         <v>11</v>
       </c>
-      <c r="F160" s="100" t="s">
+      <c r="F160" s="97" t="s">
         <v>735</v>
       </c>
       <c r="M160">
@@ -10494,10 +10493,10 @@
       <c r="C161" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E161" s="70">
+      <c r="E161" s="67">
         <v>12</v>
       </c>
-      <c r="F161" s="77" t="s">
+      <c r="F161" s="74" t="s">
         <v>630</v>
       </c>
       <c r="M161">
@@ -10519,10 +10518,10 @@
       <c r="C162" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E162" s="70">
+      <c r="E162" s="67">
         <v>13</v>
       </c>
-      <c r="F162" s="102" t="s">
+      <c r="F162" s="99" t="s">
         <v>765</v>
       </c>
       <c r="M162">
@@ -10544,10 +10543,10 @@
       <c r="C163" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E163" s="70">
+      <c r="E163" s="67">
         <v>14</v>
       </c>
-      <c r="F163" s="108" t="s">
+      <c r="F163" s="105" t="s">
         <v>580</v>
       </c>
       <c r="M163">
@@ -10569,10 +10568,10 @@
       <c r="C164" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E164" s="70">
+      <c r="E164" s="67">
         <v>15</v>
       </c>
-      <c r="F164" s="77" t="s">
+      <c r="F164" s="74" t="s">
         <v>653</v>
       </c>
       <c r="M164">
@@ -10594,10 +10593,10 @@
       <c r="C165" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E165" s="70">
+      <c r="E165" s="67">
         <v>16</v>
       </c>
-      <c r="F165" s="106" t="s">
+      <c r="F165" s="103" t="s">
         <v>707</v>
       </c>
       <c r="M165">
@@ -10619,10 +10618,10 @@
       <c r="C166" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E166" s="70">
+      <c r="E166" s="67">
         <v>17</v>
       </c>
-      <c r="F166" s="78" t="s">
+      <c r="F166" s="75" t="s">
         <v>403</v>
       </c>
       <c r="M166">
@@ -10644,10 +10643,10 @@
       <c r="C167" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E167" s="70">
+      <c r="E167" s="67">
         <v>18</v>
       </c>
-      <c r="F167" s="104" t="s">
+      <c r="F167" s="101" t="s">
         <v>694</v>
       </c>
       <c r="M167">
@@ -10663,17 +10662,17 @@
       </c>
     </row>
     <row r="168" spans="2:15" ht="12.75">
-      <c r="B168" s="109">
+      <c r="B168" s="106">
         <v>163</v>
       </c>
-      <c r="C168" s="110" t="s">
+      <c r="C168" s="107" t="s">
         <v>33</v>
       </c>
-      <c r="D168" s="111"/>
-      <c r="E168" s="109">
+      <c r="D168" s="108"/>
+      <c r="E168" s="106">
         <v>1</v>
       </c>
-      <c r="F168" s="108" t="s">
+      <c r="F168" s="105" t="s">
         <v>512</v>
       </c>
       <c r="M168">
@@ -10698,7 +10697,7 @@
       <c r="E169" s="1">
         <v>2</v>
       </c>
-      <c r="F169" s="68" t="s">
+      <c r="F169" s="65" t="s">
         <v>561</v>
       </c>
       <c r="M169">
@@ -10723,7 +10722,7 @@
       <c r="E170" s="1">
         <v>3</v>
       </c>
-      <c r="F170" s="78" t="s">
+      <c r="F170" s="75" t="s">
         <v>546</v>
       </c>
       <c r="M170">
@@ -10748,7 +10747,7 @@
       <c r="E171" s="1">
         <v>4</v>
       </c>
-      <c r="F171" s="108" t="s">
+      <c r="F171" s="105" t="s">
         <v>575</v>
       </c>
       <c r="M171">
@@ -10773,7 +10772,7 @@
       <c r="E172" s="1">
         <v>5</v>
       </c>
-      <c r="F172" s="77" t="s">
+      <c r="F172" s="74" t="s">
         <v>646</v>
       </c>
       <c r="M172">
@@ -10798,7 +10797,7 @@
       <c r="E173" s="1">
         <v>6</v>
       </c>
-      <c r="F173" s="105" t="s">
+      <c r="F173" s="102" t="s">
         <v>666</v>
       </c>
       <c r="M173">
@@ -10823,7 +10822,7 @@
       <c r="E174" s="1">
         <v>7</v>
       </c>
-      <c r="F174" s="100" t="s">
+      <c r="F174" s="97" t="s">
         <v>732</v>
       </c>
       <c r="M174">
@@ -10848,7 +10847,7 @@
       <c r="E175" s="1">
         <v>8</v>
       </c>
-      <c r="F175" s="103" t="s">
+      <c r="F175" s="100" t="s">
         <v>678</v>
       </c>
       <c r="M175">
@@ -10873,7 +10872,7 @@
       <c r="E176" s="1">
         <v>9</v>
       </c>
-      <c r="F176" s="78" t="s">
+      <c r="F176" s="75" t="s">
         <v>611</v>
       </c>
       <c r="M176">
@@ -10898,7 +10897,7 @@
       <c r="E177" s="1">
         <v>10</v>
       </c>
-      <c r="F177" s="68" t="s">
+      <c r="F177" s="65" t="s">
         <v>615</v>
       </c>
       <c r="M177">
@@ -10923,7 +10922,7 @@
       <c r="E178" s="1">
         <v>11</v>
       </c>
-      <c r="F178" s="78" t="s">
+      <c r="F178" s="75" t="s">
         <v>388</v>
       </c>
       <c r="M178">
@@ -10948,7 +10947,7 @@
       <c r="E179" s="1">
         <v>12</v>
       </c>
-      <c r="F179" s="77" t="s">
+      <c r="F179" s="74" t="s">
         <v>641</v>
       </c>
       <c r="M179">
@@ -10976,7 +10975,7 @@
       <c r="E180" s="1">
         <v>13</v>
       </c>
-      <c r="F180" s="107" t="s">
+      <c r="F180" s="104" t="s">
         <v>621</v>
       </c>
       <c r="M180">
@@ -11001,7 +11000,7 @@
       <c r="E181" s="1">
         <v>14</v>
       </c>
-      <c r="F181" s="100" t="s">
+      <c r="F181" s="97" t="s">
         <v>717</v>
       </c>
       <c r="M181">
@@ -11026,7 +11025,7 @@
       <c r="E182" s="1">
         <v>15</v>
       </c>
-      <c r="F182" s="68" t="s">
+      <c r="F182" s="65" t="s">
         <v>617</v>
       </c>
       <c r="M182">
@@ -11051,7 +11050,7 @@
       <c r="E183" s="1">
         <v>16</v>
       </c>
-      <c r="F183" s="103" t="s">
+      <c r="F183" s="100" t="s">
         <v>687</v>
       </c>
       <c r="M183">
@@ -11079,7 +11078,7 @@
       <c r="E184" s="1">
         <v>17</v>
       </c>
-      <c r="F184" s="108" t="s">
+      <c r="F184" s="105" t="s">
         <v>429</v>
       </c>
       <c r="M184">
@@ -11104,7 +11103,7 @@
       <c r="E185" s="1">
         <v>18</v>
       </c>
-      <c r="F185" s="100" t="s">
+      <c r="F185" s="97" t="s">
         <v>733</v>
       </c>
       <c r="M185">
@@ -11120,17 +11119,17 @@
       </c>
     </row>
     <row r="186" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B186" s="109">
+      <c r="B186" s="106">
         <v>181</v>
       </c>
-      <c r="C186" s="110" t="s">
+      <c r="C186" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="D186" s="111"/>
-      <c r="E186" s="109">
+      <c r="D186" s="108"/>
+      <c r="E186" s="106">
         <v>1</v>
       </c>
-      <c r="F186" s="108" t="s">
+      <c r="F186" s="105" t="s">
         <v>513</v>
       </c>
       <c r="M186">
@@ -11155,10 +11154,10 @@
       <c r="D187">
         <v>1.1100000000000001</v>
       </c>
-      <c r="E187" s="70">
+      <c r="E187" s="67">
         <v>2</v>
       </c>
-      <c r="F187" s="68" t="s">
+      <c r="F187" s="65" t="s">
         <v>750</v>
       </c>
       <c r="M187">
@@ -11180,10 +11179,10 @@
       <c r="C188" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E188" s="70">
+      <c r="E188" s="67">
         <v>3</v>
       </c>
-      <c r="F188" s="78" t="s">
+      <c r="F188" s="75" t="s">
         <v>547</v>
       </c>
       <c r="M188">
@@ -11205,10 +11204,10 @@
       <c r="C189" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E189" s="70">
+      <c r="E189" s="67">
         <v>4</v>
       </c>
-      <c r="F189" s="77" t="s">
+      <c r="F189" s="74" t="s">
         <v>647</v>
       </c>
       <c r="M189">
@@ -11230,10 +11229,10 @@
       <c r="C190" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E190" s="70">
+      <c r="E190" s="67">
         <v>5</v>
       </c>
-      <c r="F190" s="68" t="s">
+      <c r="F190" s="65" t="s">
         <v>464</v>
       </c>
       <c r="M190">
@@ -11255,10 +11254,10 @@
       <c r="C191" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E191" s="70">
+      <c r="E191" s="67">
         <v>6</v>
       </c>
-      <c r="F191" s="105" t="s">
+      <c r="F191" s="102" t="s">
         <v>668</v>
       </c>
       <c r="M191">
@@ -11280,10 +11279,10 @@
       <c r="C192" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E192" s="70">
+      <c r="E192" s="67">
         <v>7</v>
       </c>
-      <c r="F192" s="100" t="s">
+      <c r="F192" s="97" t="s">
         <v>737</v>
       </c>
       <c r="M192">
@@ -11305,10 +11304,10 @@
       <c r="C193" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E193" s="70">
+      <c r="E193" s="67">
         <v>8</v>
       </c>
-      <c r="F193" s="104" t="s">
+      <c r="F193" s="101" t="s">
         <v>699</v>
       </c>
       <c r="M193">
@@ -11330,10 +11329,10 @@
       <c r="C194" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E194" s="70">
+      <c r="E194" s="67">
         <v>9</v>
       </c>
-      <c r="F194" s="78" t="s">
+      <c r="F194" s="75" t="s">
         <v>588</v>
       </c>
       <c r="M194">
@@ -11355,10 +11354,10 @@
       <c r="C195" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E195" s="70">
+      <c r="E195" s="67">
         <v>10</v>
       </c>
-      <c r="F195" s="108" t="s">
+      <c r="F195" s="105" t="s">
         <v>572</v>
       </c>
       <c r="M195">
@@ -11380,10 +11379,10 @@
       <c r="C196" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E196" s="70">
+      <c r="E196" s="67">
         <v>11</v>
       </c>
-      <c r="F196" s="104" t="s">
+      <c r="F196" s="101" t="s">
         <v>700</v>
       </c>
       <c r="M196">
@@ -11405,10 +11404,10 @@
       <c r="C197" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E197" s="70">
+      <c r="E197" s="67">
         <v>12</v>
       </c>
-      <c r="F197" s="77" t="s">
+      <c r="F197" s="74" t="s">
         <v>626</v>
       </c>
       <c r="M197">
@@ -11433,10 +11432,10 @@
       <c r="D198">
         <v>1.22</v>
       </c>
-      <c r="E198" s="70">
+      <c r="E198" s="67">
         <v>13</v>
       </c>
-      <c r="F198" s="108" t="s">
+      <c r="F198" s="105" t="s">
         <v>429</v>
       </c>
       <c r="M198">
@@ -11458,10 +11457,10 @@
       <c r="C199" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E199" s="70">
+      <c r="E199" s="67">
         <v>14</v>
       </c>
-      <c r="F199" s="68" t="s">
+      <c r="F199" s="65" t="s">
         <v>618</v>
       </c>
       <c r="M199">
@@ -11483,10 +11482,10 @@
       <c r="C200" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E200" s="70">
+      <c r="E200" s="67">
         <v>15</v>
       </c>
-      <c r="F200" s="78" t="s">
+      <c r="F200" s="75" t="s">
         <v>585</v>
       </c>
       <c r="M200">
@@ -11508,10 +11507,10 @@
       <c r="C201" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E201" s="70">
+      <c r="E201" s="67">
         <v>16</v>
       </c>
-      <c r="F201" s="103" t="s">
+      <c r="F201" s="100" t="s">
         <v>691</v>
       </c>
       <c r="M201">
@@ -11533,10 +11532,10 @@
       <c r="C202" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E202" s="70">
+      <c r="E202" s="67">
         <v>17</v>
       </c>
-      <c r="F202" s="77" t="s">
+      <c r="F202" s="74" t="s">
         <v>636</v>
       </c>
       <c r="M202">
@@ -11558,10 +11557,10 @@
       <c r="C203" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E203" s="70">
+      <c r="E203" s="67">
         <v>18</v>
       </c>
-      <c r="F203" s="106" t="s">
+      <c r="F203" s="103" t="s">
         <v>703</v>
       </c>
       <c r="M203">
@@ -11577,17 +11576,17 @@
       </c>
     </row>
     <row r="204" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B204" s="109">
+      <c r="B204" s="106">
         <v>199</v>
       </c>
-      <c r="C204" s="110" t="s">
+      <c r="C204" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="D204" s="111"/>
-      <c r="E204" s="109">
+      <c r="D204" s="108"/>
+      <c r="E204" s="106">
         <v>1</v>
       </c>
-      <c r="F204" s="108" t="s">
+      <c r="F204" s="105" t="s">
         <v>514</v>
       </c>
       <c r="M204">
@@ -11612,7 +11611,7 @@
       <c r="E205" s="1">
         <v>2</v>
       </c>
-      <c r="F205" s="68" t="s">
+      <c r="F205" s="65" t="s">
         <v>751</v>
       </c>
       <c r="M205">
@@ -11637,7 +11636,7 @@
       <c r="E206" s="1">
         <v>3</v>
       </c>
-      <c r="F206" s="78" t="s">
+      <c r="F206" s="75" t="s">
         <v>548</v>
       </c>
       <c r="M206">
@@ -11662,7 +11661,7 @@
       <c r="E207" s="1">
         <v>4</v>
       </c>
-      <c r="F207" s="105" t="s">
+      <c r="F207" s="102" t="s">
         <v>663</v>
       </c>
       <c r="M207">
@@ -11687,7 +11686,7 @@
       <c r="E208" s="1">
         <v>5</v>
       </c>
-      <c r="F208" s="77" t="s">
+      <c r="F208" s="74" t="s">
         <v>643</v>
       </c>
       <c r="M208">
@@ -11712,7 +11711,7 @@
       <c r="E209" s="1">
         <v>6</v>
       </c>
-      <c r="F209" s="108" t="s">
+      <c r="F209" s="105" t="s">
         <v>573</v>
       </c>
       <c r="M209">
@@ -11740,7 +11739,7 @@
       <c r="E210" s="1">
         <v>7</v>
       </c>
-      <c r="F210" s="68" t="s">
+      <c r="F210" s="65" t="s">
         <v>614</v>
       </c>
       <c r="M210">
@@ -11765,7 +11764,7 @@
       <c r="E211" s="1">
         <v>8</v>
       </c>
-      <c r="F211" s="78" t="s">
+      <c r="F211" s="75" t="s">
         <v>594</v>
       </c>
       <c r="M211">
@@ -11790,7 +11789,7 @@
       <c r="E212" s="1">
         <v>9</v>
       </c>
-      <c r="F212" s="107" t="s">
+      <c r="F212" s="104" t="s">
         <v>622</v>
       </c>
       <c r="M212">
@@ -11815,7 +11814,7 @@
       <c r="E213" s="1">
         <v>10</v>
       </c>
-      <c r="F213" s="101" t="s">
+      <c r="F213" s="98" t="s">
         <v>657</v>
       </c>
       <c r="M213">
@@ -11840,7 +11839,7 @@
       <c r="E214" s="1">
         <v>11</v>
       </c>
-      <c r="F214" s="100" t="s">
+      <c r="F214" s="97" t="s">
         <v>714</v>
       </c>
       <c r="M214">
@@ -11865,7 +11864,7 @@
       <c r="E215" s="1">
         <v>12</v>
       </c>
-      <c r="F215" s="78" t="s">
+      <c r="F215" s="75" t="s">
         <v>595</v>
       </c>
       <c r="M215">
@@ -11890,7 +11889,7 @@
       <c r="E216" s="1">
         <v>13</v>
       </c>
-      <c r="F216" s="77" t="s">
+      <c r="F216" s="74" t="s">
         <v>654</v>
       </c>
       <c r="M216">
@@ -11915,7 +11914,7 @@
       <c r="E217" s="1">
         <v>14</v>
       </c>
-      <c r="F217" s="103" t="s">
+      <c r="F217" s="100" t="s">
         <v>673</v>
       </c>
       <c r="M217">
@@ -11943,7 +11942,7 @@
       <c r="E218" s="1">
         <v>15</v>
       </c>
-      <c r="F218" s="108" t="s">
+      <c r="F218" s="105" t="s">
         <v>429</v>
       </c>
       <c r="M218">
@@ -11968,7 +11967,7 @@
       <c r="E219" s="1">
         <v>16</v>
       </c>
-      <c r="F219" s="78" t="s">
+      <c r="F219" s="75" t="s">
         <v>605</v>
       </c>
       <c r="M219">
@@ -11993,7 +11992,7 @@
       <c r="E220" s="1">
         <v>17</v>
       </c>
-      <c r="F220" s="77" t="s">
+      <c r="F220" s="74" t="s">
         <v>639</v>
       </c>
       <c r="M220">
@@ -12018,7 +12017,7 @@
       <c r="E221" s="1">
         <v>18</v>
       </c>
-      <c r="F221" s="102" t="s">
+      <c r="F221" s="99" t="s">
         <v>742</v>
       </c>
       <c r="M221">
@@ -12034,19 +12033,19 @@
       </c>
     </row>
     <row r="222" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B222" s="109">
+      <c r="B222" s="106">
         <v>217</v>
       </c>
-      <c r="C222" s="110" t="s">
+      <c r="C222" s="107" t="s">
         <v>41</v>
       </c>
-      <c r="D222" s="111">
+      <c r="D222" s="108">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E222" s="109">
+      <c r="E222" s="106">
         <v>1</v>
       </c>
-      <c r="F222" s="108" t="s">
+      <c r="F222" s="105" t="s">
         <v>515</v>
       </c>
       <c r="M222">
@@ -12068,10 +12067,10 @@
       <c r="C223" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E223" s="70">
+      <c r="E223" s="67">
         <v>2</v>
       </c>
-      <c r="F223" s="68" t="s">
+      <c r="F223" s="65" t="s">
         <v>752</v>
       </c>
       <c r="M223">
@@ -12093,10 +12092,10 @@
       <c r="C224" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E224" s="70">
+      <c r="E224" s="67">
         <v>3</v>
       </c>
-      <c r="F224" s="78" t="s">
+      <c r="F224" s="75" t="s">
         <v>549</v>
       </c>
       <c r="M224">
@@ -12118,10 +12117,10 @@
       <c r="C225" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E225" s="70">
+      <c r="E225" s="67">
         <v>4</v>
       </c>
-      <c r="F225" s="105" t="s">
+      <c r="F225" s="102" t="s">
         <v>664</v>
       </c>
       <c r="M225">
@@ -12143,10 +12142,10 @@
       <c r="C226" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E226" s="70">
+      <c r="E226" s="67">
         <v>5</v>
       </c>
-      <c r="F226" s="108" t="s">
+      <c r="F226" s="105" t="s">
         <v>578</v>
       </c>
       <c r="M226">
@@ -12168,10 +12167,10 @@
       <c r="C227" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E227" s="70">
+      <c r="E227" s="67">
         <v>6</v>
       </c>
-      <c r="F227" s="100" t="s">
+      <c r="F227" s="97" t="s">
         <v>725</v>
       </c>
       <c r="M227">
@@ -12196,10 +12195,10 @@
       <c r="D228">
         <v>1.24</v>
       </c>
-      <c r="E228" s="70">
+      <c r="E228" s="67">
         <v>7</v>
       </c>
-      <c r="F228" s="108" t="s">
+      <c r="F228" s="105" t="s">
         <v>429</v>
       </c>
       <c r="M228">
@@ -12221,10 +12220,10 @@
       <c r="C229" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E229" s="70">
+      <c r="E229" s="67">
         <v>8</v>
       </c>
-      <c r="F229" s="68" t="s">
+      <c r="F229" s="65" t="s">
         <v>755</v>
       </c>
       <c r="M229">
@@ -12246,10 +12245,10 @@
       <c r="C230" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E230" s="70">
+      <c r="E230" s="67">
         <v>9</v>
       </c>
-      <c r="F230" s="78" t="s">
+      <c r="F230" s="75" t="s">
         <v>593</v>
       </c>
       <c r="M230">
@@ -12271,10 +12270,10 @@
       <c r="C231" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E231" s="70">
+      <c r="E231" s="67">
         <v>10</v>
       </c>
-      <c r="F231" s="77" t="s">
+      <c r="F231" s="74" t="s">
         <v>645</v>
       </c>
       <c r="M231">
@@ -12296,10 +12295,10 @@
       <c r="C232" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E232" s="70">
+      <c r="E232" s="67">
         <v>11</v>
       </c>
-      <c r="F232" s="103" t="s">
+      <c r="F232" s="100" t="s">
         <v>684</v>
       </c>
       <c r="M232">
@@ -12321,10 +12320,10 @@
       <c r="C233" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E233" s="70">
+      <c r="E233" s="67">
         <v>12</v>
       </c>
-      <c r="F233" s="78" t="s">
+      <c r="F233" s="75" t="s">
         <v>387</v>
       </c>
       <c r="M233">
@@ -12346,10 +12345,10 @@
       <c r="C234" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E234" s="70">
+      <c r="E234" s="67">
         <v>13</v>
       </c>
-      <c r="F234" s="103" t="s">
+      <c r="F234" s="100" t="s">
         <v>689</v>
       </c>
       <c r="M234">
@@ -12371,10 +12370,10 @@
       <c r="C235" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E235" s="70">
+      <c r="E235" s="67">
         <v>14</v>
       </c>
-      <c r="F235" s="106" t="s">
+      <c r="F235" s="103" t="s">
         <v>705</v>
       </c>
       <c r="M235">
@@ -12396,10 +12395,10 @@
       <c r="C236" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E236" s="70">
+      <c r="E236" s="67">
         <v>15</v>
       </c>
-      <c r="F236" s="78" t="s">
+      <c r="F236" s="75" t="s">
         <v>607</v>
       </c>
       <c r="M236">
@@ -12421,10 +12420,10 @@
       <c r="C237" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E237" s="70">
+      <c r="E237" s="67">
         <v>16</v>
       </c>
-      <c r="F237" s="77" t="s">
+      <c r="F237" s="74" t="s">
         <v>650</v>
       </c>
       <c r="M237">
@@ -12446,10 +12445,10 @@
       <c r="C238" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E238" s="70">
+      <c r="E238" s="67">
         <v>17</v>
       </c>
-      <c r="F238" s="100" t="s">
+      <c r="F238" s="97" t="s">
         <v>731</v>
       </c>
       <c r="M238">
@@ -12471,10 +12470,10 @@
       <c r="C239" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E239" s="70">
+      <c r="E239" s="67">
         <v>18</v>
       </c>
-      <c r="F239" s="106" t="s">
+      <c r="F239" s="103" t="s">
         <v>711</v>
       </c>
       <c r="H239">
@@ -12493,17 +12492,17 @@
       </c>
     </row>
     <row r="240" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B240" s="109">
+      <c r="B240" s="106">
         <v>235</v>
       </c>
-      <c r="C240" s="110" t="s">
+      <c r="C240" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="D240" s="111"/>
-      <c r="E240" s="109">
+      <c r="D240" s="108"/>
+      <c r="E240" s="106">
         <v>1</v>
       </c>
-      <c r="F240" s="108" t="s">
+      <c r="F240" s="105" t="s">
         <v>516</v>
       </c>
       <c r="H240">
@@ -12531,7 +12530,7 @@
       <c r="E241" s="1">
         <v>2</v>
       </c>
-      <c r="F241" s="68" t="s">
+      <c r="F241" s="65" t="s">
         <v>753</v>
       </c>
       <c r="H241">
@@ -12559,7 +12558,7 @@
       <c r="E242" s="1">
         <v>3</v>
       </c>
-      <c r="F242" s="78" t="s">
+      <c r="F242" s="75" t="s">
         <v>550</v>
       </c>
       <c r="H242" t="s">
@@ -12587,7 +12586,7 @@
       <c r="E243" s="1">
         <v>4</v>
       </c>
-      <c r="F243" s="105" t="s">
+      <c r="F243" s="102" t="s">
         <v>661</v>
       </c>
       <c r="H243" t="s">
@@ -12615,7 +12614,7 @@
       <c r="E244" s="1">
         <v>5</v>
       </c>
-      <c r="F244" s="68" t="s">
+      <c r="F244" s="65" t="s">
         <v>748</v>
       </c>
       <c r="H244" t="s">
@@ -12646,7 +12645,7 @@
       <c r="E245" s="1">
         <v>6</v>
       </c>
-      <c r="F245" s="78" t="s">
+      <c r="F245" s="75" t="s">
         <v>596</v>
       </c>
       <c r="H245" t="s">
@@ -12674,7 +12673,7 @@
       <c r="E246" s="1">
         <v>7</v>
       </c>
-      <c r="F246" s="100" t="s">
+      <c r="F246" s="97" t="s">
         <v>728</v>
       </c>
       <c r="H246" t="s">
@@ -12702,7 +12701,7 @@
       <c r="E247" s="1">
         <v>8</v>
       </c>
-      <c r="F247" s="108" t="s">
+      <c r="F247" s="105" t="s">
         <v>388</v>
       </c>
       <c r="H247" t="s">
@@ -12730,7 +12729,7 @@
       <c r="E248" s="1">
         <v>9</v>
       </c>
-      <c r="F248" s="77" t="s">
+      <c r="F248" s="74" t="s">
         <v>644</v>
       </c>
       <c r="H248" t="s">
@@ -12758,7 +12757,7 @@
       <c r="E249" s="1">
         <v>10</v>
       </c>
-      <c r="F249" s="100" t="s">
+      <c r="F249" s="97" t="s">
         <v>719</v>
       </c>
       <c r="H249" t="s">
@@ -12792,7 +12791,7 @@
       <c r="E250" s="1">
         <v>11</v>
       </c>
-      <c r="F250" s="108" t="s">
+      <c r="F250" s="105" t="s">
         <v>429</v>
       </c>
       <c r="H250" t="s">
@@ -12823,7 +12822,7 @@
       <c r="E251" s="1">
         <v>12</v>
       </c>
-      <c r="F251" s="103" t="s">
+      <c r="F251" s="100" t="s">
         <v>693</v>
       </c>
       <c r="H251" t="s">
@@ -12854,7 +12853,7 @@
       <c r="E252" s="1">
         <v>13</v>
       </c>
-      <c r="F252" s="68" t="s">
+      <c r="F252" s="65" t="s">
         <v>619</v>
       </c>
       <c r="H252" t="s">
@@ -12885,7 +12884,7 @@
       <c r="E253" s="1">
         <v>14</v>
       </c>
-      <c r="F253" s="77" t="s">
+      <c r="F253" s="74" t="s">
         <v>631</v>
       </c>
       <c r="H253" t="s">
@@ -12913,7 +12912,7 @@
       <c r="E254" s="1">
         <v>15</v>
       </c>
-      <c r="F254" s="78" t="s">
+      <c r="F254" s="75" t="s">
         <v>586</v>
       </c>
       <c r="H254" t="s">
@@ -12941,7 +12940,7 @@
       <c r="E255" s="1">
         <v>16</v>
       </c>
-      <c r="F255" s="77" t="s">
+      <c r="F255" s="74" t="s">
         <v>652</v>
       </c>
       <c r="H255" t="s">
@@ -12969,7 +12968,7 @@
       <c r="E256" s="1">
         <v>17</v>
       </c>
-      <c r="F256" s="103" t="s">
+      <c r="F256" s="100" t="s">
         <v>681</v>
       </c>
       <c r="H256" t="s">
@@ -12997,7 +12996,7 @@
       <c r="E257" s="1">
         <v>18</v>
       </c>
-      <c r="F257" s="104" t="s">
+      <c r="F257" s="101" t="s">
         <v>701</v>
       </c>
       <c r="M257">
@@ -13013,17 +13012,17 @@
       </c>
     </row>
     <row r="258" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B258" s="109">
+      <c r="B258" s="106">
         <v>253</v>
       </c>
-      <c r="C258" s="110" t="s">
+      <c r="C258" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="D258" s="111"/>
-      <c r="E258" s="109">
+      <c r="D258" s="108"/>
+      <c r="E258" s="106">
         <v>1</v>
       </c>
-      <c r="F258" s="108" t="s">
+      <c r="F258" s="105" t="s">
         <v>517</v>
       </c>
       <c r="H258">
@@ -13048,10 +13047,10 @@
       <c r="C259" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E259" s="70">
+      <c r="E259" s="67">
         <v>2</v>
       </c>
-      <c r="F259" s="68" t="s">
+      <c r="F259" s="65" t="s">
         <v>754</v>
       </c>
       <c r="H259">
@@ -13079,10 +13078,10 @@
       <c r="D260">
         <v>1.1499999999999999</v>
       </c>
-      <c r="E260" s="70">
+      <c r="E260" s="67">
         <v>3</v>
       </c>
-      <c r="F260" s="78" t="s">
+      <c r="F260" s="75" t="s">
         <v>551</v>
       </c>
       <c r="H260" t="s">
@@ -13107,10 +13106,10 @@
       <c r="C261" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E261" s="70">
+      <c r="E261" s="67">
         <v>4</v>
       </c>
-      <c r="F261" s="77" t="s">
+      <c r="F261" s="74" t="s">
         <v>655</v>
       </c>
       <c r="H261" t="s">
@@ -13135,10 +13134,10 @@
       <c r="C262" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E262" s="70">
+      <c r="E262" s="67">
         <v>5</v>
       </c>
-      <c r="F262" s="105" t="s">
+      <c r="F262" s="102" t="s">
         <v>671</v>
       </c>
       <c r="H262" t="s">
@@ -13163,10 +13162,10 @@
       <c r="C263" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E263" s="70">
+      <c r="E263" s="67">
         <v>6</v>
       </c>
-      <c r="F263" s="104" t="s">
+      <c r="F263" s="101" t="s">
         <v>697</v>
       </c>
       <c r="H263" t="s">
@@ -13180,10 +13179,10 @@
       <c r="C264" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E264" s="70">
+      <c r="E264" s="67">
         <v>7</v>
       </c>
-      <c r="F264" s="103" t="s">
+      <c r="F264" s="100" t="s">
         <v>674</v>
       </c>
       <c r="H264" t="s">
@@ -13197,10 +13196,10 @@
       <c r="C265" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E265" s="70">
+      <c r="E265" s="67">
         <v>8</v>
       </c>
-      <c r="F265" s="78" t="s">
+      <c r="F265" s="75" t="s">
         <v>610</v>
       </c>
       <c r="H265" t="s">
@@ -13214,10 +13213,10 @@
       <c r="C266" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E266" s="70">
+      <c r="E266" s="67">
         <v>9</v>
       </c>
-      <c r="F266" s="77" t="s">
+      <c r="F266" s="74" t="s">
         <v>638</v>
       </c>
       <c r="H266" t="s">
@@ -13231,10 +13230,10 @@
       <c r="C267" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E267" s="70">
+      <c r="E267" s="67">
         <v>10</v>
       </c>
-      <c r="F267" s="106" t="s">
+      <c r="F267" s="103" t="s">
         <v>704</v>
       </c>
       <c r="H267" t="s">
@@ -13248,10 +13247,10 @@
       <c r="C268" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E268" s="70">
+      <c r="E268" s="67">
         <v>11</v>
       </c>
-      <c r="F268" s="108" t="s">
+      <c r="F268" s="105" t="s">
         <v>387</v>
       </c>
       <c r="H268" t="s">
@@ -13265,10 +13264,10 @@
       <c r="C269" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E269" s="70">
+      <c r="E269" s="67">
         <v>12</v>
       </c>
-      <c r="F269" s="68" t="s">
+      <c r="F269" s="65" t="s">
         <v>620</v>
       </c>
       <c r="H269" t="s">
@@ -13282,10 +13281,10 @@
       <c r="C270" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E270" s="70">
+      <c r="E270" s="67">
         <v>13</v>
       </c>
-      <c r="F270" s="100" t="s">
+      <c r="F270" s="97" t="s">
         <v>724</v>
       </c>
       <c r="H270" t="s">
@@ -13299,10 +13298,10 @@
       <c r="C271" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E271" s="70">
+      <c r="E271" s="67">
         <v>14</v>
       </c>
-      <c r="F271" s="78" t="s">
+      <c r="F271" s="75" t="s">
         <v>387</v>
       </c>
       <c r="H271" t="s">
@@ -13319,10 +13318,10 @@
       <c r="D272">
         <v>1.26</v>
       </c>
-      <c r="E272" s="70">
+      <c r="E272" s="67">
         <v>15</v>
       </c>
-      <c r="F272" s="108" t="s">
+      <c r="F272" s="105" t="s">
         <v>429</v>
       </c>
       <c r="H272" t="s">
@@ -13336,10 +13335,10 @@
       <c r="C273" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E273" s="70">
+      <c r="E273" s="67">
         <v>16</v>
       </c>
-      <c r="F273" s="102" t="s">
+      <c r="F273" s="99" t="s">
         <v>745</v>
       </c>
       <c r="H273" t="s">
@@ -13353,10 +13352,10 @@
       <c r="C274" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E274" s="70">
+      <c r="E274" s="67">
         <v>17</v>
       </c>
-      <c r="F274" s="100" t="s">
+      <c r="F274" s="97" t="s">
         <v>721</v>
       </c>
       <c r="H274" t="s">
@@ -13370,10 +13369,10 @@
       <c r="C275" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E275" s="70">
+      <c r="E275" s="67">
         <v>18</v>
       </c>
-      <c r="F275" s="106" t="s">
+      <c r="F275" s="103" t="s">
         <v>706</v>
       </c>
       <c r="H275" t="s">
@@ -14403,7 +14402,7 @@
       <c r="E70" t="s">
         <v>802</v>
       </c>
-      <c r="F70" s="113" t="s">
+      <c r="F70" s="1" t="s">
         <v>803</v>
       </c>
     </row>
@@ -15413,15 +15412,15 @@
       </c>
     </row>
     <row r="4" spans="3:22">
-      <c r="O4" s="62" t="s">
+      <c r="O4" s="111" t="s">
         <v>235</v>
       </c>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="63"/>
-      <c r="R4" s="63"/>
-      <c r="S4" s="63"/>
-      <c r="T4" s="63"/>
-      <c r="U4" s="63"/>
+      <c r="P4" s="112"/>
+      <c r="Q4" s="112"/>
+      <c r="R4" s="112"/>
+      <c r="S4" s="112"/>
+      <c r="T4" s="112"/>
+      <c r="U4" s="112"/>
     </row>
     <row r="5" spans="3:22">
       <c r="C5" s="1" t="s">

</xml_diff>

<commit_message>
Engine upgrade to Godot 4.3
Added Chestnut and Cherry upgrade calculations
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C65ED08-08F3-4A5A-9BA9-5D5853900B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C47D44B-4ACD-47A5-B9E3-9A6F55CD2797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="7848" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,19 @@
     <sheet name="Fishing" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -3241,6 +3254,7 @@
     <xf numFmtId="0" fontId="2" fillId="44" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3248,10 +3262,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Parasts" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3478,16 +3491,16 @@
       <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" customWidth="1"/>
-    <col min="9" max="9" width="37.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" customWidth="1"/>
+    <col min="9" max="9" width="37.6640625" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" customWidth="1"/>
+    <col min="13" max="13" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:10" ht="12.75">
+    <row r="5" spans="3:10" ht="13.2">
       <c r="G5" s="1" t="s">
         <v>0</v>
       </c>
@@ -3498,7 +3511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="3:10" ht="12.75">
+    <row r="6" spans="3:10" ht="13.2">
       <c r="G6" s="1">
         <v>1</v>
       </c>
@@ -3512,7 +3525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="3:10" ht="12.75">
+    <row r="7" spans="3:10" ht="13.2">
       <c r="G7" s="1">
         <v>1</v>
       </c>
@@ -3526,7 +3539,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="3:10" ht="12.75">
+    <row r="8" spans="3:10" ht="13.2">
       <c r="G8" s="1">
         <v>1</v>
       </c>
@@ -3540,7 +3553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="3:10" ht="12.75">
+    <row r="9" spans="3:10" ht="13.2">
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
@@ -3560,7 +3573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="3:10" ht="12.75">
+    <row r="10" spans="3:10" ht="13.2">
       <c r="G10" s="1">
         <v>1</v>
       </c>
@@ -3574,7 +3587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="3:10" ht="12.75">
+    <row r="11" spans="3:10" ht="13.2">
       <c r="G11" s="1">
         <v>1</v>
       </c>
@@ -3588,7 +3601,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="3:10" ht="12.75">
+    <row r="12" spans="3:10" ht="13.2">
       <c r="G12" s="1">
         <v>1</v>
       </c>
@@ -3602,7 +3615,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="3:10" ht="12.75">
+    <row r="13" spans="3:10" ht="13.2">
       <c r="G13" s="1">
         <v>2</v>
       </c>
@@ -3616,7 +3629,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="3:10" ht="12.75">
+    <row r="14" spans="3:10" ht="13.2">
       <c r="G14" s="1">
         <v>2</v>
       </c>
@@ -3630,7 +3643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="3:10" ht="12.75">
+    <row r="15" spans="3:10" ht="13.2">
       <c r="G15" s="1">
         <v>2</v>
       </c>
@@ -3642,7 +3655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="3:10" ht="12.75">
+    <row r="16" spans="3:10" ht="13.2">
       <c r="G16" s="1">
         <v>2</v>
       </c>
@@ -3656,7 +3669,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="6:10" ht="12.75">
+    <row r="17" spans="6:10" ht="13.2">
       <c r="G17" s="1">
         <v>2</v>
       </c>
@@ -3670,7 +3683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="6:10" ht="12.75">
+    <row r="18" spans="6:10" ht="13.2">
       <c r="G18" s="1">
         <v>2</v>
       </c>
@@ -3681,7 +3694,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="6:10" ht="12.75">
+    <row r="19" spans="6:10" ht="13.2">
       <c r="G19" s="1">
         <v>2</v>
       </c>
@@ -3695,7 +3708,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="6:10" ht="12.75">
+    <row r="20" spans="6:10" ht="13.2">
       <c r="G20" s="1">
         <v>3</v>
       </c>
@@ -3709,7 +3722,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="6:10" ht="12.75">
+    <row r="21" spans="6:10" ht="13.2">
       <c r="G21" s="1">
         <v>3</v>
       </c>
@@ -3723,7 +3736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="6:10" ht="12.75">
+    <row r="22" spans="6:10" ht="13.2">
       <c r="G22" s="1">
         <v>3</v>
       </c>
@@ -3737,7 +3750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="6:10" ht="12.75">
+    <row r="23" spans="6:10" ht="13.2">
       <c r="G23" s="1">
         <v>3</v>
       </c>
@@ -3751,7 +3764,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="6:10" ht="12.75">
+    <row r="24" spans="6:10" ht="13.2">
       <c r="G24" s="1">
         <v>3</v>
       </c>
@@ -3762,7 +3775,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="6:10" ht="12.75">
+    <row r="25" spans="6:10" ht="13.2">
       <c r="G25" s="1">
         <v>3</v>
       </c>
@@ -3776,7 +3789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="6:10" ht="12.75">
+    <row r="26" spans="6:10" ht="13.2">
       <c r="G26" s="1">
         <v>3</v>
       </c>
@@ -4091,15 +4104,15 @@
       <selection activeCell="F4" sqref="F4:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="12.75">
+    <row r="2" spans="1:15" ht="13.2">
       <c r="D2" s="1" t="s">
         <v>50</v>
       </c>
@@ -4107,7 +4120,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="12.75">
+    <row r="3" spans="1:15" ht="13.2">
       <c r="C3" s="1" t="s">
         <v>52</v>
       </c>
@@ -4139,7 +4152,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="12.75">
+    <row r="4" spans="1:15" ht="13.2">
       <c r="C4" s="1">
         <v>1</v>
       </c>
@@ -4172,7 +4185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="12.75">
+    <row r="5" spans="1:15" ht="13.2">
       <c r="C5" s="1">
         <v>2</v>
       </c>
@@ -4205,7 +4218,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="12.75">
+    <row r="6" spans="1:15" ht="13.2">
       <c r="C6" s="1">
         <v>3</v>
       </c>
@@ -4238,7 +4251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="12.75">
+    <row r="7" spans="1:15" ht="13.2">
       <c r="C7" s="1">
         <v>4</v>
       </c>
@@ -4271,7 +4284,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="12.75">
+    <row r="8" spans="1:15" ht="13.2">
       <c r="C8" s="1">
         <v>5</v>
       </c>
@@ -4304,7 +4317,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="12.75">
+    <row r="9" spans="1:15" ht="13.2">
       <c r="C9" s="1">
         <v>6</v>
       </c>
@@ -4337,7 +4350,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="12.75">
+    <row r="10" spans="1:15" ht="13.2">
       <c r="C10" s="1">
         <v>7</v>
       </c>
@@ -4370,7 +4383,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="12.75">
+    <row r="11" spans="1:15" ht="13.2">
       <c r="C11" s="1">
         <v>8</v>
       </c>
@@ -4403,7 +4416,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="12.75">
+    <row r="12" spans="1:15" ht="13.2">
       <c r="C12" s="1">
         <v>9</v>
       </c>
@@ -4436,7 +4449,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="12.75">
+    <row r="13" spans="1:15" ht="13.2">
       <c r="A13" s="39" t="s">
         <v>3</v>
       </c>
@@ -4472,7 +4485,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="12.75">
+    <row r="14" spans="1:15" ht="13.2">
       <c r="A14" s="35" t="s">
         <v>18</v>
       </c>
@@ -4508,7 +4521,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="12.75">
+    <row r="15" spans="1:15" ht="13.2">
       <c r="A15" s="35" t="s">
         <v>9</v>
       </c>
@@ -4544,7 +4557,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="12.75">
+    <row r="16" spans="1:15" ht="13.2">
       <c r="A16" s="35" t="s">
         <v>14</v>
       </c>
@@ -4580,7 +4593,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="12.75">
+    <row r="17" spans="1:15" ht="13.2">
       <c r="A17" s="35" t="s">
         <v>21</v>
       </c>
@@ -4616,7 +4629,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="12.75">
+    <row r="18" spans="1:15" ht="13.2">
       <c r="A18" s="35" t="s">
         <v>16</v>
       </c>
@@ -4652,7 +4665,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="12.75">
+    <row r="19" spans="1:15" ht="13.2">
       <c r="A19" s="47" t="s">
         <v>26</v>
       </c>
@@ -4660,7 +4673,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="12.75">
+    <row r="20" spans="1:15" ht="13.2">
       <c r="A20" s="35" t="s">
         <v>29</v>
       </c>
@@ -4668,7 +4681,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="12.75">
+    <row r="21" spans="1:15" ht="13.2">
       <c r="A21" s="35" t="s">
         <v>31</v>
       </c>
@@ -4676,7 +4689,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="12.75">
+    <row r="22" spans="1:15" ht="13.2">
       <c r="A22" s="35" t="s">
         <v>33</v>
       </c>
@@ -4684,7 +4697,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="12.75">
+    <row r="23" spans="1:15" ht="13.2">
       <c r="A23" s="35" t="s">
         <v>37</v>
       </c>
@@ -4692,7 +4705,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="12.75">
+    <row r="24" spans="1:15" ht="13.2">
       <c r="A24" s="35" t="s">
         <v>39</v>
       </c>
@@ -4700,7 +4713,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="12.75">
+    <row r="25" spans="1:15" ht="13.2">
       <c r="A25" s="35" t="s">
         <v>41</v>
       </c>
@@ -4708,7 +4721,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="12.75">
+    <row r="26" spans="1:15" ht="13.2">
       <c r="A26" s="35" t="s">
         <v>45</v>
       </c>
@@ -4716,7 +4729,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="12.75">
+    <row r="27" spans="1:15" ht="13.2">
       <c r="A27" s="35" t="s">
         <v>46</v>
       </c>
@@ -4724,12 +4737,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="12.75">
+    <row r="28" spans="1:15" ht="13.2">
       <c r="O28" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="12.75">
+    <row r="29" spans="1:15" ht="13.2">
       <c r="C29" s="1">
         <v>2</v>
       </c>
@@ -4762,12 +4775,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="12.75">
+    <row r="30" spans="1:15" ht="13.2">
       <c r="O30" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="12.75">
+    <row r="32" spans="1:15" ht="13.2">
       <c r="F32" s="23" t="s">
         <v>72</v>
       </c>
@@ -4777,7 +4790,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="12.75">
+    <row r="34" spans="2:12" ht="13.2">
       <c r="F34" s="23" t="s">
         <v>74</v>
       </c>
@@ -4955,40 +4968,41 @@
   </sheetPr>
   <dimension ref="A1:X276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B78" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H84" sqref="H84"/>
+    <sheetView tabSelected="1" topLeftCell="C112" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F131" sqref="F131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="38.42578125" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="28.140625" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" customWidth="1"/>
-    <col min="21" max="21" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="1.77734375" customWidth="1"/>
+    <col min="5" max="5" width="4.21875" customWidth="1"/>
+    <col min="6" max="6" width="40" customWidth="1"/>
+    <col min="7" max="7" width="32.88671875" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="28.109375" customWidth="1"/>
+    <col min="14" max="14" width="19.44140625" customWidth="1"/>
+    <col min="15" max="15" width="20.88671875" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" customWidth="1"/>
+    <col min="17" max="17" width="18.109375" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" customWidth="1"/>
+    <col min="20" max="20" width="14.44140625" customWidth="1"/>
+    <col min="21" max="21" width="21.44140625" customWidth="1"/>
     <col min="22" max="22" width="26" customWidth="1"/>
-    <col min="23" max="23" width="23.5703125" customWidth="1"/>
-    <col min="24" max="24" width="23.28515625" customWidth="1"/>
-    <col min="25" max="25" width="22.140625" customWidth="1"/>
-    <col min="26" max="26" width="31.42578125" customWidth="1"/>
-    <col min="27" max="27" width="37.7109375" customWidth="1"/>
-    <col min="28" max="28" width="29.42578125" customWidth="1"/>
-    <col min="29" max="29" width="29.85546875" customWidth="1"/>
-    <col min="30" max="30" width="28.7109375" customWidth="1"/>
-    <col min="31" max="31" width="33.140625" customWidth="1"/>
+    <col min="23" max="23" width="23.5546875" customWidth="1"/>
+    <col min="24" max="24" width="23.33203125" customWidth="1"/>
+    <col min="25" max="25" width="22.109375" customWidth="1"/>
+    <col min="26" max="26" width="31.44140625" customWidth="1"/>
+    <col min="27" max="27" width="37.6640625" customWidth="1"/>
+    <col min="28" max="28" width="29.44140625" customWidth="1"/>
+    <col min="29" max="29" width="29.88671875" customWidth="1"/>
+    <col min="30" max="30" width="28.6640625" customWidth="1"/>
+    <col min="31" max="31" width="33.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1">
@@ -4996,7 +5010,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="12.75">
+    <row r="2" spans="1:23" ht="13.2">
       <c r="C2" s="1" t="s">
         <v>75</v>
       </c>
@@ -5057,21 +5071,21 @@
       <c r="K5" s="45" t="s">
         <v>432</v>
       </c>
-      <c r="M5" s="110" t="s">
+      <c r="M5" s="111" t="s">
         <v>78</v>
       </c>
-      <c r="N5" s="110"/>
-      <c r="O5" s="110"/>
-      <c r="P5" s="110"/>
-      <c r="Q5" s="110"/>
-      <c r="R5" s="110"/>
-      <c r="S5" s="110"/>
-      <c r="T5" s="110"/>
-      <c r="U5" s="110"/>
-      <c r="V5" s="110"/>
-      <c r="W5" s="110"/>
-    </row>
-    <row r="6" spans="1:23" ht="13.5" thickBot="1">
+      <c r="N5" s="111"/>
+      <c r="O5" s="111"/>
+      <c r="P5" s="111"/>
+      <c r="Q5" s="111"/>
+      <c r="R5" s="111"/>
+      <c r="S5" s="111"/>
+      <c r="T5" s="111"/>
+      <c r="U5" s="111"/>
+      <c r="V5" s="111"/>
+      <c r="W5" s="111"/>
+    </row>
+    <row r="6" spans="1:23" ht="13.8" thickBot="1">
       <c r="A6" s="35" t="s">
         <v>18</v>
       </c>
@@ -5140,7 +5154,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="12.75">
+    <row r="7" spans="1:23" ht="13.2">
       <c r="A7" s="35" t="s">
         <v>9</v>
       </c>
@@ -5212,7 +5226,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="12.75">
+    <row r="8" spans="1:23" ht="13.2">
       <c r="A8" s="35" t="s">
         <v>14</v>
       </c>
@@ -5283,7 +5297,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="12.75">
+    <row r="9" spans="1:23" ht="13.2">
       <c r="A9" s="35" t="s">
         <v>21</v>
       </c>
@@ -5351,7 +5365,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="12.75">
+    <row r="10" spans="1:23" ht="13.2">
       <c r="A10" s="35" t="s">
         <v>16</v>
       </c>
@@ -5406,7 +5420,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="12.75">
+    <row r="11" spans="1:23" ht="13.2">
       <c r="A11" s="47" t="s">
         <v>26</v>
       </c>
@@ -5465,7 +5479,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="12.75">
+    <row r="12" spans="1:23" ht="13.2">
       <c r="A12" s="35" t="s">
         <v>29</v>
       </c>
@@ -5519,7 +5533,7 @@
       </c>
       <c r="W12" s="40"/>
     </row>
-    <row r="13" spans="1:23" ht="12.75">
+    <row r="13" spans="1:23" ht="13.2">
       <c r="A13" s="35" t="s">
         <v>31</v>
       </c>
@@ -5566,7 +5580,7 @@
       </c>
       <c r="W13" s="40"/>
     </row>
-    <row r="14" spans="1:23" ht="12.75">
+    <row r="14" spans="1:23" ht="13.2">
       <c r="A14" s="35" t="s">
         <v>33</v>
       </c>
@@ -5600,7 +5614,7 @@
       <c r="V14" s="38"/>
       <c r="W14" s="40"/>
     </row>
-    <row r="15" spans="1:23" ht="12.75">
+    <row r="15" spans="1:23" ht="13.2">
       <c r="A15" s="35" t="s">
         <v>37</v>
       </c>
@@ -5634,7 +5648,7 @@
       <c r="V15" s="38"/>
       <c r="W15" s="40"/>
     </row>
-    <row r="16" spans="1:23" ht="12.75">
+    <row r="16" spans="1:23" ht="13.2">
       <c r="A16" s="35" t="s">
         <v>39</v>
       </c>
@@ -5668,7 +5682,7 @@
       <c r="V16" s="42"/>
       <c r="W16" s="43"/>
     </row>
-    <row r="17" spans="1:23" ht="12.75">
+    <row r="17" spans="1:23" ht="13.2">
       <c r="A17" s="35" t="s">
         <v>41</v>
       </c>
@@ -5704,7 +5718,7 @@
       <c r="V17" s="40"/>
       <c r="W17" s="40"/>
     </row>
-    <row r="18" spans="1:23" ht="12.75">
+    <row r="18" spans="1:23" ht="13.2">
       <c r="A18" s="35" t="s">
         <v>45</v>
       </c>
@@ -5736,7 +5750,7 @@
       <c r="V18" s="40"/>
       <c r="W18" s="40"/>
     </row>
-    <row r="19" spans="1:23" ht="12.75">
+    <row r="19" spans="1:23" ht="13.2">
       <c r="A19" s="35" t="s">
         <v>46</v>
       </c>
@@ -5769,7 +5783,7 @@
       <c r="V19" s="40"/>
       <c r="W19" s="40"/>
     </row>
-    <row r="20" spans="1:23" ht="12.75">
+    <row r="20" spans="1:23" ht="13.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>15</v>
@@ -5797,7 +5811,7 @@
       <c r="V20" s="40"/>
       <c r="W20" s="40"/>
     </row>
-    <row r="21" spans="1:23" ht="12.75">
+    <row r="21" spans="1:23" ht="13.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>16</v>
@@ -5828,7 +5842,7 @@
       <c r="V21" s="40"/>
       <c r="W21" s="40"/>
     </row>
-    <row r="22" spans="1:23" ht="12.75">
+    <row r="22" spans="1:23" ht="13.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>17</v>
@@ -5856,7 +5870,7 @@
       <c r="V22" s="40"/>
       <c r="W22" s="40"/>
     </row>
-    <row r="23" spans="1:23" ht="12.75">
+    <row r="23" spans="1:23" ht="13.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
         <v>18</v>
@@ -5893,7 +5907,7 @@
       <c r="V23" s="40"/>
       <c r="W23" s="40"/>
     </row>
-    <row r="24" spans="1:23" ht="12.75">
+    <row r="24" spans="1:23" ht="13.2">
       <c r="A24" s="1"/>
       <c r="B24" s="106">
         <v>19</v>
@@ -5933,7 +5947,7 @@
       <c r="V24" s="40"/>
       <c r="W24" s="40"/>
     </row>
-    <row r="25" spans="1:23" ht="12.75">
+    <row r="25" spans="1:23" ht="13.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1">
         <v>20</v>
@@ -5973,7 +5987,7 @@
       <c r="V25" s="40"/>
       <c r="W25" s="40"/>
     </row>
-    <row r="26" spans="1:23" ht="12.75">
+    <row r="26" spans="1:23" ht="13.2">
       <c r="B26" s="1">
         <v>21</v>
       </c>
@@ -6012,7 +6026,7 @@
       <c r="V26" s="40"/>
       <c r="W26" s="40"/>
     </row>
-    <row r="27" spans="1:23" ht="12.75">
+    <row r="27" spans="1:23" ht="13.2">
       <c r="B27" s="1">
         <v>22</v>
       </c>
@@ -6051,14 +6065,14 @@
       <c r="V27" s="40"/>
       <c r="W27" s="40"/>
     </row>
-    <row r="28" spans="1:23" ht="12.75">
+    <row r="28" spans="1:23" ht="13.2">
       <c r="B28" s="1">
         <v>23</v>
       </c>
       <c r="C28" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="113">
+      <c r="E28" s="110">
         <v>5</v>
       </c>
       <c r="F28" s="105" t="s">
@@ -6084,7 +6098,7 @@
       <c r="V28" s="40"/>
       <c r="W28" s="40"/>
     </row>
-    <row r="29" spans="1:23" ht="12.75">
+    <row r="29" spans="1:23" ht="13.2">
       <c r="B29" s="1">
         <v>24</v>
       </c>
@@ -6115,7 +6129,7 @@
       <c r="V29" s="40"/>
       <c r="W29" s="40"/>
     </row>
-    <row r="30" spans="1:23" ht="12.75">
+    <row r="30" spans="1:23" ht="13.2">
       <c r="B30" s="1">
         <v>25</v>
       </c>
@@ -6149,7 +6163,7 @@
       <c r="V30" s="40"/>
       <c r="W30" s="40"/>
     </row>
-    <row r="31" spans="1:23" ht="12.75">
+    <row r="31" spans="1:23" ht="13.2">
       <c r="B31" s="1">
         <v>26</v>
       </c>
@@ -6172,7 +6186,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="12.75">
+    <row r="32" spans="1:23" ht="13.2">
       <c r="B32" s="1">
         <v>27</v>
       </c>
@@ -6195,7 +6209,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="18.75" thickBot="1">
+    <row r="33" spans="1:24" ht="18" thickBot="1">
       <c r="B33" s="1">
         <v>28</v>
       </c>
@@ -6212,7 +6226,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="18.75" thickBot="1">
+    <row r="34" spans="1:24" ht="18" thickBot="1">
       <c r="B34" s="1">
         <v>29</v>
       </c>
@@ -6240,7 +6254,7 @@
       <c r="V34" s="53"/>
       <c r="W34" s="53"/>
     </row>
-    <row r="35" spans="1:24" ht="13.5" thickBot="1">
+    <row r="35" spans="1:24" ht="13.8" thickBot="1">
       <c r="B35" s="1">
         <v>30</v>
       </c>
@@ -6293,7 +6307,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="12.75">
+    <row r="36" spans="1:24" ht="13.2">
       <c r="B36" s="1">
         <v>31</v>
       </c>
@@ -6350,7 +6364,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="12.75">
+    <row r="37" spans="1:24" ht="13.2">
       <c r="B37" s="1">
         <v>32</v>
       </c>
@@ -6408,7 +6422,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="12.75">
+    <row r="38" spans="1:24" ht="13.2">
       <c r="B38" s="1">
         <v>33</v>
       </c>
@@ -6465,7 +6479,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="12.75">
+    <row r="39" spans="1:24" ht="13.2">
       <c r="B39" s="1">
         <v>34</v>
       </c>
@@ -6523,7 +6537,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="12.75">
+    <row r="40" spans="1:24" ht="13.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -6580,7 +6594,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="12.75">
+    <row r="41" spans="1:24" ht="13.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -6634,7 +6648,7 @@
       </c>
       <c r="X41" s="55"/>
     </row>
-    <row r="42" spans="1:24" ht="12.75">
+    <row r="42" spans="1:24" ht="13.2">
       <c r="A42">
         <v>7</v>
       </c>
@@ -6691,7 +6705,7 @@
       </c>
       <c r="X42" s="55"/>
     </row>
-    <row r="43" spans="1:24" ht="12.75">
+    <row r="43" spans="1:24" ht="13.2">
       <c r="A43">
         <v>10</v>
       </c>
@@ -6744,7 +6758,7 @@
       </c>
       <c r="X43" s="55"/>
     </row>
-    <row r="44" spans="1:24" ht="12.75">
+    <row r="44" spans="1:24" ht="13.2">
       <c r="A44">
         <v>13</v>
       </c>
@@ -6797,7 +6811,7 @@
       </c>
       <c r="X44" s="55"/>
     </row>
-    <row r="45" spans="1:24" ht="12.75">
+    <row r="45" spans="1:24" ht="13.2">
       <c r="A45">
         <v>16</v>
       </c>
@@ -6851,7 +6865,7 @@
       </c>
       <c r="X45" s="59"/>
     </row>
-    <row r="46" spans="1:24" ht="12.75">
+    <row r="46" spans="1:24" ht="13.2">
       <c r="A46">
         <v>19</v>
       </c>
@@ -6902,7 +6916,7 @@
       </c>
       <c r="X46" s="55"/>
     </row>
-    <row r="47" spans="1:24" ht="12.75">
+    <row r="47" spans="1:24" ht="13.2">
       <c r="A47">
         <v>22</v>
       </c>
@@ -6953,7 +6967,7 @@
       </c>
       <c r="X47" s="55"/>
     </row>
-    <row r="48" spans="1:24" ht="12.75">
+    <row r="48" spans="1:24" ht="13.2">
       <c r="A48">
         <v>25</v>
       </c>
@@ -7002,7 +7016,7 @@
       </c>
       <c r="X48" s="55"/>
     </row>
-    <row r="49" spans="1:24" ht="12.75">
+    <row r="49" spans="1:24" ht="13.2">
       <c r="A49">
         <v>28</v>
       </c>
@@ -7051,7 +7065,7 @@
       </c>
       <c r="X49" s="55"/>
     </row>
-    <row r="50" spans="1:24" ht="12.75">
+    <row r="50" spans="1:24" ht="13.2">
       <c r="A50">
         <v>31</v>
       </c>
@@ -7100,7 +7114,7 @@
       </c>
       <c r="X50" s="55"/>
     </row>
-    <row r="51" spans="1:24" ht="12.75">
+    <row r="51" spans="1:24" ht="13.2">
       <c r="A51">
         <v>34</v>
       </c>
@@ -7146,7 +7160,7 @@
       </c>
       <c r="X51" s="55"/>
     </row>
-    <row r="52" spans="1:24" ht="12.75">
+    <row r="52" spans="1:24" ht="13.2">
       <c r="A52">
         <v>37</v>
       </c>
@@ -7207,7 +7221,7 @@
       </c>
       <c r="X52" s="55"/>
     </row>
-    <row r="53" spans="1:24" ht="12.75">
+    <row r="53" spans="1:24" ht="13.2">
       <c r="A53">
         <v>40</v>
       </c>
@@ -7259,7 +7273,7 @@
       </c>
       <c r="X53" s="55"/>
     </row>
-    <row r="54" spans="1:24" ht="12.75">
+    <row r="54" spans="1:24" ht="13.2">
       <c r="A54">
         <v>43</v>
       </c>
@@ -7308,7 +7322,7 @@
       </c>
       <c r="X54" s="55"/>
     </row>
-    <row r="55" spans="1:24" ht="12.75">
+    <row r="55" spans="1:24" ht="13.2">
       <c r="A55">
         <v>46</v>
       </c>
@@ -7366,7 +7380,7 @@
       </c>
       <c r="X55" s="55"/>
     </row>
-    <row r="56" spans="1:24" ht="12.75">
+    <row r="56" spans="1:24" ht="13.2">
       <c r="A56">
         <v>49</v>
       </c>
@@ -7415,7 +7429,7 @@
       </c>
       <c r="X56" s="55"/>
     </row>
-    <row r="57" spans="1:24" ht="12.75">
+    <row r="57" spans="1:24" ht="13.2">
       <c r="A57">
         <v>52</v>
       </c>
@@ -7467,7 +7481,7 @@
       </c>
       <c r="X57" s="55"/>
     </row>
-    <row r="58" spans="1:24" ht="12.75">
+    <row r="58" spans="1:24" ht="13.2">
       <c r="A58">
         <v>55</v>
       </c>
@@ -7512,7 +7526,7 @@
       </c>
       <c r="X58" s="55"/>
     </row>
-    <row r="59" spans="1:24" ht="12.75">
+    <row r="59" spans="1:24" ht="13.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -7560,7 +7574,7 @@
       </c>
       <c r="X59" s="55"/>
     </row>
-    <row r="60" spans="1:24" ht="12.75">
+    <row r="60" spans="1:24" ht="13.2">
       <c r="A60">
         <v>61</v>
       </c>
@@ -7603,7 +7617,7 @@
       </c>
       <c r="X60" s="55"/>
     </row>
-    <row r="61" spans="1:24" ht="12.75">
+    <row r="61" spans="1:24" ht="13.2">
       <c r="A61">
         <v>64</v>
       </c>
@@ -7648,7 +7662,7 @@
       </c>
       <c r="X61" s="55"/>
     </row>
-    <row r="62" spans="1:24" ht="12.75">
+    <row r="62" spans="1:24" ht="13.2">
       <c r="A62">
         <v>9887654321</v>
       </c>
@@ -7690,7 +7704,7 @@
       </c>
       <c r="X62" s="55"/>
     </row>
-    <row r="63" spans="1:24" ht="12.75">
+    <row r="63" spans="1:24" ht="13.2">
       <c r="B63" s="1">
         <v>58</v>
       </c>
@@ -7729,7 +7743,7 @@
       </c>
       <c r="X63" s="55"/>
     </row>
-    <row r="64" spans="1:24" ht="12.75">
+    <row r="64" spans="1:24" ht="13.2">
       <c r="B64" s="1">
         <v>59</v>
       </c>
@@ -7766,7 +7780,7 @@
       <c r="W64" s="55"/>
       <c r="X64" s="55"/>
     </row>
-    <row r="65" spans="2:24" ht="12.75">
+    <row r="65" spans="2:24" ht="13.2">
       <c r="B65" s="1">
         <v>60</v>
       </c>
@@ -7803,7 +7817,7 @@
       <c r="W65" s="55"/>
       <c r="X65" s="55"/>
     </row>
-    <row r="66" spans="2:24" ht="12.75">
+    <row r="66" spans="2:24" ht="13.2">
       <c r="B66" s="1">
         <v>61</v>
       </c>
@@ -7840,7 +7854,7 @@
       <c r="W66" s="55"/>
       <c r="X66" s="55"/>
     </row>
-    <row r="67" spans="2:24" ht="12.75">
+    <row r="67" spans="2:24" ht="13.2">
       <c r="B67" s="1">
         <v>62</v>
       </c>
@@ -7877,7 +7891,7 @@
       <c r="W67" s="55"/>
       <c r="X67" s="55"/>
     </row>
-    <row r="68" spans="2:24" ht="12.75">
+    <row r="68" spans="2:24" ht="13.2">
       <c r="B68" s="1">
         <v>63</v>
       </c>
@@ -7914,7 +7928,7 @@
       <c r="W68" s="55"/>
       <c r="X68" s="55"/>
     </row>
-    <row r="69" spans="2:24" ht="12.75">
+    <row r="69" spans="2:24" ht="13.2">
       <c r="B69" s="1">
         <v>64</v>
       </c>
@@ -7949,7 +7963,7 @@
       <c r="W69" s="55"/>
       <c r="X69" s="55"/>
     </row>
-    <row r="70" spans="2:24" ht="12.75">
+    <row r="70" spans="2:24" ht="13.2">
       <c r="B70" s="1">
         <v>65</v>
       </c>
@@ -7987,7 +8001,7 @@
       <c r="W70" s="55"/>
       <c r="X70" s="55"/>
     </row>
-    <row r="71" spans="2:24" ht="12.75">
+    <row r="71" spans="2:24" ht="13.2">
       <c r="B71" s="1">
         <v>66</v>
       </c>
@@ -8020,7 +8034,7 @@
       <c r="W71" s="55"/>
       <c r="X71" s="55"/>
     </row>
-    <row r="72" spans="2:24" ht="12.75">
+    <row r="72" spans="2:24" ht="13.2">
       <c r="B72" s="1">
         <v>67</v>
       </c>
@@ -8053,7 +8067,7 @@
       <c r="W72" s="55"/>
       <c r="X72" s="55"/>
     </row>
-    <row r="73" spans="2:24" ht="12.75">
+    <row r="73" spans="2:24" ht="13.2">
       <c r="B73" s="1">
         <v>68</v>
       </c>
@@ -8086,7 +8100,7 @@
       <c r="W73" s="55"/>
       <c r="X73" s="55"/>
     </row>
-    <row r="74" spans="2:24" ht="12.75">
+    <row r="74" spans="2:24" ht="13.2">
       <c r="B74" s="1">
         <v>69</v>
       </c>
@@ -8119,7 +8133,7 @@
       <c r="W74" s="55"/>
       <c r="X74" s="55"/>
     </row>
-    <row r="75" spans="2:24" ht="12.75">
+    <row r="75" spans="2:24" ht="13.2">
       <c r="B75" s="1">
         <v>70</v>
       </c>
@@ -8152,7 +8166,7 @@
       <c r="W75" s="55"/>
       <c r="X75" s="55"/>
     </row>
-    <row r="76" spans="2:24" ht="12.75">
+    <row r="76" spans="2:24" ht="13.2">
       <c r="B76" s="1">
         <v>71</v>
       </c>
@@ -8185,7 +8199,7 @@
       <c r="W76" s="55"/>
       <c r="X76" s="55"/>
     </row>
-    <row r="77" spans="2:24" ht="12.75">
+    <row r="77" spans="2:24" ht="13.2">
       <c r="B77" s="1">
         <v>72</v>
       </c>
@@ -8218,7 +8232,7 @@
       <c r="W77" s="55"/>
       <c r="X77" s="55"/>
     </row>
-    <row r="78" spans="2:24" ht="12.75">
+    <row r="78" spans="2:24" ht="13.2">
       <c r="B78" s="106">
         <v>73</v>
       </c>
@@ -8252,7 +8266,7 @@
       <c r="W78" s="55"/>
       <c r="X78" s="55"/>
     </row>
-    <row r="79" spans="2:24" ht="12.75">
+    <row r="79" spans="2:24" ht="13.2">
       <c r="B79" s="1">
         <v>74</v>
       </c>
@@ -8285,7 +8299,7 @@
       <c r="W79" s="55"/>
       <c r="X79" s="55"/>
     </row>
-    <row r="80" spans="2:24" ht="12.75">
+    <row r="80" spans="2:24" ht="13.2">
       <c r="B80" s="1">
         <v>75</v>
       </c>
@@ -8318,7 +8332,7 @@
       <c r="W80" s="55"/>
       <c r="X80" s="55"/>
     </row>
-    <row r="81" spans="2:24" ht="12.75">
+    <row r="81" spans="2:24" ht="13.2">
       <c r="B81" s="1">
         <v>76</v>
       </c>
@@ -8349,7 +8363,7 @@
       <c r="W81" s="55"/>
       <c r="X81" s="55"/>
     </row>
-    <row r="82" spans="2:24" ht="12.75">
+    <row r="82" spans="2:24" ht="13.2">
       <c r="B82" s="1">
         <v>77</v>
       </c>
@@ -8380,7 +8394,7 @@
       <c r="W82" s="55"/>
       <c r="X82" s="55"/>
     </row>
-    <row r="83" spans="2:24" ht="12.75">
+    <row r="83" spans="2:24" ht="13.2">
       <c r="B83" s="1">
         <v>78</v>
       </c>
@@ -8414,7 +8428,7 @@
       <c r="W83" s="55"/>
       <c r="X83" s="55"/>
     </row>
-    <row r="84" spans="2:24" ht="12.75">
+    <row r="84" spans="2:24" ht="13.2">
       <c r="B84" s="1">
         <v>79</v>
       </c>
@@ -8445,7 +8459,7 @@
       <c r="W84" s="55"/>
       <c r="X84" s="55"/>
     </row>
-    <row r="85" spans="2:24" ht="12.75">
+    <row r="85" spans="2:24" ht="13.2">
       <c r="B85" s="1">
         <v>80</v>
       </c>
@@ -8476,7 +8490,7 @@
       <c r="W85" s="55"/>
       <c r="X85" s="55"/>
     </row>
-    <row r="86" spans="2:24" ht="12.75">
+    <row r="86" spans="2:24" ht="13.2">
       <c r="B86" s="1">
         <v>81</v>
       </c>
@@ -8507,7 +8521,7 @@
       <c r="W86" s="55"/>
       <c r="X86" s="55"/>
     </row>
-    <row r="87" spans="2:24" ht="12.75">
+    <row r="87" spans="2:24" ht="13.2">
       <c r="B87" s="1">
         <v>82</v>
       </c>
@@ -8557,7 +8571,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="2:24" ht="12.75">
+    <row r="88" spans="2:24" ht="13.2">
       <c r="B88" s="1">
         <v>83</v>
       </c>
@@ -8589,7 +8603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="2:24" ht="12.75">
+    <row r="89" spans="2:24" ht="13.2">
       <c r="B89" s="1">
         <v>84</v>
       </c>
@@ -8606,7 +8620,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="90" spans="2:24" ht="12.75">
+    <row r="90" spans="2:24" ht="13.2">
       <c r="B90" s="1">
         <v>85</v>
       </c>
@@ -8636,7 +8650,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="2:24" ht="12.75">
+    <row r="91" spans="2:24" ht="13.2">
       <c r="B91" s="1">
         <v>86</v>
       </c>
@@ -8666,7 +8680,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="92" spans="2:24" ht="12.75">
+    <row r="92" spans="2:24" ht="13.2">
       <c r="B92" s="1">
         <v>87</v>
       </c>
@@ -8696,7 +8710,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="2:24" ht="12.75">
+    <row r="93" spans="2:24" ht="13.2">
       <c r="B93" s="1">
         <v>88</v>
       </c>
@@ -8726,7 +8740,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="94" spans="2:24" ht="12.75">
+    <row r="94" spans="2:24" ht="13.2">
       <c r="B94" s="1">
         <v>89</v>
       </c>
@@ -8759,7 +8773,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="2:24" ht="12.75">
+    <row r="95" spans="2:24" ht="13.2">
       <c r="B95" s="1">
         <v>90</v>
       </c>
@@ -8789,7 +8803,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="2:24" ht="12.75">
+    <row r="96" spans="2:24" ht="13.2">
       <c r="B96" s="106">
         <v>91</v>
       </c>
@@ -8820,7 +8834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="2:24" ht="12.75">
+    <row r="97" spans="2:24" ht="13.2">
       <c r="B97" s="1">
         <v>92</v>
       </c>
@@ -8850,7 +8864,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="98" spans="2:24" ht="12.75">
+    <row r="98" spans="2:24" ht="13.2">
       <c r="B98" s="1">
         <v>93</v>
       </c>
@@ -8880,7 +8894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="2:24" ht="12.75">
+    <row r="99" spans="2:24" ht="13.2">
       <c r="B99" s="1">
         <v>94</v>
       </c>
@@ -8910,7 +8924,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="2:24" ht="12.75">
+    <row r="100" spans="2:24" ht="13.2">
       <c r="B100" s="1">
         <v>95</v>
       </c>
@@ -8940,7 +8954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="2:24" ht="12.75">
+    <row r="101" spans="2:24" ht="13.2">
       <c r="B101" s="1">
         <v>96</v>
       </c>
@@ -8970,7 +8984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="2:24" ht="12.75">
+    <row r="102" spans="2:24" ht="13.2">
       <c r="B102" s="1">
         <v>97</v>
       </c>
@@ -9000,7 +9014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="2:24" ht="12.75">
+    <row r="103" spans="2:24" ht="13.2">
       <c r="B103" s="1">
         <v>98</v>
       </c>
@@ -9015,7 +9029,7 @@
       </c>
       <c r="T103" s="45"/>
     </row>
-    <row r="104" spans="2:24" ht="12.75">
+    <row r="104" spans="2:24" ht="13.2">
       <c r="B104" s="1">
         <v>99</v>
       </c>
@@ -9029,7 +9043,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="105" spans="2:24" ht="12.75">
+    <row r="105" spans="2:24" ht="13.2">
       <c r="B105" s="1">
         <v>100</v>
       </c>
@@ -9043,7 +9057,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="106" spans="2:24" ht="12.75">
+    <row r="106" spans="2:24" ht="13.2">
       <c r="B106" s="1">
         <v>101</v>
       </c>
@@ -9057,7 +9071,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="107" spans="2:24" ht="12.75">
+    <row r="107" spans="2:24" ht="13.2">
       <c r="B107" s="1">
         <v>102</v>
       </c>
@@ -9071,7 +9085,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="108" spans="2:24" ht="12.75">
+    <row r="108" spans="2:24" ht="13.2">
       <c r="B108" s="1">
         <v>103</v>
       </c>
@@ -9088,7 +9102,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="109" spans="2:24" ht="12.75">
+    <row r="109" spans="2:24" ht="13.2">
       <c r="B109" s="1">
         <v>104</v>
       </c>
@@ -9114,7 +9128,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="110" spans="2:24" ht="12.75">
+    <row r="110" spans="2:24" ht="13.2">
       <c r="B110" s="1">
         <v>105</v>
       </c>
@@ -9128,7 +9142,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="111" spans="2:24" ht="12.75">
+    <row r="111" spans="2:24" ht="13.2">
       <c r="B111" s="1">
         <v>106</v>
       </c>
@@ -9142,7 +9156,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="112" spans="2:24" ht="12.75">
+    <row r="112" spans="2:24" ht="13.2">
       <c r="B112" s="1">
         <v>107</v>
       </c>
@@ -9163,7 +9177,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="113" spans="2:24" ht="12.75">
+    <row r="113" spans="2:24" ht="13.2">
       <c r="B113" s="1">
         <v>108</v>
       </c>
@@ -9209,7 +9223,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="114" spans="2:24" ht="12.75">
+    <row r="114" spans="2:24" ht="13.2">
       <c r="B114" s="106">
         <v>109</v>
       </c>
@@ -9252,7 +9266,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="2:24" ht="12.75">
+    <row r="115" spans="2:24" ht="13.2">
       <c r="B115" s="1">
         <v>110</v>
       </c>
@@ -9294,7 +9308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="2:24" ht="12.75">
+    <row r="116" spans="2:24" ht="13.2">
       <c r="B116" s="1">
         <v>111</v>
       </c>
@@ -9336,7 +9350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="2:24" ht="12.75">
+    <row r="117" spans="2:24" ht="13.2">
       <c r="B117" s="1">
         <v>112</v>
       </c>
@@ -9369,7 +9383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:24" ht="12.75">
+    <row r="118" spans="2:24" ht="13.2">
       <c r="B118" s="1">
         <v>113</v>
       </c>
@@ -9401,7 +9415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:24" ht="12.75">
+    <row r="119" spans="2:24" ht="13.2">
       <c r="B119" s="1">
         <v>114</v>
       </c>
@@ -9435,7 +9449,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="120" spans="2:24" ht="12.75">
+    <row r="120" spans="2:24" ht="13.2">
       <c r="B120" s="1">
         <v>115</v>
       </c>
@@ -9460,7 +9474,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="121" spans="2:24" ht="12.75">
+    <row r="121" spans="2:24" ht="13.2">
       <c r="B121" s="1">
         <v>116</v>
       </c>
@@ -9485,7 +9499,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="122" spans="2:24" ht="12.75">
+    <row r="122" spans="2:24" ht="13.2">
       <c r="B122" s="1">
         <v>117</v>
       </c>
@@ -9510,7 +9524,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="123" spans="2:24" ht="12.75">
+    <row r="123" spans="2:24" ht="13.2">
       <c r="B123" s="1">
         <v>118</v>
       </c>
@@ -9535,7 +9549,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="124" spans="2:24" ht="12.75">
+    <row r="124" spans="2:24" ht="13.2">
       <c r="B124" s="1">
         <v>119</v>
       </c>
@@ -9560,7 +9574,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="125" spans="2:24" ht="12.75">
+    <row r="125" spans="2:24" ht="13.2">
       <c r="B125" s="1">
         <v>120</v>
       </c>
@@ -9585,7 +9599,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="126" spans="2:24" ht="12.75">
+    <row r="126" spans="2:24" ht="13.2">
       <c r="B126" s="1">
         <v>121</v>
       </c>
@@ -9610,7 +9624,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="127" spans="2:24" ht="12.75">
+    <row r="127" spans="2:24" ht="13.2">
       <c r="B127" s="1">
         <v>122</v>
       </c>
@@ -9635,7 +9649,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="128" spans="2:24" ht="12.75">
+    <row r="128" spans="2:24" ht="13.2">
       <c r="B128" s="1">
         <v>123</v>
       </c>
@@ -9660,7 +9674,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="129" spans="2:15" ht="12.75">
+    <row r="129" spans="2:15" ht="13.2">
       <c r="B129" s="1">
         <v>124</v>
       </c>
@@ -9688,7 +9702,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="130" spans="2:15" ht="12.75">
+    <row r="130" spans="2:15" ht="13.2">
       <c r="B130" s="1">
         <v>125</v>
       </c>
@@ -9713,7 +9727,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="131" spans="2:15" ht="12.75">
+    <row r="131" spans="2:15" ht="13.2">
       <c r="B131" s="1">
         <v>126</v>
       </c>
@@ -9738,7 +9752,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="132" spans="2:15" ht="12.75">
+    <row r="132" spans="2:15" ht="13.2">
       <c r="B132" s="106">
         <v>127</v>
       </c>
@@ -9767,7 +9781,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="133" spans="2:15" ht="12.75">
+    <row r="133" spans="2:15" ht="13.2">
       <c r="B133" s="1">
         <v>128</v>
       </c>
@@ -9795,7 +9809,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="134" spans="2:15" ht="12.75">
+    <row r="134" spans="2:15" ht="13.2">
       <c r="B134" s="1">
         <v>129</v>
       </c>
@@ -9823,7 +9837,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="135" spans="2:15" ht="12.75">
+    <row r="135" spans="2:15" ht="13.2">
       <c r="B135" s="1">
         <v>130</v>
       </c>
@@ -9848,7 +9862,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="136" spans="2:15" ht="12.75">
+    <row r="136" spans="2:15" ht="13.2">
       <c r="B136" s="1">
         <v>131</v>
       </c>
@@ -9876,7 +9890,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="137" spans="2:15" ht="12.75">
+    <row r="137" spans="2:15" ht="13.2">
       <c r="B137" s="1">
         <v>132</v>
       </c>
@@ -9901,7 +9915,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="138" spans="2:15" ht="12.75">
+    <row r="138" spans="2:15" ht="13.2">
       <c r="B138" s="1">
         <v>133</v>
       </c>
@@ -9926,7 +9940,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="139" spans="2:15" ht="12.75">
+    <row r="139" spans="2:15" ht="13.2">
       <c r="B139" s="1">
         <v>134</v>
       </c>
@@ -9951,7 +9965,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="140" spans="2:15" ht="12.75">
+    <row r="140" spans="2:15" ht="13.2">
       <c r="B140" s="1">
         <v>135</v>
       </c>
@@ -9976,7 +9990,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="141" spans="2:15" ht="12.75">
+    <row r="141" spans="2:15" ht="13.2">
       <c r="B141" s="1">
         <v>136</v>
       </c>
@@ -10001,7 +10015,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="142" spans="2:15" ht="12.75">
+    <row r="142" spans="2:15" ht="13.2">
       <c r="B142" s="1">
         <v>137</v>
       </c>
@@ -10026,7 +10040,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="143" spans="2:15" ht="12.75">
+    <row r="143" spans="2:15" ht="13.2">
       <c r="B143" s="1">
         <v>138</v>
       </c>
@@ -10051,7 +10065,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="144" spans="2:15" ht="12.75">
+    <row r="144" spans="2:15" ht="13.2">
       <c r="B144" s="1">
         <v>139</v>
       </c>
@@ -10076,7 +10090,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="145" spans="2:15" ht="12.75">
+    <row r="145" spans="2:15" ht="13.2">
       <c r="B145" s="1">
         <v>140</v>
       </c>
@@ -10101,7 +10115,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="146" spans="2:15" ht="12.75">
+    <row r="146" spans="2:15" ht="13.2">
       <c r="B146" s="1">
         <v>141</v>
       </c>
@@ -10126,7 +10140,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="147" spans="2:15" ht="12.75">
+    <row r="147" spans="2:15" ht="13.2">
       <c r="B147" s="1">
         <v>142</v>
       </c>
@@ -10151,7 +10165,7 @@
         <v>1493</v>
       </c>
     </row>
-    <row r="148" spans="2:15" ht="12.75">
+    <row r="148" spans="2:15" ht="13.2">
       <c r="B148" s="1">
         <v>143</v>
       </c>
@@ -10176,7 +10190,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="149" spans="2:15" ht="12.75">
+    <row r="149" spans="2:15" ht="13.2">
       <c r="B149" s="1">
         <v>144</v>
       </c>
@@ -10204,7 +10218,7 @@
         <v>1723</v>
       </c>
     </row>
-    <row r="150" spans="2:15" ht="12.75">
+    <row r="150" spans="2:15" ht="13.2">
       <c r="B150" s="106">
         <v>145</v>
       </c>
@@ -10230,7 +10244,7 @@
         <v>1851</v>
       </c>
     </row>
-    <row r="151" spans="2:15" ht="12.75">
+    <row r="151" spans="2:15" ht="13.2">
       <c r="B151" s="1">
         <v>146</v>
       </c>
@@ -10255,7 +10269,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="152" spans="2:15" ht="12.75">
+    <row r="152" spans="2:15" ht="13.2">
       <c r="B152" s="1">
         <v>147</v>
       </c>
@@ -10280,7 +10294,7 @@
         <v>2139</v>
       </c>
     </row>
-    <row r="153" spans="2:15" ht="12.75">
+    <row r="153" spans="2:15" ht="13.2">
       <c r="B153" s="1">
         <v>148</v>
       </c>
@@ -10308,7 +10322,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="154" spans="2:15" ht="12.75">
+    <row r="154" spans="2:15" ht="13.2">
       <c r="B154" s="1">
         <v>149</v>
       </c>
@@ -10333,7 +10347,7 @@
         <v>2477</v>
       </c>
     </row>
-    <row r="155" spans="2:15" ht="12.75">
+    <row r="155" spans="2:15" ht="13.2">
       <c r="B155" s="1">
         <v>150</v>
       </c>
@@ -10361,7 +10375,7 @@
         <v>2668</v>
       </c>
     </row>
-    <row r="156" spans="2:15" ht="12.75">
+    <row r="156" spans="2:15" ht="13.2">
       <c r="B156" s="1">
         <v>151</v>
       </c>
@@ -10386,7 +10400,7 @@
         <v>2878</v>
       </c>
     </row>
-    <row r="157" spans="2:15" ht="12.75">
+    <row r="157" spans="2:15" ht="13.2">
       <c r="B157" s="1">
         <v>152</v>
       </c>
@@ -10411,7 +10425,7 @@
         <v>3109</v>
       </c>
     </row>
-    <row r="158" spans="2:15" ht="12.75">
+    <row r="158" spans="2:15" ht="13.2">
       <c r="B158" s="1">
         <v>153</v>
       </c>
@@ -10436,7 +10450,7 @@
         <v>3362</v>
       </c>
     </row>
-    <row r="159" spans="2:15" ht="12.75">
+    <row r="159" spans="2:15" ht="13.2">
       <c r="B159" s="1">
         <v>154</v>
       </c>
@@ -10461,7 +10475,7 @@
         <v>3642</v>
       </c>
     </row>
-    <row r="160" spans="2:15" ht="12.75">
+    <row r="160" spans="2:15" ht="13.2">
       <c r="B160" s="1">
         <v>155</v>
       </c>
@@ -10486,7 +10500,7 @@
         <v>3952</v>
       </c>
     </row>
-    <row r="161" spans="2:15" ht="12.75">
+    <row r="161" spans="2:15" ht="13.2">
       <c r="B161" s="1">
         <v>156</v>
       </c>
@@ -10511,7 +10525,7 @@
         <v>4296</v>
       </c>
     </row>
-    <row r="162" spans="2:15" ht="12.75">
+    <row r="162" spans="2:15" ht="13.2">
       <c r="B162" s="1">
         <v>157</v>
       </c>
@@ -10536,7 +10550,7 @@
         <v>4680</v>
       </c>
     </row>
-    <row r="163" spans="2:15" ht="12.75">
+    <row r="163" spans="2:15" ht="13.2">
       <c r="B163" s="1">
         <v>158</v>
       </c>
@@ -10561,7 +10575,7 @@
         <v>5108</v>
       </c>
     </row>
-    <row r="164" spans="2:15" ht="12.75">
+    <row r="164" spans="2:15" ht="13.2">
       <c r="B164" s="1">
         <v>159</v>
       </c>
@@ -10586,7 +10600,7 @@
         <v>5587</v>
       </c>
     </row>
-    <row r="165" spans="2:15" ht="12.75">
+    <row r="165" spans="2:15" ht="13.2">
       <c r="B165" s="1">
         <v>160</v>
       </c>
@@ -10611,7 +10625,7 @@
         <v>6124</v>
       </c>
     </row>
-    <row r="166" spans="2:15" ht="12.75">
+    <row r="166" spans="2:15" ht="13.2">
       <c r="B166" s="1">
         <v>161</v>
       </c>
@@ -10636,7 +10650,7 @@
         <v>6728</v>
       </c>
     </row>
-    <row r="167" spans="2:15" ht="12.75">
+    <row r="167" spans="2:15" ht="13.2">
       <c r="B167" s="1">
         <v>162</v>
       </c>
@@ -10661,7 +10675,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="168" spans="2:15" ht="12.75">
+    <row r="168" spans="2:15" ht="13.2">
       <c r="B168" s="106">
         <v>163</v>
       </c>
@@ -10687,7 +10701,7 @@
         <v>8178</v>
       </c>
     </row>
-    <row r="169" spans="2:15" ht="12.75">
+    <row r="169" spans="2:15" ht="13.2">
       <c r="B169" s="1">
         <v>164</v>
       </c>
@@ -10712,7 +10726,7 @@
         <v>9047</v>
       </c>
     </row>
-    <row r="170" spans="2:15" ht="12.75">
+    <row r="170" spans="2:15" ht="13.2">
       <c r="B170" s="1">
         <v>165</v>
       </c>
@@ -10737,7 +10751,7 @@
         <v>10032</v>
       </c>
     </row>
-    <row r="171" spans="2:15" ht="12.75">
+    <row r="171" spans="2:15" ht="13.2">
       <c r="B171" s="1">
         <v>166</v>
       </c>
@@ -10762,7 +10776,7 @@
         <v>11149</v>
       </c>
     </row>
-    <row r="172" spans="2:15" ht="12.75">
+    <row r="172" spans="2:15" ht="13.2">
       <c r="B172" s="1">
         <v>167</v>
       </c>
@@ -10787,7 +10801,7 @@
         <v>12418</v>
       </c>
     </row>
-    <row r="173" spans="2:15" ht="12.75">
+    <row r="173" spans="2:15" ht="13.2">
       <c r="B173" s="1">
         <v>168</v>
       </c>
@@ -13408,18 +13422,18 @@
       <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="6" max="6" width="38.85546875" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
+    <col min="6" max="6" width="38.88671875" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10" ht="12.75">
+    <row r="2" spans="3:10" ht="13.2">
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="3:10" ht="12.75">
+    <row r="4" spans="3:10" ht="13.2">
       <c r="C4" s="1" t="s">
         <v>52</v>
       </c>
@@ -13445,7 +13459,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="3:10" ht="12.75">
+    <row r="5" spans="3:10" ht="13.2">
       <c r="C5" s="1">
         <v>1</v>
       </c>
@@ -13465,7 +13479,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="3:10" ht="12.75">
+    <row r="6" spans="3:10" ht="13.2">
       <c r="C6" s="1">
         <v>2</v>
       </c>
@@ -13479,7 +13493,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="7" spans="3:10" ht="12.75">
+    <row r="7" spans="3:10" ht="13.2">
       <c r="C7" s="1">
         <v>3</v>
       </c>
@@ -13493,7 +13507,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="8" spans="3:10" ht="12.75">
+    <row r="8" spans="3:10" ht="13.2">
       <c r="C8" s="1">
         <v>4</v>
       </c>
@@ -13507,7 +13521,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="9" spans="3:10" ht="12.75">
+    <row r="9" spans="3:10" ht="13.2">
       <c r="C9" s="1">
         <v>5</v>
       </c>
@@ -13521,7 +13535,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="10" spans="3:10" ht="12.75">
+    <row r="10" spans="3:10" ht="13.2">
       <c r="C10" s="1">
         <v>6</v>
       </c>
@@ -13535,7 +13549,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="11" spans="3:10" ht="12.75">
+    <row r="11" spans="3:10" ht="13.2">
       <c r="C11" s="1">
         <v>7</v>
       </c>
@@ -13549,7 +13563,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="12" spans="3:10" ht="12.75">
+    <row r="12" spans="3:10" ht="13.2">
       <c r="C12" s="1">
         <v>8</v>
       </c>
@@ -13563,7 +13577,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="13" spans="3:10" ht="12.75">
+    <row r="13" spans="3:10" ht="13.2">
       <c r="C13" s="1">
         <v>9</v>
       </c>
@@ -13577,7 +13591,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="3:10" ht="12.75">
+    <row r="14" spans="3:10" ht="13.2">
       <c r="C14" s="1">
         <v>10</v>
       </c>
@@ -13591,7 +13605,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="15" spans="3:10" ht="12.75">
+    <row r="15" spans="3:10" ht="13.2">
       <c r="C15" s="1">
         <v>11</v>
       </c>
@@ -13605,7 +13619,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="16" spans="3:10" ht="12.75">
+    <row r="16" spans="3:10" ht="13.2">
       <c r="C16" s="1">
         <v>12</v>
       </c>
@@ -13619,7 +13633,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="17" spans="3:9" ht="12.75">
+    <row r="17" spans="3:9" ht="13.2">
       <c r="C17" s="1">
         <v>13</v>
       </c>
@@ -13633,7 +13647,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="18" spans="3:9" ht="12.75">
+    <row r="18" spans="3:9" ht="13.2">
       <c r="C18" s="1">
         <v>14</v>
       </c>
@@ -13647,7 +13661,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="19" spans="3:9" ht="12.75">
+    <row r="19" spans="3:9" ht="13.2">
       <c r="C19" s="1">
         <v>15</v>
       </c>
@@ -13661,7 +13675,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="20" spans="3:9" ht="12.75">
+    <row r="20" spans="3:9" ht="13.2">
       <c r="C20" s="1">
         <v>16</v>
       </c>
@@ -13675,7 +13689,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="21" spans="3:9" ht="12.75">
+    <row r="21" spans="3:9" ht="13.2">
       <c r="C21" s="1">
         <v>17</v>
       </c>
@@ -13689,7 +13703,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="22" spans="3:9" ht="12.75">
+    <row r="22" spans="3:9" ht="13.2">
       <c r="C22" s="1">
         <v>18</v>
       </c>
@@ -13703,7 +13717,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="23" spans="3:9" ht="12.75">
+    <row r="23" spans="3:9" ht="13.2">
       <c r="C23" s="1">
         <v>19</v>
       </c>
@@ -13717,7 +13731,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="24" spans="3:9" ht="12.75">
+    <row r="24" spans="3:9" ht="13.2">
       <c r="C24" s="1">
         <v>20</v>
       </c>
@@ -13731,7 +13745,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="25" spans="3:9" ht="12.75">
+    <row r="25" spans="3:9" ht="13.2">
       <c r="C25" s="1">
         <v>21</v>
       </c>
@@ -13745,7 +13759,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="26" spans="3:9" ht="12.75">
+    <row r="26" spans="3:9" ht="13.2">
       <c r="C26" s="1">
         <v>22</v>
       </c>
@@ -13759,7 +13773,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="27" spans="3:9" ht="12.75">
+    <row r="27" spans="3:9" ht="13.2">
       <c r="C27" s="1">
         <v>23</v>
       </c>
@@ -13773,7 +13787,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="3:9" ht="12.75">
+    <row r="28" spans="3:9" ht="13.2">
       <c r="C28" s="1">
         <v>24</v>
       </c>
@@ -13787,7 +13801,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="29" spans="3:9" ht="12.75">
+    <row r="29" spans="3:9" ht="13.2">
       <c r="C29" s="1">
         <v>25</v>
       </c>
@@ -13801,7 +13815,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="30" spans="3:9" ht="12.75">
+    <row r="30" spans="3:9" ht="13.2">
       <c r="C30" s="1">
         <v>26</v>
       </c>
@@ -13815,7 +13829,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="31" spans="3:9" ht="12.75">
+    <row r="31" spans="3:9" ht="13.2">
       <c r="C31" s="1">
         <v>27</v>
       </c>
@@ -13829,7 +13843,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="3:9" ht="12.75">
+    <row r="32" spans="3:9" ht="13.2">
       <c r="C32" s="1">
         <v>28</v>
       </c>
@@ -13844,7 +13858,7 @@
       </c>
       <c r="I32" s="26"/>
     </row>
-    <row r="33" spans="3:9" ht="12.75">
+    <row r="33" spans="3:9" ht="13.2">
       <c r="C33" s="1">
         <v>29</v>
       </c>
@@ -13859,7 +13873,7 @@
       </c>
       <c r="I33" s="27"/>
     </row>
-    <row r="34" spans="3:9" ht="12.75">
+    <row r="34" spans="3:9" ht="13.2">
       <c r="C34" s="1">
         <v>30</v>
       </c>
@@ -13874,7 +13888,7 @@
       </c>
       <c r="I34" s="27"/>
     </row>
-    <row r="35" spans="3:9" ht="12.75">
+    <row r="35" spans="3:9" ht="13.2">
       <c r="C35" s="1">
         <v>31</v>
       </c>
@@ -13889,7 +13903,7 @@
       </c>
       <c r="I35" s="27"/>
     </row>
-    <row r="36" spans="3:9" ht="12.75">
+    <row r="36" spans="3:9" ht="13.2">
       <c r="C36" s="1">
         <v>32</v>
       </c>
@@ -13906,7 +13920,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="3:9" ht="12.75">
+    <row r="37" spans="3:9" ht="13.2">
       <c r="C37" s="1">
         <v>33</v>
       </c>
@@ -13923,7 +13937,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="3:9" ht="12.75">
+    <row r="38" spans="3:9" ht="13.2">
       <c r="C38" s="1">
         <v>34</v>
       </c>
@@ -13940,7 +13954,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="3:9" ht="12.75">
+    <row r="39" spans="3:9" ht="13.2">
       <c r="C39" s="1">
         <v>35</v>
       </c>
@@ -13957,7 +13971,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="40" spans="3:9" ht="12.75">
+    <row r="40" spans="3:9" ht="13.2">
       <c r="C40" s="1">
         <v>36</v>
       </c>
@@ -13974,7 +13988,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="41" spans="3:9" ht="12.75">
+    <row r="41" spans="3:9" ht="13.2">
       <c r="C41" s="1">
         <v>37</v>
       </c>
@@ -13991,7 +14005,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="42" spans="3:9" ht="12.75">
+    <row r="42" spans="3:9" ht="13.2">
       <c r="C42" s="1">
         <v>38</v>
       </c>
@@ -14008,7 +14022,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="43" spans="3:9" ht="12.75">
+    <row r="43" spans="3:9" ht="13.2">
       <c r="C43" s="1">
         <v>39</v>
       </c>
@@ -14025,7 +14039,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="3:9" ht="12.75">
+    <row r="44" spans="3:9" ht="13.2">
       <c r="C44" s="1">
         <v>40</v>
       </c>
@@ -14042,7 +14056,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="45" spans="3:9" ht="12.75">
+    <row r="45" spans="3:9" ht="13.2">
       <c r="C45" s="1">
         <v>41</v>
       </c>
@@ -14059,7 +14073,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="46" spans="3:9" ht="12.75">
+    <row r="46" spans="3:9" ht="13.2">
       <c r="C46" s="1">
         <v>42</v>
       </c>
@@ -14076,7 +14090,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="47" spans="3:9" ht="12.75">
+    <row r="47" spans="3:9" ht="13.2">
       <c r="C47" s="1">
         <v>43</v>
       </c>
@@ -14093,7 +14107,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="48" spans="3:9" ht="12.75">
+    <row r="48" spans="3:9" ht="13.2">
       <c r="C48" s="1">
         <v>44</v>
       </c>
@@ -14110,7 +14124,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="49" spans="3:9" ht="12.75">
+    <row r="49" spans="3:9" ht="13.2">
       <c r="C49" s="1">
         <v>45</v>
       </c>
@@ -14127,7 +14141,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="50" spans="3:9" ht="12.75">
+    <row r="50" spans="3:9" ht="13.2">
       <c r="C50" s="1">
         <v>46</v>
       </c>
@@ -14144,7 +14158,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="51" spans="3:9" ht="12.75">
+    <row r="51" spans="3:9" ht="13.2">
       <c r="C51" s="1">
         <v>47</v>
       </c>
@@ -14161,7 +14175,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="52" spans="3:9" ht="12.75">
+    <row r="52" spans="3:9" ht="13.2">
       <c r="C52" s="1">
         <v>48</v>
       </c>
@@ -14178,7 +14192,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="53" spans="3:9" ht="12.75">
+    <row r="53" spans="3:9" ht="13.2">
       <c r="C53" s="1">
         <v>49</v>
       </c>
@@ -14195,7 +14209,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="54" spans="3:9" ht="12.75">
+    <row r="54" spans="3:9" ht="13.2">
       <c r="C54" s="1">
         <v>50</v>
       </c>
@@ -14209,7 +14223,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="55" spans="3:9" ht="12.75">
+    <row r="55" spans="3:9" ht="13.2">
       <c r="C55" s="1">
         <v>51</v>
       </c>
@@ -14223,7 +14237,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="56" spans="3:9" ht="12.75">
+    <row r="56" spans="3:9" ht="13.2">
       <c r="C56" s="1">
         <v>52</v>
       </c>
@@ -14237,7 +14251,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="57" spans="3:9" ht="12.75">
+    <row r="57" spans="3:9" ht="13.2">
       <c r="C57" s="1">
         <v>53</v>
       </c>
@@ -14251,7 +14265,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="58" spans="3:9" ht="12.75">
+    <row r="58" spans="3:9" ht="13.2">
       <c r="C58" s="1">
         <v>54</v>
       </c>
@@ -14265,7 +14279,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="3:9" ht="12.75">
+    <row r="59" spans="3:9" ht="13.2">
       <c r="C59" s="1">
         <v>55</v>
       </c>
@@ -14279,7 +14293,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="60" spans="3:9" ht="12.75">
+    <row r="60" spans="3:9" ht="13.2">
       <c r="C60" s="1">
         <v>56</v>
       </c>
@@ -14293,7 +14307,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="3:9" ht="12.75">
+    <row r="61" spans="3:9" ht="13.2">
       <c r="C61" s="1">
         <v>57</v>
       </c>
@@ -14307,7 +14321,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="62" spans="3:9" ht="12.75">
+    <row r="62" spans="3:9" ht="13.2">
       <c r="C62" s="1">
         <v>58</v>
       </c>
@@ -14318,7 +14332,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="63" spans="3:9" ht="12.75">
+    <row r="63" spans="3:9" ht="13.2">
       <c r="C63" s="1">
         <v>59</v>
       </c>
@@ -14329,7 +14343,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="64" spans="3:9" ht="12.75">
+    <row r="64" spans="3:9" ht="13.2">
       <c r="C64" s="1">
         <v>60</v>
       </c>
@@ -14340,7 +14354,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="65" spans="3:6" ht="12.75">
+    <row r="65" spans="3:6" ht="13.2">
       <c r="C65" s="1">
         <v>61</v>
       </c>
@@ -14482,10 +14496,10 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:9">
@@ -14936,10 +14950,10 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:7">
@@ -15310,10 +15324,10 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="5" max="5" width="69.85546875" customWidth="1"/>
-    <col min="8" max="8" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="69.88671875" customWidth="1"/>
+    <col min="8" max="8" width="39.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:8">
@@ -15395,10 +15409,10 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="26" customWidth="1"/>
   </cols>
@@ -15412,15 +15426,15 @@
       </c>
     </row>
     <row r="4" spans="3:22">
-      <c r="O4" s="111" t="s">
+      <c r="O4" s="112" t="s">
         <v>235</v>
       </c>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="112"/>
-      <c r="R4" s="112"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
+      <c r="P4" s="113"/>
+      <c r="Q4" s="113"/>
+      <c r="R4" s="113"/>
+      <c r="S4" s="113"/>
+      <c r="T4" s="113"/>
+      <c r="U4" s="113"/>
     </row>
     <row r="5" spans="3:22">
       <c r="C5" s="1" t="s">
@@ -16244,11 +16258,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:20">

</xml_diff>

<commit_message>
Effect calculation fix, unlocks, repo clean-up
Removed all V1 code
Fixed a lot of upgrade calculations that where wrong
Made logic that will be used for unlocking different parts of the game
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479A49CF-CB1E-4CC1-B6D9-747CC55AF1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752F1CE1-4ADD-42D7-B854-012B13125E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4955,8 +4955,8 @@
   </sheetPr>
   <dimension ref="A1:X276"/>
   <sheetViews>
-    <sheetView topLeftCell="A260" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F274" sqref="F274"/>
+    <sheetView topLeftCell="A155" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -13405,8 +13405,8 @@
   </sheetPr>
   <dimension ref="C2:J76"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A64" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -14933,8 +14933,8 @@
   </sheetPr>
   <dimension ref="C4:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Bots, Fish and small fixes
Implemented buying bots and bot sell logic
Hide magic upgrades after bought
Changed/Fixed some of the bot upgrade effects
Implemented simple fish logic
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803F1F21-99A9-4E55-A60B-9B777E57EA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6394049A-364D-4B32-A359-5C06CED42297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1817" uniqueCount="839">
   <si>
     <t xml:space="preserve">Tier </t>
   </si>
@@ -2490,9 +2490,6 @@
     <t>upgrade click beaver</t>
   </si>
   <si>
-    <t>2+ beavers from woodcamps</t>
-  </si>
-  <si>
     <t>wood per second 2% increase per level</t>
   </si>
   <si>
@@ -2533,6 +2530,30 @@
   </si>
   <si>
     <t>Wpc 0.2% per achievement</t>
+  </si>
+  <si>
+    <t>change bot better sell price to better wood price</t>
+  </si>
+  <si>
+    <t>Better wood price 0.5%</t>
+  </si>
+  <si>
+    <t>Better wood price 0.3%</t>
+  </si>
+  <si>
+    <t>Better wood price 2.6%</t>
+  </si>
+  <si>
+    <t>FoS better all wood sell 0.02%</t>
+  </si>
+  <si>
+    <t>FoS better all wood sell 0.05%</t>
+  </si>
+  <si>
+    <t>Better wood price 3.1%</t>
+  </si>
+  <si>
+    <t>1+ beavers from woodcamps</t>
   </si>
 </sst>
 </file>
@@ -3275,6 +3296,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="46" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3282,7 +3304,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="46" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4989,8 +5010,8 @@
   </sheetPr>
   <dimension ref="A1:X276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A254" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L262" sqref="L262"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5092,19 +5113,19 @@
       <c r="K5" s="45" t="s">
         <v>432</v>
       </c>
-      <c r="M5" s="111" t="s">
+      <c r="M5" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="N5" s="111"/>
-      <c r="O5" s="111"/>
-      <c r="P5" s="111"/>
-      <c r="Q5" s="111"/>
-      <c r="R5" s="111"/>
-      <c r="S5" s="111"/>
-      <c r="T5" s="111"/>
-      <c r="U5" s="111"/>
-      <c r="V5" s="111"/>
-      <c r="W5" s="111"/>
+      <c r="N5" s="112"/>
+      <c r="O5" s="112"/>
+      <c r="P5" s="112"/>
+      <c r="Q5" s="112"/>
+      <c r="R5" s="112"/>
+      <c r="S5" s="112"/>
+      <c r="T5" s="112"/>
+      <c r="U5" s="112"/>
+      <c r="V5" s="112"/>
+      <c r="W5" s="112"/>
     </row>
     <row r="6" spans="1:23" ht="13.5" thickBot="1">
       <c r="A6" s="35" t="s">
@@ -5458,7 +5479,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="75" t="s">
-        <v>817</v>
+        <v>838</v>
       </c>
       <c r="H11">
         <v>750</v>
@@ -5753,7 +5774,7 @@
         <v>13</v>
       </c>
       <c r="F18" s="75" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="M18" s="40"/>
       <c r="N18" s="40" t="s">
@@ -5790,6 +5811,9 @@
       <c r="F19" s="74" t="s">
         <v>622</v>
       </c>
+      <c r="G19" t="s">
+        <v>831</v>
+      </c>
       <c r="M19" s="40"/>
       <c r="N19" s="40"/>
       <c r="O19" s="40"/>
@@ -5816,7 +5840,7 @@
         <v>15</v>
       </c>
       <c r="F20" s="105" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="M20" s="35"/>
       <c r="N20" s="40"/>
@@ -6341,7 +6365,7 @@
       <c r="F36" s="97" t="s">
         <v>717</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>130</v>
       </c>
       <c r="K36" s="45"/>
@@ -6398,10 +6422,10 @@
       <c r="F37" s="74" t="s">
         <v>631</v>
       </c>
-      <c r="G37" s="45" t="s">
+      <c r="H37" s="45"/>
+      <c r="I37" s="45" t="s">
         <v>465</v>
       </c>
-      <c r="H37" s="45"/>
       <c r="K37" s="45"/>
       <c r="L37" s="40">
         <v>2</v>
@@ -6456,10 +6480,10 @@
       <c r="F38" s="100" t="s">
         <v>689</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" s="45"/>
+      <c r="I38" t="s">
         <v>439</v>
       </c>
-      <c r="H38" s="45"/>
       <c r="L38" s="40">
         <v>3</v>
       </c>
@@ -6513,10 +6537,10 @@
       <c r="F39" s="101" t="s">
         <v>694</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="45"/>
+      <c r="I39" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H39" s="45"/>
       <c r="K39" s="45"/>
       <c r="L39" s="40">
         <v>4</v>
@@ -6574,7 +6598,7 @@
       <c r="F40" s="100" t="s">
         <v>674</v>
       </c>
-      <c r="G40" t="s">
+      <c r="I40" t="s">
         <v>436</v>
       </c>
       <c r="L40" s="40">
@@ -6900,7 +6924,7 @@
         <v>5</v>
       </c>
       <c r="F46" s="105" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="G46" s="1"/>
       <c r="L46" s="40">
@@ -7197,9 +7221,7 @@
       <c r="F52" s="74" t="s">
         <v>634</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="G52" s="1"/>
       <c r="H52" t="s">
         <v>396</v>
       </c>
@@ -7258,9 +7280,7 @@
       <c r="F53" s="75" t="s">
         <v>591</v>
       </c>
-      <c r="G53" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="G53" s="1"/>
       <c r="H53" s="45" t="s">
         <v>410</v>
       </c>
@@ -7310,9 +7330,7 @@
       <c r="F54" s="100" t="s">
         <v>676</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="G54" s="1"/>
       <c r="L54" s="40">
         <v>19</v>
       </c>
@@ -7359,9 +7377,7 @@
       <c r="F55" s="74" t="s">
         <v>627</v>
       </c>
-      <c r="G55" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="G55" s="1"/>
       <c r="H55" t="s">
         <v>92</v>
       </c>
@@ -7417,9 +7433,7 @@
       <c r="F56" s="97" t="s">
         <v>735</v>
       </c>
-      <c r="G56" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="G56" s="1"/>
       <c r="L56" s="40">
         <v>21</v>
       </c>
@@ -7469,9 +7483,7 @@
       <c r="F57" s="105" t="s">
         <v>429</v>
       </c>
-      <c r="G57" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="G57" s="1"/>
       <c r="L57" s="40">
         <v>22</v>
       </c>
@@ -7518,9 +7530,7 @@
       <c r="F58" s="65" t="s">
         <v>618</v>
       </c>
-      <c r="G58" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="G58" s="1"/>
       <c r="L58" s="40">
         <v>23</v>
       </c>
@@ -7563,9 +7573,7 @@
       <c r="F59" s="103" t="s">
         <v>762</v>
       </c>
-      <c r="G59" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="G59" s="1"/>
       <c r="H59" s="45" t="s">
         <v>411</v>
       </c>
@@ -8231,6 +8239,9 @@
         <v>18</v>
       </c>
       <c r="F77" s="74" t="s">
+        <v>832</v>
+      </c>
+      <c r="G77" t="s">
         <v>641</v>
       </c>
       <c r="L77" s="40">
@@ -8522,7 +8533,7 @@
         <v>9</v>
       </c>
       <c r="F86" s="74" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="L86" s="40">
         <v>51</v>
@@ -8652,7 +8663,7 @@
         <v>13</v>
       </c>
       <c r="F90" s="97" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="T90" s="58" t="s">
         <v>518</v>
@@ -9134,6 +9145,9 @@
         <v>14</v>
       </c>
       <c r="F109" s="74" t="s">
+        <v>833</v>
+      </c>
+      <c r="G109" t="s">
         <v>639</v>
       </c>
       <c r="U109">
@@ -9415,7 +9429,7 @@
         <v>5</v>
       </c>
       <c r="F118" s="98" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="M118">
         <v>6</v>
@@ -9631,7 +9645,7 @@
         <v>13</v>
       </c>
       <c r="F126" s="105" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="M126">
         <v>14</v>
@@ -10482,7 +10496,7 @@
         <v>10</v>
       </c>
       <c r="F159" s="75" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="M159">
         <v>47</v>
@@ -10609,9 +10623,6 @@
       <c r="F164" s="74" t="s">
         <v>616</v>
       </c>
-      <c r="G164" t="s">
-        <v>616</v>
-      </c>
       <c r="M164">
         <v>52</v>
       </c>
@@ -10660,7 +10671,7 @@
         <v>17</v>
       </c>
       <c r="F166" s="75" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="M166">
         <v>54</v>
@@ -10961,7 +10972,7 @@
         <v>11</v>
       </c>
       <c r="F178" s="75" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="M178">
         <v>66</v>
@@ -10986,6 +10997,9 @@
         <v>12</v>
       </c>
       <c r="F179" s="74" t="s">
+        <v>834</v>
+      </c>
+      <c r="G179" t="s">
         <v>640</v>
       </c>
       <c r="M179">
@@ -11066,9 +11080,6 @@
       <c r="F182" s="65" t="s">
         <v>652</v>
       </c>
-      <c r="G182" t="s">
-        <v>652</v>
-      </c>
       <c r="M182">
         <v>70</v>
       </c>
@@ -11147,9 +11158,6 @@
       <c r="F185" s="97" t="s">
         <v>699</v>
       </c>
-      <c r="G185" t="s">
-        <v>699</v>
-      </c>
       <c r="M185">
         <v>73</v>
       </c>
@@ -11429,9 +11437,6 @@
       <c r="F196" s="101" t="s">
         <v>732</v>
       </c>
-      <c r="G196" t="s">
-        <v>732</v>
-      </c>
       <c r="M196">
         <v>84</v>
       </c>
@@ -11912,7 +11917,7 @@
         <v>12</v>
       </c>
       <c r="F215" s="75" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="M215">
         <v>103</v>
@@ -11937,7 +11942,7 @@
         <v>13</v>
       </c>
       <c r="F216" s="74" t="s">
-        <v>653</v>
+        <v>835</v>
       </c>
       <c r="M216">
         <v>104</v>
@@ -12039,11 +12044,8 @@
       <c r="E220" s="1">
         <v>17</v>
       </c>
-      <c r="F220" s="114" t="s">
-        <v>831</v>
-      </c>
-      <c r="G220" t="s">
-        <v>388</v>
+      <c r="F220" s="111" t="s">
+        <v>830</v>
       </c>
       <c r="M220">
         <v>108</v>
@@ -12754,9 +12756,6 @@
       <c r="F247" s="105" t="s">
         <v>577</v>
       </c>
-      <c r="G247" t="s">
-        <v>577</v>
-      </c>
       <c r="H247" t="s">
         <v>452</v>
       </c>
@@ -13163,7 +13162,7 @@
         <v>4</v>
       </c>
       <c r="F261" s="74" t="s">
-        <v>654</v>
+        <v>836</v>
       </c>
       <c r="H261" t="s">
         <v>441</v>
@@ -13270,6 +13269,9 @@
         <v>9</v>
       </c>
       <c r="F266" s="74" t="s">
+        <v>837</v>
+      </c>
+      <c r="G266" t="s">
         <v>637</v>
       </c>
       <c r="H266" t="s">
@@ -13865,7 +13867,7 @@
         <v>26</v>
       </c>
       <c r="F30" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="31" spans="3:9" ht="12.75">
@@ -15330,7 +15332,7 @@
         <v>29</v>
       </c>
       <c r="D35" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="G35" s="28" t="s">
         <v>224</v>
@@ -15465,15 +15467,15 @@
       </c>
     </row>
     <row r="4" spans="3:22">
-      <c r="O4" s="112" t="s">
+      <c r="O4" s="113" t="s">
         <v>235</v>
       </c>
-      <c r="P4" s="113"/>
-      <c r="Q4" s="113"/>
-      <c r="R4" s="113"/>
-      <c r="S4" s="113"/>
-      <c r="T4" s="113"/>
-      <c r="U4" s="113"/>
+      <c r="P4" s="114"/>
+      <c r="Q4" s="114"/>
+      <c r="R4" s="114"/>
+      <c r="S4" s="114"/>
+      <c r="T4" s="114"/>
+      <c r="U4" s="114"/>
     </row>
     <row r="5" spans="3:22">
       <c r="C5" s="1" t="s">

</xml_diff>

<commit_message>
Start pacing, removing levels and fishing updates
Implemented bait buying and the displaying of owned bait.
Started implementing fishing spots
Started creating pacing for the start of the game (oak, apple, maple)
Updated upgrade, research and woodcamp prices, names and effects
Started removing levels from the game, replacing it with beavers
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FFF4EB-C132-45FD-A55D-5364B463217F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C9EA3D-6824-4F9A-8B46-68E199E1EBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="Dam" sheetId="7" r:id="rId7"/>
     <sheet name="Achievements" sheetId="8" r:id="rId8"/>
     <sheet name="Fishing" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1847" uniqueCount="912">
   <si>
     <t xml:space="preserve">Tier </t>
   </si>
@@ -2769,6 +2770,21 @@
   </si>
   <si>
     <t>(0.5 - bait FP) * spot%</t>
+  </si>
+  <si>
+    <t>round(pow(1.6, level) + 1.5 * pow(level, 4.3)) + 1 * (level + 1) * 7 + 2</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>2^C5 + 2 * (C5^2) + 1 * (C5 + 1) * 7 + 2</t>
+  </si>
+  <si>
+    <t>2^C5 + 2 * (C5^3) + 1 * (C5 + 1) * 7 + 2</t>
+  </si>
+  <si>
+    <t>3^C5 + 2 * (C5^2) + 1 * (C5 + 1) * 7 + 2</t>
   </si>
 </sst>
 </file>
@@ -4365,6 +4381,759 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE76D2E-FEA3-454F-BC35-ED3E32220B6F}">
+  <dimension ref="C3:F46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="4" max="4" width="57" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:6">
+      <c r="D3" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="C4" t="s">
+        <v>908</v>
+      </c>
+      <c r="D4" t="s">
+        <v>909</v>
+      </c>
+      <c r="E4" t="s">
+        <v>911</v>
+      </c>
+      <c r="F4" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f>2^C5 + 2 * (C5^2) + 1 * (C5+ 1) * 7 + 2</f>
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <f>3^C5 + 2 * (C5^2) + 1 * (C5+ 1) * 7 + 2</f>
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <f>2^C5 + 2 * (C5^3) + 1 * (C5 + 1) * 7 + 2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D46" si="0">2^C6 + 2 * (C6^2) + 1 * (C6+ 1) * 7 + 2</f>
+        <v>35</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E46" si="1">3^C6 + 2 * (C6^2) + 1 * (C6+ 1) * 7 + 2</f>
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F46" si="2">2^C6 + 2 * (C6^3) + 1 * (C6 + 1) * 7 + 2</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>337</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>852</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>547</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6">
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>284</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>2343</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>872</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6">
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>449</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>6754</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6">
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>746</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>19917</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6">
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1303</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>59328</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>3103</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6">
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>2376</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>177475</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>4796</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6">
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>4477</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>531822</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>7645</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>8630</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>1594761</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>12686</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>16883</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>4783468</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>21979</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>33332</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>14349471</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>39632</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>66169</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>43047354</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>73849</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6">
+      <c r="C21">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>131778</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>129140869</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>141026</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="C22">
+        <v>18</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>262927</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>387421272</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>273943</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="C23">
+        <v>19</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>525152</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>1162262331</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>538148</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="C24">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>1049525</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>3486785350</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>1064725</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6">
+      <c r="C25">
+        <v>21</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>2098190</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>10460354241</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>2115830</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6">
+      <c r="C26">
+        <v>22</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>4195435</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>31381060740</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>4215763</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6">
+      <c r="C27">
+        <v>23</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>8389836</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>94143180055</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>8413112</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="C28">
+        <v>24</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>16778545</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>282429537810</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>16805041</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6">
+      <c r="C29">
+        <v>25</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>33555866</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>847288610877</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>33585866</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6">
+      <c r="C30">
+        <v>26</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>67110407</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>2541865829872</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>67144207</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6">
+      <c r="C31">
+        <v>27</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>134219384</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>7625597486643</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>134257292</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6">
+      <c r="C32">
+        <v>28</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>268437229</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>22876792456734</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>268479565</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6">
+      <c r="C33">
+        <v>29</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>536872806</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>68630377366777</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>536919902</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6">
+      <c r="C34">
+        <v>30</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>1073743843</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>205891132096668</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>1073796043</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6">
+      <c r="C35">
+        <v>31</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>2147485796</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>617673396286095</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>2147543456</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6">
+      <c r="C36">
+        <v>32</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>4294969577</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>1853020188854122</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>4295033065</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6">
+      <c r="C37">
+        <v>33</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>8589937010</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>5559060566557941</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
+        <v>8590006706</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6">
+      <c r="C38">
+        <v>34</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>17179871743</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>1.6677181699669126E+16</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
+        <v>17179948039</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6">
+      <c r="C39">
+        <v>35</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>34359741072</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>5.00315450990024E+16</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
+        <v>34359824372</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6">
+      <c r="C40">
+        <v>36</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>68719479589</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>1.5009463529700198E+17</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="2"/>
+        <v>68719570309</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6">
+      <c r="C41">
+        <v>37</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>137438956478</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>4.5028390589100038E+17</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="2"/>
+        <v>137439055046</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6">
+      <c r="C42">
+        <v>38</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>274877910107</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>1.3508517176729951E+18</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="2"/>
+        <v>274878016963</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6">
+      <c r="C43">
+        <v>39</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>549755817212</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>4.0525551530189798E+18</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="2"/>
+        <v>549755932808</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6">
+      <c r="C44">
+        <v>40</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>1099511631265</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>1.2157665459056933E+19</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="2"/>
+        <v>1099511756065</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6">
+      <c r="C45">
+        <v>41</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>2199023259210</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>3.6472996377170792E+19</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="2"/>
+        <v>2199023393690</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6">
+      <c r="C46">
+        <v>42</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>4398046514935</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>1.0941898913151237E+20</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="2"/>
+        <v>4398046659583</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
@@ -16527,7 +17296,7 @@
   </sheetPr>
   <dimension ref="C3:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="B8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Started creating Dam tab
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67896D1B-93B7-4B4C-A4ED-8CEBE69647C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F777FDA-72F8-4CB8-9694-BAF287F92725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="1035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="1063">
   <si>
     <t xml:space="preserve">Tier </t>
   </si>
@@ -3154,6 +3154,90 @@
   </si>
   <si>
     <t>Total Wood Sold With Bots</t>
+  </si>
+  <si>
+    <t>Mega Dam</t>
+  </si>
+  <si>
+    <t>Sub 1</t>
+  </si>
+  <si>
+    <t>Sub 4</t>
+  </si>
+  <si>
+    <t>Sub 3</t>
+  </si>
+  <si>
+    <t>Sub 2</t>
+  </si>
+  <si>
+    <t>Foundations</t>
+  </si>
+  <si>
+    <t>Site Appreizal</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Finishing Toches</t>
+  </si>
+  <si>
+    <t>Fund Rasing</t>
+  </si>
+  <si>
+    <t>Buying Oligargcs</t>
+  </si>
+  <si>
+    <t>Getting a Team of Beavers</t>
+  </si>
+  <si>
+    <t>Planing</t>
+  </si>
+  <si>
+    <t>Arhitecture</t>
+  </si>
+  <si>
+    <t>Plan Excecution</t>
+  </si>
+  <si>
+    <t>Weight Testing</t>
+  </si>
+  <si>
+    <t>Atracting Investors</t>
+  </si>
+  <si>
+    <t>Over throwing the Government</t>
+  </si>
+  <si>
+    <t>Subjecation</t>
+  </si>
+  <si>
+    <t>Excecuting the master plan</t>
+  </si>
+  <si>
+    <t>Grand Opening</t>
+  </si>
+  <si>
+    <t>Creating Logistics lines</t>
+  </si>
+  <si>
+    <t>Environmental Impact Studies</t>
+  </si>
+  <si>
+    <t>Careful Wood Stacking</t>
+  </si>
+  <si>
+    <t>Patching leaks/ holes</t>
+  </si>
+  <si>
+    <t>Build Multiple Dams at the same time with unlocks, all current constructions if stages active suck other resources (suck speed can be improved with upgrades, resource amount needed lowered with research, like an inovation in the construction process</t>
+  </si>
+  <si>
+    <t>To start building a dam there is some upfront cost</t>
+  </si>
+  <si>
+    <t>Maybe make magic like a skill tree to be more interesting open one and then adjesent magic upgrades are shown and be able to be unlocked</t>
   </si>
 </sst>
 </file>
@@ -17703,10 +17787,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="C4:G36"/>
+  <dimension ref="C4:G39"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -18067,6 +18151,11 @@
         <v>225</v>
       </c>
     </row>
+    <row r="39" spans="3:7" ht="15.75" customHeight="1">
+      <c r="D39" t="s">
+        <v>1062</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18077,44 +18166,85 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="C3:H9"/>
+  <dimension ref="C3:T16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="5" max="5" width="69.85546875" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
     <col min="8" max="8" width="39.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8">
+    <row r="3" spans="3:20">
       <c r="C3" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="3:8">
+    <row r="5" spans="3:20">
       <c r="C5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" t="s">
+        <v>1039</v>
+      </c>
+      <c r="I5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J5" t="s">
+        <v>135</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="L5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M5" t="s">
+        <v>135</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1037</v>
+      </c>
+      <c r="O5" t="s">
+        <v>77</v>
+      </c>
+      <c r="P5" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="6" spans="3:8">
+    <row r="6" spans="3:20">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -18122,34 +18252,112 @@
         <v>229</v>
       </c>
       <c r="E6" t="s">
+        <v>1046</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1040</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1058</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1059</v>
+      </c>
+      <c r="Q6" t="s">
         <v>428</v>
       </c>
-      <c r="H6" t="s">
+      <c r="T6" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="7" spans="3:8">
+    <row r="7" spans="3:20">
       <c r="C7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="8" spans="3:8">
+      <c r="E7" t="s">
+        <v>1041</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1047</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1049</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="8" spans="3:20">
       <c r="C8" s="1">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="9" spans="3:8">
+      <c r="E8" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1056</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1042</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="9" spans="3:20">
       <c r="C9" s="1">
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>232</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1051</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1057</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="10" spans="3:20" ht="15.75" customHeight="1">
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1045</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1052</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1053</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20" ht="15.75" customHeight="1">
+      <c r="D15" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="16" spans="3:20" ht="15.75" customHeight="1">
+      <c r="D16" t="s">
+        <v>1061</v>
       </c>
     </row>
   </sheetData>
@@ -18164,7 +18372,7 @@
   </sheetPr>
   <dimension ref="C3:V105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="E8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Save info and other small improvements
Improved info displayed about saves
Updated dam data saving, added more detailed dam prices
Changed some of the Research and upgrade names and descriptions
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11921FAC-31D2-4FAD-AF60-B5EB95CCB638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB715DD-0B62-4512-A1E7-67FB0132B863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="7848" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -25,11 +25,24 @@
     <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="1066">
   <si>
     <t xml:space="preserve">Tier </t>
   </si>
@@ -2730,24 +2743,9 @@
     <t>Oak storage +100</t>
   </si>
   <si>
-    <t>10% cheaper beavers</t>
-  </si>
-  <si>
     <t>12% storage from woodcamps</t>
   </si>
   <si>
-    <t>cheaper bots 6%</t>
-  </si>
-  <si>
-    <t>WC 7% cheaper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wpc add 2% wps </t>
-  </si>
-  <si>
-    <t>1+ beavers per WC</t>
-  </si>
-  <si>
     <t>ideas</t>
   </si>
   <si>
@@ -2763,30 +2761,12 @@
     <t>changed position</t>
   </si>
   <si>
-    <t>1.5x storage</t>
-  </si>
-  <si>
-    <t>fish sell for more 5%</t>
-  </si>
-  <si>
-    <t>cheaper bots 4%</t>
-  </si>
-  <si>
-    <t>faster research 2%</t>
-  </si>
-  <si>
     <t>10+ beavers for each wood type</t>
   </si>
   <si>
     <t>2% more fish</t>
   </si>
   <si>
-    <t>More magic 5%</t>
-  </si>
-  <si>
-    <t>13% storage</t>
-  </si>
-  <si>
     <t>change?</t>
   </si>
   <si>
@@ -2865,18 +2845,9 @@
     <t>Apple storage +110</t>
   </si>
   <si>
-    <t>Unlock Research / wps 5.5%</t>
-  </si>
-  <si>
     <t>9% cheaper beavers</t>
   </si>
   <si>
-    <t>beaver +0.25 more wood</t>
-  </si>
-  <si>
-    <t>beaver +0.3 more wood</t>
-  </si>
-  <si>
     <t>WC use 2.5% less wood</t>
   </si>
   <si>
@@ -2889,9 +2860,6 @@
     <t>wpc</t>
   </si>
   <si>
-    <t>Unlock Apple Wood / 2% wpc tp wps</t>
-  </si>
-  <si>
     <t>Woodcamp production 8.5%</t>
   </si>
   <si>
@@ -3238,6 +3206,60 @@
   </si>
   <si>
     <t>Subjugation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oak per Beaver +0.25 </t>
+  </si>
+  <si>
+    <t>Woodcamp WPS +0.5</t>
+  </si>
+  <si>
+    <t>1.5% wpc tp wps</t>
+  </si>
+  <si>
+    <t>Unlock Apple Wood / 10% cheaper Beavers</t>
+  </si>
+  <si>
+    <t>Per WC +1 Beaver</t>
+  </si>
+  <si>
+    <t>Faster research 2%</t>
+  </si>
+  <si>
+    <t>7% cheaper WC's</t>
+  </si>
+  <si>
+    <t>6% Cheaper bots</t>
+  </si>
+  <si>
+    <t>5% More Magic</t>
+  </si>
+  <si>
+    <t>add 2% WPC to WPS</t>
+  </si>
+  <si>
+    <t>Better wood price 0.005</t>
+  </si>
+  <si>
+    <t>4.5% storage</t>
+  </si>
+  <si>
+    <t>Cheaper bots 4%</t>
+  </si>
+  <si>
+    <t>Fish price 5%</t>
+  </si>
+  <si>
+    <t>Apple per Beaver +0.3</t>
+  </si>
+  <si>
+    <t>Woodcamp WPS +1</t>
+  </si>
+  <si>
+    <t>WPS 4.5%</t>
+  </si>
+  <si>
+    <t>Unlock Research / 7.5% Storage</t>
   </si>
 </sst>
 </file>
@@ -4005,7 +4027,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Parasts" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4232,16 +4254,16 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" customWidth="1"/>
-    <col min="9" max="9" width="37.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" customWidth="1"/>
+    <col min="9" max="9" width="37.6640625" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" customWidth="1"/>
+    <col min="13" max="13" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:10" ht="12.75">
+    <row r="5" spans="2:10" ht="13.2">
       <c r="G5" s="1" t="s">
         <v>0</v>
       </c>
@@ -4252,7 +4274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="12.75">
+    <row r="6" spans="2:10" ht="13.2">
       <c r="G6" s="1">
         <v>1</v>
       </c>
@@ -4266,7 +4288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="12.75">
+    <row r="7" spans="2:10" ht="13.2">
       <c r="G7" s="1">
         <v>1</v>
       </c>
@@ -4280,7 +4302,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="12.75">
+    <row r="8" spans="2:10" ht="13.2">
       <c r="G8" s="1">
         <v>1</v>
       </c>
@@ -4294,7 +4316,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="12.75">
+    <row r="9" spans="2:10" ht="13.2">
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
@@ -4314,7 +4336,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="12.75">
+    <row r="10" spans="2:10" ht="13.2">
       <c r="G10" s="1">
         <v>1</v>
       </c>
@@ -4328,7 +4350,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="12.75">
+    <row r="11" spans="2:10" ht="13.2">
       <c r="G11" s="1">
         <v>1</v>
       </c>
@@ -4342,9 +4364,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="12.75">
+    <row r="12" spans="2:10" ht="13.2">
       <c r="C12" t="s">
-        <v>944</v>
+        <v>930</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -4362,7 +4384,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="12.75">
+    <row r="13" spans="2:10" ht="13.2">
       <c r="B13" t="s">
         <v>81</v>
       </c>
@@ -4385,7 +4407,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="12.75">
+    <row r="14" spans="2:10" ht="13.2">
       <c r="B14" t="s">
         <v>468</v>
       </c>
@@ -4408,9 +4430,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="12.75">
+    <row r="15" spans="2:10" ht="13.2">
       <c r="B15" t="s">
-        <v>945</v>
+        <v>931</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -4429,7 +4451,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="12.75">
+    <row r="16" spans="2:10" ht="13.2">
       <c r="G16" s="1">
         <v>2</v>
       </c>
@@ -4443,7 +4465,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="6:10" ht="12.75">
+    <row r="17" spans="6:10" ht="13.2">
       <c r="G17" s="1">
         <v>2</v>
       </c>
@@ -4457,7 +4479,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="6:10" ht="12.75">
+    <row r="18" spans="6:10" ht="13.2">
       <c r="G18" s="1">
         <v>2</v>
       </c>
@@ -4468,7 +4490,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="6:10" ht="12.75">
+    <row r="19" spans="6:10" ht="13.2">
       <c r="G19" s="1">
         <v>2</v>
       </c>
@@ -4482,7 +4504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="6:10" ht="12.75">
+    <row r="20" spans="6:10" ht="13.2">
       <c r="G20" s="1">
         <v>3</v>
       </c>
@@ -4496,7 +4518,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="6:10" ht="12.75">
+    <row r="21" spans="6:10" ht="13.2">
       <c r="G21" s="1">
         <v>3</v>
       </c>
@@ -4510,7 +4532,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="6:10" ht="12.75">
+    <row r="22" spans="6:10" ht="13.2">
       <c r="G22" s="1">
         <v>3</v>
       </c>
@@ -4524,7 +4546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="6:10" ht="12.75">
+    <row r="23" spans="6:10" ht="13.2">
       <c r="G23" s="1">
         <v>3</v>
       </c>
@@ -4538,7 +4560,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="6:10" ht="12.75">
+    <row r="24" spans="6:10" ht="13.2">
       <c r="G24" s="1">
         <v>3</v>
       </c>
@@ -4549,7 +4571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="6:10" ht="12.75">
+    <row r="25" spans="6:10" ht="13.2">
       <c r="G25" s="1">
         <v>3</v>
       </c>
@@ -4563,7 +4585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="6:10" ht="12.75">
+    <row r="26" spans="6:10" ht="13.2">
       <c r="G26" s="1">
         <v>3</v>
       </c>
@@ -4875,11 +4897,11 @@
       <selection activeCell="K149" sqref="K149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="4" max="4" width="57" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
-    <col min="6" max="6" width="35.85546875" customWidth="1"/>
+    <col min="6" max="6" width="35.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10">
@@ -6696,15 +6718,15 @@
       <selection activeCell="F4" sqref="F4:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="12.75">
+    <row r="2" spans="1:15" ht="13.2">
       <c r="D2" s="1" t="s">
         <v>50</v>
       </c>
@@ -6712,7 +6734,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="12.75">
+    <row r="3" spans="1:15" ht="13.2">
       <c r="C3" s="1" t="s">
         <v>52</v>
       </c>
@@ -6744,7 +6766,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="12.75">
+    <row r="4" spans="1:15" ht="13.2">
       <c r="C4" s="1">
         <v>1</v>
       </c>
@@ -6777,7 +6799,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="12.75">
+    <row r="5" spans="1:15" ht="13.2">
       <c r="C5" s="1">
         <v>2</v>
       </c>
@@ -6810,7 +6832,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="12.75">
+    <row r="6" spans="1:15" ht="13.2">
       <c r="C6" s="1">
         <v>3</v>
       </c>
@@ -6843,7 +6865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="12.75">
+    <row r="7" spans="1:15" ht="13.2">
       <c r="C7" s="1">
         <v>4</v>
       </c>
@@ -6876,7 +6898,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="12.75">
+    <row r="8" spans="1:15" ht="13.2">
       <c r="C8" s="1">
         <v>5</v>
       </c>
@@ -6909,7 +6931,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="12.75">
+    <row r="9" spans="1:15" ht="13.2">
       <c r="C9" s="1">
         <v>6</v>
       </c>
@@ -6942,7 +6964,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="12.75">
+    <row r="10" spans="1:15" ht="13.2">
       <c r="C10" s="1">
         <v>7</v>
       </c>
@@ -6975,7 +6997,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="12.75">
+    <row r="11" spans="1:15" ht="13.2">
       <c r="C11" s="1">
         <v>8</v>
       </c>
@@ -7008,7 +7030,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="12.75">
+    <row r="12" spans="1:15" ht="13.2">
       <c r="C12" s="1">
         <v>9</v>
       </c>
@@ -7041,7 +7063,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="12.75">
+    <row r="13" spans="1:15" ht="13.2">
       <c r="A13" s="39" t="s">
         <v>3</v>
       </c>
@@ -7077,7 +7099,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="12.75">
+    <row r="14" spans="1:15" ht="13.2">
       <c r="A14" s="35" t="s">
         <v>18</v>
       </c>
@@ -7113,7 +7135,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="12.75">
+    <row r="15" spans="1:15" ht="13.2">
       <c r="A15" s="35" t="s">
         <v>9</v>
       </c>
@@ -7149,7 +7171,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="12.75">
+    <row r="16" spans="1:15" ht="13.2">
       <c r="A16" s="35" t="s">
         <v>14</v>
       </c>
@@ -7185,7 +7207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="12.75">
+    <row r="17" spans="1:15" ht="13.2">
       <c r="A17" s="35" t="s">
         <v>21</v>
       </c>
@@ -7221,7 +7243,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="12.75">
+    <row r="18" spans="1:15" ht="13.2">
       <c r="A18" s="35" t="s">
         <v>16</v>
       </c>
@@ -7257,7 +7279,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="12.75">
+    <row r="19" spans="1:15" ht="13.2">
       <c r="A19" s="47" t="s">
         <v>26</v>
       </c>
@@ -7265,7 +7287,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="12.75">
+    <row r="20" spans="1:15" ht="13.2">
       <c r="A20" s="35" t="s">
         <v>29</v>
       </c>
@@ -7273,7 +7295,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="12.75">
+    <row r="21" spans="1:15" ht="13.2">
       <c r="A21" s="35" t="s">
         <v>31</v>
       </c>
@@ -7281,7 +7303,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="12.75">
+    <row r="22" spans="1:15" ht="13.2">
       <c r="A22" s="35" t="s">
         <v>33</v>
       </c>
@@ -7289,7 +7311,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="12.75">
+    <row r="23" spans="1:15" ht="13.2">
       <c r="A23" s="35" t="s">
         <v>37</v>
       </c>
@@ -7297,7 +7319,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="12.75">
+    <row r="24" spans="1:15" ht="13.2">
       <c r="A24" s="35" t="s">
         <v>39</v>
       </c>
@@ -7305,7 +7327,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="12.75">
+    <row r="25" spans="1:15" ht="13.2">
       <c r="A25" s="35" t="s">
         <v>41</v>
       </c>
@@ -7313,7 +7335,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="12.75">
+    <row r="26" spans="1:15" ht="13.2">
       <c r="A26" s="35" t="s">
         <v>45</v>
       </c>
@@ -7321,7 +7343,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="12.75">
+    <row r="27" spans="1:15" ht="13.2">
       <c r="A27" s="35" t="s">
         <v>46</v>
       </c>
@@ -7329,12 +7351,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="12.75">
+    <row r="28" spans="1:15" ht="13.2">
       <c r="O28" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="12.75">
+    <row r="29" spans="1:15" ht="13.2">
       <c r="C29" s="1">
         <v>2</v>
       </c>
@@ -7367,12 +7389,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="12.75">
+    <row r="30" spans="1:15" ht="13.2">
       <c r="O30" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="12.75">
+    <row r="32" spans="1:15" ht="13.2">
       <c r="F32" s="23" t="s">
         <v>72</v>
       </c>
@@ -7382,7 +7404,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="12.75">
+    <row r="34" spans="2:12" ht="13.2">
       <c r="F34" s="23" t="s">
         <v>74</v>
       </c>
@@ -7560,41 +7582,41 @@
   </sheetPr>
   <dimension ref="A1:X295"/>
   <sheetViews>
-    <sheetView topLeftCell="C280" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F295" sqref="F295"/>
+    <sheetView tabSelected="1" topLeftCell="C21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="1.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="1.6640625" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" customWidth="1"/>
     <col min="6" max="6" width="40" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="28.140625" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" customWidth="1"/>
-    <col min="21" max="21" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="32.88671875" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="28.109375" customWidth="1"/>
+    <col min="14" max="14" width="19.44140625" customWidth="1"/>
+    <col min="15" max="15" width="20.88671875" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" customWidth="1"/>
+    <col min="17" max="17" width="18.109375" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" customWidth="1"/>
+    <col min="20" max="20" width="14.44140625" customWidth="1"/>
+    <col min="21" max="21" width="21.44140625" customWidth="1"/>
     <col min="22" max="22" width="26" customWidth="1"/>
-    <col min="23" max="23" width="23.5703125" customWidth="1"/>
-    <col min="24" max="24" width="23.28515625" customWidth="1"/>
-    <col min="25" max="25" width="22.140625" customWidth="1"/>
-    <col min="26" max="26" width="31.42578125" customWidth="1"/>
-    <col min="27" max="27" width="37.7109375" customWidth="1"/>
-    <col min="28" max="28" width="29.42578125" customWidth="1"/>
-    <col min="29" max="29" width="29.85546875" customWidth="1"/>
-    <col min="30" max="30" width="28.7109375" customWidth="1"/>
-    <col min="31" max="31" width="33.140625" customWidth="1"/>
+    <col min="23" max="23" width="23.5546875" customWidth="1"/>
+    <col min="24" max="24" width="23.33203125" customWidth="1"/>
+    <col min="25" max="25" width="22.109375" customWidth="1"/>
+    <col min="26" max="26" width="31.44140625" customWidth="1"/>
+    <col min="27" max="27" width="37.6640625" customWidth="1"/>
+    <col min="28" max="28" width="29.44140625" customWidth="1"/>
+    <col min="29" max="29" width="29.88671875" customWidth="1"/>
+    <col min="30" max="30" width="28.6640625" customWidth="1"/>
+    <col min="31" max="31" width="33.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1">
@@ -7602,7 +7624,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="12.75">
+    <row r="2" spans="1:23" ht="13.2">
       <c r="C2" s="1" t="s">
         <v>75</v>
       </c>
@@ -7677,7 +7699,7 @@
       <c r="V5" s="114"/>
       <c r="W5" s="114"/>
     </row>
-    <row r="6" spans="1:23" ht="13.5" thickBot="1">
+    <row r="6" spans="1:23" ht="13.8" thickBot="1">
       <c r="A6" s="35" t="s">
         <v>18</v>
       </c>
@@ -7694,7 +7716,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="105" t="s">
-        <v>940</v>
+        <v>1048</v>
       </c>
       <c r="G6" s="45" t="s">
         <v>360</v>
@@ -7746,7 +7768,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="12.75">
+    <row r="7" spans="1:23" ht="13.2">
       <c r="A7" s="35" t="s">
         <v>9</v>
       </c>
@@ -7818,7 +7840,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="12.75">
+    <row r="8" spans="1:23" ht="13.2">
       <c r="A8" s="35" t="s">
         <v>14</v>
       </c>
@@ -7835,7 +7857,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="75" t="s">
-        <v>470</v>
+        <v>1049</v>
       </c>
       <c r="G8" s="45" t="s">
         <v>413</v>
@@ -7889,7 +7911,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="12.75">
+    <row r="9" spans="1:23" ht="13.2">
       <c r="A9" s="35" t="s">
         <v>21</v>
       </c>
@@ -7906,7 +7928,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="105" t="s">
-        <v>893</v>
+        <v>1050</v>
       </c>
       <c r="G9" s="45" t="s">
         <v>365</v>
@@ -7957,7 +7979,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="12.75">
+    <row r="10" spans="1:23" ht="13.2">
       <c r="A10" s="35" t="s">
         <v>16</v>
       </c>
@@ -7974,7 +7996,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="104" t="s">
-        <v>946</v>
+        <v>1051</v>
       </c>
       <c r="G10" s="45" t="s">
         <v>367</v>
@@ -8012,7 +8034,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="12.75">
+    <row r="11" spans="1:23" ht="13.2">
       <c r="A11" s="47" t="s">
         <v>26</v>
       </c>
@@ -8029,7 +8051,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="75" t="s">
-        <v>898</v>
+        <v>1052</v>
       </c>
       <c r="H11">
         <v>750</v>
@@ -8071,7 +8093,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="12.75">
+    <row r="12" spans="1:23" ht="13.2">
       <c r="A12" s="35" t="s">
         <v>29</v>
       </c>
@@ -8088,7 +8110,7 @@
         <v>7</v>
       </c>
       <c r="F12" s="102" t="s">
-        <v>907</v>
+        <v>1053</v>
       </c>
       <c r="H12">
         <v>1400</v>
@@ -8125,7 +8147,7 @@
       </c>
       <c r="W12" s="40"/>
     </row>
-    <row r="13" spans="1:23" ht="12.75">
+    <row r="13" spans="1:23" ht="13.2">
       <c r="A13" s="35" t="s">
         <v>31</v>
       </c>
@@ -8142,7 +8164,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="65" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H13" s="1">
         <v>10000</v>
@@ -8172,7 +8194,7 @@
       </c>
       <c r="W13" s="40"/>
     </row>
-    <row r="14" spans="1:23" ht="12.75">
+    <row r="14" spans="1:23" ht="13.2">
       <c r="A14" s="35" t="s">
         <v>33</v>
       </c>
@@ -8186,7 +8208,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="97" t="s">
-        <v>896</v>
+        <v>1054</v>
       </c>
       <c r="M14" s="27" t="s">
         <v>293</v>
@@ -8206,7 +8228,7 @@
       <c r="V14" s="38"/>
       <c r="W14" s="40"/>
     </row>
-    <row r="15" spans="1:23" ht="12.75">
+    <row r="15" spans="1:23" ht="13.2">
       <c r="A15" s="35" t="s">
         <v>37</v>
       </c>
@@ -8220,7 +8242,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="98" t="s">
-        <v>936</v>
+        <v>925</v>
       </c>
       <c r="M15" s="40" t="s">
         <v>325</v>
@@ -8240,7 +8262,7 @@
       <c r="V15" s="38"/>
       <c r="W15" s="40"/>
     </row>
-    <row r="16" spans="1:23" ht="12.75">
+    <row r="16" spans="1:23" ht="13.2">
       <c r="A16" s="35" t="s">
         <v>39</v>
       </c>
@@ -8254,7 +8276,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="99" t="s">
-        <v>895</v>
+        <v>1055</v>
       </c>
       <c r="M16" s="40" t="s">
         <v>326</v>
@@ -8274,7 +8296,7 @@
       <c r="V16" s="42"/>
       <c r="W16" s="43"/>
     </row>
-    <row r="17" spans="1:23" ht="12.75">
+    <row r="17" spans="1:23" ht="13.2">
       <c r="A17" s="35" t="s">
         <v>41</v>
       </c>
@@ -8288,7 +8310,7 @@
         <v>12</v>
       </c>
       <c r="F17" s="97" t="s">
-        <v>910</v>
+        <v>1056</v>
       </c>
       <c r="G17" t="e">
         <f>log</f>
@@ -8310,7 +8332,7 @@
       <c r="V17" s="40"/>
       <c r="W17" s="40"/>
     </row>
-    <row r="18" spans="1:23" ht="12.75">
+    <row r="18" spans="1:23" ht="13.2">
       <c r="A18" s="35" t="s">
         <v>45</v>
       </c>
@@ -8324,7 +8346,7 @@
         <v>13</v>
       </c>
       <c r="F18" s="75" t="s">
-        <v>897</v>
+        <v>1057</v>
       </c>
       <c r="M18" s="40"/>
       <c r="N18" s="40" t="s">
@@ -8342,7 +8364,7 @@
       <c r="V18" s="40"/>
       <c r="W18" s="40"/>
     </row>
-    <row r="19" spans="1:23" ht="12.75">
+    <row r="19" spans="1:23" ht="13.2">
       <c r="A19" s="35" t="s">
         <v>46</v>
       </c>
@@ -8359,7 +8381,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="74" t="s">
-        <v>556</v>
+        <v>1058</v>
       </c>
       <c r="G19" t="s">
         <v>761</v>
@@ -8378,7 +8400,7 @@
       <c r="V19" s="40"/>
       <c r="W19" s="40"/>
     </row>
-    <row r="20" spans="1:23" ht="12.75">
+    <row r="20" spans="1:23" ht="13.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>15</v>
@@ -8390,7 +8412,7 @@
         <v>15</v>
       </c>
       <c r="F20" s="105" t="s">
-        <v>909</v>
+        <v>900</v>
       </c>
       <c r="M20" s="35"/>
       <c r="N20" s="40"/>
@@ -8406,7 +8428,7 @@
       <c r="V20" s="40"/>
       <c r="W20" s="40"/>
     </row>
-    <row r="21" spans="1:23" ht="12.75">
+    <row r="21" spans="1:23" ht="13.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>16</v>
@@ -8421,7 +8443,7 @@
         <v>16</v>
       </c>
       <c r="F21" s="65" t="s">
-        <v>904</v>
+        <v>1059</v>
       </c>
       <c r="M21" s="40"/>
       <c r="N21" s="40"/>
@@ -8437,7 +8459,7 @@
       <c r="V21" s="40"/>
       <c r="W21" s="40"/>
     </row>
-    <row r="22" spans="1:23" ht="12.75">
+    <row r="22" spans="1:23" ht="13.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>17</v>
@@ -8449,7 +8471,7 @@
         <v>17</v>
       </c>
       <c r="F22" s="74" t="s">
-        <v>906</v>
+        <v>1060</v>
       </c>
       <c r="M22" s="40"/>
       <c r="N22" s="40"/>
@@ -8465,7 +8487,7 @@
       <c r="V22" s="40"/>
       <c r="W22" s="40"/>
     </row>
-    <row r="23" spans="1:23" ht="12.75">
+    <row r="23" spans="1:23" ht="13.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
         <v>18</v>
@@ -8477,7 +8499,7 @@
         <v>18</v>
       </c>
       <c r="F23" s="100" t="s">
-        <v>905</v>
+        <v>1061</v>
       </c>
       <c r="H23" s="44">
         <v>4.11E+17</v>
@@ -8502,7 +8524,7 @@
       <c r="V23" s="40"/>
       <c r="W23" s="40"/>
     </row>
-    <row r="24" spans="1:23" ht="12.75">
+    <row r="24" spans="1:23" ht="13.2">
       <c r="A24" s="1"/>
       <c r="B24" s="106">
         <v>19</v>
@@ -8517,7 +8539,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="105" t="s">
-        <v>941</v>
+        <v>1062</v>
       </c>
       <c r="H24">
         <v>20</v>
@@ -8542,7 +8564,7 @@
       <c r="V24" s="40"/>
       <c r="W24" s="40"/>
     </row>
-    <row r="25" spans="1:23" ht="12.75">
+    <row r="25" spans="1:23" ht="13.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1">
         <v>20</v>
@@ -8557,7 +8579,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="65" t="s">
-        <v>937</v>
+        <v>926</v>
       </c>
       <c r="H25">
         <v>30</v>
@@ -8582,7 +8604,7 @@
       <c r="V25" s="40"/>
       <c r="W25" s="40"/>
     </row>
-    <row r="26" spans="1:23" ht="12.75">
+    <row r="26" spans="1:23" ht="13.2">
       <c r="B26" s="1">
         <v>21</v>
       </c>
@@ -8596,7 +8618,7 @@
         <v>3</v>
       </c>
       <c r="F26" s="75" t="s">
-        <v>471</v>
+        <v>1063</v>
       </c>
       <c r="H26">
         <v>150</v>
@@ -8621,7 +8643,7 @@
       <c r="V26" s="40"/>
       <c r="W26" s="40"/>
     </row>
-    <row r="27" spans="1:23" ht="12.75">
+    <row r="27" spans="1:23" ht="13.2">
       <c r="B27" s="1">
         <v>22</v>
       </c>
@@ -8635,7 +8657,7 @@
         <v>4</v>
       </c>
       <c r="F27" s="65" t="s">
-        <v>911</v>
+        <v>1064</v>
       </c>
       <c r="H27">
         <v>300</v>
@@ -8660,7 +8682,7 @@
       <c r="V27" s="40"/>
       <c r="W27" s="40"/>
     </row>
-    <row r="28" spans="1:23" ht="12.75">
+    <row r="28" spans="1:23" ht="13.2">
       <c r="B28" s="1">
         <v>23</v>
       </c>
@@ -8671,10 +8693,10 @@
         <v>5</v>
       </c>
       <c r="F28" s="105" t="s">
-        <v>931</v>
+        <v>920</v>
       </c>
       <c r="G28" t="s">
-        <v>912</v>
+        <v>901</v>
       </c>
       <c r="H28">
         <v>400</v>
@@ -8696,7 +8718,7 @@
       <c r="V28" s="40"/>
       <c r="W28" s="40"/>
     </row>
-    <row r="29" spans="1:23" ht="12.75">
+    <row r="29" spans="1:23" ht="13.2">
       <c r="B29" s="1">
         <v>24</v>
       </c>
@@ -8710,10 +8732,10 @@
         <v>6</v>
       </c>
       <c r="F29" s="104" t="s">
-        <v>938</v>
+        <v>1065</v>
       </c>
       <c r="G29" t="s">
-        <v>913</v>
+        <v>902</v>
       </c>
       <c r="H29">
         <v>1000</v>
@@ -8730,7 +8752,7 @@
       <c r="V29" s="40"/>
       <c r="W29" s="40"/>
     </row>
-    <row r="30" spans="1:23" ht="12.75">
+    <row r="30" spans="1:23" ht="13.2">
       <c r="B30" s="1">
         <v>25</v>
       </c>
@@ -8744,7 +8766,7 @@
         <v>7</v>
       </c>
       <c r="F30" s="105" t="s">
-        <v>939</v>
+        <v>927</v>
       </c>
       <c r="H30">
         <v>1200</v>
@@ -8764,7 +8786,7 @@
       <c r="V30" s="40"/>
       <c r="W30" s="40"/>
     </row>
-    <row r="31" spans="1:23" ht="12.75">
+    <row r="31" spans="1:23" ht="13.2">
       <c r="B31" s="1">
         <v>26</v>
       </c>
@@ -8775,7 +8797,7 @@
         <v>8</v>
       </c>
       <c r="F31" s="65" t="s">
-        <v>932</v>
+        <v>921</v>
       </c>
       <c r="H31">
         <v>2000</v>
@@ -8787,7 +8809,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="12.75">
+    <row r="32" spans="1:23" ht="13.2">
       <c r="B32" s="1">
         <v>27</v>
       </c>
@@ -8801,10 +8823,10 @@
         <v>9</v>
       </c>
       <c r="F32" s="75" t="s">
-        <v>942</v>
+        <v>928</v>
       </c>
       <c r="G32" t="s">
-        <v>914</v>
+        <v>903</v>
       </c>
       <c r="H32">
         <v>2200</v>
@@ -8813,7 +8835,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="18.75" thickBot="1">
+    <row r="33" spans="1:24" ht="18" thickBot="1">
       <c r="B33" s="1">
         <v>28</v>
       </c>
@@ -8824,13 +8846,13 @@
         <v>10</v>
       </c>
       <c r="F33" s="102" t="s">
-        <v>915</v>
+        <v>904</v>
       </c>
       <c r="O33" s="79" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="18.75" thickBot="1">
+    <row r="34" spans="1:24" ht="18" thickBot="1">
       <c r="B34" s="1">
         <v>29</v>
       </c>
@@ -8858,7 +8880,7 @@
       <c r="V34" s="53"/>
       <c r="W34" s="53"/>
     </row>
-    <row r="35" spans="1:24" ht="13.5" thickBot="1">
+    <row r="35" spans="1:24" ht="13.8" thickBot="1">
       <c r="B35" s="1">
         <v>30</v>
       </c>
@@ -8911,7 +8933,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="12.75">
+    <row r="36" spans="1:24" ht="13.2">
       <c r="B36" s="1">
         <v>31</v>
       </c>
@@ -8922,7 +8944,7 @@
         <v>13</v>
       </c>
       <c r="F36" s="97" t="s">
-        <v>934</v>
+        <v>923</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>130</v>
@@ -8968,7 +8990,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="12.75">
+    <row r="37" spans="1:24" ht="13.2">
       <c r="B37" s="1">
         <v>32</v>
       </c>
@@ -9026,7 +9048,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="12.75">
+    <row r="38" spans="1:24" ht="13.2">
       <c r="B38" s="1">
         <v>33</v>
       </c>
@@ -9037,7 +9059,7 @@
         <v>15</v>
       </c>
       <c r="F38" s="100" t="s">
-        <v>933</v>
+        <v>922</v>
       </c>
       <c r="H38" s="45"/>
       <c r="I38" t="s">
@@ -9083,7 +9105,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="12.75">
+    <row r="39" spans="1:24" ht="13.2">
       <c r="B39" s="1">
         <v>34</v>
       </c>
@@ -9094,7 +9116,7 @@
         <v>16</v>
       </c>
       <c r="F39" s="101" t="s">
-        <v>943</v>
+        <v>929</v>
       </c>
       <c r="H39" s="45"/>
       <c r="I39" s="1" t="s">
@@ -9141,7 +9163,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="12.75">
+    <row r="40" spans="1:24" ht="13.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -9198,7 +9220,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="12.75">
+    <row r="41" spans="1:24" ht="13.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -9212,7 +9234,7 @@
         <v>18</v>
       </c>
       <c r="F41" s="97" t="s">
-        <v>935</v>
+        <v>924</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="45"/>
@@ -9252,7 +9274,7 @@
       </c>
       <c r="X41" s="55"/>
     </row>
-    <row r="42" spans="1:24" ht="12.75">
+    <row r="42" spans="1:24" ht="13.2">
       <c r="A42">
         <v>7</v>
       </c>
@@ -9267,7 +9289,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="105" t="s">
-        <v>916</v>
+        <v>905</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="45">
@@ -9309,7 +9331,7 @@
       </c>
       <c r="X42" s="55"/>
     </row>
-    <row r="43" spans="1:24" ht="12.75">
+    <row r="43" spans="1:24" ht="13.2">
       <c r="A43">
         <v>10</v>
       </c>
@@ -9362,7 +9384,7 @@
       </c>
       <c r="X43" s="55"/>
     </row>
-    <row r="44" spans="1:24" ht="12.75">
+    <row r="44" spans="1:24" ht="13.2">
       <c r="A44">
         <v>13</v>
       </c>
@@ -9415,7 +9437,7 @@
       </c>
       <c r="X44" s="55"/>
     </row>
-    <row r="45" spans="1:24" ht="12.75">
+    <row r="45" spans="1:24" ht="13.2">
       <c r="A45">
         <v>16</v>
       </c>
@@ -9432,7 +9454,7 @@
         <v>4</v>
       </c>
       <c r="F45" s="75" t="s">
-        <v>917</v>
+        <v>906</v>
       </c>
       <c r="G45" s="1"/>
       <c r="L45" s="40">
@@ -9469,7 +9491,7 @@
       </c>
       <c r="X45" s="59"/>
     </row>
-    <row r="46" spans="1:24" ht="12.75">
+    <row r="46" spans="1:24" ht="13.2">
       <c r="A46">
         <v>19</v>
       </c>
@@ -9520,7 +9542,7 @@
       </c>
       <c r="X46" s="55"/>
     </row>
-    <row r="47" spans="1:24" ht="12.75">
+    <row r="47" spans="1:24" ht="13.2">
       <c r="A47">
         <v>22</v>
       </c>
@@ -9571,7 +9593,7 @@
       </c>
       <c r="X47" s="55"/>
     </row>
-    <row r="48" spans="1:24" ht="12.75">
+    <row r="48" spans="1:24" ht="13.2">
       <c r="A48">
         <v>25</v>
       </c>
@@ -9620,7 +9642,7 @@
       </c>
       <c r="X48" s="55"/>
     </row>
-    <row r="49" spans="1:24" ht="12.75">
+    <row r="49" spans="1:24" ht="13.2">
       <c r="A49">
         <v>28</v>
       </c>
@@ -9669,7 +9691,7 @@
       </c>
       <c r="X49" s="55"/>
     </row>
-    <row r="50" spans="1:24" ht="12.75">
+    <row r="50" spans="1:24" ht="13.2">
       <c r="A50">
         <v>31</v>
       </c>
@@ -9718,7 +9740,7 @@
       </c>
       <c r="X50" s="55"/>
     </row>
-    <row r="51" spans="1:24" ht="12.75">
+    <row r="51" spans="1:24" ht="13.2">
       <c r="A51">
         <v>34</v>
       </c>
@@ -9764,7 +9786,7 @@
       </c>
       <c r="X51" s="55"/>
     </row>
-    <row r="52" spans="1:24" ht="12.75">
+    <row r="52" spans="1:24" ht="13.2">
       <c r="A52">
         <v>37</v>
       </c>
@@ -9823,7 +9845,7 @@
       </c>
       <c r="X52" s="55"/>
     </row>
-    <row r="53" spans="1:24" ht="12.75">
+    <row r="53" spans="1:24" ht="13.2">
       <c r="A53">
         <v>40</v>
       </c>
@@ -9873,7 +9895,7 @@
       </c>
       <c r="X53" s="55"/>
     </row>
-    <row r="54" spans="1:24" ht="12.75">
+    <row r="54" spans="1:24" ht="13.2">
       <c r="A54">
         <v>43</v>
       </c>
@@ -9920,7 +9942,7 @@
       </c>
       <c r="X54" s="55"/>
     </row>
-    <row r="55" spans="1:24" ht="12.75">
+    <row r="55" spans="1:24" ht="13.2">
       <c r="A55">
         <v>46</v>
       </c>
@@ -9976,7 +9998,7 @@
       </c>
       <c r="X55" s="55"/>
     </row>
-    <row r="56" spans="1:24" ht="12.75">
+    <row r="56" spans="1:24" ht="13.2">
       <c r="A56">
         <v>49</v>
       </c>
@@ -10023,7 +10045,7 @@
       </c>
       <c r="X56" s="55"/>
     </row>
-    <row r="57" spans="1:24" ht="12.75">
+    <row r="57" spans="1:24" ht="13.2">
       <c r="A57">
         <v>52</v>
       </c>
@@ -10073,7 +10095,7 @@
       </c>
       <c r="X57" s="55"/>
     </row>
-    <row r="58" spans="1:24" ht="12.75">
+    <row r="58" spans="1:24" ht="13.2">
       <c r="A58">
         <v>55</v>
       </c>
@@ -10116,7 +10138,7 @@
       </c>
       <c r="X58" s="55"/>
     </row>
-    <row r="59" spans="1:24" ht="12.75">
+    <row r="59" spans="1:24" ht="13.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -10162,7 +10184,7 @@
       </c>
       <c r="X59" s="55"/>
     </row>
-    <row r="60" spans="1:24" ht="12.75">
+    <row r="60" spans="1:24" ht="13.2">
       <c r="A60">
         <v>61</v>
       </c>
@@ -10205,7 +10227,7 @@
       </c>
       <c r="X60" s="55"/>
     </row>
-    <row r="61" spans="1:24" ht="12.75">
+    <row r="61" spans="1:24" ht="13.2">
       <c r="A61">
         <v>64</v>
       </c>
@@ -10250,7 +10272,7 @@
       </c>
       <c r="X61" s="55"/>
     </row>
-    <row r="62" spans="1:24" ht="12.75">
+    <row r="62" spans="1:24" ht="13.2">
       <c r="A62">
         <v>9887654321</v>
       </c>
@@ -10292,7 +10314,7 @@
       </c>
       <c r="X62" s="55"/>
     </row>
-    <row r="63" spans="1:24" ht="12.75">
+    <row r="63" spans="1:24" ht="13.2">
       <c r="B63" s="1">
         <v>58</v>
       </c>
@@ -10331,7 +10353,7 @@
       </c>
       <c r="X63" s="55"/>
     </row>
-    <row r="64" spans="1:24" ht="12.75">
+    <row r="64" spans="1:24" ht="13.2">
       <c r="B64" s="1">
         <v>59</v>
       </c>
@@ -10368,7 +10390,7 @@
       <c r="W64" s="55"/>
       <c r="X64" s="55"/>
     </row>
-    <row r="65" spans="2:24" ht="12.75">
+    <row r="65" spans="2:24" ht="13.2">
       <c r="B65" s="1">
         <v>60</v>
       </c>
@@ -10405,7 +10427,7 @@
       <c r="W65" s="55"/>
       <c r="X65" s="55"/>
     </row>
-    <row r="66" spans="2:24" ht="12.75">
+    <row r="66" spans="2:24" ht="13.2">
       <c r="B66" s="1">
         <v>61</v>
       </c>
@@ -10442,7 +10464,7 @@
       <c r="W66" s="55"/>
       <c r="X66" s="55"/>
     </row>
-    <row r="67" spans="2:24" ht="12.75">
+    <row r="67" spans="2:24" ht="13.2">
       <c r="B67" s="1">
         <v>62</v>
       </c>
@@ -10479,7 +10501,7 @@
       <c r="W67" s="55"/>
       <c r="X67" s="55"/>
     </row>
-    <row r="68" spans="2:24" ht="12.75">
+    <row r="68" spans="2:24" ht="13.2">
       <c r="B68" s="1">
         <v>63</v>
       </c>
@@ -10516,7 +10538,7 @@
       <c r="W68" s="55"/>
       <c r="X68" s="55"/>
     </row>
-    <row r="69" spans="2:24" ht="12.75">
+    <row r="69" spans="2:24" ht="13.2">
       <c r="B69" s="1">
         <v>64</v>
       </c>
@@ -10551,7 +10573,7 @@
       <c r="W69" s="55"/>
       <c r="X69" s="55"/>
     </row>
-    <row r="70" spans="2:24" ht="12.75">
+    <row r="70" spans="2:24" ht="13.2">
       <c r="B70" s="1">
         <v>65</v>
       </c>
@@ -10589,7 +10611,7 @@
       <c r="W70" s="55"/>
       <c r="X70" s="55"/>
     </row>
-    <row r="71" spans="2:24" ht="12.75">
+    <row r="71" spans="2:24" ht="13.2">
       <c r="B71" s="1">
         <v>66</v>
       </c>
@@ -10622,7 +10644,7 @@
       <c r="W71" s="55"/>
       <c r="X71" s="55"/>
     </row>
-    <row r="72" spans="2:24" ht="12.75">
+    <row r="72" spans="2:24" ht="13.2">
       <c r="B72" s="1">
         <v>67</v>
       </c>
@@ -10655,7 +10677,7 @@
       <c r="W72" s="55"/>
       <c r="X72" s="55"/>
     </row>
-    <row r="73" spans="2:24" ht="12.75">
+    <row r="73" spans="2:24" ht="13.2">
       <c r="B73" s="1">
         <v>68</v>
       </c>
@@ -10688,7 +10710,7 @@
       <c r="W73" s="55"/>
       <c r="X73" s="55"/>
     </row>
-    <row r="74" spans="2:24" ht="12.75">
+    <row r="74" spans="2:24" ht="13.2">
       <c r="B74" s="1">
         <v>69</v>
       </c>
@@ -10721,7 +10743,7 @@
       <c r="W74" s="55"/>
       <c r="X74" s="55"/>
     </row>
-    <row r="75" spans="2:24" ht="12.75">
+    <row r="75" spans="2:24" ht="13.2">
       <c r="B75" s="1">
         <v>70</v>
       </c>
@@ -10754,7 +10776,7 @@
       <c r="W75" s="55"/>
       <c r="X75" s="55"/>
     </row>
-    <row r="76" spans="2:24" ht="12.75">
+    <row r="76" spans="2:24" ht="13.2">
       <c r="B76" s="1">
         <v>71</v>
       </c>
@@ -10787,7 +10809,7 @@
       <c r="W76" s="55"/>
       <c r="X76" s="55"/>
     </row>
-    <row r="77" spans="2:24" ht="12.75">
+    <row r="77" spans="2:24" ht="13.2">
       <c r="B77" s="1">
         <v>72</v>
       </c>
@@ -10823,7 +10845,7 @@
       <c r="W77" s="55"/>
       <c r="X77" s="55"/>
     </row>
-    <row r="78" spans="2:24" ht="12.75">
+    <row r="78" spans="2:24" ht="13.2">
       <c r="B78" s="106">
         <v>73</v>
       </c>
@@ -10857,7 +10879,7 @@
       <c r="W78" s="55"/>
       <c r="X78" s="55"/>
     </row>
-    <row r="79" spans="2:24" ht="12.75">
+    <row r="79" spans="2:24" ht="13.2">
       <c r="B79" s="1">
         <v>74</v>
       </c>
@@ -10890,7 +10912,7 @@
       <c r="W79" s="55"/>
       <c r="X79" s="55"/>
     </row>
-    <row r="80" spans="2:24" ht="12.75">
+    <row r="80" spans="2:24" ht="13.2">
       <c r="B80" s="1">
         <v>75</v>
       </c>
@@ -10923,7 +10945,7 @@
       <c r="W80" s="55"/>
       <c r="X80" s="55"/>
     </row>
-    <row r="81" spans="2:24" ht="12.75">
+    <row r="81" spans="2:24" ht="13.2">
       <c r="B81" s="1">
         <v>76</v>
       </c>
@@ -10954,7 +10976,7 @@
       <c r="W81" s="55"/>
       <c r="X81" s="55"/>
     </row>
-    <row r="82" spans="2:24" ht="12.75">
+    <row r="82" spans="2:24" ht="13.2">
       <c r="B82" s="1">
         <v>77</v>
       </c>
@@ -10985,7 +11007,7 @@
       <c r="W82" s="55"/>
       <c r="X82" s="55"/>
     </row>
-    <row r="83" spans="2:24" ht="12.75">
+    <row r="83" spans="2:24" ht="13.2">
       <c r="B83" s="1">
         <v>78</v>
       </c>
@@ -11019,7 +11041,7 @@
       <c r="W83" s="55"/>
       <c r="X83" s="55"/>
     </row>
-    <row r="84" spans="2:24" ht="12.75">
+    <row r="84" spans="2:24" ht="13.2">
       <c r="B84" s="1">
         <v>79</v>
       </c>
@@ -11050,7 +11072,7 @@
       <c r="W84" s="55"/>
       <c r="X84" s="55"/>
     </row>
-    <row r="85" spans="2:24" ht="12.75">
+    <row r="85" spans="2:24" ht="13.2">
       <c r="B85" s="1">
         <v>80</v>
       </c>
@@ -11081,7 +11103,7 @@
       <c r="W85" s="55"/>
       <c r="X85" s="55"/>
     </row>
-    <row r="86" spans="2:24" ht="12.75">
+    <row r="86" spans="2:24" ht="13.2">
       <c r="B86" s="1">
         <v>81</v>
       </c>
@@ -11112,7 +11134,7 @@
       <c r="W86" s="55"/>
       <c r="X86" s="55"/>
     </row>
-    <row r="87" spans="2:24" ht="12.75">
+    <row r="87" spans="2:24" ht="13.2">
       <c r="B87" s="1">
         <v>82</v>
       </c>
@@ -11162,7 +11184,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="2:24" ht="12.75">
+    <row r="88" spans="2:24" ht="13.2">
       <c r="B88" s="1">
         <v>83</v>
       </c>
@@ -11194,7 +11216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="2:24" ht="12.75">
+    <row r="89" spans="2:24" ht="13.2">
       <c r="B89" s="1">
         <v>84</v>
       </c>
@@ -11211,7 +11233,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="90" spans="2:24" ht="12.75">
+    <row r="90" spans="2:24" ht="13.2">
       <c r="B90" s="1">
         <v>85</v>
       </c>
@@ -11241,7 +11263,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="2:24" ht="12.75">
+    <row r="91" spans="2:24" ht="13.2">
       <c r="B91" s="1">
         <v>86</v>
       </c>
@@ -11271,7 +11293,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="92" spans="2:24" ht="12.75">
+    <row r="92" spans="2:24" ht="13.2">
       <c r="B92" s="1">
         <v>87</v>
       </c>
@@ -11301,7 +11323,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="2:24" ht="12.75">
+    <row r="93" spans="2:24" ht="13.2">
       <c r="B93" s="1">
         <v>88</v>
       </c>
@@ -11331,7 +11353,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="94" spans="2:24" ht="12.75">
+    <row r="94" spans="2:24" ht="13.2">
       <c r="B94" s="1">
         <v>89</v>
       </c>
@@ -11364,7 +11386,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="2:24" ht="12.75">
+    <row r="95" spans="2:24" ht="13.2">
       <c r="B95" s="1">
         <v>90</v>
       </c>
@@ -11394,7 +11416,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="2:24" ht="12.75">
+    <row r="96" spans="2:24" ht="13.2">
       <c r="B96" s="106">
         <v>91</v>
       </c>
@@ -11425,7 +11447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="2:24" ht="12.75">
+    <row r="97" spans="2:24" ht="13.2">
       <c r="B97" s="1">
         <v>92</v>
       </c>
@@ -11455,7 +11477,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="98" spans="2:24" ht="12.75">
+    <row r="98" spans="2:24" ht="13.2">
       <c r="B98" s="1">
         <v>93</v>
       </c>
@@ -11485,7 +11507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="2:24" ht="12.75">
+    <row r="99" spans="2:24" ht="13.2">
       <c r="B99" s="1">
         <v>94</v>
       </c>
@@ -11515,7 +11537,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="2:24" ht="12.75">
+    <row r="100" spans="2:24" ht="13.2">
       <c r="B100" s="1">
         <v>95</v>
       </c>
@@ -11545,7 +11567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="2:24" ht="12.75">
+    <row r="101" spans="2:24" ht="13.2">
       <c r="B101" s="1">
         <v>96</v>
       </c>
@@ -11575,7 +11597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="2:24" ht="12.75">
+    <row r="102" spans="2:24" ht="13.2">
       <c r="B102" s="1">
         <v>97</v>
       </c>
@@ -11605,7 +11627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="2:24" ht="12.75">
+    <row r="103" spans="2:24" ht="13.2">
       <c r="B103" s="1">
         <v>98</v>
       </c>
@@ -11620,7 +11642,7 @@
       </c>
       <c r="T103" s="45"/>
     </row>
-    <row r="104" spans="2:24" ht="12.75">
+    <row r="104" spans="2:24" ht="13.2">
       <c r="B104" s="1">
         <v>99</v>
       </c>
@@ -11634,7 +11656,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="105" spans="2:24" ht="12.75">
+    <row r="105" spans="2:24" ht="13.2">
       <c r="B105" s="1">
         <v>100</v>
       </c>
@@ -11648,7 +11670,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="106" spans="2:24" ht="12.75">
+    <row r="106" spans="2:24" ht="13.2">
       <c r="B106" s="1">
         <v>101</v>
       </c>
@@ -11662,7 +11684,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="107" spans="2:24" ht="12.75">
+    <row r="107" spans="2:24" ht="13.2">
       <c r="B107" s="1">
         <v>102</v>
       </c>
@@ -11676,7 +11698,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="108" spans="2:24" ht="12.75">
+    <row r="108" spans="2:24" ht="13.2">
       <c r="B108" s="1">
         <v>103</v>
       </c>
@@ -11693,7 +11715,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="109" spans="2:24" ht="12.75">
+    <row r="109" spans="2:24" ht="13.2">
       <c r="B109" s="1">
         <v>104</v>
       </c>
@@ -11722,7 +11744,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="110" spans="2:24" ht="12.75">
+    <row r="110" spans="2:24" ht="13.2">
       <c r="B110" s="1">
         <v>105</v>
       </c>
@@ -11736,7 +11758,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="111" spans="2:24" ht="12.75">
+    <row r="111" spans="2:24" ht="13.2">
       <c r="B111" s="1">
         <v>106</v>
       </c>
@@ -11750,7 +11772,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="112" spans="2:24" ht="12.75">
+    <row r="112" spans="2:24" ht="13.2">
       <c r="B112" s="1">
         <v>107</v>
       </c>
@@ -11771,7 +11793,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="113" spans="2:24" ht="12.75">
+    <row r="113" spans="2:24" ht="13.2">
       <c r="B113" s="1">
         <v>108</v>
       </c>
@@ -11817,7 +11839,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="114" spans="2:24" ht="12.75">
+    <row r="114" spans="2:24" ht="13.2">
       <c r="B114" s="106">
         <v>109</v>
       </c>
@@ -11860,7 +11882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="2:24" ht="12.75">
+    <row r="115" spans="2:24" ht="13.2">
       <c r="B115" s="1">
         <v>110</v>
       </c>
@@ -11902,7 +11924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="2:24" ht="12.75">
+    <row r="116" spans="2:24" ht="13.2">
       <c r="B116" s="1">
         <v>111</v>
       </c>
@@ -11944,7 +11966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="2:24" ht="12.75">
+    <row r="117" spans="2:24" ht="13.2">
       <c r="B117" s="1">
         <v>112</v>
       </c>
@@ -11977,7 +11999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:24" ht="12.75">
+    <row r="118" spans="2:24" ht="13.2">
       <c r="B118" s="1">
         <v>113</v>
       </c>
@@ -12009,7 +12031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:24" ht="12.75">
+    <row r="119" spans="2:24" ht="13.2">
       <c r="B119" s="1">
         <v>114</v>
       </c>
@@ -12043,7 +12065,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="120" spans="2:24" ht="12.75">
+    <row r="120" spans="2:24" ht="13.2">
       <c r="B120" s="1">
         <v>115</v>
       </c>
@@ -12068,7 +12090,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="121" spans="2:24" ht="12.75">
+    <row r="121" spans="2:24" ht="13.2">
       <c r="B121" s="1">
         <v>116</v>
       </c>
@@ -12093,7 +12115,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="122" spans="2:24" ht="12.75">
+    <row r="122" spans="2:24" ht="13.2">
       <c r="B122" s="1">
         <v>117</v>
       </c>
@@ -12118,7 +12140,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="123" spans="2:24" ht="12.75">
+    <row r="123" spans="2:24" ht="13.2">
       <c r="B123" s="1">
         <v>118</v>
       </c>
@@ -12143,7 +12165,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="124" spans="2:24" ht="12.75">
+    <row r="124" spans="2:24" ht="13.2">
       <c r="B124" s="1">
         <v>119</v>
       </c>
@@ -12168,7 +12190,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="125" spans="2:24" ht="12.75">
+    <row r="125" spans="2:24" ht="13.2">
       <c r="B125" s="1">
         <v>120</v>
       </c>
@@ -12193,7 +12215,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="126" spans="2:24" ht="12.75">
+    <row r="126" spans="2:24" ht="13.2">
       <c r="B126" s="1">
         <v>121</v>
       </c>
@@ -12218,7 +12240,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="127" spans="2:24" ht="12.75">
+    <row r="127" spans="2:24" ht="13.2">
       <c r="B127" s="1">
         <v>122</v>
       </c>
@@ -12243,7 +12265,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="128" spans="2:24" ht="12.75">
+    <row r="128" spans="2:24" ht="13.2">
       <c r="B128" s="1">
         <v>123</v>
       </c>
@@ -12268,7 +12290,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="129" spans="2:15" ht="12.75">
+    <row r="129" spans="2:15" ht="13.2">
       <c r="B129" s="1">
         <v>124</v>
       </c>
@@ -12296,7 +12318,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="130" spans="2:15" ht="12.75">
+    <row r="130" spans="2:15" ht="13.2">
       <c r="B130" s="1">
         <v>125</v>
       </c>
@@ -12321,7 +12343,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="131" spans="2:15" ht="12.75">
+    <row r="131" spans="2:15" ht="13.2">
       <c r="B131" s="1">
         <v>126</v>
       </c>
@@ -12346,7 +12368,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="132" spans="2:15" ht="12.75">
+    <row r="132" spans="2:15" ht="13.2">
       <c r="B132" s="106">
         <v>127</v>
       </c>
@@ -12375,7 +12397,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="133" spans="2:15" ht="12.75">
+    <row r="133" spans="2:15" ht="13.2">
       <c r="B133" s="1">
         <v>128</v>
       </c>
@@ -12403,7 +12425,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="134" spans="2:15" ht="12.75">
+    <row r="134" spans="2:15" ht="13.2">
       <c r="B134" s="1">
         <v>129</v>
       </c>
@@ -12431,7 +12453,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="135" spans="2:15" ht="12.75">
+    <row r="135" spans="2:15" ht="13.2">
       <c r="B135" s="1">
         <v>130</v>
       </c>
@@ -12456,7 +12478,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="136" spans="2:15" ht="12.75">
+    <row r="136" spans="2:15" ht="13.2">
       <c r="B136" s="1">
         <v>131</v>
       </c>
@@ -12484,7 +12506,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="137" spans="2:15" ht="12.75">
+    <row r="137" spans="2:15" ht="13.2">
       <c r="B137" s="1">
         <v>132</v>
       </c>
@@ -12509,7 +12531,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="138" spans="2:15" ht="12.75">
+    <row r="138" spans="2:15" ht="13.2">
       <c r="B138" s="1">
         <v>133</v>
       </c>
@@ -12534,7 +12556,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="139" spans="2:15" ht="12.75">
+    <row r="139" spans="2:15" ht="13.2">
       <c r="B139" s="1">
         <v>134</v>
       </c>
@@ -12559,7 +12581,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="140" spans="2:15" ht="12.75">
+    <row r="140" spans="2:15" ht="13.2">
       <c r="B140" s="1">
         <v>135</v>
       </c>
@@ -12584,7 +12606,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="141" spans="2:15" ht="12.75">
+    <row r="141" spans="2:15" ht="13.2">
       <c r="B141" s="1">
         <v>136</v>
       </c>
@@ -12609,7 +12631,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="142" spans="2:15" ht="12.75">
+    <row r="142" spans="2:15" ht="13.2">
       <c r="B142" s="1">
         <v>137</v>
       </c>
@@ -12634,7 +12656,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="143" spans="2:15" ht="12.75">
+    <row r="143" spans="2:15" ht="13.2">
       <c r="B143" s="1">
         <v>138</v>
       </c>
@@ -12659,7 +12681,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="144" spans="2:15" ht="12.75">
+    <row r="144" spans="2:15" ht="13.2">
       <c r="B144" s="1">
         <v>139</v>
       </c>
@@ -12684,7 +12706,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="145" spans="2:15" ht="12.75">
+    <row r="145" spans="2:15" ht="13.2">
       <c r="B145" s="1">
         <v>140</v>
       </c>
@@ -12709,7 +12731,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="146" spans="2:15" ht="12.75">
+    <row r="146" spans="2:15" ht="13.2">
       <c r="B146" s="1">
         <v>141</v>
       </c>
@@ -12734,7 +12756,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="147" spans="2:15" ht="12.75">
+    <row r="147" spans="2:15" ht="13.2">
       <c r="B147" s="1">
         <v>142</v>
       </c>
@@ -12759,7 +12781,7 @@
         <v>1493</v>
       </c>
     </row>
-    <row r="148" spans="2:15" ht="12.75">
+    <row r="148" spans="2:15" ht="13.2">
       <c r="B148" s="1">
         <v>143</v>
       </c>
@@ -12784,7 +12806,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="149" spans="2:15" ht="12.75">
+    <row r="149" spans="2:15" ht="13.2">
       <c r="B149" s="1">
         <v>144</v>
       </c>
@@ -12812,7 +12834,7 @@
         <v>1723</v>
       </c>
     </row>
-    <row r="150" spans="2:15" ht="12.75">
+    <row r="150" spans="2:15" ht="13.2">
       <c r="B150" s="106">
         <v>145</v>
       </c>
@@ -12838,7 +12860,7 @@
         <v>1851</v>
       </c>
     </row>
-    <row r="151" spans="2:15" ht="12.75">
+    <row r="151" spans="2:15" ht="13.2">
       <c r="B151" s="1">
         <v>146</v>
       </c>
@@ -12863,7 +12885,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="152" spans="2:15" ht="12.75">
+    <row r="152" spans="2:15" ht="13.2">
       <c r="B152" s="1">
         <v>147</v>
       </c>
@@ -12888,7 +12910,7 @@
         <v>2139</v>
       </c>
     </row>
-    <row r="153" spans="2:15" ht="12.75">
+    <row r="153" spans="2:15" ht="13.2">
       <c r="B153" s="1">
         <v>148</v>
       </c>
@@ -12916,7 +12938,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="154" spans="2:15" ht="12.75">
+    <row r="154" spans="2:15" ht="13.2">
       <c r="B154" s="1">
         <v>149</v>
       </c>
@@ -12941,7 +12963,7 @@
         <v>2477</v>
       </c>
     </row>
-    <row r="155" spans="2:15" ht="12.75">
+    <row r="155" spans="2:15" ht="13.2">
       <c r="B155" s="1">
         <v>150</v>
       </c>
@@ -12969,7 +12991,7 @@
         <v>2668</v>
       </c>
     </row>
-    <row r="156" spans="2:15" ht="12.75">
+    <row r="156" spans="2:15" ht="13.2">
       <c r="B156" s="1">
         <v>151</v>
       </c>
@@ -12994,7 +13016,7 @@
         <v>2878</v>
       </c>
     </row>
-    <row r="157" spans="2:15" ht="12.75">
+    <row r="157" spans="2:15" ht="13.2">
       <c r="B157" s="1">
         <v>152</v>
       </c>
@@ -13019,7 +13041,7 @@
         <v>3109</v>
       </c>
     </row>
-    <row r="158" spans="2:15" ht="12.75">
+    <row r="158" spans="2:15" ht="13.2">
       <c r="B158" s="1">
         <v>153</v>
       </c>
@@ -13044,7 +13066,7 @@
         <v>3362</v>
       </c>
     </row>
-    <row r="159" spans="2:15" ht="12.75">
+    <row r="159" spans="2:15" ht="13.2">
       <c r="B159" s="1">
         <v>154</v>
       </c>
@@ -13069,7 +13091,7 @@
         <v>3642</v>
       </c>
     </row>
-    <row r="160" spans="2:15" ht="12.75">
+    <row r="160" spans="2:15" ht="13.2">
       <c r="B160" s="1">
         <v>155</v>
       </c>
@@ -13094,7 +13116,7 @@
         <v>3952</v>
       </c>
     </row>
-    <row r="161" spans="2:15" ht="12.75">
+    <row r="161" spans="2:15" ht="13.2">
       <c r="B161" s="1">
         <v>156</v>
       </c>
@@ -13119,7 +13141,7 @@
         <v>4296</v>
       </c>
     </row>
-    <row r="162" spans="2:15" ht="12.75">
+    <row r="162" spans="2:15" ht="13.2">
       <c r="B162" s="1">
         <v>157</v>
       </c>
@@ -13144,7 +13166,7 @@
         <v>4680</v>
       </c>
     </row>
-    <row r="163" spans="2:15" ht="12.75">
+    <row r="163" spans="2:15" ht="13.2">
       <c r="B163" s="1">
         <v>158</v>
       </c>
@@ -13169,7 +13191,7 @@
         <v>5108</v>
       </c>
     </row>
-    <row r="164" spans="2:15" ht="12.75">
+    <row r="164" spans="2:15" ht="13.2">
       <c r="B164" s="1">
         <v>159</v>
       </c>
@@ -13194,7 +13216,7 @@
         <v>5587</v>
       </c>
     </row>
-    <row r="165" spans="2:15" ht="12.75">
+    <row r="165" spans="2:15" ht="13.2">
       <c r="B165" s="1">
         <v>160</v>
       </c>
@@ -13219,7 +13241,7 @@
         <v>6124</v>
       </c>
     </row>
-    <row r="166" spans="2:15" ht="12.75">
+    <row r="166" spans="2:15" ht="13.2">
       <c r="B166" s="1">
         <v>161</v>
       </c>
@@ -13244,7 +13266,7 @@
         <v>6728</v>
       </c>
     </row>
-    <row r="167" spans="2:15" ht="12.75">
+    <row r="167" spans="2:15" ht="13.2">
       <c r="B167" s="1">
         <v>162</v>
       </c>
@@ -13269,7 +13291,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="168" spans="2:15" ht="12.75">
+    <row r="168" spans="2:15" ht="13.2">
       <c r="B168" s="106">
         <v>163</v>
       </c>
@@ -13295,7 +13317,7 @@
         <v>8178</v>
       </c>
     </row>
-    <row r="169" spans="2:15" ht="12.75">
+    <row r="169" spans="2:15" ht="13.2">
       <c r="B169" s="1">
         <v>164</v>
       </c>
@@ -13320,7 +13342,7 @@
         <v>9047</v>
       </c>
     </row>
-    <row r="170" spans="2:15" ht="12.75">
+    <row r="170" spans="2:15" ht="13.2">
       <c r="B170" s="1">
         <v>165</v>
       </c>
@@ -13345,7 +13367,7 @@
         <v>10032</v>
       </c>
     </row>
-    <row r="171" spans="2:15" ht="12.75">
+    <row r="171" spans="2:15" ht="13.2">
       <c r="B171" s="1">
         <v>166</v>
       </c>
@@ -13370,7 +13392,7 @@
         <v>11149</v>
       </c>
     </row>
-    <row r="172" spans="2:15" ht="12.75">
+    <row r="172" spans="2:15" ht="13.2">
       <c r="B172" s="1">
         <v>167</v>
       </c>
@@ -13395,7 +13417,7 @@
         <v>12418</v>
       </c>
     </row>
-    <row r="173" spans="2:15" ht="12.75">
+    <row r="173" spans="2:15" ht="13.2">
       <c r="B173" s="1">
         <v>168</v>
       </c>
@@ -16005,32 +16027,32 @@
     <row r="278" spans="2:8" ht="15.75" customHeight="1">
       <c r="B278" s="106"/>
       <c r="C278" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="D278" s="108"/>
       <c r="E278" s="106">
         <v>1</v>
       </c>
       <c r="F278" s="105" t="s">
-        <v>919</v>
+        <v>908</v>
       </c>
     </row>
     <row r="279" spans="2:8" ht="15.75" customHeight="1">
       <c r="B279" s="1"/>
       <c r="C279" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E279" s="67">
         <v>2</v>
       </c>
       <c r="F279" s="65" t="s">
-        <v>947</v>
+        <v>932</v>
       </c>
     </row>
     <row r="280" spans="2:8" ht="15.75" customHeight="1">
       <c r="B280" s="1"/>
       <c r="C280" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="D280">
         <v>1.1499999999999999</v>
@@ -16039,61 +16061,61 @@
         <v>3</v>
       </c>
       <c r="F280" s="75" t="s">
-        <v>920</v>
+        <v>909</v>
       </c>
     </row>
     <row r="281" spans="2:8" ht="15.75" customHeight="1">
       <c r="B281" s="1"/>
       <c r="C281" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E281" s="67">
         <v>4</v>
       </c>
       <c r="F281" s="74" t="s">
-        <v>948</v>
+        <v>933</v>
       </c>
     </row>
     <row r="282" spans="2:8" ht="15.75" customHeight="1">
       <c r="B282" s="1"/>
       <c r="C282" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E282" s="67">
         <v>5</v>
       </c>
       <c r="F282" s="102" t="s">
-        <v>949</v>
+        <v>934</v>
       </c>
     </row>
     <row r="283" spans="2:8" ht="15.75" customHeight="1">
       <c r="B283" s="1"/>
       <c r="C283" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E283" s="67">
         <v>6</v>
       </c>
       <c r="F283" s="101" t="s">
-        <v>952</v>
+        <v>937</v>
       </c>
     </row>
     <row r="284" spans="2:8" ht="15.75" customHeight="1">
       <c r="B284" s="1"/>
       <c r="C284" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E284" s="67">
         <v>7</v>
       </c>
       <c r="F284" s="100" t="s">
-        <v>923</v>
+        <v>912</v>
       </c>
     </row>
     <row r="285" spans="2:8" ht="15.75" customHeight="1">
       <c r="B285" s="1"/>
       <c r="C285" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E285" s="67">
         <v>8</v>
@@ -16105,7 +16127,7 @@
     <row r="286" spans="2:8" ht="15.75" customHeight="1">
       <c r="B286" s="1"/>
       <c r="C286" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E286" s="67">
         <v>9</v>
@@ -16117,31 +16139,31 @@
     <row r="287" spans="2:8" ht="15.75" customHeight="1">
       <c r="B287" s="1"/>
       <c r="C287" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E287" s="67">
         <v>10</v>
       </c>
       <c r="F287" s="103" t="s">
-        <v>929</v>
+        <v>918</v>
       </c>
     </row>
     <row r="288" spans="2:8" ht="15.75" customHeight="1">
       <c r="B288" s="1"/>
       <c r="C288" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E288" s="67">
         <v>11</v>
       </c>
       <c r="F288" s="105" t="s">
-        <v>951</v>
+        <v>936</v>
       </c>
     </row>
     <row r="289" spans="2:6" ht="15.75" customHeight="1">
       <c r="B289" s="1"/>
       <c r="C289" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E289" s="67">
         <v>12</v>
@@ -16153,31 +16175,31 @@
     <row r="290" spans="2:6" ht="15.75" customHeight="1">
       <c r="B290" s="1"/>
       <c r="C290" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E290" s="67">
         <v>13</v>
       </c>
       <c r="F290" s="97" t="s">
-        <v>950</v>
+        <v>935</v>
       </c>
     </row>
     <row r="291" spans="2:6" ht="15.75" customHeight="1">
       <c r="B291" s="1"/>
       <c r="C291" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E291" s="67">
         <v>14</v>
       </c>
       <c r="F291" s="75" t="s">
-        <v>930</v>
+        <v>919</v>
       </c>
     </row>
     <row r="292" spans="2:6" ht="15.75" customHeight="1">
       <c r="B292" s="1"/>
       <c r="C292" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="D292">
         <v>1.26</v>
@@ -16186,43 +16208,43 @@
         <v>15</v>
       </c>
       <c r="F292" s="105" t="s">
-        <v>926</v>
+        <v>915</v>
       </c>
     </row>
     <row r="293" spans="2:6" ht="15.75" customHeight="1">
       <c r="B293" s="1"/>
       <c r="C293" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E293" s="67">
         <v>16</v>
       </c>
       <c r="F293" s="99" t="s">
-        <v>925</v>
+        <v>914</v>
       </c>
     </row>
     <row r="294" spans="2:6" ht="15.75" customHeight="1">
       <c r="B294" s="1"/>
       <c r="C294" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E294" s="67">
         <v>17</v>
       </c>
       <c r="F294" s="97" t="s">
-        <v>924</v>
+        <v>913</v>
       </c>
     </row>
     <row r="295" spans="2:6" ht="15.75" customHeight="1">
       <c r="B295" s="1"/>
       <c r="C295" s="107" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
       <c r="E295" s="67">
         <v>18</v>
       </c>
       <c r="F295" s="103" t="s">
-        <v>921</v>
+        <v>910</v>
       </c>
     </row>
   </sheetData>
@@ -16245,23 +16267,23 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="6" max="6" width="38.85546875" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
+    <col min="6" max="6" width="38.88671875" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:12" ht="12.75">
+    <row r="2" spans="3:12" ht="13.2">
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="3:12" ht="15.75" customHeight="1">
       <c r="L3" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="4" spans="3:12" ht="12.75">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" ht="13.2">
       <c r="C4" s="1" t="s">
         <v>52</v>
       </c>
@@ -16287,10 +16309,10 @@
         <v>136</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="5" spans="3:12" ht="12.75">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" ht="13.2">
       <c r="C5" s="1">
         <v>1</v>
       </c>
@@ -16310,10 +16332,10 @@
         <v>208</v>
       </c>
       <c r="L5" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="6" spans="3:12" ht="12.75">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" ht="13.2">
       <c r="C6" s="1">
         <v>2</v>
       </c>
@@ -16327,10 +16349,10 @@
         <v>407</v>
       </c>
       <c r="L6" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12" ht="12.75">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" ht="13.2">
       <c r="C7" s="1">
         <v>3</v>
       </c>
@@ -16344,7 +16366,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="8" spans="3:12" ht="12.75">
+    <row r="8" spans="3:12" ht="13.2">
       <c r="C8" s="1">
         <v>4</v>
       </c>
@@ -16358,7 +16380,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="9" spans="3:12" ht="12.75">
+    <row r="9" spans="3:12" ht="13.2">
       <c r="C9" s="1">
         <v>5</v>
       </c>
@@ -16372,7 +16394,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="10" spans="3:12" ht="12.75">
+    <row r="10" spans="3:12" ht="13.2">
       <c r="C10" s="1">
         <v>6</v>
       </c>
@@ -16386,10 +16408,10 @@
         <v>116</v>
       </c>
       <c r="G10" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="11" spans="3:12" ht="12.75">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" ht="13.2">
       <c r="C11" s="1">
         <v>7</v>
       </c>
@@ -16400,13 +16422,13 @@
         <v>6</v>
       </c>
       <c r="F11" s="46" t="s">
-        <v>901</v>
+        <v>896</v>
       </c>
       <c r="G11" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="12" spans="3:12" ht="12.75">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" ht="13.2">
       <c r="C12" s="1">
         <v>8</v>
       </c>
@@ -16420,7 +16442,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="13" spans="3:12" ht="12.75">
+    <row r="13" spans="3:12" ht="13.2">
       <c r="C13" s="1">
         <v>9</v>
       </c>
@@ -16434,7 +16456,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="14" spans="3:12" ht="12.75">
+    <row r="14" spans="3:12" ht="13.2">
       <c r="C14" s="1">
         <v>10</v>
       </c>
@@ -16448,7 +16470,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="15" spans="3:12" ht="12.75">
+    <row r="15" spans="3:12" ht="13.2">
       <c r="C15" s="1">
         <v>11</v>
       </c>
@@ -16462,7 +16484,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="16" spans="3:12" ht="12.75">
+    <row r="16" spans="3:12" ht="13.2">
       <c r="C16" s="1">
         <v>12</v>
       </c>
@@ -16476,7 +16498,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="17" spans="3:9" ht="12.75">
+    <row r="17" spans="3:9" ht="13.2">
       <c r="C17" s="1">
         <v>13</v>
       </c>
@@ -16490,7 +16512,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="18" spans="3:9" ht="12.75">
+    <row r="18" spans="3:9" ht="13.2">
       <c r="C18" s="1">
         <v>14</v>
       </c>
@@ -16504,7 +16526,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="19" spans="3:9" ht="12.75">
+    <row r="19" spans="3:9" ht="13.2">
       <c r="C19" s="1">
         <v>15</v>
       </c>
@@ -16518,7 +16540,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="20" spans="3:9" ht="12.75">
+    <row r="20" spans="3:9" ht="13.2">
       <c r="C20" s="1">
         <v>16</v>
       </c>
@@ -16532,7 +16554,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="21" spans="3:9" ht="12.75">
+    <row r="21" spans="3:9" ht="13.2">
       <c r="C21" s="1">
         <v>17</v>
       </c>
@@ -16546,7 +16568,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="22" spans="3:9" ht="12.75">
+    <row r="22" spans="3:9" ht="13.2">
       <c r="C22" s="1">
         <v>18</v>
       </c>
@@ -16560,7 +16582,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="23" spans="3:9" ht="12.75">
+    <row r="23" spans="3:9" ht="13.2">
       <c r="C23" s="1">
         <v>19</v>
       </c>
@@ -16574,7 +16596,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="24" spans="3:9" ht="12.75">
+    <row r="24" spans="3:9" ht="13.2">
       <c r="C24" s="1">
         <v>20</v>
       </c>
@@ -16588,7 +16610,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="25" spans="3:9" ht="12.75">
+    <row r="25" spans="3:9" ht="13.2">
       <c r="C25" s="1">
         <v>21</v>
       </c>
@@ -16602,7 +16624,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="26" spans="3:9" ht="12.75">
+    <row r="26" spans="3:9" ht="13.2">
       <c r="C26" s="1">
         <v>22</v>
       </c>
@@ -16616,7 +16638,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="27" spans="3:9" ht="12.75">
+    <row r="27" spans="3:9" ht="13.2">
       <c r="C27" s="1">
         <v>23</v>
       </c>
@@ -16630,7 +16652,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="3:9" ht="12.75">
+    <row r="28" spans="3:9" ht="13.2">
       <c r="C28" s="1">
         <v>24</v>
       </c>
@@ -16644,7 +16666,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="29" spans="3:9" ht="12.75">
+    <row r="29" spans="3:9" ht="13.2">
       <c r="C29" s="1">
         <v>25</v>
       </c>
@@ -16658,7 +16680,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="30" spans="3:9" ht="12.75">
+    <row r="30" spans="3:9" ht="13.2">
       <c r="C30" s="1">
         <v>26</v>
       </c>
@@ -16672,7 +16694,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="31" spans="3:9" ht="12.75">
+    <row r="31" spans="3:9" ht="13.2">
       <c r="C31" s="1">
         <v>27</v>
       </c>
@@ -16686,7 +16708,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="3:9" ht="12.75">
+    <row r="32" spans="3:9" ht="13.2">
       <c r="C32" s="1">
         <v>28</v>
       </c>
@@ -16701,7 +16723,7 @@
       </c>
       <c r="I32" s="26"/>
     </row>
-    <row r="33" spans="3:9" ht="12.75">
+    <row r="33" spans="3:9" ht="13.2">
       <c r="C33" s="1">
         <v>29</v>
       </c>
@@ -16716,7 +16738,7 @@
       </c>
       <c r="I33" s="27"/>
     </row>
-    <row r="34" spans="3:9" ht="12.75">
+    <row r="34" spans="3:9" ht="13.2">
       <c r="C34" s="1">
         <v>30</v>
       </c>
@@ -16731,7 +16753,7 @@
       </c>
       <c r="I34" s="27"/>
     </row>
-    <row r="35" spans="3:9" ht="12.75">
+    <row r="35" spans="3:9" ht="13.2">
       <c r="C35" s="1">
         <v>31</v>
       </c>
@@ -16746,7 +16768,7 @@
       </c>
       <c r="I35" s="27"/>
     </row>
-    <row r="36" spans="3:9" ht="12.75">
+    <row r="36" spans="3:9" ht="13.2">
       <c r="C36" s="1">
         <v>32</v>
       </c>
@@ -16763,7 +16785,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="3:9" ht="12.75">
+    <row r="37" spans="3:9" ht="13.2">
       <c r="C37" s="1">
         <v>33</v>
       </c>
@@ -16780,7 +16802,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="3:9" ht="12.75">
+    <row r="38" spans="3:9" ht="13.2">
       <c r="C38" s="1">
         <v>34</v>
       </c>
@@ -16797,7 +16819,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="3:9" ht="12.75">
+    <row r="39" spans="3:9" ht="13.2">
       <c r="C39" s="1">
         <v>35</v>
       </c>
@@ -16814,7 +16836,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="40" spans="3:9" ht="12.75">
+    <row r="40" spans="3:9" ht="13.2">
       <c r="C40" s="1">
         <v>36</v>
       </c>
@@ -16831,7 +16853,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="41" spans="3:9" ht="12.75">
+    <row r="41" spans="3:9" ht="13.2">
       <c r="C41" s="1">
         <v>37</v>
       </c>
@@ -16848,7 +16870,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="42" spans="3:9" ht="12.75">
+    <row r="42" spans="3:9" ht="13.2">
       <c r="C42" s="1">
         <v>38</v>
       </c>
@@ -16865,7 +16887,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="43" spans="3:9" ht="12.75">
+    <row r="43" spans="3:9" ht="13.2">
       <c r="C43" s="1">
         <v>39</v>
       </c>
@@ -16882,7 +16904,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="44" spans="3:9" ht="12.75">
+    <row r="44" spans="3:9" ht="13.2">
       <c r="C44" s="1">
         <v>40</v>
       </c>
@@ -16899,7 +16921,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="45" spans="3:9" ht="12.75">
+    <row r="45" spans="3:9" ht="13.2">
       <c r="C45" s="1">
         <v>41</v>
       </c>
@@ -16916,7 +16938,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="46" spans="3:9" ht="12.75">
+    <row r="46" spans="3:9" ht="13.2">
       <c r="C46" s="1">
         <v>42</v>
       </c>
@@ -16933,7 +16955,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="47" spans="3:9" ht="12.75">
+    <row r="47" spans="3:9" ht="13.2">
       <c r="C47" s="1">
         <v>43</v>
       </c>
@@ -16950,7 +16972,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="48" spans="3:9" ht="12.75">
+    <row r="48" spans="3:9" ht="13.2">
       <c r="C48" s="1">
         <v>44</v>
       </c>
@@ -16967,7 +16989,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="49" spans="3:9" ht="12.75">
+    <row r="49" spans="3:9" ht="13.2">
       <c r="C49" s="1">
         <v>45</v>
       </c>
@@ -16984,7 +17006,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="50" spans="3:9" ht="12.75">
+    <row r="50" spans="3:9" ht="13.2">
       <c r="C50" s="1">
         <v>46</v>
       </c>
@@ -17001,7 +17023,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="51" spans="3:9" ht="12.75">
+    <row r="51" spans="3:9" ht="13.2">
       <c r="C51" s="1">
         <v>47</v>
       </c>
@@ -17018,7 +17040,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="52" spans="3:9" ht="12.75">
+    <row r="52" spans="3:9" ht="13.2">
       <c r="C52" s="1">
         <v>48</v>
       </c>
@@ -17035,7 +17057,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="53" spans="3:9" ht="12.75">
+    <row r="53" spans="3:9" ht="13.2">
       <c r="C53" s="1">
         <v>49</v>
       </c>
@@ -17052,7 +17074,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="54" spans="3:9" ht="12.75">
+    <row r="54" spans="3:9" ht="13.2">
       <c r="C54" s="1">
         <v>50</v>
       </c>
@@ -17066,7 +17088,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="55" spans="3:9" ht="12.75">
+    <row r="55" spans="3:9" ht="13.2">
       <c r="C55" s="1">
         <v>51</v>
       </c>
@@ -17080,7 +17102,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="56" spans="3:9" ht="12.75">
+    <row r="56" spans="3:9" ht="13.2">
       <c r="C56" s="1">
         <v>52</v>
       </c>
@@ -17094,7 +17116,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="57" spans="3:9" ht="12.75">
+    <row r="57" spans="3:9" ht="13.2">
       <c r="C57" s="1">
         <v>53</v>
       </c>
@@ -17108,7 +17130,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="58" spans="3:9" ht="12.75">
+    <row r="58" spans="3:9" ht="13.2">
       <c r="C58" s="1">
         <v>54</v>
       </c>
@@ -17122,7 +17144,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="3:9" ht="12.75">
+    <row r="59" spans="3:9" ht="13.2">
       <c r="C59" s="1">
         <v>55</v>
       </c>
@@ -17136,7 +17158,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="60" spans="3:9" ht="12.75">
+    <row r="60" spans="3:9" ht="13.2">
       <c r="C60" s="1">
         <v>56</v>
       </c>
@@ -17150,7 +17172,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="3:9" ht="12.75">
+    <row r="61" spans="3:9" ht="13.2">
       <c r="C61" s="1">
         <v>57</v>
       </c>
@@ -17164,7 +17186,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="62" spans="3:9" ht="12.75">
+    <row r="62" spans="3:9" ht="13.2">
       <c r="C62" s="1">
         <v>58</v>
       </c>
@@ -17175,7 +17197,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="63" spans="3:9" ht="12.75">
+    <row r="63" spans="3:9" ht="13.2">
       <c r="C63" s="1">
         <v>59</v>
       </c>
@@ -17186,7 +17208,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="64" spans="3:9" ht="12.75">
+    <row r="64" spans="3:9" ht="13.2">
       <c r="C64" s="1">
         <v>60</v>
       </c>
@@ -17197,7 +17219,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="65" spans="3:6" ht="12.75">
+    <row r="65" spans="3:6" ht="13.2">
       <c r="C65" s="1">
         <v>61</v>
       </c>
@@ -17339,10 +17361,10 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:9">
@@ -17793,18 +17815,18 @@
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" ht="12.75">
+    <row r="4" spans="3:7" ht="13.2">
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="12.75">
+    <row r="6" spans="3:7" ht="13.2">
       <c r="C6" s="1" t="s">
         <v>52</v>
       </c>
@@ -17821,7 +17843,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="12.75">
+    <row r="7" spans="3:7" ht="13.2">
       <c r="C7" s="1">
         <v>1</v>
       </c>
@@ -17832,7 +17854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="12.75">
+    <row r="8" spans="3:7" ht="13.2">
       <c r="C8" s="1">
         <v>2</v>
       </c>
@@ -17843,7 +17865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="12.75">
+    <row r="9" spans="3:7" ht="13.2">
       <c r="C9" s="1">
         <v>3</v>
       </c>
@@ -17854,7 +17876,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="3:7" ht="12.75">
+    <row r="10" spans="3:7" ht="13.2">
       <c r="C10" s="1">
         <v>4</v>
       </c>
@@ -17865,7 +17887,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="3:7" ht="12.75">
+    <row r="11" spans="3:7" ht="13.2">
       <c r="C11" s="1">
         <v>5</v>
       </c>
@@ -17876,7 +17898,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="3:7" ht="12.75">
+    <row r="12" spans="3:7" ht="13.2">
       <c r="C12" s="1">
         <v>6</v>
       </c>
@@ -17887,7 +17909,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="3:7" ht="12.75">
+    <row r="13" spans="3:7" ht="13.2">
       <c r="C13" s="1">
         <v>7</v>
       </c>
@@ -17898,7 +17920,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="3:7" ht="12.75">
+    <row r="14" spans="3:7" ht="13.2">
       <c r="C14" s="1">
         <v>8</v>
       </c>
@@ -17909,7 +17931,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="15" spans="3:7" ht="12.75">
+    <row r="15" spans="3:7" ht="13.2">
       <c r="C15" s="1">
         <v>9</v>
       </c>
@@ -17920,7 +17942,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="16" spans="3:7" ht="12.75">
+    <row r="16" spans="3:7" ht="13.2">
       <c r="C16" s="1">
         <v>10</v>
       </c>
@@ -17931,7 +17953,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="17" spans="3:7" ht="12.75">
+    <row r="17" spans="3:7" ht="13.2">
       <c r="C17" s="1">
         <v>11</v>
       </c>
@@ -17942,7 +17964,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="18" spans="3:7" ht="12.75">
+    <row r="18" spans="3:7" ht="13.2">
       <c r="C18" s="1">
         <v>12</v>
       </c>
@@ -17953,7 +17975,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="19" spans="3:7" ht="12.75">
+    <row r="19" spans="3:7" ht="13.2">
       <c r="C19" s="1">
         <v>13</v>
       </c>
@@ -17964,7 +17986,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="20" spans="3:7" ht="12.75">
+    <row r="20" spans="3:7" ht="13.2">
       <c r="C20" s="1">
         <v>14</v>
       </c>
@@ -17975,7 +17997,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="3:7" ht="12.75">
+    <row r="21" spans="3:7" ht="13.2">
       <c r="C21" s="1">
         <v>15</v>
       </c>
@@ -17986,7 +18008,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="3:7" ht="12.75">
+    <row r="22" spans="3:7" ht="13.2">
       <c r="C22" s="1">
         <v>16</v>
       </c>
@@ -17997,7 +18019,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="3:7" ht="12.75">
+    <row r="23" spans="3:7" ht="13.2">
       <c r="C23" s="1">
         <v>17</v>
       </c>
@@ -18008,7 +18030,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="3:7" ht="12.75">
+    <row r="24" spans="3:7" ht="13.2">
       <c r="C24" s="1">
         <v>18</v>
       </c>
@@ -18019,7 +18041,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="3:7" ht="12.75">
+    <row r="25" spans="3:7" ht="13.2">
       <c r="C25" s="1">
         <v>19</v>
       </c>
@@ -18030,7 +18052,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="3:7" ht="12.75">
+    <row r="26" spans="3:7" ht="13.2">
       <c r="C26" s="1">
         <v>20</v>
       </c>
@@ -18041,7 +18063,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="3:7" ht="12.75">
+    <row r="27" spans="3:7" ht="13.2">
       <c r="C27" s="1">
         <v>21</v>
       </c>
@@ -18052,7 +18074,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="28" spans="3:7" ht="12.75">
+    <row r="28" spans="3:7" ht="13.2">
       <c r="C28" s="1">
         <v>22</v>
       </c>
@@ -18063,7 +18085,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="3:7" ht="12.75">
+    <row r="29" spans="3:7" ht="13.2">
       <c r="C29" s="1">
         <v>23</v>
       </c>
@@ -18074,7 +18096,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="30" spans="3:7" ht="12.75">
+    <row r="30" spans="3:7" ht="13.2">
       <c r="C30" s="1">
         <v>24</v>
       </c>
@@ -18085,7 +18107,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="3:7" ht="12.75">
+    <row r="31" spans="3:7" ht="13.2">
       <c r="C31" s="1">
         <v>25</v>
       </c>
@@ -18096,7 +18118,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="3:7" ht="12.75">
+    <row r="32" spans="3:7" ht="13.2">
       <c r="C32" s="1">
         <v>26</v>
       </c>
@@ -18107,7 +18129,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="33" spans="3:7" ht="12.75">
+    <row r="33" spans="3:7" ht="13.2">
       <c r="C33" s="1">
         <v>27</v>
       </c>
@@ -18118,7 +18140,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="34" spans="3:7" ht="12.75">
+    <row r="34" spans="3:7" ht="13.2">
       <c r="C34" s="1">
         <v>28</v>
       </c>
@@ -18129,7 +18151,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="35" spans="3:7" ht="12.75">
+    <row r="35" spans="3:7" ht="13.2">
       <c r="C35" s="1">
         <v>29</v>
       </c>
@@ -18140,7 +18162,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="3:7" ht="12.75">
+    <row r="36" spans="3:7" ht="13.2">
       <c r="C36" s="1">
         <v>30</v>
       </c>
@@ -18153,7 +18175,7 @@
     </row>
     <row r="39" spans="3:7" ht="15.75" customHeight="1">
       <c r="D39" t="s">
-        <v>1059</v>
+        <v>1044</v>
       </c>
     </row>
   </sheetData>
@@ -18168,27 +18190,27 @@
   </sheetPr>
   <dimension ref="C3:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" customWidth="1"/>
-    <col min="2" max="2" width="3.5703125" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="8" max="8" width="39.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="8" max="8" width="39.44140625" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="14" max="14" width="16.5546875" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:20" ht="12.75">
+    <row r="3" spans="3:20" ht="13.2">
       <c r="C3" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="3:20" ht="12.75">
+    <row r="5" spans="3:20" ht="13.2">
       <c r="C5" s="1" t="s">
         <v>52</v>
       </c>
@@ -18196,7 +18218,7 @@
         <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>1036</v>
+        <v>1021</v>
       </c>
       <c r="F5" t="s">
         <v>77</v>
@@ -18205,7 +18227,7 @@
         <v>135</v>
       </c>
       <c r="H5" t="s">
-        <v>1039</v>
+        <v>1024</v>
       </c>
       <c r="I5" t="s">
         <v>77</v>
@@ -18214,7 +18236,7 @@
         <v>135</v>
       </c>
       <c r="K5" t="s">
-        <v>1038</v>
+        <v>1023</v>
       </c>
       <c r="L5" t="s">
         <v>77</v>
@@ -18223,7 +18245,7 @@
         <v>135</v>
       </c>
       <c r="N5" t="s">
-        <v>1037</v>
+        <v>1022</v>
       </c>
       <c r="O5" t="s">
         <v>77</v>
@@ -18244,7 +18266,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="6" spans="3:20" ht="12.75">
+    <row r="6" spans="3:20" ht="13.2">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -18252,16 +18274,16 @@
         <v>229</v>
       </c>
       <c r="E6" t="s">
-        <v>1044</v>
+        <v>1029</v>
       </c>
       <c r="H6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="K6" t="s">
         <v>1040</v>
       </c>
-      <c r="K6" t="s">
-        <v>1055</v>
-      </c>
       <c r="N6" t="s">
-        <v>1056</v>
+        <v>1041</v>
       </c>
       <c r="Q6" t="s">
         <v>428</v>
@@ -18270,7 +18292,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="7" spans="3:20" ht="12.75">
+    <row r="7" spans="3:20" ht="13.2">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -18278,19 +18300,19 @@
         <v>230</v>
       </c>
       <c r="E7" t="s">
-        <v>1060</v>
+        <v>1045</v>
       </c>
       <c r="H7" t="s">
-        <v>1045</v>
+        <v>1030</v>
       </c>
       <c r="K7" t="s">
-        <v>1047</v>
+        <v>1032</v>
       </c>
       <c r="N7" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="8" spans="3:20" ht="12.75">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="8" spans="3:20" ht="13.2">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -18298,19 +18320,19 @@
         <v>231</v>
       </c>
       <c r="E8" t="s">
-        <v>1043</v>
+        <v>1028</v>
       </c>
       <c r="H8" t="s">
-        <v>1053</v>
+        <v>1038</v>
       </c>
       <c r="K8" t="s">
-        <v>1041</v>
+        <v>1026</v>
       </c>
       <c r="N8" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="9" spans="3:20" ht="12.75">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="9" spans="3:20" ht="13.2">
       <c r="C9" s="1">
         <v>4</v>
       </c>
@@ -18318,16 +18340,16 @@
         <v>232</v>
       </c>
       <c r="E9" t="s">
-        <v>1049</v>
+        <v>1034</v>
       </c>
       <c r="H9" t="s">
-        <v>1054</v>
+        <v>1039</v>
       </c>
       <c r="K9" t="s">
-        <v>1046</v>
+        <v>1031</v>
       </c>
       <c r="N9" t="s">
-        <v>1052</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="10" spans="3:20" ht="15.75" customHeight="1">
@@ -18335,29 +18357,29 @@
         <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1046</v>
+      </c>
+      <c r="H10" t="s">
         <v>1035</v>
       </c>
-      <c r="E10" t="s">
-        <v>1061</v>
-      </c>
-      <c r="H10" t="s">
-        <v>1050</v>
-      </c>
       <c r="K10" t="s">
-        <v>1062</v>
+        <v>1047</v>
       </c>
       <c r="N10" t="s">
-        <v>1051</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="15" spans="3:20" ht="15.75" customHeight="1">
       <c r="D15" t="s">
-        <v>1057</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="16" spans="3:20" ht="15.75" customHeight="1">
       <c r="D16" t="s">
-        <v>1058</v>
+        <v>1043</v>
       </c>
     </row>
   </sheetData>
@@ -18376,11 +18398,11 @@
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="9" max="9" width="33.6640625" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="26" customWidth="1"/>
   </cols>
@@ -18471,13 +18493,13 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>953</v>
+        <v>938</v>
       </c>
       <c r="L6" s="1">
         <v>1</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>1026</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="7" spans="3:22">
@@ -18491,13 +18513,13 @@
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>954</v>
+        <v>939</v>
       </c>
       <c r="L7" s="1">
         <v>2</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>1025</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="8" spans="3:22">
@@ -18511,13 +18533,13 @@
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>971</v>
+        <v>956</v>
       </c>
       <c r="L8" s="1">
         <v>3</v>
       </c>
       <c r="M8" t="s">
-        <v>1033</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="9" spans="3:22">
@@ -18531,13 +18553,13 @@
         <v>4</v>
       </c>
       <c r="I9" t="s">
-        <v>955</v>
+        <v>940</v>
       </c>
       <c r="L9" s="1">
         <v>4</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>1034</v>
+        <v>1019</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>247</v>
@@ -18581,7 +18603,7 @@
         <v>5</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>1012</v>
+        <v>997</v>
       </c>
     </row>
     <row r="11" spans="3:22">
@@ -18601,7 +18623,7 @@
         <v>6</v>
       </c>
       <c r="M11" t="s">
-        <v>1031</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="12" spans="3:22">
@@ -18621,7 +18643,7 @@
         <v>7</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>1021</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="13" spans="3:22">
@@ -18644,7 +18666,7 @@
         <v>8</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>1022</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="14" spans="3:22">
@@ -18667,7 +18689,7 @@
         <v>9</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>1024</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="15" spans="3:22">
@@ -18687,7 +18709,7 @@
         <v>10</v>
       </c>
       <c r="M15" t="s">
-        <v>1032</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="16" spans="3:22">
@@ -18707,7 +18729,7 @@
         <v>11</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>1027</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="17" spans="3:16">
@@ -18727,7 +18749,7 @@
         <v>12</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>1028</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="18" spans="3:16">
@@ -18741,13 +18763,13 @@
         <v>13</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>956</v>
+        <v>941</v>
       </c>
       <c r="L18" s="1">
         <v>13</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>1029</v>
+        <v>1014</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>253</v>
@@ -18764,7 +18786,7 @@
         <v>14</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>957</v>
+        <v>942</v>
       </c>
       <c r="L19" s="1">
         <v>14</v>
@@ -18787,13 +18809,13 @@
         <v>15</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>958</v>
+        <v>943</v>
       </c>
       <c r="L20" s="1">
         <v>15</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>1020</v>
+        <v>1005</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>251</v>
@@ -18810,7 +18832,7 @@
         <v>16</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>959</v>
+        <v>944</v>
       </c>
       <c r="L21" s="1">
         <v>16</v>
@@ -18833,13 +18855,13 @@
         <v>17</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>960</v>
+        <v>945</v>
       </c>
       <c r="L22" s="1">
         <v>17</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>1023</v>
+        <v>1008</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>250</v>
@@ -18856,13 +18878,13 @@
         <v>18</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>961</v>
+        <v>946</v>
       </c>
       <c r="L23" s="1">
         <v>18</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>244</v>
@@ -18879,7 +18901,7 @@
         <v>19</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>962</v>
+        <v>947</v>
       </c>
       <c r="L24" s="1"/>
       <c r="P24" s="1" t="s">
@@ -18897,7 +18919,7 @@
         <v>20</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>963</v>
+        <v>948</v>
       </c>
       <c r="L25" s="1"/>
     </row>
@@ -18912,7 +18934,7 @@
         <v>21</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>964</v>
+        <v>949</v>
       </c>
     </row>
     <row r="27" spans="3:16">
@@ -18926,10 +18948,10 @@
         <v>22</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>965</v>
+        <v>950</v>
       </c>
       <c r="N27" t="s">
-        <v>1011</v>
+        <v>996</v>
       </c>
     </row>
     <row r="28" spans="3:16">
@@ -18943,10 +18965,10 @@
         <v>23</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>966</v>
+        <v>951</v>
       </c>
       <c r="N28" t="s">
-        <v>1011</v>
+        <v>996</v>
       </c>
     </row>
     <row r="29" spans="3:16">
@@ -18960,10 +18982,10 @@
         <v>24</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>967</v>
+        <v>952</v>
       </c>
       <c r="J29" t="s">
-        <v>969</v>
+        <v>954</v>
       </c>
     </row>
     <row r="30" spans="3:16">
@@ -18974,10 +18996,10 @@
         <v>25</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>968</v>
+        <v>953</v>
       </c>
       <c r="M30" t="s">
-        <v>899</v>
+        <v>894</v>
       </c>
     </row>
     <row r="31" spans="3:16">
@@ -18991,10 +19013,10 @@
         <v>26</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>970</v>
+        <v>955</v>
       </c>
       <c r="M31" t="s">
-        <v>927</v>
+        <v>916</v>
       </c>
     </row>
     <row r="32" spans="3:16">
@@ -19005,10 +19027,10 @@
         <v>27</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>972</v>
+        <v>957</v>
       </c>
       <c r="M32" t="s">
-        <v>928</v>
+        <v>917</v>
       </c>
     </row>
     <row r="33" spans="3:9">
@@ -19019,7 +19041,7 @@
         <v>28</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>973</v>
+        <v>958</v>
       </c>
     </row>
     <row r="34" spans="3:9">
@@ -19030,7 +19052,7 @@
         <v>29</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>974</v>
+        <v>959</v>
       </c>
     </row>
     <row r="35" spans="3:9">
@@ -19041,7 +19063,7 @@
         <v>30</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>975</v>
+        <v>960</v>
       </c>
     </row>
     <row r="36" spans="3:9">
@@ -19052,7 +19074,7 @@
         <v>31</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>976</v>
+        <v>961</v>
       </c>
     </row>
     <row r="37" spans="3:9">
@@ -19063,7 +19085,7 @@
         <v>32</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>977</v>
+        <v>962</v>
       </c>
     </row>
     <row r="38" spans="3:9">
@@ -19074,7 +19096,7 @@
         <v>33</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>978</v>
+        <v>963</v>
       </c>
     </row>
     <row r="39" spans="3:9">
@@ -19091,7 +19113,7 @@
         <v>34</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>979</v>
+        <v>964</v>
       </c>
     </row>
     <row r="40" spans="3:9">
@@ -19102,7 +19124,7 @@
         <v>35</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>980</v>
+        <v>965</v>
       </c>
     </row>
     <row r="41" spans="3:9">
@@ -19113,7 +19135,7 @@
         <v>36</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>981</v>
+        <v>966</v>
       </c>
     </row>
     <row r="42" spans="3:9">
@@ -19124,7 +19146,7 @@
         <v>37</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>982</v>
+        <v>967</v>
       </c>
     </row>
     <row r="43" spans="3:9">
@@ -19135,7 +19157,7 @@
         <v>38</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>983</v>
+        <v>968</v>
       </c>
     </row>
     <row r="44" spans="3:9">
@@ -19146,7 +19168,7 @@
         <v>39</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>984</v>
+        <v>969</v>
       </c>
     </row>
     <row r="45" spans="3:9">
@@ -19157,7 +19179,7 @@
         <v>40</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>985</v>
+        <v>970</v>
       </c>
     </row>
     <row r="46" spans="3:9">
@@ -19168,7 +19190,7 @@
         <v>41</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>986</v>
+        <v>971</v>
       </c>
     </row>
     <row r="47" spans="3:9">
@@ -19179,7 +19201,7 @@
         <v>42</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>987</v>
+        <v>972</v>
       </c>
     </row>
     <row r="48" spans="3:9">
@@ -19190,7 +19212,7 @@
         <v>43</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>988</v>
+        <v>973</v>
       </c>
     </row>
     <row r="49" spans="3:13">
@@ -19201,7 +19223,7 @@
         <v>44</v>
       </c>
       <c r="I49" t="s">
-        <v>989</v>
+        <v>974</v>
       </c>
     </row>
     <row r="50" spans="3:13">
@@ -19212,7 +19234,7 @@
         <v>45</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>990</v>
+        <v>975</v>
       </c>
     </row>
     <row r="51" spans="3:13">
@@ -19223,7 +19245,7 @@
         <v>46</v>
       </c>
       <c r="I51" t="s">
-        <v>991</v>
+        <v>976</v>
       </c>
     </row>
     <row r="52" spans="3:13">
@@ -19234,7 +19256,7 @@
         <v>47</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>992</v>
+        <v>977</v>
       </c>
     </row>
     <row r="53" spans="3:13">
@@ -19245,7 +19267,7 @@
         <v>48</v>
       </c>
       <c r="I53" t="s">
-        <v>993</v>
+        <v>978</v>
       </c>
     </row>
     <row r="54" spans="3:13">
@@ -19256,10 +19278,10 @@
         <v>49</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>994</v>
+        <v>979</v>
       </c>
       <c r="M54" t="s">
-        <v>1007</v>
+        <v>992</v>
       </c>
     </row>
     <row r="55" spans="3:13">
@@ -19270,7 +19292,7 @@
         <v>50</v>
       </c>
       <c r="I55" t="s">
-        <v>995</v>
+        <v>980</v>
       </c>
     </row>
     <row r="56" spans="3:13">
@@ -19281,7 +19303,7 @@
         <v>51</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>996</v>
+        <v>981</v>
       </c>
     </row>
     <row r="57" spans="3:13">
@@ -19292,7 +19314,7 @@
         <v>52</v>
       </c>
       <c r="I57" t="s">
-        <v>997</v>
+        <v>982</v>
       </c>
     </row>
     <row r="58" spans="3:13">
@@ -19303,7 +19325,7 @@
         <v>53</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
     </row>
     <row r="59" spans="3:13">
@@ -19314,7 +19336,7 @@
         <v>54</v>
       </c>
       <c r="I59" t="s">
-        <v>999</v>
+        <v>984</v>
       </c>
     </row>
     <row r="60" spans="3:13">
@@ -19325,7 +19347,7 @@
         <v>55</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>1000</v>
+        <v>985</v>
       </c>
     </row>
     <row r="61" spans="3:13">
@@ -19336,7 +19358,7 @@
         <v>56</v>
       </c>
       <c r="I61" t="s">
-        <v>1001</v>
+        <v>986</v>
       </c>
     </row>
     <row r="62" spans="3:13">
@@ -19347,7 +19369,7 @@
         <v>57</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>1002</v>
+        <v>987</v>
       </c>
     </row>
     <row r="63" spans="3:13">
@@ -19358,7 +19380,7 @@
         <v>58</v>
       </c>
       <c r="I63" t="s">
-        <v>1003</v>
+        <v>988</v>
       </c>
     </row>
     <row r="64" spans="3:13">
@@ -19369,7 +19391,7 @@
         <v>59</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>1004</v>
+        <v>989</v>
       </c>
     </row>
     <row r="65" spans="3:10">
@@ -19380,10 +19402,10 @@
         <v>60</v>
       </c>
       <c r="I65" t="s">
-        <v>1006</v>
+        <v>991</v>
       </c>
       <c r="J65" t="s">
-        <v>1005</v>
+        <v>990</v>
       </c>
     </row>
     <row r="66" spans="3:10">
@@ -19394,7 +19416,7 @@
         <v>61</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>1008</v>
+        <v>993</v>
       </c>
     </row>
     <row r="67" spans="3:10">
@@ -19405,7 +19427,7 @@
         <v>62</v>
       </c>
       <c r="I67" t="s">
-        <v>1009</v>
+        <v>994</v>
       </c>
     </row>
     <row r="68" spans="3:10">
@@ -19416,7 +19438,7 @@
         <v>63</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>1010</v>
+        <v>995</v>
       </c>
     </row>
     <row r="69" spans="3:10">
@@ -19424,7 +19446,7 @@
         <v>64</v>
       </c>
       <c r="I69" t="s">
-        <v>1013</v>
+        <v>998</v>
       </c>
     </row>
     <row r="70" spans="3:10">
@@ -19432,7 +19454,7 @@
         <v>65</v>
       </c>
       <c r="I70" t="s">
-        <v>1014</v>
+        <v>999</v>
       </c>
     </row>
     <row r="71" spans="3:10">
@@ -19440,7 +19462,7 @@
         <v>66</v>
       </c>
       <c r="I71" t="s">
-        <v>1015</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="72" spans="3:10">
@@ -19448,7 +19470,7 @@
         <v>67</v>
       </c>
       <c r="I72" t="s">
-        <v>1016</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="73" spans="3:10">
@@ -19456,7 +19478,7 @@
         <v>68</v>
       </c>
       <c r="I73" t="s">
-        <v>1017</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="74" spans="3:10">
@@ -19464,7 +19486,7 @@
         <v>69</v>
       </c>
       <c r="I74" t="s">
-        <v>1018</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="75" spans="3:10">
@@ -19472,7 +19494,7 @@
         <v>70</v>
       </c>
       <c r="I75" t="s">
-        <v>1019</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="76" spans="3:10">
@@ -19645,22 +19667,22 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" customWidth="1"/>
-    <col min="11" max="11" width="51.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" customWidth="1"/>
+    <col min="11" max="11" width="51.88671875" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
-    <col min="16" max="16" width="24.28515625" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" customWidth="1"/>
-    <col min="18" max="18" width="29.42578125" customWidth="1"/>
+    <col min="16" max="16" width="24.33203125" customWidth="1"/>
+    <col min="17" max="17" width="19.109375" customWidth="1"/>
+    <col min="18" max="18" width="29.44140625" customWidth="1"/>
     <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" customWidth="1"/>
-    <col min="21" max="21" width="3.5703125" customWidth="1"/>
-    <col min="22" max="22" width="2.140625" customWidth="1"/>
-    <col min="25" max="25" width="14.7109375" customWidth="1"/>
+    <col min="20" max="20" width="10.88671875" customWidth="1"/>
+    <col min="21" max="21" width="3.5546875" customWidth="1"/>
+    <col min="22" max="22" width="2.109375" customWidth="1"/>
+    <col min="25" max="25" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:20">

</xml_diff>

<commit_message>
Balancing, Fishing timeout, Bugfix
Research and Upgrade Balancing
Fixed small bug with saving
Added fishing timeout
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB715DD-0B62-4512-A1E7-67FB0132B863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD99B11-51A1-47B1-9A96-A8D9803BAC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="7848" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -25,24 +25,11 @@
     <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="1066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="1068">
   <si>
     <t xml:space="preserve">Tier </t>
   </si>
@@ -3260,6 +3247,12 @@
   </si>
   <si>
     <t>Unlock Research / 7.5% Storage</t>
+  </si>
+  <si>
+    <t>New idea in december</t>
+  </si>
+  <si>
+    <t>After unlocking all wood types have 0 wood</t>
   </si>
 </sst>
 </file>
@@ -4027,7 +4020,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Parasts" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4254,16 +4247,16 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="26.5546875" customWidth="1"/>
-    <col min="8" max="8" width="23.44140625" customWidth="1"/>
-    <col min="9" max="9" width="37.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" customWidth="1"/>
-    <col min="13" max="13" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="37.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:10" ht="13.2">
+    <row r="5" spans="2:10" ht="12.75">
       <c r="G5" s="1" t="s">
         <v>0</v>
       </c>
@@ -4274,7 +4267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="13.2">
+    <row r="6" spans="2:10" ht="12.75">
       <c r="G6" s="1">
         <v>1</v>
       </c>
@@ -4288,7 +4281,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="13.2">
+    <row r="7" spans="2:10" ht="12.75">
       <c r="G7" s="1">
         <v>1</v>
       </c>
@@ -4302,7 +4295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="13.2">
+    <row r="8" spans="2:10" ht="12.75">
       <c r="G8" s="1">
         <v>1</v>
       </c>
@@ -4316,7 +4309,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="13.2">
+    <row r="9" spans="2:10" ht="12.75">
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
@@ -4336,7 +4329,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="13.2">
+    <row r="10" spans="2:10" ht="12.75">
       <c r="G10" s="1">
         <v>1</v>
       </c>
@@ -4350,7 +4343,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="13.2">
+    <row r="11" spans="2:10" ht="12.75">
       <c r="G11" s="1">
         <v>1</v>
       </c>
@@ -4364,7 +4357,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="13.2">
+    <row r="12" spans="2:10" ht="12.75">
       <c r="C12" t="s">
         <v>930</v>
       </c>
@@ -4384,7 +4377,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="13.2">
+    <row r="13" spans="2:10" ht="12.75">
       <c r="B13" t="s">
         <v>81</v>
       </c>
@@ -4407,7 +4400,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="13.2">
+    <row r="14" spans="2:10" ht="12.75">
       <c r="B14" t="s">
         <v>468</v>
       </c>
@@ -4430,7 +4423,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="13.2">
+    <row r="15" spans="2:10" ht="12.75">
       <c r="B15" t="s">
         <v>931</v>
       </c>
@@ -4451,7 +4444,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="13.2">
+    <row r="16" spans="2:10" ht="12.75">
       <c r="G16" s="1">
         <v>2</v>
       </c>
@@ -4465,7 +4458,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="6:10" ht="13.2">
+    <row r="17" spans="6:10" ht="12.75">
       <c r="G17" s="1">
         <v>2</v>
       </c>
@@ -4479,7 +4472,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="6:10" ht="13.2">
+    <row r="18" spans="6:10" ht="12.75">
       <c r="G18" s="1">
         <v>2</v>
       </c>
@@ -4490,7 +4483,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="6:10" ht="13.2">
+    <row r="19" spans="6:10" ht="12.75">
       <c r="G19" s="1">
         <v>2</v>
       </c>
@@ -4504,7 +4497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="6:10" ht="13.2">
+    <row r="20" spans="6:10" ht="12.75">
       <c r="G20" s="1">
         <v>3</v>
       </c>
@@ -4518,7 +4511,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="6:10" ht="13.2">
+    <row r="21" spans="6:10" ht="12.75">
       <c r="G21" s="1">
         <v>3</v>
       </c>
@@ -4532,7 +4525,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="6:10" ht="13.2">
+    <row r="22" spans="6:10" ht="12.75">
       <c r="G22" s="1">
         <v>3</v>
       </c>
@@ -4546,7 +4539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="6:10" ht="13.2">
+    <row r="23" spans="6:10" ht="12.75">
       <c r="G23" s="1">
         <v>3</v>
       </c>
@@ -4560,7 +4553,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="6:10" ht="13.2">
+    <row r="24" spans="6:10" ht="12.75">
       <c r="G24" s="1">
         <v>3</v>
       </c>
@@ -4571,7 +4564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="6:10" ht="13.2">
+    <row r="25" spans="6:10" ht="12.75">
       <c r="G25" s="1">
         <v>3</v>
       </c>
@@ -4585,7 +4578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="6:10" ht="13.2">
+    <row r="26" spans="6:10" ht="12.75">
       <c r="G26" s="1">
         <v>3</v>
       </c>
@@ -4897,11 +4890,11 @@
       <selection activeCell="K149" sqref="K149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="4" max="4" width="57" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
-    <col min="6" max="6" width="35.88671875" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10">
@@ -6718,15 +6711,15 @@
       <selection activeCell="F4" sqref="F4:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="13.2">
+    <row r="2" spans="1:15" ht="12.75">
       <c r="D2" s="1" t="s">
         <v>50</v>
       </c>
@@ -6734,7 +6727,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="13.2">
+    <row r="3" spans="1:15" ht="12.75">
       <c r="C3" s="1" t="s">
         <v>52</v>
       </c>
@@ -6766,7 +6759,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="13.2">
+    <row r="4" spans="1:15" ht="12.75">
       <c r="C4" s="1">
         <v>1</v>
       </c>
@@ -6799,7 +6792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="13.2">
+    <row r="5" spans="1:15" ht="12.75">
       <c r="C5" s="1">
         <v>2</v>
       </c>
@@ -6832,7 +6825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="13.2">
+    <row r="6" spans="1:15" ht="12.75">
       <c r="C6" s="1">
         <v>3</v>
       </c>
@@ -6865,7 +6858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="13.2">
+    <row r="7" spans="1:15" ht="12.75">
       <c r="C7" s="1">
         <v>4</v>
       </c>
@@ -6898,7 +6891,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="13.2">
+    <row r="8" spans="1:15" ht="12.75">
       <c r="C8" s="1">
         <v>5</v>
       </c>
@@ -6931,7 +6924,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="13.2">
+    <row r="9" spans="1:15" ht="12.75">
       <c r="C9" s="1">
         <v>6</v>
       </c>
@@ -6964,7 +6957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="13.2">
+    <row r="10" spans="1:15" ht="12.75">
       <c r="C10" s="1">
         <v>7</v>
       </c>
@@ -6997,7 +6990,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="13.2">
+    <row r="11" spans="1:15" ht="12.75">
       <c r="C11" s="1">
         <v>8</v>
       </c>
@@ -7030,7 +7023,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="13.2">
+    <row r="12" spans="1:15" ht="12.75">
       <c r="C12" s="1">
         <v>9</v>
       </c>
@@ -7063,7 +7056,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="13.2">
+    <row r="13" spans="1:15" ht="12.75">
       <c r="A13" s="39" t="s">
         <v>3</v>
       </c>
@@ -7099,7 +7092,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="13.2">
+    <row r="14" spans="1:15" ht="12.75">
       <c r="A14" s="35" t="s">
         <v>18</v>
       </c>
@@ -7135,7 +7128,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="13.2">
+    <row r="15" spans="1:15" ht="12.75">
       <c r="A15" s="35" t="s">
         <v>9</v>
       </c>
@@ -7171,7 +7164,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="13.2">
+    <row r="16" spans="1:15" ht="12.75">
       <c r="A16" s="35" t="s">
         <v>14</v>
       </c>
@@ -7207,7 +7200,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="13.2">
+    <row r="17" spans="1:15" ht="12.75">
       <c r="A17" s="35" t="s">
         <v>21</v>
       </c>
@@ -7243,7 +7236,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="13.2">
+    <row r="18" spans="1:15" ht="12.75">
       <c r="A18" s="35" t="s">
         <v>16</v>
       </c>
@@ -7279,7 +7272,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="13.2">
+    <row r="19" spans="1:15" ht="12.75">
       <c r="A19" s="47" t="s">
         <v>26</v>
       </c>
@@ -7287,7 +7280,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="13.2">
+    <row r="20" spans="1:15" ht="12.75">
       <c r="A20" s="35" t="s">
         <v>29</v>
       </c>
@@ -7295,7 +7288,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="13.2">
+    <row r="21" spans="1:15" ht="12.75">
       <c r="A21" s="35" t="s">
         <v>31</v>
       </c>
@@ -7303,7 +7296,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="13.2">
+    <row r="22" spans="1:15" ht="12.75">
       <c r="A22" s="35" t="s">
         <v>33</v>
       </c>
@@ -7311,7 +7304,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="13.2">
+    <row r="23" spans="1:15" ht="12.75">
       <c r="A23" s="35" t="s">
         <v>37</v>
       </c>
@@ -7319,7 +7312,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="13.2">
+    <row r="24" spans="1:15" ht="12.75">
       <c r="A24" s="35" t="s">
         <v>39</v>
       </c>
@@ -7327,7 +7320,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="13.2">
+    <row r="25" spans="1:15" ht="12.75">
       <c r="A25" s="35" t="s">
         <v>41</v>
       </c>
@@ -7335,7 +7328,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="13.2">
+    <row r="26" spans="1:15" ht="12.75">
       <c r="A26" s="35" t="s">
         <v>45</v>
       </c>
@@ -7343,7 +7336,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="13.2">
+    <row r="27" spans="1:15" ht="12.75">
       <c r="A27" s="35" t="s">
         <v>46</v>
       </c>
@@ -7351,12 +7344,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="13.2">
+    <row r="28" spans="1:15" ht="12.75">
       <c r="O28" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="13.2">
+    <row r="29" spans="1:15" ht="12.75">
       <c r="C29" s="1">
         <v>2</v>
       </c>
@@ -7389,12 +7382,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="13.2">
+    <row r="30" spans="1:15" ht="12.75">
       <c r="O30" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="13.2">
+    <row r="32" spans="1:15" ht="12.75">
       <c r="F32" s="23" t="s">
         <v>72</v>
       </c>
@@ -7404,7 +7397,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="13.2">
+    <row r="34" spans="2:12" ht="12.75">
       <c r="F34" s="23" t="s">
         <v>74</v>
       </c>
@@ -7582,41 +7575,41 @@
   </sheetPr>
   <dimension ref="A1:X295"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C21" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="1.6640625" customWidth="1"/>
-    <col min="5" max="5" width="4.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" customWidth="1"/>
     <col min="6" max="6" width="40" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" customWidth="1"/>
-    <col min="9" max="9" width="25.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" customWidth="1"/>
-    <col min="13" max="13" width="28.109375" customWidth="1"/>
-    <col min="14" max="14" width="19.44140625" customWidth="1"/>
-    <col min="15" max="15" width="20.88671875" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1"/>
-    <col min="17" max="17" width="18.109375" customWidth="1"/>
-    <col min="18" max="18" width="16.6640625" customWidth="1"/>
-    <col min="19" max="19" width="15.6640625" customWidth="1"/>
-    <col min="20" max="20" width="14.44140625" customWidth="1"/>
-    <col min="21" max="21" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="18.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" customWidth="1"/>
+    <col min="21" max="21" width="21.42578125" customWidth="1"/>
     <col min="22" max="22" width="26" customWidth="1"/>
-    <col min="23" max="23" width="23.5546875" customWidth="1"/>
-    <col min="24" max="24" width="23.33203125" customWidth="1"/>
-    <col min="25" max="25" width="22.109375" customWidth="1"/>
-    <col min="26" max="26" width="31.44140625" customWidth="1"/>
-    <col min="27" max="27" width="37.6640625" customWidth="1"/>
-    <col min="28" max="28" width="29.44140625" customWidth="1"/>
-    <col min="29" max="29" width="29.88671875" customWidth="1"/>
-    <col min="30" max="30" width="28.6640625" customWidth="1"/>
-    <col min="31" max="31" width="33.109375" customWidth="1"/>
+    <col min="23" max="23" width="23.5703125" customWidth="1"/>
+    <col min="24" max="24" width="23.28515625" customWidth="1"/>
+    <col min="25" max="25" width="22.140625" customWidth="1"/>
+    <col min="26" max="26" width="31.42578125" customWidth="1"/>
+    <col min="27" max="27" width="37.7109375" customWidth="1"/>
+    <col min="28" max="28" width="29.42578125" customWidth="1"/>
+    <col min="29" max="29" width="29.85546875" customWidth="1"/>
+    <col min="30" max="30" width="28.7109375" customWidth="1"/>
+    <col min="31" max="31" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1">
@@ -7624,7 +7617,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="13.2">
+    <row r="2" spans="1:23" ht="12.75">
       <c r="C2" s="1" t="s">
         <v>75</v>
       </c>
@@ -7699,7 +7692,7 @@
       <c r="V5" s="114"/>
       <c r="W5" s="114"/>
     </row>
-    <row r="6" spans="1:23" ht="13.8" thickBot="1">
+    <row r="6" spans="1:23" ht="13.5" thickBot="1">
       <c r="A6" s="35" t="s">
         <v>18</v>
       </c>
@@ -7768,7 +7761,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="13.2">
+    <row r="7" spans="1:23" ht="12.75">
       <c r="A7" s="35" t="s">
         <v>9</v>
       </c>
@@ -7840,7 +7833,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="13.2">
+    <row r="8" spans="1:23" ht="12.75">
       <c r="A8" s="35" t="s">
         <v>14</v>
       </c>
@@ -7911,7 +7904,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="13.2">
+    <row r="9" spans="1:23" ht="12.75">
       <c r="A9" s="35" t="s">
         <v>21</v>
       </c>
@@ -7979,7 +7972,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="13.2">
+    <row r="10" spans="1:23" ht="12.75">
       <c r="A10" s="35" t="s">
         <v>16</v>
       </c>
@@ -8034,7 +8027,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="13.2">
+    <row r="11" spans="1:23" ht="12.75">
       <c r="A11" s="47" t="s">
         <v>26</v>
       </c>
@@ -8093,7 +8086,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="13.2">
+    <row r="12" spans="1:23" ht="12.75">
       <c r="A12" s="35" t="s">
         <v>29</v>
       </c>
@@ -8147,7 +8140,7 @@
       </c>
       <c r="W12" s="40"/>
     </row>
-    <row r="13" spans="1:23" ht="13.2">
+    <row r="13" spans="1:23" ht="12.75">
       <c r="A13" s="35" t="s">
         <v>31</v>
       </c>
@@ -8194,7 +8187,7 @@
       </c>
       <c r="W13" s="40"/>
     </row>
-    <row r="14" spans="1:23" ht="13.2">
+    <row r="14" spans="1:23" ht="12.75">
       <c r="A14" s="35" t="s">
         <v>33</v>
       </c>
@@ -8228,7 +8221,7 @@
       <c r="V14" s="38"/>
       <c r="W14" s="40"/>
     </row>
-    <row r="15" spans="1:23" ht="13.2">
+    <row r="15" spans="1:23" ht="12.75">
       <c r="A15" s="35" t="s">
         <v>37</v>
       </c>
@@ -8262,7 +8255,7 @@
       <c r="V15" s="38"/>
       <c r="W15" s="40"/>
     </row>
-    <row r="16" spans="1:23" ht="13.2">
+    <row r="16" spans="1:23" ht="12.75">
       <c r="A16" s="35" t="s">
         <v>39</v>
       </c>
@@ -8296,7 +8289,7 @@
       <c r="V16" s="42"/>
       <c r="W16" s="43"/>
     </row>
-    <row r="17" spans="1:23" ht="13.2">
+    <row r="17" spans="1:23" ht="12.75">
       <c r="A17" s="35" t="s">
         <v>41</v>
       </c>
@@ -8332,7 +8325,7 @@
       <c r="V17" s="40"/>
       <c r="W17" s="40"/>
     </row>
-    <row r="18" spans="1:23" ht="13.2">
+    <row r="18" spans="1:23" ht="12.75">
       <c r="A18" s="35" t="s">
         <v>45</v>
       </c>
@@ -8364,7 +8357,7 @@
       <c r="V18" s="40"/>
       <c r="W18" s="40"/>
     </row>
-    <row r="19" spans="1:23" ht="13.2">
+    <row r="19" spans="1:23" ht="12.75">
       <c r="A19" s="35" t="s">
         <v>46</v>
       </c>
@@ -8400,7 +8393,7 @@
       <c r="V19" s="40"/>
       <c r="W19" s="40"/>
     </row>
-    <row r="20" spans="1:23" ht="13.2">
+    <row r="20" spans="1:23" ht="12.75">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>15</v>
@@ -8428,7 +8421,7 @@
       <c r="V20" s="40"/>
       <c r="W20" s="40"/>
     </row>
-    <row r="21" spans="1:23" ht="13.2">
+    <row r="21" spans="1:23" ht="12.75">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>16</v>
@@ -8459,7 +8452,7 @@
       <c r="V21" s="40"/>
       <c r="W21" s="40"/>
     </row>
-    <row r="22" spans="1:23" ht="13.2">
+    <row r="22" spans="1:23" ht="12.75">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>17</v>
@@ -8487,7 +8480,7 @@
       <c r="V22" s="40"/>
       <c r="W22" s="40"/>
     </row>
-    <row r="23" spans="1:23" ht="13.2">
+    <row r="23" spans="1:23" ht="12.75">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
         <v>18</v>
@@ -8524,7 +8517,7 @@
       <c r="V23" s="40"/>
       <c r="W23" s="40"/>
     </row>
-    <row r="24" spans="1:23" ht="13.2">
+    <row r="24" spans="1:23" ht="12.75">
       <c r="A24" s="1"/>
       <c r="B24" s="106">
         <v>19</v>
@@ -8564,7 +8557,7 @@
       <c r="V24" s="40"/>
       <c r="W24" s="40"/>
     </row>
-    <row r="25" spans="1:23" ht="13.2">
+    <row r="25" spans="1:23" ht="12.75">
       <c r="A25" s="1"/>
       <c r="B25" s="1">
         <v>20</v>
@@ -8604,7 +8597,7 @@
       <c r="V25" s="40"/>
       <c r="W25" s="40"/>
     </row>
-    <row r="26" spans="1:23" ht="13.2">
+    <row r="26" spans="1:23" ht="12.75">
       <c r="B26" s="1">
         <v>21</v>
       </c>
@@ -8643,7 +8636,7 @@
       <c r="V26" s="40"/>
       <c r="W26" s="40"/>
     </row>
-    <row r="27" spans="1:23" ht="13.2">
+    <row r="27" spans="1:23" ht="12.75">
       <c r="B27" s="1">
         <v>22</v>
       </c>
@@ -8682,7 +8675,7 @@
       <c r="V27" s="40"/>
       <c r="W27" s="40"/>
     </row>
-    <row r="28" spans="1:23" ht="13.2">
+    <row r="28" spans="1:23" ht="12.75">
       <c r="B28" s="1">
         <v>23</v>
       </c>
@@ -8718,7 +8711,7 @@
       <c r="V28" s="40"/>
       <c r="W28" s="40"/>
     </row>
-    <row r="29" spans="1:23" ht="13.2">
+    <row r="29" spans="1:23" ht="12.75">
       <c r="B29" s="1">
         <v>24</v>
       </c>
@@ -8752,7 +8745,7 @@
       <c r="V29" s="40"/>
       <c r="W29" s="40"/>
     </row>
-    <row r="30" spans="1:23" ht="13.2">
+    <row r="30" spans="1:23" ht="12.75">
       <c r="B30" s="1">
         <v>25</v>
       </c>
@@ -8786,7 +8779,7 @@
       <c r="V30" s="40"/>
       <c r="W30" s="40"/>
     </row>
-    <row r="31" spans="1:23" ht="13.2">
+    <row r="31" spans="1:23" ht="12.75">
       <c r="B31" s="1">
         <v>26</v>
       </c>
@@ -8809,7 +8802,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="13.2">
+    <row r="32" spans="1:23" ht="12.75">
       <c r="B32" s="1">
         <v>27</v>
       </c>
@@ -8835,7 +8828,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="18" thickBot="1">
+    <row r="33" spans="1:24" ht="18.75" thickBot="1">
       <c r="B33" s="1">
         <v>28</v>
       </c>
@@ -8852,7 +8845,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="18" thickBot="1">
+    <row r="34" spans="1:24" ht="18.75" thickBot="1">
       <c r="B34" s="1">
         <v>29</v>
       </c>
@@ -8880,7 +8873,7 @@
       <c r="V34" s="53"/>
       <c r="W34" s="53"/>
     </row>
-    <row r="35" spans="1:24" ht="13.8" thickBot="1">
+    <row r="35" spans="1:24" ht="13.5" thickBot="1">
       <c r="B35" s="1">
         <v>30</v>
       </c>
@@ -8933,7 +8926,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="13.2">
+    <row r="36" spans="1:24" ht="12.75">
       <c r="B36" s="1">
         <v>31</v>
       </c>
@@ -8990,7 +8983,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="13.2">
+    <row r="37" spans="1:24" ht="12.75">
       <c r="B37" s="1">
         <v>32</v>
       </c>
@@ -9048,7 +9041,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="13.2">
+    <row r="38" spans="1:24" ht="12.75">
       <c r="B38" s="1">
         <v>33</v>
       </c>
@@ -9105,7 +9098,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="13.2">
+    <row r="39" spans="1:24" ht="12.75">
       <c r="B39" s="1">
         <v>34</v>
       </c>
@@ -9163,7 +9156,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="13.2">
+    <row r="40" spans="1:24" ht="12.75">
       <c r="A40">
         <v>1</v>
       </c>
@@ -9220,7 +9213,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="13.2">
+    <row r="41" spans="1:24" ht="12.75">
       <c r="A41">
         <v>4</v>
       </c>
@@ -9274,7 +9267,7 @@
       </c>
       <c r="X41" s="55"/>
     </row>
-    <row r="42" spans="1:24" ht="13.2">
+    <row r="42" spans="1:24" ht="12.75">
       <c r="A42">
         <v>7</v>
       </c>
@@ -9331,7 +9324,7 @@
       </c>
       <c r="X42" s="55"/>
     </row>
-    <row r="43" spans="1:24" ht="13.2">
+    <row r="43" spans="1:24" ht="12.75">
       <c r="A43">
         <v>10</v>
       </c>
@@ -9384,7 +9377,7 @@
       </c>
       <c r="X43" s="55"/>
     </row>
-    <row r="44" spans="1:24" ht="13.2">
+    <row r="44" spans="1:24" ht="12.75">
       <c r="A44">
         <v>13</v>
       </c>
@@ -9437,7 +9430,7 @@
       </c>
       <c r="X44" s="55"/>
     </row>
-    <row r="45" spans="1:24" ht="13.2">
+    <row r="45" spans="1:24" ht="12.75">
       <c r="A45">
         <v>16</v>
       </c>
@@ -9491,7 +9484,7 @@
       </c>
       <c r="X45" s="59"/>
     </row>
-    <row r="46" spans="1:24" ht="13.2">
+    <row r="46" spans="1:24" ht="12.75">
       <c r="A46">
         <v>19</v>
       </c>
@@ -9542,7 +9535,7 @@
       </c>
       <c r="X46" s="55"/>
     </row>
-    <row r="47" spans="1:24" ht="13.2">
+    <row r="47" spans="1:24" ht="12.75">
       <c r="A47">
         <v>22</v>
       </c>
@@ -9593,7 +9586,7 @@
       </c>
       <c r="X47" s="55"/>
     </row>
-    <row r="48" spans="1:24" ht="13.2">
+    <row r="48" spans="1:24" ht="12.75">
       <c r="A48">
         <v>25</v>
       </c>
@@ -9642,7 +9635,7 @@
       </c>
       <c r="X48" s="55"/>
     </row>
-    <row r="49" spans="1:24" ht="13.2">
+    <row r="49" spans="1:24" ht="12.75">
       <c r="A49">
         <v>28</v>
       </c>
@@ -9691,7 +9684,7 @@
       </c>
       <c r="X49" s="55"/>
     </row>
-    <row r="50" spans="1:24" ht="13.2">
+    <row r="50" spans="1:24" ht="12.75">
       <c r="A50">
         <v>31</v>
       </c>
@@ -9740,7 +9733,7 @@
       </c>
       <c r="X50" s="55"/>
     </row>
-    <row r="51" spans="1:24" ht="13.2">
+    <row r="51" spans="1:24" ht="12.75">
       <c r="A51">
         <v>34</v>
       </c>
@@ -9786,7 +9779,7 @@
       </c>
       <c r="X51" s="55"/>
     </row>
-    <row r="52" spans="1:24" ht="13.2">
+    <row r="52" spans="1:24" ht="12.75">
       <c r="A52">
         <v>37</v>
       </c>
@@ -9845,7 +9838,7 @@
       </c>
       <c r="X52" s="55"/>
     </row>
-    <row r="53" spans="1:24" ht="13.2">
+    <row r="53" spans="1:24" ht="12.75">
       <c r="A53">
         <v>40</v>
       </c>
@@ -9895,7 +9888,7 @@
       </c>
       <c r="X53" s="55"/>
     </row>
-    <row r="54" spans="1:24" ht="13.2">
+    <row r="54" spans="1:24" ht="12.75">
       <c r="A54">
         <v>43</v>
       </c>
@@ -9942,7 +9935,7 @@
       </c>
       <c r="X54" s="55"/>
     </row>
-    <row r="55" spans="1:24" ht="13.2">
+    <row r="55" spans="1:24" ht="12.75">
       <c r="A55">
         <v>46</v>
       </c>
@@ -9998,7 +9991,7 @@
       </c>
       <c r="X55" s="55"/>
     </row>
-    <row r="56" spans="1:24" ht="13.2">
+    <row r="56" spans="1:24" ht="12.75">
       <c r="A56">
         <v>49</v>
       </c>
@@ -10045,7 +10038,7 @@
       </c>
       <c r="X56" s="55"/>
     </row>
-    <row r="57" spans="1:24" ht="13.2">
+    <row r="57" spans="1:24" ht="12.75">
       <c r="A57">
         <v>52</v>
       </c>
@@ -10095,7 +10088,7 @@
       </c>
       <c r="X57" s="55"/>
     </row>
-    <row r="58" spans="1:24" ht="13.2">
+    <row r="58" spans="1:24" ht="12.75">
       <c r="A58">
         <v>55</v>
       </c>
@@ -10138,7 +10131,7 @@
       </c>
       <c r="X58" s="55"/>
     </row>
-    <row r="59" spans="1:24" ht="13.2">
+    <row r="59" spans="1:24" ht="12.75">
       <c r="A59">
         <v>58</v>
       </c>
@@ -10184,7 +10177,7 @@
       </c>
       <c r="X59" s="55"/>
     </row>
-    <row r="60" spans="1:24" ht="13.2">
+    <row r="60" spans="1:24" ht="12.75">
       <c r="A60">
         <v>61</v>
       </c>
@@ -10227,7 +10220,7 @@
       </c>
       <c r="X60" s="55"/>
     </row>
-    <row r="61" spans="1:24" ht="13.2">
+    <row r="61" spans="1:24" ht="12.75">
       <c r="A61">
         <v>64</v>
       </c>
@@ -10272,7 +10265,7 @@
       </c>
       <c r="X61" s="55"/>
     </row>
-    <row r="62" spans="1:24" ht="13.2">
+    <row r="62" spans="1:24" ht="12.75">
       <c r="A62">
         <v>9887654321</v>
       </c>
@@ -10314,7 +10307,7 @@
       </c>
       <c r="X62" s="55"/>
     </row>
-    <row r="63" spans="1:24" ht="13.2">
+    <row r="63" spans="1:24" ht="12.75">
       <c r="B63" s="1">
         <v>58</v>
       </c>
@@ -10353,7 +10346,7 @@
       </c>
       <c r="X63" s="55"/>
     </row>
-    <row r="64" spans="1:24" ht="13.2">
+    <row r="64" spans="1:24" ht="12.75">
       <c r="B64" s="1">
         <v>59</v>
       </c>
@@ -10390,7 +10383,7 @@
       <c r="W64" s="55"/>
       <c r="X64" s="55"/>
     </row>
-    <row r="65" spans="2:24" ht="13.2">
+    <row r="65" spans="2:24" ht="12.75">
       <c r="B65" s="1">
         <v>60</v>
       </c>
@@ -10427,7 +10420,7 @@
       <c r="W65" s="55"/>
       <c r="X65" s="55"/>
     </row>
-    <row r="66" spans="2:24" ht="13.2">
+    <row r="66" spans="2:24" ht="12.75">
       <c r="B66" s="1">
         <v>61</v>
       </c>
@@ -10464,7 +10457,7 @@
       <c r="W66" s="55"/>
       <c r="X66" s="55"/>
     </row>
-    <row r="67" spans="2:24" ht="13.2">
+    <row r="67" spans="2:24" ht="12.75">
       <c r="B67" s="1">
         <v>62</v>
       </c>
@@ -10501,7 +10494,7 @@
       <c r="W67" s="55"/>
       <c r="X67" s="55"/>
     </row>
-    <row r="68" spans="2:24" ht="13.2">
+    <row r="68" spans="2:24" ht="12.75">
       <c r="B68" s="1">
         <v>63</v>
       </c>
@@ -10538,7 +10531,7 @@
       <c r="W68" s="55"/>
       <c r="X68" s="55"/>
     </row>
-    <row r="69" spans="2:24" ht="13.2">
+    <row r="69" spans="2:24" ht="12.75">
       <c r="B69" s="1">
         <v>64</v>
       </c>
@@ -10573,7 +10566,7 @@
       <c r="W69" s="55"/>
       <c r="X69" s="55"/>
     </row>
-    <row r="70" spans="2:24" ht="13.2">
+    <row r="70" spans="2:24" ht="12.75">
       <c r="B70" s="1">
         <v>65</v>
       </c>
@@ -10611,7 +10604,7 @@
       <c r="W70" s="55"/>
       <c r="X70" s="55"/>
     </row>
-    <row r="71" spans="2:24" ht="13.2">
+    <row r="71" spans="2:24" ht="12.75">
       <c r="B71" s="1">
         <v>66</v>
       </c>
@@ -10644,7 +10637,7 @@
       <c r="W71" s="55"/>
       <c r="X71" s="55"/>
     </row>
-    <row r="72" spans="2:24" ht="13.2">
+    <row r="72" spans="2:24" ht="12.75">
       <c r="B72" s="1">
         <v>67</v>
       </c>
@@ -10677,7 +10670,7 @@
       <c r="W72" s="55"/>
       <c r="X72" s="55"/>
     </row>
-    <row r="73" spans="2:24" ht="13.2">
+    <row r="73" spans="2:24" ht="12.75">
       <c r="B73" s="1">
         <v>68</v>
       </c>
@@ -10710,7 +10703,7 @@
       <c r="W73" s="55"/>
       <c r="X73" s="55"/>
     </row>
-    <row r="74" spans="2:24" ht="13.2">
+    <row r="74" spans="2:24" ht="12.75">
       <c r="B74" s="1">
         <v>69</v>
       </c>
@@ -10743,7 +10736,7 @@
       <c r="W74" s="55"/>
       <c r="X74" s="55"/>
     </row>
-    <row r="75" spans="2:24" ht="13.2">
+    <row r="75" spans="2:24" ht="12.75">
       <c r="B75" s="1">
         <v>70</v>
       </c>
@@ -10776,7 +10769,7 @@
       <c r="W75" s="55"/>
       <c r="X75" s="55"/>
     </row>
-    <row r="76" spans="2:24" ht="13.2">
+    <row r="76" spans="2:24" ht="12.75">
       <c r="B76" s="1">
         <v>71</v>
       </c>
@@ -10809,7 +10802,7 @@
       <c r="W76" s="55"/>
       <c r="X76" s="55"/>
     </row>
-    <row r="77" spans="2:24" ht="13.2">
+    <row r="77" spans="2:24" ht="12.75">
       <c r="B77" s="1">
         <v>72</v>
       </c>
@@ -10845,7 +10838,7 @@
       <c r="W77" s="55"/>
       <c r="X77" s="55"/>
     </row>
-    <row r="78" spans="2:24" ht="13.2">
+    <row r="78" spans="2:24" ht="12.75">
       <c r="B78" s="106">
         <v>73</v>
       </c>
@@ -10879,7 +10872,7 @@
       <c r="W78" s="55"/>
       <c r="X78" s="55"/>
     </row>
-    <row r="79" spans="2:24" ht="13.2">
+    <row r="79" spans="2:24" ht="12.75">
       <c r="B79" s="1">
         <v>74</v>
       </c>
@@ -10912,7 +10905,7 @@
       <c r="W79" s="55"/>
       <c r="X79" s="55"/>
     </row>
-    <row r="80" spans="2:24" ht="13.2">
+    <row r="80" spans="2:24" ht="12.75">
       <c r="B80" s="1">
         <v>75</v>
       </c>
@@ -10945,7 +10938,7 @@
       <c r="W80" s="55"/>
       <c r="X80" s="55"/>
     </row>
-    <row r="81" spans="2:24" ht="13.2">
+    <row r="81" spans="2:24" ht="12.75">
       <c r="B81" s="1">
         <v>76</v>
       </c>
@@ -10976,7 +10969,7 @@
       <c r="W81" s="55"/>
       <c r="X81" s="55"/>
     </row>
-    <row r="82" spans="2:24" ht="13.2">
+    <row r="82" spans="2:24" ht="12.75">
       <c r="B82" s="1">
         <v>77</v>
       </c>
@@ -11007,7 +11000,7 @@
       <c r="W82" s="55"/>
       <c r="X82" s="55"/>
     </row>
-    <row r="83" spans="2:24" ht="13.2">
+    <row r="83" spans="2:24" ht="12.75">
       <c r="B83" s="1">
         <v>78</v>
       </c>
@@ -11041,7 +11034,7 @@
       <c r="W83" s="55"/>
       <c r="X83" s="55"/>
     </row>
-    <row r="84" spans="2:24" ht="13.2">
+    <row r="84" spans="2:24" ht="12.75">
       <c r="B84" s="1">
         <v>79</v>
       </c>
@@ -11072,7 +11065,7 @@
       <c r="W84" s="55"/>
       <c r="X84" s="55"/>
     </row>
-    <row r="85" spans="2:24" ht="13.2">
+    <row r="85" spans="2:24" ht="12.75">
       <c r="B85" s="1">
         <v>80</v>
       </c>
@@ -11103,7 +11096,7 @@
       <c r="W85" s="55"/>
       <c r="X85" s="55"/>
     </row>
-    <row r="86" spans="2:24" ht="13.2">
+    <row r="86" spans="2:24" ht="12.75">
       <c r="B86" s="1">
         <v>81</v>
       </c>
@@ -11134,7 +11127,7 @@
       <c r="W86" s="55"/>
       <c r="X86" s="55"/>
     </row>
-    <row r="87" spans="2:24" ht="13.2">
+    <row r="87" spans="2:24" ht="12.75">
       <c r="B87" s="1">
         <v>82</v>
       </c>
@@ -11184,7 +11177,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="2:24" ht="13.2">
+    <row r="88" spans="2:24" ht="12.75">
       <c r="B88" s="1">
         <v>83</v>
       </c>
@@ -11216,7 +11209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="2:24" ht="13.2">
+    <row r="89" spans="2:24" ht="12.75">
       <c r="B89" s="1">
         <v>84</v>
       </c>
@@ -11233,7 +11226,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="90" spans="2:24" ht="13.2">
+    <row r="90" spans="2:24" ht="12.75">
       <c r="B90" s="1">
         <v>85</v>
       </c>
@@ -11263,7 +11256,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="2:24" ht="13.2">
+    <row r="91" spans="2:24" ht="12.75">
       <c r="B91" s="1">
         <v>86</v>
       </c>
@@ -11293,7 +11286,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="92" spans="2:24" ht="13.2">
+    <row r="92" spans="2:24" ht="12.75">
       <c r="B92" s="1">
         <v>87</v>
       </c>
@@ -11323,7 +11316,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="2:24" ht="13.2">
+    <row r="93" spans="2:24" ht="12.75">
       <c r="B93" s="1">
         <v>88</v>
       </c>
@@ -11353,7 +11346,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="94" spans="2:24" ht="13.2">
+    <row r="94" spans="2:24" ht="12.75">
       <c r="B94" s="1">
         <v>89</v>
       </c>
@@ -11386,7 +11379,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="2:24" ht="13.2">
+    <row r="95" spans="2:24" ht="12.75">
       <c r="B95" s="1">
         <v>90</v>
       </c>
@@ -11416,7 +11409,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="2:24" ht="13.2">
+    <row r="96" spans="2:24" ht="12.75">
       <c r="B96" s="106">
         <v>91</v>
       </c>
@@ -11447,7 +11440,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="2:24" ht="13.2">
+    <row r="97" spans="2:24" ht="12.75">
       <c r="B97" s="1">
         <v>92</v>
       </c>
@@ -11477,7 +11470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="98" spans="2:24" ht="13.2">
+    <row r="98" spans="2:24" ht="12.75">
       <c r="B98" s="1">
         <v>93</v>
       </c>
@@ -11507,7 +11500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="2:24" ht="13.2">
+    <row r="99" spans="2:24" ht="12.75">
       <c r="B99" s="1">
         <v>94</v>
       </c>
@@ -11537,7 +11530,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="2:24" ht="13.2">
+    <row r="100" spans="2:24" ht="12.75">
       <c r="B100" s="1">
         <v>95</v>
       </c>
@@ -11567,7 +11560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="2:24" ht="13.2">
+    <row r="101" spans="2:24" ht="12.75">
       <c r="B101" s="1">
         <v>96</v>
       </c>
@@ -11597,7 +11590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="2:24" ht="13.2">
+    <row r="102" spans="2:24" ht="12.75">
       <c r="B102" s="1">
         <v>97</v>
       </c>
@@ -11627,7 +11620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="2:24" ht="13.2">
+    <row r="103" spans="2:24" ht="12.75">
       <c r="B103" s="1">
         <v>98</v>
       </c>
@@ -11642,7 +11635,7 @@
       </c>
       <c r="T103" s="45"/>
     </row>
-    <row r="104" spans="2:24" ht="13.2">
+    <row r="104" spans="2:24" ht="12.75">
       <c r="B104" s="1">
         <v>99</v>
       </c>
@@ -11656,7 +11649,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="105" spans="2:24" ht="13.2">
+    <row r="105" spans="2:24" ht="12.75">
       <c r="B105" s="1">
         <v>100</v>
       </c>
@@ -11670,7 +11663,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="106" spans="2:24" ht="13.2">
+    <row r="106" spans="2:24" ht="12.75">
       <c r="B106" s="1">
         <v>101</v>
       </c>
@@ -11684,7 +11677,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="107" spans="2:24" ht="13.2">
+    <row r="107" spans="2:24" ht="12.75">
       <c r="B107" s="1">
         <v>102</v>
       </c>
@@ -11698,7 +11691,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="108" spans="2:24" ht="13.2">
+    <row r="108" spans="2:24" ht="12.75">
       <c r="B108" s="1">
         <v>103</v>
       </c>
@@ -11715,7 +11708,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="109" spans="2:24" ht="13.2">
+    <row r="109" spans="2:24" ht="12.75">
       <c r="B109" s="1">
         <v>104</v>
       </c>
@@ -11744,7 +11737,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="110" spans="2:24" ht="13.2">
+    <row r="110" spans="2:24" ht="12.75">
       <c r="B110" s="1">
         <v>105</v>
       </c>
@@ -11758,7 +11751,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="111" spans="2:24" ht="13.2">
+    <row r="111" spans="2:24" ht="12.75">
       <c r="B111" s="1">
         <v>106</v>
       </c>
@@ -11772,7 +11765,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="112" spans="2:24" ht="13.2">
+    <row r="112" spans="2:24" ht="12.75">
       <c r="B112" s="1">
         <v>107</v>
       </c>
@@ -11793,7 +11786,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="113" spans="2:24" ht="13.2">
+    <row r="113" spans="2:24" ht="12.75">
       <c r="B113" s="1">
         <v>108</v>
       </c>
@@ -11839,7 +11832,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="114" spans="2:24" ht="13.2">
+    <row r="114" spans="2:24" ht="12.75">
       <c r="B114" s="106">
         <v>109</v>
       </c>
@@ -11882,7 +11875,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="2:24" ht="13.2">
+    <row r="115" spans="2:24" ht="12.75">
       <c r="B115" s="1">
         <v>110</v>
       </c>
@@ -11924,7 +11917,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="2:24" ht="13.2">
+    <row r="116" spans="2:24" ht="12.75">
       <c r="B116" s="1">
         <v>111</v>
       </c>
@@ -11966,7 +11959,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="2:24" ht="13.2">
+    <row r="117" spans="2:24" ht="12.75">
       <c r="B117" s="1">
         <v>112</v>
       </c>
@@ -11999,7 +11992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:24" ht="13.2">
+    <row r="118" spans="2:24" ht="12.75">
       <c r="B118" s="1">
         <v>113</v>
       </c>
@@ -12031,7 +12024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:24" ht="13.2">
+    <row r="119" spans="2:24" ht="12.75">
       <c r="B119" s="1">
         <v>114</v>
       </c>
@@ -12065,7 +12058,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="120" spans="2:24" ht="13.2">
+    <row r="120" spans="2:24" ht="12.75">
       <c r="B120" s="1">
         <v>115</v>
       </c>
@@ -12090,7 +12083,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="121" spans="2:24" ht="13.2">
+    <row r="121" spans="2:24" ht="12.75">
       <c r="B121" s="1">
         <v>116</v>
       </c>
@@ -12115,7 +12108,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="122" spans="2:24" ht="13.2">
+    <row r="122" spans="2:24" ht="12.75">
       <c r="B122" s="1">
         <v>117</v>
       </c>
@@ -12140,7 +12133,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="123" spans="2:24" ht="13.2">
+    <row r="123" spans="2:24" ht="12.75">
       <c r="B123" s="1">
         <v>118</v>
       </c>
@@ -12165,7 +12158,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="124" spans="2:24" ht="13.2">
+    <row r="124" spans="2:24" ht="12.75">
       <c r="B124" s="1">
         <v>119</v>
       </c>
@@ -12190,7 +12183,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="125" spans="2:24" ht="13.2">
+    <row r="125" spans="2:24" ht="12.75">
       <c r="B125" s="1">
         <v>120</v>
       </c>
@@ -12215,7 +12208,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="126" spans="2:24" ht="13.2">
+    <row r="126" spans="2:24" ht="12.75">
       <c r="B126" s="1">
         <v>121</v>
       </c>
@@ -12240,7 +12233,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="127" spans="2:24" ht="13.2">
+    <row r="127" spans="2:24" ht="12.75">
       <c r="B127" s="1">
         <v>122</v>
       </c>
@@ -12265,7 +12258,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="128" spans="2:24" ht="13.2">
+    <row r="128" spans="2:24" ht="12.75">
       <c r="B128" s="1">
         <v>123</v>
       </c>
@@ -12290,7 +12283,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="129" spans="2:15" ht="13.2">
+    <row r="129" spans="2:15" ht="12.75">
       <c r="B129" s="1">
         <v>124</v>
       </c>
@@ -12318,7 +12311,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="130" spans="2:15" ht="13.2">
+    <row r="130" spans="2:15" ht="12.75">
       <c r="B130" s="1">
         <v>125</v>
       </c>
@@ -12343,7 +12336,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="131" spans="2:15" ht="13.2">
+    <row r="131" spans="2:15" ht="12.75">
       <c r="B131" s="1">
         <v>126</v>
       </c>
@@ -12368,7 +12361,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="132" spans="2:15" ht="13.2">
+    <row r="132" spans="2:15" ht="12.75">
       <c r="B132" s="106">
         <v>127</v>
       </c>
@@ -12397,7 +12390,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="133" spans="2:15" ht="13.2">
+    <row r="133" spans="2:15" ht="12.75">
       <c r="B133" s="1">
         <v>128</v>
       </c>
@@ -12425,7 +12418,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="134" spans="2:15" ht="13.2">
+    <row r="134" spans="2:15" ht="12.75">
       <c r="B134" s="1">
         <v>129</v>
       </c>
@@ -12453,7 +12446,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="135" spans="2:15" ht="13.2">
+    <row r="135" spans="2:15" ht="12.75">
       <c r="B135" s="1">
         <v>130</v>
       </c>
@@ -12478,7 +12471,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="136" spans="2:15" ht="13.2">
+    <row r="136" spans="2:15" ht="12.75">
       <c r="B136" s="1">
         <v>131</v>
       </c>
@@ -12506,7 +12499,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="137" spans="2:15" ht="13.2">
+    <row r="137" spans="2:15" ht="12.75">
       <c r="B137" s="1">
         <v>132</v>
       </c>
@@ -12531,7 +12524,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="138" spans="2:15" ht="13.2">
+    <row r="138" spans="2:15" ht="12.75">
       <c r="B138" s="1">
         <v>133</v>
       </c>
@@ -12556,7 +12549,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="139" spans="2:15" ht="13.2">
+    <row r="139" spans="2:15" ht="12.75">
       <c r="B139" s="1">
         <v>134</v>
       </c>
@@ -12581,7 +12574,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="140" spans="2:15" ht="13.2">
+    <row r="140" spans="2:15" ht="12.75">
       <c r="B140" s="1">
         <v>135</v>
       </c>
@@ -12606,7 +12599,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="141" spans="2:15" ht="13.2">
+    <row r="141" spans="2:15" ht="12.75">
       <c r="B141" s="1">
         <v>136</v>
       </c>
@@ -12631,7 +12624,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="142" spans="2:15" ht="13.2">
+    <row r="142" spans="2:15" ht="12.75">
       <c r="B142" s="1">
         <v>137</v>
       </c>
@@ -12656,7 +12649,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="143" spans="2:15" ht="13.2">
+    <row r="143" spans="2:15" ht="12.75">
       <c r="B143" s="1">
         <v>138</v>
       </c>
@@ -12681,7 +12674,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="144" spans="2:15" ht="13.2">
+    <row r="144" spans="2:15" ht="12.75">
       <c r="B144" s="1">
         <v>139</v>
       </c>
@@ -12706,7 +12699,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="145" spans="2:15" ht="13.2">
+    <row r="145" spans="2:15" ht="12.75">
       <c r="B145" s="1">
         <v>140</v>
       </c>
@@ -12731,7 +12724,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="146" spans="2:15" ht="13.2">
+    <row r="146" spans="2:15" ht="12.75">
       <c r="B146" s="1">
         <v>141</v>
       </c>
@@ -12756,7 +12749,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="147" spans="2:15" ht="13.2">
+    <row r="147" spans="2:15" ht="12.75">
       <c r="B147" s="1">
         <v>142</v>
       </c>
@@ -12781,7 +12774,7 @@
         <v>1493</v>
       </c>
     </row>
-    <row r="148" spans="2:15" ht="13.2">
+    <row r="148" spans="2:15" ht="12.75">
       <c r="B148" s="1">
         <v>143</v>
       </c>
@@ -12806,7 +12799,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="149" spans="2:15" ht="13.2">
+    <row r="149" spans="2:15" ht="12.75">
       <c r="B149" s="1">
         <v>144</v>
       </c>
@@ -12834,7 +12827,7 @@
         <v>1723</v>
       </c>
     </row>
-    <row r="150" spans="2:15" ht="13.2">
+    <row r="150" spans="2:15" ht="12.75">
       <c r="B150" s="106">
         <v>145</v>
       </c>
@@ -12860,7 +12853,7 @@
         <v>1851</v>
       </c>
     </row>
-    <row r="151" spans="2:15" ht="13.2">
+    <row r="151" spans="2:15" ht="12.75">
       <c r="B151" s="1">
         <v>146</v>
       </c>
@@ -12885,7 +12878,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="152" spans="2:15" ht="13.2">
+    <row r="152" spans="2:15" ht="12.75">
       <c r="B152" s="1">
         <v>147</v>
       </c>
@@ -12910,7 +12903,7 @@
         <v>2139</v>
       </c>
     </row>
-    <row r="153" spans="2:15" ht="13.2">
+    <row r="153" spans="2:15" ht="12.75">
       <c r="B153" s="1">
         <v>148</v>
       </c>
@@ -12938,7 +12931,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="154" spans="2:15" ht="13.2">
+    <row r="154" spans="2:15" ht="12.75">
       <c r="B154" s="1">
         <v>149</v>
       </c>
@@ -12963,7 +12956,7 @@
         <v>2477</v>
       </c>
     </row>
-    <row r="155" spans="2:15" ht="13.2">
+    <row r="155" spans="2:15" ht="12.75">
       <c r="B155" s="1">
         <v>150</v>
       </c>
@@ -12991,7 +12984,7 @@
         <v>2668</v>
       </c>
     </row>
-    <row r="156" spans="2:15" ht="13.2">
+    <row r="156" spans="2:15" ht="12.75">
       <c r="B156" s="1">
         <v>151</v>
       </c>
@@ -13016,7 +13009,7 @@
         <v>2878</v>
       </c>
     </row>
-    <row r="157" spans="2:15" ht="13.2">
+    <row r="157" spans="2:15" ht="12.75">
       <c r="B157" s="1">
         <v>152</v>
       </c>
@@ -13041,7 +13034,7 @@
         <v>3109</v>
       </c>
     </row>
-    <row r="158" spans="2:15" ht="13.2">
+    <row r="158" spans="2:15" ht="12.75">
       <c r="B158" s="1">
         <v>153</v>
       </c>
@@ -13066,7 +13059,7 @@
         <v>3362</v>
       </c>
     </row>
-    <row r="159" spans="2:15" ht="13.2">
+    <row r="159" spans="2:15" ht="12.75">
       <c r="B159" s="1">
         <v>154</v>
       </c>
@@ -13091,7 +13084,7 @@
         <v>3642</v>
       </c>
     </row>
-    <row r="160" spans="2:15" ht="13.2">
+    <row r="160" spans="2:15" ht="12.75">
       <c r="B160" s="1">
         <v>155</v>
       </c>
@@ -13116,7 +13109,7 @@
         <v>3952</v>
       </c>
     </row>
-    <row r="161" spans="2:15" ht="13.2">
+    <row r="161" spans="2:15" ht="12.75">
       <c r="B161" s="1">
         <v>156</v>
       </c>
@@ -13141,7 +13134,7 @@
         <v>4296</v>
       </c>
     </row>
-    <row r="162" spans="2:15" ht="13.2">
+    <row r="162" spans="2:15" ht="12.75">
       <c r="B162" s="1">
         <v>157</v>
       </c>
@@ -13166,7 +13159,7 @@
         <v>4680</v>
       </c>
     </row>
-    <row r="163" spans="2:15" ht="13.2">
+    <row r="163" spans="2:15" ht="12.75">
       <c r="B163" s="1">
         <v>158</v>
       </c>
@@ -13191,7 +13184,7 @@
         <v>5108</v>
       </c>
     </row>
-    <row r="164" spans="2:15" ht="13.2">
+    <row r="164" spans="2:15" ht="12.75">
       <c r="B164" s="1">
         <v>159</v>
       </c>
@@ -13216,7 +13209,7 @@
         <v>5587</v>
       </c>
     </row>
-    <row r="165" spans="2:15" ht="13.2">
+    <row r="165" spans="2:15" ht="12.75">
       <c r="B165" s="1">
         <v>160</v>
       </c>
@@ -13241,7 +13234,7 @@
         <v>6124</v>
       </c>
     </row>
-    <row r="166" spans="2:15" ht="13.2">
+    <row r="166" spans="2:15" ht="12.75">
       <c r="B166" s="1">
         <v>161</v>
       </c>
@@ -13266,7 +13259,7 @@
         <v>6728</v>
       </c>
     </row>
-    <row r="167" spans="2:15" ht="13.2">
+    <row r="167" spans="2:15" ht="12.75">
       <c r="B167" s="1">
         <v>162</v>
       </c>
@@ -13291,7 +13284,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="168" spans="2:15" ht="13.2">
+    <row r="168" spans="2:15" ht="12.75">
       <c r="B168" s="106">
         <v>163</v>
       </c>
@@ -13317,7 +13310,7 @@
         <v>8178</v>
       </c>
     </row>
-    <row r="169" spans="2:15" ht="13.2">
+    <row r="169" spans="2:15" ht="12.75">
       <c r="B169" s="1">
         <v>164</v>
       </c>
@@ -13342,7 +13335,7 @@
         <v>9047</v>
       </c>
     </row>
-    <row r="170" spans="2:15" ht="13.2">
+    <row r="170" spans="2:15" ht="12.75">
       <c r="B170" s="1">
         <v>165</v>
       </c>
@@ -13367,7 +13360,7 @@
         <v>10032</v>
       </c>
     </row>
-    <row r="171" spans="2:15" ht="13.2">
+    <row r="171" spans="2:15" ht="12.75">
       <c r="B171" s="1">
         <v>166</v>
       </c>
@@ -13392,7 +13385,7 @@
         <v>11149</v>
       </c>
     </row>
-    <row r="172" spans="2:15" ht="13.2">
+    <row r="172" spans="2:15" ht="12.75">
       <c r="B172" s="1">
         <v>167</v>
       </c>
@@ -13417,7 +13410,7 @@
         <v>12418</v>
       </c>
     </row>
-    <row r="173" spans="2:15" ht="13.2">
+    <row r="173" spans="2:15" ht="12.75">
       <c r="B173" s="1">
         <v>168</v>
       </c>
@@ -16267,13 +16260,13 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="6" max="6" width="38.88671875" customWidth="1"/>
-    <col min="9" max="9" width="26.88671875" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:12" ht="13.2">
+    <row r="2" spans="3:12" ht="12.75">
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
@@ -16283,7 +16276,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="4" spans="3:12" ht="13.2">
+    <row r="4" spans="3:12" ht="12.75">
       <c r="C4" s="1" t="s">
         <v>52</v>
       </c>
@@ -16312,7 +16305,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="5" spans="3:12" ht="13.2">
+    <row r="5" spans="3:12" ht="12.75">
       <c r="C5" s="1">
         <v>1</v>
       </c>
@@ -16335,7 +16328,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="6" spans="3:12" ht="13.2">
+    <row r="6" spans="3:12" ht="12.75">
       <c r="C6" s="1">
         <v>2</v>
       </c>
@@ -16352,7 +16345,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="7" spans="3:12" ht="13.2">
+    <row r="7" spans="3:12" ht="12.75">
       <c r="C7" s="1">
         <v>3</v>
       </c>
@@ -16366,7 +16359,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="8" spans="3:12" ht="13.2">
+    <row r="8" spans="3:12" ht="12.75">
       <c r="C8" s="1">
         <v>4</v>
       </c>
@@ -16380,7 +16373,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="9" spans="3:12" ht="13.2">
+    <row r="9" spans="3:12" ht="12.75">
       <c r="C9" s="1">
         <v>5</v>
       </c>
@@ -16394,7 +16387,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="10" spans="3:12" ht="13.2">
+    <row r="10" spans="3:12" ht="12.75">
       <c r="C10" s="1">
         <v>6</v>
       </c>
@@ -16411,7 +16404,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="11" spans="3:12" ht="13.2">
+    <row r="11" spans="3:12" ht="12.75">
       <c r="C11" s="1">
         <v>7</v>
       </c>
@@ -16428,7 +16421,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="12" spans="3:12" ht="13.2">
+    <row r="12" spans="3:12" ht="12.75">
       <c r="C12" s="1">
         <v>8</v>
       </c>
@@ -16442,7 +16435,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="13" spans="3:12" ht="13.2">
+    <row r="13" spans="3:12" ht="12.75">
       <c r="C13" s="1">
         <v>9</v>
       </c>
@@ -16456,7 +16449,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="14" spans="3:12" ht="13.2">
+    <row r="14" spans="3:12" ht="12.75">
       <c r="C14" s="1">
         <v>10</v>
       </c>
@@ -16470,7 +16463,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="15" spans="3:12" ht="13.2">
+    <row r="15" spans="3:12" ht="12.75">
       <c r="C15" s="1">
         <v>11</v>
       </c>
@@ -16484,7 +16477,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="16" spans="3:12" ht="13.2">
+    <row r="16" spans="3:12" ht="12.75">
       <c r="C16" s="1">
         <v>12</v>
       </c>
@@ -16498,7 +16491,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="17" spans="3:9" ht="13.2">
+    <row r="17" spans="3:9" ht="12.75">
       <c r="C17" s="1">
         <v>13</v>
       </c>
@@ -16512,7 +16505,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="18" spans="3:9" ht="13.2">
+    <row r="18" spans="3:9" ht="12.75">
       <c r="C18" s="1">
         <v>14</v>
       </c>
@@ -16526,7 +16519,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="19" spans="3:9" ht="13.2">
+    <row r="19" spans="3:9" ht="12.75">
       <c r="C19" s="1">
         <v>15</v>
       </c>
@@ -16540,7 +16533,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="20" spans="3:9" ht="13.2">
+    <row r="20" spans="3:9" ht="12.75">
       <c r="C20" s="1">
         <v>16</v>
       </c>
@@ -16554,7 +16547,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="21" spans="3:9" ht="13.2">
+    <row r="21" spans="3:9" ht="12.75">
       <c r="C21" s="1">
         <v>17</v>
       </c>
@@ -16568,7 +16561,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="22" spans="3:9" ht="13.2">
+    <row r="22" spans="3:9" ht="12.75">
       <c r="C22" s="1">
         <v>18</v>
       </c>
@@ -16582,7 +16575,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="23" spans="3:9" ht="13.2">
+    <row r="23" spans="3:9" ht="12.75">
       <c r="C23" s="1">
         <v>19</v>
       </c>
@@ -16596,7 +16589,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="24" spans="3:9" ht="13.2">
+    <row r="24" spans="3:9" ht="12.75">
       <c r="C24" s="1">
         <v>20</v>
       </c>
@@ -16610,7 +16603,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="25" spans="3:9" ht="13.2">
+    <row r="25" spans="3:9" ht="12.75">
       <c r="C25" s="1">
         <v>21</v>
       </c>
@@ -16624,7 +16617,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="26" spans="3:9" ht="13.2">
+    <row r="26" spans="3:9" ht="12.75">
       <c r="C26" s="1">
         <v>22</v>
       </c>
@@ -16638,7 +16631,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="27" spans="3:9" ht="13.2">
+    <row r="27" spans="3:9" ht="12.75">
       <c r="C27" s="1">
         <v>23</v>
       </c>
@@ -16652,7 +16645,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="3:9" ht="13.2">
+    <row r="28" spans="3:9" ht="12.75">
       <c r="C28" s="1">
         <v>24</v>
       </c>
@@ -16666,7 +16659,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="29" spans="3:9" ht="13.2">
+    <row r="29" spans="3:9" ht="12.75">
       <c r="C29" s="1">
         <v>25</v>
       </c>
@@ -16680,7 +16673,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="30" spans="3:9" ht="13.2">
+    <row r="30" spans="3:9" ht="12.75">
       <c r="C30" s="1">
         <v>26</v>
       </c>
@@ -16694,7 +16687,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="31" spans="3:9" ht="13.2">
+    <row r="31" spans="3:9" ht="12.75">
       <c r="C31" s="1">
         <v>27</v>
       </c>
@@ -16708,7 +16701,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="3:9" ht="13.2">
+    <row r="32" spans="3:9" ht="12.75">
       <c r="C32" s="1">
         <v>28</v>
       </c>
@@ -16723,7 +16716,7 @@
       </c>
       <c r="I32" s="26"/>
     </row>
-    <row r="33" spans="3:9" ht="13.2">
+    <row r="33" spans="3:9" ht="12.75">
       <c r="C33" s="1">
         <v>29</v>
       </c>
@@ -16738,7 +16731,7 @@
       </c>
       <c r="I33" s="27"/>
     </row>
-    <row r="34" spans="3:9" ht="13.2">
+    <row r="34" spans="3:9" ht="12.75">
       <c r="C34" s="1">
         <v>30</v>
       </c>
@@ -16753,7 +16746,7 @@
       </c>
       <c r="I34" s="27"/>
     </row>
-    <row r="35" spans="3:9" ht="13.2">
+    <row r="35" spans="3:9" ht="12.75">
       <c r="C35" s="1">
         <v>31</v>
       </c>
@@ -16768,7 +16761,7 @@
       </c>
       <c r="I35" s="27"/>
     </row>
-    <row r="36" spans="3:9" ht="13.2">
+    <row r="36" spans="3:9" ht="12.75">
       <c r="C36" s="1">
         <v>32</v>
       </c>
@@ -16785,7 +16778,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="3:9" ht="13.2">
+    <row r="37" spans="3:9" ht="12.75">
       <c r="C37" s="1">
         <v>33</v>
       </c>
@@ -16802,7 +16795,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="3:9" ht="13.2">
+    <row r="38" spans="3:9" ht="12.75">
       <c r="C38" s="1">
         <v>34</v>
       </c>
@@ -16819,7 +16812,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="3:9" ht="13.2">
+    <row r="39" spans="3:9" ht="12.75">
       <c r="C39" s="1">
         <v>35</v>
       </c>
@@ -16836,7 +16829,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="40" spans="3:9" ht="13.2">
+    <row r="40" spans="3:9" ht="12.75">
       <c r="C40" s="1">
         <v>36</v>
       </c>
@@ -16853,7 +16846,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="41" spans="3:9" ht="13.2">
+    <row r="41" spans="3:9" ht="12.75">
       <c r="C41" s="1">
         <v>37</v>
       </c>
@@ -16870,7 +16863,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="42" spans="3:9" ht="13.2">
+    <row r="42" spans="3:9" ht="12.75">
       <c r="C42" s="1">
         <v>38</v>
       </c>
@@ -16887,7 +16880,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="43" spans="3:9" ht="13.2">
+    <row r="43" spans="3:9" ht="12.75">
       <c r="C43" s="1">
         <v>39</v>
       </c>
@@ -16904,7 +16897,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="44" spans="3:9" ht="13.2">
+    <row r="44" spans="3:9" ht="12.75">
       <c r="C44" s="1">
         <v>40</v>
       </c>
@@ -16921,7 +16914,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="45" spans="3:9" ht="13.2">
+    <row r="45" spans="3:9" ht="12.75">
       <c r="C45" s="1">
         <v>41</v>
       </c>
@@ -16938,7 +16931,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="46" spans="3:9" ht="13.2">
+    <row r="46" spans="3:9" ht="12.75">
       <c r="C46" s="1">
         <v>42</v>
       </c>
@@ -16955,7 +16948,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="47" spans="3:9" ht="13.2">
+    <row r="47" spans="3:9" ht="12.75">
       <c r="C47" s="1">
         <v>43</v>
       </c>
@@ -16972,7 +16965,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="48" spans="3:9" ht="13.2">
+    <row r="48" spans="3:9" ht="12.75">
       <c r="C48" s="1">
         <v>44</v>
       </c>
@@ -16989,7 +16982,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="49" spans="3:9" ht="13.2">
+    <row r="49" spans="3:9" ht="12.75">
       <c r="C49" s="1">
         <v>45</v>
       </c>
@@ -17006,7 +16999,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="50" spans="3:9" ht="13.2">
+    <row r="50" spans="3:9" ht="12.75">
       <c r="C50" s="1">
         <v>46</v>
       </c>
@@ -17023,7 +17016,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="51" spans="3:9" ht="13.2">
+    <row r="51" spans="3:9" ht="12.75">
       <c r="C51" s="1">
         <v>47</v>
       </c>
@@ -17040,7 +17033,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="52" spans="3:9" ht="13.2">
+    <row r="52" spans="3:9" ht="12.75">
       <c r="C52" s="1">
         <v>48</v>
       </c>
@@ -17057,7 +17050,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="53" spans="3:9" ht="13.2">
+    <row r="53" spans="3:9" ht="12.75">
       <c r="C53" s="1">
         <v>49</v>
       </c>
@@ -17074,7 +17067,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="54" spans="3:9" ht="13.2">
+    <row r="54" spans="3:9" ht="12.75">
       <c r="C54" s="1">
         <v>50</v>
       </c>
@@ -17088,7 +17081,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="55" spans="3:9" ht="13.2">
+    <row r="55" spans="3:9" ht="12.75">
       <c r="C55" s="1">
         <v>51</v>
       </c>
@@ -17102,7 +17095,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="56" spans="3:9" ht="13.2">
+    <row r="56" spans="3:9" ht="12.75">
       <c r="C56" s="1">
         <v>52</v>
       </c>
@@ -17116,7 +17109,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="57" spans="3:9" ht="13.2">
+    <row r="57" spans="3:9" ht="12.75">
       <c r="C57" s="1">
         <v>53</v>
       </c>
@@ -17130,7 +17123,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="58" spans="3:9" ht="13.2">
+    <row r="58" spans="3:9" ht="12.75">
       <c r="C58" s="1">
         <v>54</v>
       </c>
@@ -17144,7 +17137,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="3:9" ht="13.2">
+    <row r="59" spans="3:9" ht="12.75">
       <c r="C59" s="1">
         <v>55</v>
       </c>
@@ -17158,7 +17151,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="60" spans="3:9" ht="13.2">
+    <row r="60" spans="3:9" ht="12.75">
       <c r="C60" s="1">
         <v>56</v>
       </c>
@@ -17172,7 +17165,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="3:9" ht="13.2">
+    <row r="61" spans="3:9" ht="12.75">
       <c r="C61" s="1">
         <v>57</v>
       </c>
@@ -17186,7 +17179,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="62" spans="3:9" ht="13.2">
+    <row r="62" spans="3:9" ht="12.75">
       <c r="C62" s="1">
         <v>58</v>
       </c>
@@ -17197,7 +17190,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="63" spans="3:9" ht="13.2">
+    <row r="63" spans="3:9" ht="12.75">
       <c r="C63" s="1">
         <v>59</v>
       </c>
@@ -17208,7 +17201,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="64" spans="3:9" ht="13.2">
+    <row r="64" spans="3:9" ht="12.75">
       <c r="C64" s="1">
         <v>60</v>
       </c>
@@ -17219,7 +17212,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="65" spans="3:6" ht="13.2">
+    <row r="65" spans="3:6" ht="12.75">
       <c r="C65" s="1">
         <v>61</v>
       </c>
@@ -17361,10 +17354,10 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="7" max="7" width="18.44140625" customWidth="1"/>
-    <col min="9" max="9" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:9">
@@ -17815,18 +17808,18 @@
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" ht="13.2">
+    <row r="4" spans="3:7" ht="12.75">
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="13.2">
+    <row r="6" spans="3:7" ht="12.75">
       <c r="C6" s="1" t="s">
         <v>52</v>
       </c>
@@ -17843,7 +17836,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="13.2">
+    <row r="7" spans="3:7" ht="12.75">
       <c r="C7" s="1">
         <v>1</v>
       </c>
@@ -17854,7 +17847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="13.2">
+    <row r="8" spans="3:7" ht="12.75">
       <c r="C8" s="1">
         <v>2</v>
       </c>
@@ -17865,7 +17858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="13.2">
+    <row r="9" spans="3:7" ht="12.75">
       <c r="C9" s="1">
         <v>3</v>
       </c>
@@ -17876,7 +17869,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="3:7" ht="13.2">
+    <row r="10" spans="3:7" ht="12.75">
       <c r="C10" s="1">
         <v>4</v>
       </c>
@@ -17887,7 +17880,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="3:7" ht="13.2">
+    <row r="11" spans="3:7" ht="12.75">
       <c r="C11" s="1">
         <v>5</v>
       </c>
@@ -17898,7 +17891,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="3:7" ht="13.2">
+    <row r="12" spans="3:7" ht="12.75">
       <c r="C12" s="1">
         <v>6</v>
       </c>
@@ -17909,7 +17902,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="3:7" ht="13.2">
+    <row r="13" spans="3:7" ht="12.75">
       <c r="C13" s="1">
         <v>7</v>
       </c>
@@ -17920,7 +17913,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="3:7" ht="13.2">
+    <row r="14" spans="3:7" ht="12.75">
       <c r="C14" s="1">
         <v>8</v>
       </c>
@@ -17931,7 +17924,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="15" spans="3:7" ht="13.2">
+    <row r="15" spans="3:7" ht="12.75">
       <c r="C15" s="1">
         <v>9</v>
       </c>
@@ -17942,7 +17935,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="16" spans="3:7" ht="13.2">
+    <row r="16" spans="3:7" ht="12.75">
       <c r="C16" s="1">
         <v>10</v>
       </c>
@@ -17953,7 +17946,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="17" spans="3:7" ht="13.2">
+    <row r="17" spans="3:7" ht="12.75">
       <c r="C17" s="1">
         <v>11</v>
       </c>
@@ -17964,7 +17957,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="18" spans="3:7" ht="13.2">
+    <row r="18" spans="3:7" ht="12.75">
       <c r="C18" s="1">
         <v>12</v>
       </c>
@@ -17975,7 +17968,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="19" spans="3:7" ht="13.2">
+    <row r="19" spans="3:7" ht="12.75">
       <c r="C19" s="1">
         <v>13</v>
       </c>
@@ -17986,7 +17979,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="20" spans="3:7" ht="13.2">
+    <row r="20" spans="3:7" ht="12.75">
       <c r="C20" s="1">
         <v>14</v>
       </c>
@@ -17997,7 +17990,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="3:7" ht="13.2">
+    <row r="21" spans="3:7" ht="12.75">
       <c r="C21" s="1">
         <v>15</v>
       </c>
@@ -18008,7 +18001,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="3:7" ht="13.2">
+    <row r="22" spans="3:7" ht="12.75">
       <c r="C22" s="1">
         <v>16</v>
       </c>
@@ -18019,7 +18012,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="3:7" ht="13.2">
+    <row r="23" spans="3:7" ht="12.75">
       <c r="C23" s="1">
         <v>17</v>
       </c>
@@ -18030,7 +18023,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="3:7" ht="13.2">
+    <row r="24" spans="3:7" ht="12.75">
       <c r="C24" s="1">
         <v>18</v>
       </c>
@@ -18041,7 +18034,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="3:7" ht="13.2">
+    <row r="25" spans="3:7" ht="12.75">
       <c r="C25" s="1">
         <v>19</v>
       </c>
@@ -18052,7 +18045,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="3:7" ht="13.2">
+    <row r="26" spans="3:7" ht="12.75">
       <c r="C26" s="1">
         <v>20</v>
       </c>
@@ -18063,7 +18056,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="3:7" ht="13.2">
+    <row r="27" spans="3:7" ht="12.75">
       <c r="C27" s="1">
         <v>21</v>
       </c>
@@ -18074,7 +18067,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="28" spans="3:7" ht="13.2">
+    <row r="28" spans="3:7" ht="12.75">
       <c r="C28" s="1">
         <v>22</v>
       </c>
@@ -18085,7 +18078,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="3:7" ht="13.2">
+    <row r="29" spans="3:7" ht="12.75">
       <c r="C29" s="1">
         <v>23</v>
       </c>
@@ -18096,7 +18089,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="30" spans="3:7" ht="13.2">
+    <row r="30" spans="3:7" ht="12.75">
       <c r="C30" s="1">
         <v>24</v>
       </c>
@@ -18107,7 +18100,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="3:7" ht="13.2">
+    <row r="31" spans="3:7" ht="12.75">
       <c r="C31" s="1">
         <v>25</v>
       </c>
@@ -18118,7 +18111,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="3:7" ht="13.2">
+    <row r="32" spans="3:7" ht="12.75">
       <c r="C32" s="1">
         <v>26</v>
       </c>
@@ -18129,7 +18122,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="33" spans="3:7" ht="13.2">
+    <row r="33" spans="3:7" ht="12.75">
       <c r="C33" s="1">
         <v>27</v>
       </c>
@@ -18140,7 +18133,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="34" spans="3:7" ht="13.2">
+    <row r="34" spans="3:7" ht="12.75">
       <c r="C34" s="1">
         <v>28</v>
       </c>
@@ -18151,7 +18144,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="35" spans="3:7" ht="13.2">
+    <row r="35" spans="3:7" ht="12.75">
       <c r="C35" s="1">
         <v>29</v>
       </c>
@@ -18162,7 +18155,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="3:7" ht="13.2">
+    <row r="36" spans="3:7" ht="12.75">
       <c r="C36" s="1">
         <v>30</v>
       </c>
@@ -18194,23 +18187,23 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.88671875" customWidth="1"/>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
-    <col min="8" max="8" width="39.44140625" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.5546875" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="39.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:20" ht="13.2">
+    <row r="3" spans="3:20" ht="12.75">
       <c r="C3" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="3:20" ht="13.2">
+    <row r="5" spans="3:20" ht="12.75">
       <c r="C5" s="1" t="s">
         <v>52</v>
       </c>
@@ -18266,7 +18259,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="6" spans="3:20" ht="13.2">
+    <row r="6" spans="3:20" ht="12.75">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -18292,7 +18285,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="7" spans="3:20" ht="13.2">
+    <row r="7" spans="3:20" ht="12.75">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -18312,7 +18305,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="8" spans="3:20" ht="13.2">
+    <row r="8" spans="3:20" ht="12.75">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -18332,7 +18325,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="9" spans="3:20" ht="13.2">
+    <row r="9" spans="3:20" ht="12.75">
       <c r="C9" s="1">
         <v>4</v>
       </c>
@@ -18394,15 +18387,15 @@
   </sheetPr>
   <dimension ref="C3:V105"/>
   <sheetViews>
-    <sheetView topLeftCell="E8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="E22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="26.88671875" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
-    <col min="9" max="9" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="26" customWidth="1"/>
   </cols>
@@ -19033,7 +19026,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="33" spans="3:9">
+    <row r="33" spans="3:12">
       <c r="C33" s="1">
         <v>28</v>
       </c>
@@ -19044,7 +19037,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="34" spans="3:9">
+    <row r="34" spans="3:12">
       <c r="C34" s="1">
         <v>29</v>
       </c>
@@ -19055,7 +19048,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="35" spans="3:9">
+    <row r="35" spans="3:12">
       <c r="C35" s="1">
         <v>30</v>
       </c>
@@ -19066,7 +19059,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="36" spans="3:9">
+    <row r="36" spans="3:12">
       <c r="C36" s="1">
         <v>31</v>
       </c>
@@ -19076,8 +19069,11 @@
       <c r="I36" s="1" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="37" spans="3:9">
+      <c r="L36" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12">
       <c r="C37" s="1">
         <v>32</v>
       </c>
@@ -19087,8 +19083,11 @@
       <c r="I37" s="1" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="38" spans="3:9">
+      <c r="L37" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12">
       <c r="C38" s="1">
         <v>33</v>
       </c>
@@ -19099,7 +19098,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="39" spans="3:9">
+    <row r="39" spans="3:12">
       <c r="C39" s="1">
         <v>34</v>
       </c>
@@ -19116,7 +19115,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="40" spans="3:9">
+    <row r="40" spans="3:12">
       <c r="C40" s="1">
         <v>35</v>
       </c>
@@ -19127,7 +19126,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="41" spans="3:9">
+    <row r="41" spans="3:12">
       <c r="C41" s="1">
         <v>36</v>
       </c>
@@ -19138,7 +19137,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="42" spans="3:9">
+    <row r="42" spans="3:12">
       <c r="C42" s="1">
         <v>37</v>
       </c>
@@ -19149,7 +19148,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="43" spans="3:9">
+    <row r="43" spans="3:12">
       <c r="C43" s="1">
         <v>38</v>
       </c>
@@ -19160,7 +19159,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="44" spans="3:9">
+    <row r="44" spans="3:12">
       <c r="C44" s="1">
         <v>39</v>
       </c>
@@ -19171,7 +19170,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="45" spans="3:9">
+    <row r="45" spans="3:12">
       <c r="C45" s="1">
         <v>40</v>
       </c>
@@ -19182,7 +19181,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="46" spans="3:9">
+    <row r="46" spans="3:12">
       <c r="C46" s="1">
         <v>41</v>
       </c>
@@ -19193,7 +19192,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="47" spans="3:9">
+    <row r="47" spans="3:12">
       <c r="C47" s="1">
         <v>42</v>
       </c>
@@ -19204,7 +19203,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="48" spans="3:9">
+    <row r="48" spans="3:12">
       <c r="C48" s="1">
         <v>43</v>
       </c>
@@ -19667,22 +19666,22 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
-    <col min="10" max="10" width="19.109375" customWidth="1"/>
-    <col min="11" max="11" width="51.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="51.85546875" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
-    <col min="16" max="16" width="24.33203125" customWidth="1"/>
-    <col min="17" max="17" width="19.109375" customWidth="1"/>
-    <col min="18" max="18" width="29.44140625" customWidth="1"/>
+    <col min="16" max="16" width="24.28515625" customWidth="1"/>
+    <col min="17" max="17" width="19.140625" customWidth="1"/>
+    <col min="18" max="18" width="29.42578125" customWidth="1"/>
     <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="20" width="10.88671875" customWidth="1"/>
-    <col min="21" max="21" width="3.5546875" customWidth="1"/>
-    <col min="22" max="22" width="2.109375" customWidth="1"/>
-    <col min="25" max="25" width="14.6640625" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" customWidth="1"/>
+    <col min="21" max="21" width="3.5703125" customWidth="1"/>
+    <col min="22" max="22" width="2.140625" customWidth="1"/>
+    <col min="25" max="25" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:20">

</xml_diff>

<commit_message>
Displaying resources, Colours, Balancing and Bug fixes
Added No Fish! Indicator
Added Secondary Colours to Market and Wood Bars
Added Magic count to Resource screen
Added Gold count to save info
More Balancing
Fixed resource bars not having correct production after load
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F814DE-DF7D-4832-AA13-91244ACF03B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1706D4F-E0BF-4288-8D57-1377BEECEAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="5292" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="5292" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2698" uniqueCount="1235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2714" uniqueCount="1249">
   <si>
     <t xml:space="preserve">Tier </t>
   </si>
@@ -3767,6 +3767,48 @@
   </si>
   <si>
     <t>beaver +0.7 wood per woodcamp</t>
+  </si>
+  <si>
+    <t>New Magic</t>
+  </si>
+  <si>
+    <t>Unlock Gold upgrades</t>
+  </si>
+  <si>
+    <t>Unlock Magic Store</t>
+  </si>
+  <si>
+    <t>Unlock Baits</t>
+  </si>
+  <si>
+    <t>Unlock Fishing Spots</t>
+  </si>
+  <si>
+    <t>Unlock Storage Overdrives</t>
+  </si>
+  <si>
+    <t>Unlock Research slot 2</t>
+  </si>
+  <si>
+    <t>Unlock Research slot 3</t>
+  </si>
+  <si>
+    <t>Unlock Auto Research</t>
+  </si>
+  <si>
+    <t>Unlock Achievements and FoS</t>
+  </si>
+  <si>
+    <t>1 Magic Bonus</t>
+  </si>
+  <si>
+    <t>1% WPS</t>
+  </si>
+  <si>
+    <t>1% WPC</t>
+  </si>
+  <si>
+    <t>1% Storage</t>
   </si>
 </sst>
 </file>
@@ -8097,7 +8139,7 @@
   </sheetPr>
   <dimension ref="A1:AL295"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD142" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AD142" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AH157" sqref="AH157"/>
     </sheetView>
   </sheetViews>
@@ -22508,24 +22550,28 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="C4:G39"/>
+  <dimension ref="A4:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" ht="12.75">
+    <row r="4" spans="1:9" ht="12.75">
+      <c r="A4" t="s">
+        <v>1235</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="12.75">
+    <row r="6" spans="1:9" ht="12.75">
       <c r="C6" s="1" t="s">
         <v>52</v>
       </c>
@@ -22541,8 +22587,17 @@
       <c r="G6" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="7" spans="3:7" ht="12.75">
+      <c r="I6" s="1" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="12.75">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1236</v>
+      </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
@@ -22553,7 +22608,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="12.75">
+    <row r="8" spans="1:9" ht="12.75">
+      <c r="B8" t="s">
+        <v>1237</v>
+      </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
@@ -22563,8 +22621,14 @@
       <c r="G8" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="3:7" ht="12.75">
+      <c r="I8" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="12.75">
+      <c r="B9" t="s">
+        <v>1244</v>
+      </c>
       <c r="C9" s="1">
         <v>3</v>
       </c>
@@ -22574,8 +22638,14 @@
       <c r="G9" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="3:7" ht="12.75">
+      <c r="I9" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="12.75">
+      <c r="B10" t="s">
+        <v>140</v>
+      </c>
       <c r="C10" s="1">
         <v>4</v>
       </c>
@@ -22585,8 +22655,14 @@
       <c r="G10" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="3:7" ht="12.75">
+      <c r="I10" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="12.75">
+      <c r="B11" t="s">
+        <v>138</v>
+      </c>
       <c r="C11" s="1">
         <v>5</v>
       </c>
@@ -22597,7 +22673,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="3:7" ht="12.75">
+    <row r="12" spans="1:9" ht="12.75">
+      <c r="B12" t="s">
+        <v>1238</v>
+      </c>
       <c r="C12" s="1">
         <v>6</v>
       </c>
@@ -22608,7 +22687,10 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="3:7" ht="12.75">
+    <row r="13" spans="1:9" ht="12.75">
+      <c r="B13" t="s">
+        <v>1239</v>
+      </c>
       <c r="C13" s="1">
         <v>7</v>
       </c>
@@ -22619,7 +22701,10 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="3:7" ht="12.75">
+    <row r="14" spans="1:9" ht="12.75">
+      <c r="B14" t="s">
+        <v>1240</v>
+      </c>
       <c r="C14" s="1">
         <v>8</v>
       </c>
@@ -22630,7 +22715,10 @@
         <v>444</v>
       </c>
     </row>
-    <row r="15" spans="3:7" ht="12.75">
+    <row r="15" spans="1:9" ht="12.75">
+      <c r="B15" t="s">
+        <v>1241</v>
+      </c>
       <c r="C15" s="1">
         <v>9</v>
       </c>
@@ -22641,7 +22729,10 @@
         <v>666</v>
       </c>
     </row>
-    <row r="16" spans="3:7" ht="12.75">
+    <row r="16" spans="1:9" ht="12.75">
+      <c r="B16" t="s">
+        <v>1242</v>
+      </c>
       <c r="C16" s="1">
         <v>10</v>
       </c>
@@ -22652,7 +22743,10 @@
         <v>700</v>
       </c>
     </row>
-    <row r="17" spans="3:7" ht="12.75">
+    <row r="17" spans="2:7" ht="12.75">
+      <c r="B17" t="s">
+        <v>1243</v>
+      </c>
       <c r="C17" s="1">
         <v>11</v>
       </c>
@@ -22663,7 +22757,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="18" spans="3:7" ht="12.75">
+    <row r="18" spans="2:7" ht="12.75">
       <c r="C18" s="1">
         <v>12</v>
       </c>
@@ -22674,7 +22768,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="19" spans="3:7" ht="12.75">
+    <row r="19" spans="2:7" ht="12.75">
       <c r="C19" s="1">
         <v>13</v>
       </c>
@@ -22685,7 +22779,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="20" spans="3:7" ht="12.75">
+    <row r="20" spans="2:7" ht="12.75">
       <c r="C20" s="1">
         <v>14</v>
       </c>
@@ -22696,7 +22790,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="3:7" ht="12.75">
+    <row r="21" spans="2:7" ht="12.75">
       <c r="C21" s="1">
         <v>15</v>
       </c>
@@ -22707,7 +22801,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="3:7" ht="12.75">
+    <row r="22" spans="2:7" ht="12.75">
       <c r="C22" s="1">
         <v>16</v>
       </c>
@@ -22718,7 +22812,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="3:7" ht="12.75">
+    <row r="23" spans="2:7" ht="12.75">
       <c r="C23" s="1">
         <v>17</v>
       </c>
@@ -22729,7 +22823,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="3:7" ht="12.75">
+    <row r="24" spans="2:7" ht="12.75">
       <c r="C24" s="1">
         <v>18</v>
       </c>
@@ -22740,7 +22834,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="3:7" ht="12.75">
+    <row r="25" spans="2:7" ht="12.75">
       <c r="C25" s="1">
         <v>19</v>
       </c>
@@ -22751,7 +22845,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="3:7" ht="12.75">
+    <row r="26" spans="2:7" ht="12.75">
       <c r="C26" s="1">
         <v>20</v>
       </c>
@@ -22762,7 +22856,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="3:7" ht="12.75">
+    <row r="27" spans="2:7" ht="12.75">
       <c r="C27" s="1">
         <v>21</v>
       </c>
@@ -22773,7 +22867,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="28" spans="3:7" ht="12.75">
+    <row r="28" spans="2:7" ht="12.75">
       <c r="C28" s="1">
         <v>22</v>
       </c>
@@ -22784,7 +22878,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="3:7" ht="12.75">
+    <row r="29" spans="2:7" ht="12.75">
       <c r="C29" s="1">
         <v>23</v>
       </c>
@@ -22795,7 +22889,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="30" spans="3:7" ht="12.75">
+    <row r="30" spans="2:7" ht="12.75">
       <c r="C30" s="1">
         <v>24</v>
       </c>
@@ -22806,7 +22900,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="3:7" ht="12.75">
+    <row r="31" spans="2:7" ht="12.75">
       <c r="C31" s="1">
         <v>25</v>
       </c>
@@ -22817,7 +22911,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="3:7" ht="12.75">
+    <row r="32" spans="2:7" ht="12.75">
       <c r="C32" s="1">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Mixed notation, Extra beavers and WC, balancing and Bug fixes
Added Mixed notation
Display separate extra beavers and WC
Balancing and new research and magic upgrades
Updated save info and other minor updates
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BEFFDB-C5B7-4B58-87B5-2FB6823E8530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EFBC34-7FB8-44C5-9661-58B5D737C5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6645" windowWidth="29040" windowHeight="17520" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -25,24 +25,11 @@
     <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="1523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3013" uniqueCount="1527">
   <si>
     <t xml:space="preserve">Tier </t>
   </si>
@@ -4631,6 +4618,18 @@
   </si>
   <si>
     <t>Have 10^26 Maple</t>
+  </si>
+  <si>
+    <t>25% Woodcamp Price</t>
+  </si>
+  <si>
+    <t>Woodcamps use 10% less wood</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>1c</t>
   </si>
 </sst>
 </file>
@@ -5410,7 +5409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Parasts" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5637,16 +5636,16 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="26.5546875" customWidth="1"/>
-    <col min="8" max="8" width="23.44140625" customWidth="1"/>
-    <col min="9" max="9" width="37.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" customWidth="1"/>
-    <col min="13" max="13" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="37.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:10" ht="13.2">
+    <row r="5" spans="2:10" ht="12.75">
       <c r="G5" s="1" t="s">
         <v>0</v>
       </c>
@@ -5657,7 +5656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="13.2">
+    <row r="6" spans="2:10" ht="12.75">
       <c r="G6" s="1">
         <v>1</v>
       </c>
@@ -5671,7 +5670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="13.2">
+    <row r="7" spans="2:10" ht="12.75">
       <c r="G7" s="1">
         <v>1</v>
       </c>
@@ -5685,7 +5684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="13.2">
+    <row r="8" spans="2:10" ht="12.75">
       <c r="G8" s="1">
         <v>1</v>
       </c>
@@ -5699,7 +5698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="13.2">
+    <row r="9" spans="2:10" ht="12.75">
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
@@ -5719,7 +5718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="13.2">
+    <row r="10" spans="2:10" ht="12.75">
       <c r="G10" s="1">
         <v>1</v>
       </c>
@@ -5733,7 +5732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="13.2">
+    <row r="11" spans="2:10" ht="12.75">
       <c r="G11" s="1">
         <v>1</v>
       </c>
@@ -5747,7 +5746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="13.2">
+    <row r="12" spans="2:10" ht="12.75">
       <c r="C12" t="s">
         <v>898</v>
       </c>
@@ -5767,7 +5766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="13.2">
+    <row r="13" spans="2:10" ht="12.75">
       <c r="B13" t="s">
         <v>81</v>
       </c>
@@ -5790,7 +5789,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="13.2">
+    <row r="14" spans="2:10" ht="12.75">
       <c r="B14" t="s">
         <v>456</v>
       </c>
@@ -5813,7 +5812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="13.2">
+    <row r="15" spans="2:10" ht="12.75">
       <c r="B15" t="s">
         <v>899</v>
       </c>
@@ -5834,7 +5833,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="13.2">
+    <row r="16" spans="2:10" ht="12.75">
       <c r="G16" s="1">
         <v>2</v>
       </c>
@@ -5848,7 +5847,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="6:10" ht="13.2">
+    <row r="17" spans="6:10" ht="12.75">
       <c r="G17" s="1">
         <v>2</v>
       </c>
@@ -5862,7 +5861,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="6:10" ht="13.2">
+    <row r="18" spans="6:10" ht="12.75">
       <c r="G18" s="1">
         <v>2</v>
       </c>
@@ -5873,7 +5872,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="6:10" ht="13.2">
+    <row r="19" spans="6:10" ht="12.75">
       <c r="G19" s="1">
         <v>2</v>
       </c>
@@ -5887,7 +5886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="6:10" ht="13.2">
+    <row r="20" spans="6:10" ht="12.75">
       <c r="G20" s="1">
         <v>3</v>
       </c>
@@ -5901,7 +5900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="6:10" ht="13.2">
+    <row r="21" spans="6:10" ht="12.75">
       <c r="G21" s="1">
         <v>3</v>
       </c>
@@ -5915,7 +5914,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="6:10" ht="13.2">
+    <row r="22" spans="6:10" ht="12.75">
       <c r="G22" s="1">
         <v>3</v>
       </c>
@@ -5929,7 +5928,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="6:10" ht="13.2">
+    <row r="23" spans="6:10" ht="12.75">
       <c r="G23" s="1">
         <v>3</v>
       </c>
@@ -5943,7 +5942,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="6:10" ht="13.2">
+    <row r="24" spans="6:10" ht="12.75">
       <c r="G24" s="1">
         <v>3</v>
       </c>
@@ -5954,7 +5953,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="6:10" ht="13.2">
+    <row r="25" spans="6:10" ht="12.75">
       <c r="G25" s="1">
         <v>3</v>
       </c>
@@ -5968,7 +5967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="6:10" ht="13.2">
+    <row r="26" spans="6:10" ht="12.75">
       <c r="G26" s="1">
         <v>3</v>
       </c>
@@ -6280,11 +6279,11 @@
       <selection activeCell="K149" sqref="K149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="4" max="4" width="57" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
-    <col min="6" max="6" width="35.88671875" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10">
@@ -8101,15 +8100,15 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="13.2">
+    <row r="2" spans="1:15" ht="12.75">
       <c r="D2" s="1" t="s">
         <v>50</v>
       </c>
@@ -8117,7 +8116,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="13.2">
+    <row r="3" spans="1:15" ht="12.75">
       <c r="C3" s="1" t="s">
         <v>52</v>
       </c>
@@ -8149,7 +8148,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="13.2">
+    <row r="4" spans="1:15" ht="12.75">
       <c r="C4" s="1">
         <v>1</v>
       </c>
@@ -8182,7 +8181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="13.2">
+    <row r="5" spans="1:15" ht="12.75">
       <c r="C5" s="1">
         <v>2</v>
       </c>
@@ -8215,7 +8214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="13.2">
+    <row r="6" spans="1:15" ht="12.75">
       <c r="C6" s="1">
         <v>3</v>
       </c>
@@ -8248,7 +8247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="13.2">
+    <row r="7" spans="1:15" ht="12.75">
       <c r="C7" s="1">
         <v>4</v>
       </c>
@@ -8281,7 +8280,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="13.2">
+    <row r="8" spans="1:15" ht="12.75">
       <c r="C8" s="1">
         <v>5</v>
       </c>
@@ -8314,7 +8313,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="13.2">
+    <row r="9" spans="1:15" ht="12.75">
       <c r="C9" s="1">
         <v>6</v>
       </c>
@@ -8347,7 +8346,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="13.2">
+    <row r="10" spans="1:15" ht="12.75">
       <c r="C10" s="1">
         <v>7</v>
       </c>
@@ -8380,7 +8379,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="13.2">
+    <row r="11" spans="1:15" ht="12.75">
       <c r="C11" s="1">
         <v>8</v>
       </c>
@@ -8413,7 +8412,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="13.2">
+    <row r="12" spans="1:15" ht="12.75">
       <c r="C12" s="1">
         <v>9</v>
       </c>
@@ -8446,7 +8445,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="13.2">
+    <row r="13" spans="1:15" ht="12.75">
       <c r="A13" s="39" t="s">
         <v>3</v>
       </c>
@@ -8482,7 +8481,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="13.2">
+    <row r="14" spans="1:15" ht="12.75">
       <c r="A14" s="35" t="s">
         <v>18</v>
       </c>
@@ -8518,7 +8517,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="13.2">
+    <row r="15" spans="1:15" ht="12.75">
       <c r="A15" s="35" t="s">
         <v>9</v>
       </c>
@@ -8554,7 +8553,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="13.2">
+    <row r="16" spans="1:15" ht="12.75">
       <c r="A16" s="35" t="s">
         <v>14</v>
       </c>
@@ -8590,7 +8589,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="13.2">
+    <row r="17" spans="1:15" ht="12.75">
       <c r="A17" s="35" t="s">
         <v>21</v>
       </c>
@@ -8626,7 +8625,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="13.2">
+    <row r="18" spans="1:15" ht="12.75">
       <c r="A18" s="35" t="s">
         <v>16</v>
       </c>
@@ -8662,7 +8661,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="13.2">
+    <row r="19" spans="1:15" ht="12.75">
       <c r="A19" s="47" t="s">
         <v>26</v>
       </c>
@@ -8670,7 +8669,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="13.2">
+    <row r="20" spans="1:15" ht="12.75">
       <c r="A20" s="35" t="s">
         <v>29</v>
       </c>
@@ -8678,7 +8677,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="13.2">
+    <row r="21" spans="1:15" ht="12.75">
       <c r="A21" s="35" t="s">
         <v>31</v>
       </c>
@@ -8686,7 +8685,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="13.2">
+    <row r="22" spans="1:15" ht="12.75">
       <c r="A22" s="35" t="s">
         <v>33</v>
       </c>
@@ -8694,7 +8693,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="13.2">
+    <row r="23" spans="1:15" ht="12.75">
       <c r="A23" s="35" t="s">
         <v>37</v>
       </c>
@@ -8702,7 +8701,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="13.2">
+    <row r="24" spans="1:15" ht="12.75">
       <c r="A24" s="35" t="s">
         <v>39</v>
       </c>
@@ -8710,7 +8709,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="13.2">
+    <row r="25" spans="1:15" ht="12.75">
       <c r="A25" s="35" t="s">
         <v>41</v>
       </c>
@@ -8718,7 +8717,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="13.2">
+    <row r="26" spans="1:15" ht="12.75">
       <c r="A26" s="35" t="s">
         <v>45</v>
       </c>
@@ -8726,7 +8725,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="13.2">
+    <row r="27" spans="1:15" ht="12.75">
       <c r="A27" s="35" t="s">
         <v>46</v>
       </c>
@@ -8734,12 +8733,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="13.2">
+    <row r="28" spans="1:15" ht="12.75">
       <c r="O28" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="13.2">
+    <row r="29" spans="1:15" ht="12.75">
       <c r="C29" s="1">
         <v>2</v>
       </c>
@@ -8772,12 +8771,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="13.2">
+    <row r="30" spans="1:15" ht="12.75">
       <c r="O30" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="13.2">
+    <row r="32" spans="1:15" ht="12.75">
       <c r="F32" s="23" t="s">
         <v>72</v>
       </c>
@@ -8787,7 +8786,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="13.2">
+    <row r="34" spans="2:12" ht="12.75">
       <c r="F34" s="23" t="s">
         <v>74</v>
       </c>
@@ -8969,40 +8968,40 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="1.6640625" customWidth="1"/>
-    <col min="5" max="5" width="4.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" customWidth="1"/>
     <col min="6" max="6" width="40" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" customWidth="1"/>
-    <col min="9" max="9" width="25.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" customWidth="1"/>
-    <col min="13" max="13" width="28.109375" customWidth="1"/>
-    <col min="14" max="14" width="19.44140625" customWidth="1"/>
-    <col min="15" max="15" width="20.88671875" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1"/>
-    <col min="17" max="17" width="18.109375" customWidth="1"/>
-    <col min="18" max="18" width="16.6640625" customWidth="1"/>
-    <col min="19" max="19" width="15.6640625" customWidth="1"/>
-    <col min="20" max="20" width="14.44140625" customWidth="1"/>
-    <col min="21" max="21" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="18.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" customWidth="1"/>
+    <col min="21" max="21" width="21.42578125" customWidth="1"/>
     <col min="22" max="22" width="26" customWidth="1"/>
-    <col min="23" max="23" width="23.5546875" customWidth="1"/>
-    <col min="24" max="24" width="23.33203125" customWidth="1"/>
-    <col min="25" max="25" width="22.109375" customWidth="1"/>
-    <col min="26" max="26" width="31.44140625" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" customWidth="1"/>
-    <col min="28" max="28" width="12.44140625" customWidth="1"/>
-    <col min="29" max="29" width="15.6640625" customWidth="1"/>
-    <col min="30" max="30" width="28.6640625" customWidth="1"/>
-    <col min="31" max="31" width="12.88671875" customWidth="1"/>
-    <col min="33" max="33" width="36.88671875" customWidth="1"/>
-    <col min="34" max="34" width="19.5546875" customWidth="1"/>
-    <col min="35" max="35" width="21.109375" customWidth="1"/>
+    <col min="23" max="23" width="23.5703125" customWidth="1"/>
+    <col min="24" max="24" width="23.28515625" customWidth="1"/>
+    <col min="25" max="25" width="22.140625" customWidth="1"/>
+    <col min="26" max="26" width="31.42578125" customWidth="1"/>
+    <col min="27" max="27" width="4.7109375" customWidth="1"/>
+    <col min="28" max="28" width="12.42578125" customWidth="1"/>
+    <col min="29" max="29" width="15.7109375" customWidth="1"/>
+    <col min="30" max="30" width="28.7109375" customWidth="1"/>
+    <col min="31" max="31" width="12.85546875" customWidth="1"/>
+    <col min="33" max="33" width="36.85546875" customWidth="1"/>
+    <col min="34" max="34" width="19.5703125" customWidth="1"/>
+    <col min="35" max="35" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75" customHeight="1">
@@ -9010,7 +9009,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="13.2">
+    <row r="2" spans="1:33" ht="12.75">
       <c r="C2" s="1" t="s">
         <v>75</v>
       </c>
@@ -9106,7 +9105,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="13.8" thickBot="1">
+    <row r="6" spans="1:33" ht="13.5" thickBot="1">
       <c r="A6" s="35" t="s">
         <v>18</v>
       </c>
@@ -9193,7 +9192,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="13.2">
+    <row r="7" spans="1:33" ht="12.75">
       <c r="A7" s="35" t="s">
         <v>9</v>
       </c>
@@ -9283,7 +9282,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="13.2">
+    <row r="8" spans="1:33" ht="12.75">
       <c r="A8" s="35" t="s">
         <v>14</v>
       </c>
@@ -9372,7 +9371,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="13.2">
+    <row r="9" spans="1:33" ht="12.75">
       <c r="A9" s="35" t="s">
         <v>21</v>
       </c>
@@ -9458,7 +9457,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="13.2">
+    <row r="10" spans="1:33" ht="12.75">
       <c r="A10" s="35" t="s">
         <v>16</v>
       </c>
@@ -9531,7 +9530,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="13.2">
+    <row r="11" spans="1:33" ht="12.75">
       <c r="A11" s="47" t="s">
         <v>26</v>
       </c>
@@ -9608,7 +9607,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="13.2">
+    <row r="12" spans="1:33" ht="12.75">
       <c r="A12" s="35" t="s">
         <v>29</v>
       </c>
@@ -9680,7 +9679,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="13.2">
+    <row r="13" spans="1:33" ht="12.75">
       <c r="A13" s="35" t="s">
         <v>31</v>
       </c>
@@ -9745,7 +9744,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="13.2">
+    <row r="14" spans="1:33" ht="12.75">
       <c r="A14" s="35" t="s">
         <v>33</v>
       </c>
@@ -9797,7 +9796,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="13.2">
+    <row r="15" spans="1:33" ht="12.75">
       <c r="A15" s="35" t="s">
         <v>37</v>
       </c>
@@ -9849,7 +9848,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="13.2">
+    <row r="16" spans="1:33" ht="12.75">
       <c r="A16" s="35" t="s">
         <v>39</v>
       </c>
@@ -9901,7 +9900,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="13.2">
+    <row r="17" spans="1:33" ht="12.75">
       <c r="A17" s="35" t="s">
         <v>41</v>
       </c>
@@ -9955,7 +9954,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="13.2">
+    <row r="18" spans="1:33" ht="12.75">
       <c r="A18" s="35" t="s">
         <v>45</v>
       </c>
@@ -10006,7 +10005,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="13.2">
+    <row r="19" spans="1:33" ht="12.75">
       <c r="A19" s="35" t="s">
         <v>46</v>
       </c>
@@ -10061,7 +10060,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="13.2">
+    <row r="20" spans="1:33" ht="12.75">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>15</v>
@@ -10108,7 +10107,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="21" spans="1:33" ht="13.2">
+    <row r="21" spans="1:33" ht="12.75">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>16</v>
@@ -10157,7 +10156,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="13.2">
+    <row r="22" spans="1:33" ht="12.75">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>17</v>
@@ -10203,7 +10202,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="13.2">
+    <row r="23" spans="1:33" ht="12.75">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
         <v>18</v>
@@ -10258,7 +10257,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="13.2">
+    <row r="24" spans="1:33" ht="12.75">
       <c r="A24" s="1"/>
       <c r="B24" s="106">
         <v>19</v>
@@ -10316,7 +10315,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="13.2">
+    <row r="25" spans="1:33" ht="12.75">
       <c r="A25" s="1"/>
       <c r="B25" s="1">
         <v>20</v>
@@ -10375,7 +10374,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="13.2">
+    <row r="26" spans="1:33" ht="12.75">
       <c r="B26" s="1">
         <v>21</v>
       </c>
@@ -10433,7 +10432,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="13.2">
+    <row r="27" spans="1:33" ht="12.75">
       <c r="B27" s="1">
         <v>22</v>
       </c>
@@ -10490,7 +10489,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="13.2">
+    <row r="28" spans="1:33" ht="12.75">
       <c r="B28" s="1">
         <v>23</v>
       </c>
@@ -10544,7 +10543,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="13.2">
+    <row r="29" spans="1:33" ht="12.75">
       <c r="B29" s="1">
         <v>24</v>
       </c>
@@ -10596,7 +10595,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="30" spans="1:33" ht="13.2">
+    <row r="30" spans="1:33" ht="12.75">
       <c r="B30" s="1">
         <v>25</v>
       </c>
@@ -10648,7 +10647,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="31" spans="1:33" ht="13.2">
+    <row r="31" spans="1:33" ht="12.75">
       <c r="B31" s="1">
         <v>26</v>
       </c>
@@ -10689,7 +10688,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="32" spans="1:33" ht="13.2">
+    <row r="32" spans="1:33" ht="12.75">
       <c r="B32" s="1">
         <v>27</v>
       </c>
@@ -10734,7 +10733,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="18" thickBot="1">
+    <row r="33" spans="1:33" ht="18.75" thickBot="1">
       <c r="B33" s="1">
         <v>28</v>
       </c>
@@ -10769,7 +10768,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="18" thickBot="1">
+    <row r="34" spans="1:33" ht="18.75" thickBot="1">
       <c r="B34" s="1">
         <v>29</v>
       </c>
@@ -10815,7 +10814,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="35" spans="1:33" ht="13.8" thickBot="1">
+    <row r="35" spans="1:33" ht="13.5" thickBot="1">
       <c r="B35" s="1">
         <v>30</v>
       </c>
@@ -10886,7 +10885,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="36" spans="1:33" ht="13.2">
+    <row r="36" spans="1:33" ht="12.75">
       <c r="B36" s="1">
         <v>31</v>
       </c>
@@ -10962,7 +10961,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="37" spans="1:33" ht="13.2">
+    <row r="37" spans="1:33" ht="12.75">
       <c r="B37" s="1">
         <v>32</v>
       </c>
@@ -11039,7 +11038,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="38" spans="1:33" ht="13.2">
+    <row r="38" spans="1:33" ht="12.75">
       <c r="B38" s="1">
         <v>33</v>
       </c>
@@ -11115,7 +11114,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="39" spans="1:33" ht="13.2">
+    <row r="39" spans="1:33" ht="12.75">
       <c r="B39" s="1">
         <v>34</v>
       </c>
@@ -11191,7 +11190,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="40" spans="1:33" ht="13.2">
+    <row r="40" spans="1:33" ht="12.75">
       <c r="A40">
         <v>1</v>
       </c>
@@ -11266,7 +11265,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="41" spans="1:33" ht="13.2">
+    <row r="41" spans="1:33" ht="12.75">
       <c r="A41">
         <v>4</v>
       </c>
@@ -11339,7 +11338,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="42" spans="1:33" ht="13.2">
+    <row r="42" spans="1:33" ht="12.75">
       <c r="A42">
         <v>7</v>
       </c>
@@ -11414,7 +11413,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="43" spans="1:33" ht="13.2">
+    <row r="43" spans="1:33" ht="12.75">
       <c r="A43">
         <v>10</v>
       </c>
@@ -11481,7 +11480,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="44" spans="1:33" ht="13.2">
+    <row r="44" spans="1:33" ht="12.75">
       <c r="A44">
         <v>13</v>
       </c>
@@ -11548,7 +11547,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="45" spans="1:33" ht="13.2">
+    <row r="45" spans="1:33" ht="12.75">
       <c r="A45">
         <v>16</v>
       </c>
@@ -11616,7 +11615,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="46" spans="1:33" ht="13.2">
+    <row r="46" spans="1:33" ht="12.75">
       <c r="A46">
         <v>19</v>
       </c>
@@ -11681,7 +11680,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="47" spans="1:33" ht="13.2">
+    <row r="47" spans="1:33" ht="12.75">
       <c r="A47">
         <v>22</v>
       </c>
@@ -11747,7 +11746,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="48" spans="1:33" ht="13.2">
+    <row r="48" spans="1:33" ht="12.75">
       <c r="A48">
         <v>25</v>
       </c>
@@ -11810,7 +11809,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="49" spans="1:33" ht="13.2">
+    <row r="49" spans="1:33" ht="12.75">
       <c r="A49">
         <v>28</v>
       </c>
@@ -11877,7 +11876,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="50" spans="1:33" ht="13.2">
+    <row r="50" spans="1:33" ht="12.75">
       <c r="A50">
         <v>31</v>
       </c>
@@ -11944,7 +11943,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="51" spans="1:33" ht="13.2">
+    <row r="51" spans="1:33" ht="12.75">
       <c r="A51">
         <v>34</v>
       </c>
@@ -12008,7 +12007,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="52" spans="1:33" ht="13.2">
+    <row r="52" spans="1:33" ht="12.75">
       <c r="A52">
         <v>37</v>
       </c>
@@ -12085,7 +12084,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="53" spans="1:33" ht="13.2">
+    <row r="53" spans="1:33" ht="12.75">
       <c r="A53">
         <v>40</v>
       </c>
@@ -12153,7 +12152,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="54" spans="1:33" ht="13.2">
+    <row r="54" spans="1:33" ht="12.75">
       <c r="A54">
         <v>43</v>
       </c>
@@ -12218,7 +12217,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="55" spans="1:33" ht="13.2">
+    <row r="55" spans="1:33" ht="12.75">
       <c r="A55">
         <v>46</v>
       </c>
@@ -12292,7 +12291,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="56" spans="1:33" ht="13.2">
+    <row r="56" spans="1:33" ht="12.75">
       <c r="A56">
         <v>49</v>
       </c>
@@ -12357,7 +12356,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="57" spans="1:33" ht="13.2">
+    <row r="57" spans="1:33" ht="12.75">
       <c r="A57">
         <v>52</v>
       </c>
@@ -12425,7 +12424,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="58" spans="1:33" ht="13.2">
+    <row r="58" spans="1:33" ht="12.75">
       <c r="A58">
         <v>55</v>
       </c>
@@ -12487,7 +12486,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="59" spans="1:33" ht="13.2">
+    <row r="59" spans="1:33" ht="12.75">
       <c r="A59">
         <v>58</v>
       </c>
@@ -12552,7 +12551,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="60" spans="1:33" ht="13.2">
+    <row r="60" spans="1:33" ht="12.75">
       <c r="A60">
         <v>61</v>
       </c>
@@ -12613,7 +12612,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="61" spans="1:33" ht="13.2">
+    <row r="61" spans="1:33" ht="12.75">
       <c r="A61">
         <v>64</v>
       </c>
@@ -12676,7 +12675,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="62" spans="1:33" ht="13.2">
+    <row r="62" spans="1:33" ht="12.75">
       <c r="A62">
         <v>9887654321</v>
       </c>
@@ -12737,7 +12736,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="63" spans="1:33" ht="13.2">
+    <row r="63" spans="1:33" ht="12.75">
       <c r="B63" s="1">
         <v>58</v>
       </c>
@@ -12795,7 +12794,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="64" spans="1:33" ht="13.2">
+    <row r="64" spans="1:33" ht="12.75">
       <c r="B64" s="1">
         <v>59</v>
       </c>
@@ -12851,7 +12850,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="65" spans="2:33" ht="13.2">
+    <row r="65" spans="2:33" ht="12.75">
       <c r="B65" s="1">
         <v>60</v>
       </c>
@@ -12906,7 +12905,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="66" spans="2:33" ht="13.2">
+    <row r="66" spans="2:33" ht="12.75">
       <c r="B66" s="1">
         <v>61</v>
       </c>
@@ -12962,7 +12961,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="67" spans="2:33" ht="13.2">
+    <row r="67" spans="2:33" ht="12.75">
       <c r="B67" s="1">
         <v>62</v>
       </c>
@@ -13018,7 +13017,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="68" spans="2:33" ht="13.2">
+    <row r="68" spans="2:33" ht="12.75">
       <c r="B68" s="1">
         <v>63</v>
       </c>
@@ -13074,7 +13073,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="69" spans="2:33" ht="13.2">
+    <row r="69" spans="2:33" ht="12.75">
       <c r="B69" s="1">
         <v>64</v>
       </c>
@@ -13127,7 +13126,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="70" spans="2:33" ht="13.2">
+    <row r="70" spans="2:33" ht="12.75">
       <c r="B70" s="1">
         <v>65</v>
       </c>
@@ -13183,7 +13182,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="71" spans="2:33" ht="13.2">
+    <row r="71" spans="2:33" ht="12.75">
       <c r="B71" s="1">
         <v>66</v>
       </c>
@@ -13235,7 +13234,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="72" spans="2:33" ht="13.2">
+    <row r="72" spans="2:33" ht="12.75">
       <c r="B72" s="1">
         <v>67</v>
       </c>
@@ -13287,7 +13286,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="73" spans="2:33" ht="13.2">
+    <row r="73" spans="2:33" ht="12.75">
       <c r="B73" s="1">
         <v>68</v>
       </c>
@@ -13338,7 +13337,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="74" spans="2:33" ht="13.2">
+    <row r="74" spans="2:33" ht="12.75">
       <c r="B74" s="1">
         <v>69</v>
       </c>
@@ -13389,7 +13388,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="75" spans="2:33" ht="13.2">
+    <row r="75" spans="2:33" ht="12.75">
       <c r="B75" s="1">
         <v>70</v>
       </c>
@@ -13440,7 +13439,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="76" spans="2:33" ht="13.2">
+    <row r="76" spans="2:33" ht="12.75">
       <c r="B76" s="1">
         <v>71</v>
       </c>
@@ -13491,7 +13490,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="77" spans="2:33" ht="13.2">
+    <row r="77" spans="2:33" ht="12.75">
       <c r="B77" s="1">
         <v>72</v>
       </c>
@@ -13546,7 +13545,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="78" spans="2:33" ht="13.2">
+    <row r="78" spans="2:33" ht="12.75">
       <c r="B78" s="106">
         <v>73</v>
       </c>
@@ -13598,7 +13597,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="79" spans="2:33" ht="13.2">
+    <row r="79" spans="2:33" ht="12.75">
       <c r="B79" s="1">
         <v>74</v>
       </c>
@@ -13650,7 +13649,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="80" spans="2:33" ht="13.2">
+    <row r="80" spans="2:33" ht="12.75">
       <c r="B80" s="1">
         <v>75</v>
       </c>
@@ -13702,7 +13701,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="81" spans="2:35" ht="13.2">
+    <row r="81" spans="2:35" ht="12.75">
       <c r="B81" s="1">
         <v>76</v>
       </c>
@@ -13755,7 +13754,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="82" spans="2:35" ht="13.2">
+    <row r="82" spans="2:35" ht="12.75">
       <c r="B82" s="1">
         <v>77</v>
       </c>
@@ -13805,7 +13804,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="83" spans="2:35" ht="13.2">
+    <row r="83" spans="2:35" ht="12.75">
       <c r="B83" s="1">
         <v>78</v>
       </c>
@@ -13857,7 +13856,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="84" spans="2:35" ht="13.2">
+    <row r="84" spans="2:35" ht="12.75">
       <c r="B84" s="1">
         <v>79</v>
       </c>
@@ -13907,7 +13906,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="85" spans="2:35" ht="13.2">
+    <row r="85" spans="2:35" ht="12.75">
       <c r="B85" s="1">
         <v>80</v>
       </c>
@@ -13957,7 +13956,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="86" spans="2:35" ht="13.2">
+    <row r="86" spans="2:35" ht="12.75">
       <c r="B86" s="1">
         <v>81</v>
       </c>
@@ -14006,7 +14005,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="87" spans="2:35" ht="13.2">
+    <row r="87" spans="2:35" ht="12.75">
       <c r="B87" s="1">
         <v>82</v>
       </c>
@@ -14074,7 +14073,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="88" spans="2:35" ht="13.2">
+    <row r="88" spans="2:35" ht="12.75">
       <c r="B88" s="1">
         <v>83</v>
       </c>
@@ -14124,7 +14123,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="89" spans="2:35" ht="13.2">
+    <row r="89" spans="2:35" ht="12.75">
       <c r="B89" s="1">
         <v>84</v>
       </c>
@@ -14159,7 +14158,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="90" spans="2:35" ht="13.2">
+    <row r="90" spans="2:35" ht="12.75">
       <c r="B90" s="1">
         <v>85</v>
       </c>
@@ -14207,7 +14206,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="91" spans="2:35" ht="13.2">
+    <row r="91" spans="2:35" ht="12.75">
       <c r="B91" s="1">
         <v>86</v>
       </c>
@@ -14255,7 +14254,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="92" spans="2:35" ht="13.2">
+    <row r="92" spans="2:35" ht="12.75">
       <c r="B92" s="1">
         <v>87</v>
       </c>
@@ -14304,7 +14303,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="93" spans="2:35" ht="13.2">
+    <row r="93" spans="2:35" ht="12.75">
       <c r="B93" s="1">
         <v>88</v>
       </c>
@@ -14352,7 +14351,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="94" spans="2:35" ht="13.2">
+    <row r="94" spans="2:35" ht="12.75">
       <c r="B94" s="1">
         <v>89</v>
       </c>
@@ -14404,7 +14403,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="95" spans="2:35" ht="13.2">
+    <row r="95" spans="2:35" ht="12.75">
       <c r="B95" s="1">
         <v>90</v>
       </c>
@@ -14452,7 +14451,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="96" spans="2:35" ht="13.2">
+    <row r="96" spans="2:35" ht="12.75">
       <c r="B96" s="106">
         <v>91</v>
       </c>
@@ -14502,7 +14501,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="97" spans="2:33" ht="13.2">
+    <row r="97" spans="2:33" ht="12.75">
       <c r="B97" s="1">
         <v>92</v>
       </c>
@@ -14550,7 +14549,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="98" spans="2:33" ht="13.2">
+    <row r="98" spans="2:33" ht="12.75">
       <c r="B98" s="1">
         <v>93</v>
       </c>
@@ -14599,7 +14598,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="99" spans="2:33" ht="13.2">
+    <row r="99" spans="2:33" ht="12.75">
       <c r="B99" s="1">
         <v>94</v>
       </c>
@@ -14648,7 +14647,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="100" spans="2:33" ht="13.2">
+    <row r="100" spans="2:33" ht="12.75">
       <c r="B100" s="1">
         <v>95</v>
       </c>
@@ -14697,7 +14696,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="101" spans="2:33" ht="13.2">
+    <row r="101" spans="2:33" ht="12.75">
       <c r="B101" s="1">
         <v>96</v>
       </c>
@@ -14746,7 +14745,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="102" spans="2:33" ht="13.2">
+    <row r="102" spans="2:33" ht="12.75">
       <c r="B102" s="1">
         <v>97</v>
       </c>
@@ -14795,7 +14794,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="103" spans="2:33" ht="13.2">
+    <row r="103" spans="2:33" ht="12.75">
       <c r="B103" s="1">
         <v>98</v>
       </c>
@@ -14828,7 +14827,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="104" spans="2:33" ht="13.2">
+    <row r="104" spans="2:33" ht="12.75">
       <c r="B104" s="1">
         <v>99</v>
       </c>
@@ -14861,7 +14860,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="105" spans="2:33" ht="13.2">
+    <row r="105" spans="2:33" ht="12.75">
       <c r="B105" s="1">
         <v>100</v>
       </c>
@@ -14893,7 +14892,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="106" spans="2:33" ht="13.2">
+    <row r="106" spans="2:33" ht="12.75">
       <c r="B106" s="1">
         <v>101</v>
       </c>
@@ -14926,7 +14925,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="107" spans="2:33" ht="13.2">
+    <row r="107" spans="2:33" ht="12.75">
       <c r="B107" s="1">
         <v>102</v>
       </c>
@@ -14958,7 +14957,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="108" spans="2:33" ht="13.2">
+    <row r="108" spans="2:33" ht="12.75">
       <c r="B108" s="1">
         <v>103</v>
       </c>
@@ -14994,7 +14993,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="109" spans="2:33" ht="13.2">
+    <row r="109" spans="2:33" ht="12.75">
       <c r="B109" s="1">
         <v>104</v>
       </c>
@@ -15042,7 +15041,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="110" spans="2:33" ht="13.2">
+    <row r="110" spans="2:33" ht="12.75">
       <c r="B110" s="1">
         <v>105</v>
       </c>
@@ -15074,7 +15073,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="111" spans="2:33" ht="13.2">
+    <row r="111" spans="2:33" ht="12.75">
       <c r="B111" s="1">
         <v>106</v>
       </c>
@@ -15107,7 +15106,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="112" spans="2:33" ht="13.2">
+    <row r="112" spans="2:33" ht="12.75">
       <c r="B112" s="1">
         <v>107</v>
       </c>
@@ -15147,7 +15146,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="113" spans="2:38" ht="13.2">
+    <row r="113" spans="2:38" ht="12.75">
       <c r="B113" s="1">
         <v>108</v>
       </c>
@@ -15214,7 +15213,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="114" spans="2:38" ht="13.2">
+    <row r="114" spans="2:38" ht="12.75">
       <c r="B114" s="106">
         <v>109</v>
       </c>
@@ -15278,7 +15277,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="115" spans="2:38" ht="13.2">
+    <row r="115" spans="2:38" ht="12.75">
       <c r="B115" s="1">
         <v>110</v>
       </c>
@@ -15339,7 +15338,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="116" spans="2:38" ht="13.2">
+    <row r="116" spans="2:38" ht="12.75">
       <c r="B116" s="1">
         <v>111</v>
       </c>
@@ -15406,7 +15405,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="2:38" ht="13.2">
+    <row r="117" spans="2:38" ht="12.75">
       <c r="B117" s="1">
         <v>112</v>
       </c>
@@ -15464,7 +15463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="2:38" ht="13.2">
+    <row r="118" spans="2:38" ht="12.75">
       <c r="B118" s="1">
         <v>113</v>
       </c>
@@ -15521,7 +15520,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="2:38" ht="13.2">
+    <row r="119" spans="2:38" ht="12.75">
       <c r="B119" s="1">
         <v>114</v>
       </c>
@@ -15580,7 +15579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="2:38" ht="13.2">
+    <row r="120" spans="2:38" ht="12.75">
       <c r="B120" s="1">
         <v>115</v>
       </c>
@@ -15633,7 +15632,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="121" spans="2:38" ht="13.2">
+    <row r="121" spans="2:38" ht="12.75">
       <c r="B121" s="1">
         <v>116</v>
       </c>
@@ -15686,7 +15685,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="122" spans="2:38" ht="13.2">
+    <row r="122" spans="2:38" ht="12.75">
       <c r="B122" s="1">
         <v>117</v>
       </c>
@@ -15739,7 +15738,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="123" spans="2:38" ht="13.2">
+    <row r="123" spans="2:38" ht="12.75">
       <c r="B123" s="1">
         <v>118</v>
       </c>
@@ -15794,7 +15793,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="124" spans="2:38" ht="13.2">
+    <row r="124" spans="2:38" ht="12.75">
       <c r="B124" s="1">
         <v>119</v>
       </c>
@@ -15847,7 +15846,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="125" spans="2:38" ht="13.2">
+    <row r="125" spans="2:38" ht="12.75">
       <c r="B125" s="1">
         <v>120</v>
       </c>
@@ -15900,7 +15899,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="126" spans="2:38" ht="13.2">
+    <row r="126" spans="2:38" ht="12.75">
       <c r="B126" s="1">
         <v>121</v>
       </c>
@@ -15952,7 +15951,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="127" spans="2:38" ht="13.2">
+    <row r="127" spans="2:38" ht="12.75">
       <c r="B127" s="1">
         <v>122</v>
       </c>
@@ -16007,7 +16006,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="128" spans="2:38" ht="13.2">
+    <row r="128" spans="2:38" ht="12.75">
       <c r="B128" s="1">
         <v>123</v>
       </c>
@@ -16060,7 +16059,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="129" spans="2:38" ht="13.2">
+    <row r="129" spans="2:38" ht="12.75">
       <c r="B129" s="1">
         <v>124</v>
       </c>
@@ -16114,7 +16113,7 @@
       </c>
       <c r="AL129" s="74"/>
     </row>
-    <row r="130" spans="2:38" ht="13.2">
+    <row r="130" spans="2:38" ht="12.75">
       <c r="B130" s="1">
         <v>125</v>
       </c>
@@ -16169,7 +16168,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="131" spans="2:38" ht="13.2">
+    <row r="131" spans="2:38" ht="12.75">
       <c r="B131" s="1">
         <v>126</v>
       </c>
@@ -16224,7 +16223,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="132" spans="2:38" ht="13.2">
+    <row r="132" spans="2:38" ht="12.75">
       <c r="B132" s="106">
         <v>127</v>
       </c>
@@ -16281,7 +16280,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="133" spans="2:38" ht="13.2">
+    <row r="133" spans="2:38" ht="12.75">
       <c r="B133" s="1">
         <v>128</v>
       </c>
@@ -16337,7 +16336,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="134" spans="2:38" ht="13.2">
+    <row r="134" spans="2:38" ht="12.75">
       <c r="B134" s="1">
         <v>129</v>
       </c>
@@ -16393,7 +16392,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="135" spans="2:38" ht="13.2">
+    <row r="135" spans="2:38" ht="12.75">
       <c r="B135" s="1">
         <v>130</v>
       </c>
@@ -16446,7 +16445,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="136" spans="2:38" ht="13.2">
+    <row r="136" spans="2:38" ht="12.75">
       <c r="B136" s="1">
         <v>131</v>
       </c>
@@ -16502,7 +16501,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="137" spans="2:38" ht="13.2">
+    <row r="137" spans="2:38" ht="12.75">
       <c r="B137" s="1">
         <v>132</v>
       </c>
@@ -16554,7 +16553,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="138" spans="2:38" ht="13.2">
+    <row r="138" spans="2:38" ht="12.75">
       <c r="B138" s="1">
         <v>133</v>
       </c>
@@ -16607,7 +16606,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="139" spans="2:38" ht="13.2">
+    <row r="139" spans="2:38" ht="12.75">
       <c r="B139" s="1">
         <v>134</v>
       </c>
@@ -16660,7 +16659,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="140" spans="2:38" ht="13.2">
+    <row r="140" spans="2:38" ht="12.75">
       <c r="B140" s="1">
         <v>135</v>
       </c>
@@ -16713,7 +16712,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="141" spans="2:38" ht="13.2">
+    <row r="141" spans="2:38" ht="12.75">
       <c r="B141" s="1">
         <v>136</v>
       </c>
@@ -16765,7 +16764,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="142" spans="2:38" ht="13.2">
+    <row r="142" spans="2:38" ht="12.75">
       <c r="B142" s="1">
         <v>137</v>
       </c>
@@ -16817,7 +16816,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="143" spans="2:38" ht="13.2">
+    <row r="143" spans="2:38" ht="12.75">
       <c r="B143" s="1">
         <v>138</v>
       </c>
@@ -16866,7 +16865,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="144" spans="2:38" ht="13.2">
+    <row r="144" spans="2:38" ht="12.75">
       <c r="B144" s="1">
         <v>139</v>
       </c>
@@ -16916,7 +16915,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="145" spans="2:38" ht="13.2">
+    <row r="145" spans="2:38" ht="12.75">
       <c r="B145" s="1">
         <v>140</v>
       </c>
@@ -16971,7 +16970,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="146" spans="2:38" ht="13.2">
+    <row r="146" spans="2:38" ht="12.75">
       <c r="B146" s="1">
         <v>141</v>
       </c>
@@ -17021,7 +17020,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="147" spans="2:38" ht="13.2">
+    <row r="147" spans="2:38" ht="12.75">
       <c r="B147" s="1">
         <v>142</v>
       </c>
@@ -17073,7 +17072,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="148" spans="2:38" ht="13.2">
+    <row r="148" spans="2:38" ht="12.75">
       <c r="B148" s="1">
         <v>143</v>
       </c>
@@ -17125,7 +17124,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="149" spans="2:38" ht="13.2">
+    <row r="149" spans="2:38" ht="12.75">
       <c r="B149" s="1">
         <v>144</v>
       </c>
@@ -17183,7 +17182,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="150" spans="2:38" ht="13.2">
+    <row r="150" spans="2:38" ht="12.75">
       <c r="B150" s="106">
         <v>145</v>
       </c>
@@ -17236,7 +17235,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="151" spans="2:38" ht="13.2">
+    <row r="151" spans="2:38" ht="12.75">
       <c r="B151" s="1">
         <v>146</v>
       </c>
@@ -17291,7 +17290,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="152" spans="2:38" ht="13.2">
+    <row r="152" spans="2:38" ht="12.75">
       <c r="B152" s="1">
         <v>147</v>
       </c>
@@ -17343,7 +17342,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="153" spans="2:38" ht="13.2">
+    <row r="153" spans="2:38" ht="12.75">
       <c r="B153" s="1">
         <v>148</v>
       </c>
@@ -17398,7 +17397,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="154" spans="2:38" ht="13.2">
+    <row r="154" spans="2:38" ht="12.75">
       <c r="B154" s="1">
         <v>149</v>
       </c>
@@ -17448,7 +17447,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="155" spans="2:38" ht="13.2">
+    <row r="155" spans="2:38" ht="12.75">
       <c r="B155" s="1">
         <v>150</v>
       </c>
@@ -17501,7 +17500,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="156" spans="2:38" ht="13.2">
+    <row r="156" spans="2:38" ht="12.75">
       <c r="B156" s="1">
         <v>151</v>
       </c>
@@ -17553,7 +17552,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="157" spans="2:38" ht="13.2">
+    <row r="157" spans="2:38" ht="12.75">
       <c r="B157" s="1">
         <v>152</v>
       </c>
@@ -17605,7 +17604,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="158" spans="2:38" ht="13.2">
+    <row r="158" spans="2:38" ht="12.75">
       <c r="B158" s="1">
         <v>153</v>
       </c>
@@ -17655,7 +17654,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="159" spans="2:38" ht="13.2">
+    <row r="159" spans="2:38" ht="12.75">
       <c r="B159" s="1">
         <v>154</v>
       </c>
@@ -17704,7 +17703,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="160" spans="2:38" ht="13.2">
+    <row r="160" spans="2:38" ht="12.75">
       <c r="B160" s="1">
         <v>155</v>
       </c>
@@ -17753,7 +17752,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="161" spans="2:37" ht="13.2">
+    <row r="161" spans="2:37" ht="12.75">
       <c r="B161" s="1">
         <v>156</v>
       </c>
@@ -17803,7 +17802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="2:37" ht="13.2">
+    <row r="162" spans="2:37" ht="12.75">
       <c r="B162" s="1">
         <v>157</v>
       </c>
@@ -17850,7 +17849,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="163" spans="2:37" ht="13.2">
+    <row r="163" spans="2:37" ht="12.75">
       <c r="B163" s="1">
         <v>158</v>
       </c>
@@ -17899,7 +17898,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="164" spans="2:37" ht="13.2">
+    <row r="164" spans="2:37" ht="12.75">
       <c r="B164" s="1">
         <v>159</v>
       </c>
@@ -17948,7 +17947,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="165" spans="2:37" ht="13.2">
+    <row r="165" spans="2:37" ht="12.75">
       <c r="B165" s="1">
         <v>160</v>
       </c>
@@ -17997,7 +17996,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="166" spans="2:37" ht="13.2">
+    <row r="166" spans="2:37" ht="12.75">
       <c r="B166" s="1">
         <v>161</v>
       </c>
@@ -18035,7 +18034,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="167" spans="2:37" ht="13.2">
+    <row r="167" spans="2:37" ht="12.75">
       <c r="B167" s="1">
         <v>162</v>
       </c>
@@ -18075,7 +18074,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="168" spans="2:37" ht="13.2">
+    <row r="168" spans="2:37" ht="12.75">
       <c r="B168" s="106">
         <v>163</v>
       </c>
@@ -18114,7 +18113,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="169" spans="2:37" ht="13.2">
+    <row r="169" spans="2:37" ht="12.75">
       <c r="B169" s="1">
         <v>164</v>
       </c>
@@ -18152,7 +18151,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="170" spans="2:37" ht="13.2">
+    <row r="170" spans="2:37" ht="12.75">
       <c r="B170" s="1">
         <v>165</v>
       </c>
@@ -18192,7 +18191,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="171" spans="2:37" ht="13.2">
+    <row r="171" spans="2:37" ht="12.75">
       <c r="B171" s="1">
         <v>166</v>
       </c>
@@ -18229,7 +18228,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="172" spans="2:37" ht="13.2">
+    <row r="172" spans="2:37" ht="12.75">
       <c r="B172" s="1">
         <v>167</v>
       </c>
@@ -18266,7 +18265,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="173" spans="2:37" ht="13.2">
+    <row r="173" spans="2:37" ht="12.75">
       <c r="B173" s="1">
         <v>168</v>
       </c>
@@ -21834,13 +21833,13 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="6" max="6" width="38.88671875" customWidth="1"/>
-    <col min="9" max="9" width="26.88671875" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:12" ht="13.2">
+    <row r="2" spans="3:12" ht="12.75">
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
@@ -21850,7 +21849,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="4" spans="3:12" ht="13.2">
+    <row r="4" spans="3:12" ht="12.75">
       <c r="C4" s="1" t="s">
         <v>52</v>
       </c>
@@ -21879,7 +21878,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="5" spans="3:12" ht="13.2">
+    <row r="5" spans="3:12" ht="12.75">
       <c r="C5" s="1">
         <v>1</v>
       </c>
@@ -21902,7 +21901,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="6" spans="3:12" ht="13.2">
+    <row r="6" spans="3:12" ht="12.75">
       <c r="C6" s="1">
         <v>2</v>
       </c>
@@ -21919,7 +21918,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="7" spans="3:12" ht="13.2">
+    <row r="7" spans="3:12" ht="12.75">
       <c r="C7" s="1">
         <v>3</v>
       </c>
@@ -21933,7 +21932,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="3:12" ht="13.2">
+    <row r="8" spans="3:12" ht="12.75">
       <c r="C8" s="1">
         <v>4</v>
       </c>
@@ -21947,7 +21946,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="9" spans="3:12" ht="13.2">
+    <row r="9" spans="3:12" ht="12.75">
       <c r="C9" s="1">
         <v>5</v>
       </c>
@@ -21961,7 +21960,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="10" spans="3:12" ht="13.2">
+    <row r="10" spans="3:12" ht="12.75">
       <c r="C10" s="1">
         <v>6</v>
       </c>
@@ -21978,7 +21977,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="11" spans="3:12" ht="13.2">
+    <row r="11" spans="3:12" ht="12.75">
       <c r="C11" s="1">
         <v>7</v>
       </c>
@@ -21995,7 +21994,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="12" spans="3:12" ht="13.2">
+    <row r="12" spans="3:12" ht="12.75">
       <c r="C12" s="1">
         <v>8</v>
       </c>
@@ -22009,7 +22008,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="13" spans="3:12" ht="13.2">
+    <row r="13" spans="3:12" ht="12.75">
       <c r="C13" s="1">
         <v>9</v>
       </c>
@@ -22023,7 +22022,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="14" spans="3:12" ht="13.2">
+    <row r="14" spans="3:12" ht="12.75">
       <c r="C14" s="1">
         <v>10</v>
       </c>
@@ -22040,7 +22039,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="15" spans="3:12" ht="13.2">
+    <row r="15" spans="3:12" ht="12.75">
       <c r="C15" s="1">
         <v>11</v>
       </c>
@@ -22057,7 +22056,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="16" spans="3:12" ht="13.2">
+    <row r="16" spans="3:12" ht="12.75">
       <c r="C16" s="1">
         <v>12</v>
       </c>
@@ -22074,7 +22073,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="3:9" ht="13.2">
+    <row r="17" spans="3:9" ht="12.75">
       <c r="C17" s="1">
         <v>13</v>
       </c>
@@ -22088,7 +22087,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="18" spans="3:9" ht="13.2">
+    <row r="18" spans="3:9" ht="12.75">
       <c r="C18" s="1">
         <v>14</v>
       </c>
@@ -22102,7 +22101,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="19" spans="3:9" ht="13.2">
+    <row r="19" spans="3:9" ht="12.75">
       <c r="C19" s="1">
         <v>15</v>
       </c>
@@ -22116,7 +22115,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="20" spans="3:9" ht="13.2">
+    <row r="20" spans="3:9" ht="12.75">
       <c r="C20" s="1">
         <v>16</v>
       </c>
@@ -22130,7 +22129,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="21" spans="3:9" ht="13.2">
+    <row r="21" spans="3:9" ht="12.75">
       <c r="C21" s="1">
         <v>17</v>
       </c>
@@ -22144,7 +22143,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="22" spans="3:9" ht="13.2">
+    <row r="22" spans="3:9" ht="12.75">
       <c r="C22" s="1">
         <v>18</v>
       </c>
@@ -22158,7 +22157,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="23" spans="3:9" ht="13.2">
+    <row r="23" spans="3:9" ht="12.75">
       <c r="C23" s="1">
         <v>19</v>
       </c>
@@ -22169,7 +22168,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="3:9" ht="13.2">
+    <row r="24" spans="3:9" ht="12.75">
       <c r="C24" s="1">
         <v>20</v>
       </c>
@@ -22183,7 +22182,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="25" spans="3:9" ht="13.2">
+    <row r="25" spans="3:9" ht="12.75">
       <c r="C25" s="1">
         <v>21</v>
       </c>
@@ -22194,7 +22193,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="3:9" ht="13.2">
+    <row r="26" spans="3:9" ht="12.75">
       <c r="C26" s="1">
         <v>22</v>
       </c>
@@ -22206,7 +22205,7 @@
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="3:9" ht="13.2">
+    <row r="27" spans="3:9" ht="12.75">
       <c r="C27" s="1">
         <v>23</v>
       </c>
@@ -22220,7 +22219,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="28" spans="3:9" ht="13.2">
+    <row r="28" spans="3:9" ht="12.75">
       <c r="C28" s="1">
         <v>24</v>
       </c>
@@ -22234,7 +22233,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="29" spans="3:9" ht="13.2">
+    <row r="29" spans="3:9" ht="12.75">
       <c r="C29" s="1">
         <v>25</v>
       </c>
@@ -22248,7 +22247,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="30" spans="3:9" ht="13.2">
+    <row r="30" spans="3:9" ht="12.75">
       <c r="C30" s="1">
         <v>26</v>
       </c>
@@ -22262,7 +22261,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="31" spans="3:9" ht="13.2">
+    <row r="31" spans="3:9" ht="12.75">
       <c r="C31" s="1">
         <v>27</v>
       </c>
@@ -22276,7 +22275,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="32" spans="3:9" ht="13.2">
+    <row r="32" spans="3:9" ht="12.75">
       <c r="C32" s="1">
         <v>28</v>
       </c>
@@ -22291,7 +22290,7 @@
       </c>
       <c r="I32" s="26"/>
     </row>
-    <row r="33" spans="3:9" ht="13.2">
+    <row r="33" spans="3:9" ht="12.75">
       <c r="C33" s="1">
         <v>29</v>
       </c>
@@ -22306,7 +22305,7 @@
       </c>
       <c r="I33" s="27"/>
     </row>
-    <row r="34" spans="3:9" ht="13.2">
+    <row r="34" spans="3:9" ht="12.75">
       <c r="C34" s="1">
         <v>30</v>
       </c>
@@ -22321,7 +22320,7 @@
       </c>
       <c r="I34" s="27"/>
     </row>
-    <row r="35" spans="3:9" ht="13.2">
+    <row r="35" spans="3:9" ht="12.75">
       <c r="C35" s="1">
         <v>31</v>
       </c>
@@ -22336,7 +22335,7 @@
       </c>
       <c r="I35" s="27"/>
     </row>
-    <row r="36" spans="3:9" ht="13.2">
+    <row r="36" spans="3:9" ht="12.75">
       <c r="C36" s="1">
         <v>32</v>
       </c>
@@ -22353,7 +22352,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="3:9" ht="13.2">
+    <row r="37" spans="3:9" ht="12.75">
       <c r="C37" s="1">
         <v>33</v>
       </c>
@@ -22370,7 +22369,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="3:9" ht="13.2">
+    <row r="38" spans="3:9" ht="12.75">
       <c r="C38" s="1">
         <v>34</v>
       </c>
@@ -22387,7 +22386,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="3:9" ht="13.2">
+    <row r="39" spans="3:9" ht="12.75">
       <c r="C39" s="1">
         <v>35</v>
       </c>
@@ -22404,7 +22403,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="40" spans="3:9" ht="13.2">
+    <row r="40" spans="3:9" ht="12.75">
       <c r="C40" s="1">
         <v>36</v>
       </c>
@@ -22421,7 +22420,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="3:9" ht="13.2">
+    <row r="41" spans="3:9" ht="12.75">
       <c r="C41" s="1">
         <v>37</v>
       </c>
@@ -22438,7 +22437,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="42" spans="3:9" ht="13.2">
+    <row r="42" spans="3:9" ht="12.75">
       <c r="C42" s="1">
         <v>38</v>
       </c>
@@ -22455,7 +22454,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="43" spans="3:9" ht="13.2">
+    <row r="43" spans="3:9" ht="12.75">
       <c r="C43" s="1">
         <v>39</v>
       </c>
@@ -22472,7 +22471,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="44" spans="3:9" ht="13.2">
+    <row r="44" spans="3:9" ht="12.75">
       <c r="C44" s="1">
         <v>40</v>
       </c>
@@ -22489,7 +22488,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="45" spans="3:9" ht="13.2">
+    <row r="45" spans="3:9" ht="12.75">
       <c r="C45" s="1">
         <v>41</v>
       </c>
@@ -22506,7 +22505,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="46" spans="3:9" ht="13.2">
+    <row r="46" spans="3:9" ht="12.75">
       <c r="C46" s="1">
         <v>42</v>
       </c>
@@ -22523,7 +22522,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="47" spans="3:9" ht="13.2">
+    <row r="47" spans="3:9" ht="12.75">
       <c r="C47" s="1">
         <v>43</v>
       </c>
@@ -22540,7 +22539,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="48" spans="3:9" ht="13.2">
+    <row r="48" spans="3:9" ht="12.75">
       <c r="C48" s="1">
         <v>44</v>
       </c>
@@ -22557,7 +22556,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="49" spans="3:9" ht="13.2">
+    <row r="49" spans="3:9" ht="12.75">
       <c r="C49" s="1">
         <v>45</v>
       </c>
@@ -22574,7 +22573,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="50" spans="3:9" ht="13.2">
+    <row r="50" spans="3:9" ht="12.75">
       <c r="C50" s="1">
         <v>46</v>
       </c>
@@ -22591,7 +22590,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="51" spans="3:9" ht="13.2">
+    <row r="51" spans="3:9" ht="12.75">
       <c r="C51" s="1">
         <v>47</v>
       </c>
@@ -22608,7 +22607,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="52" spans="3:9" ht="13.2">
+    <row r="52" spans="3:9" ht="12.75">
       <c r="C52" s="1">
         <v>48</v>
       </c>
@@ -22625,7 +22624,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="53" spans="3:9" ht="13.2">
+    <row r="53" spans="3:9" ht="12.75">
       <c r="C53" s="1">
         <v>49</v>
       </c>
@@ -22642,7 +22641,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="54" spans="3:9" ht="13.2">
+    <row r="54" spans="3:9" ht="12.75">
       <c r="C54" s="1">
         <v>50</v>
       </c>
@@ -22656,7 +22655,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="55" spans="3:9" ht="13.2">
+    <row r="55" spans="3:9" ht="12.75">
       <c r="C55" s="1">
         <v>51</v>
       </c>
@@ -22670,7 +22669,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="3:9" ht="13.2">
+    <row r="56" spans="3:9" ht="12.75">
       <c r="C56" s="1">
         <v>52</v>
       </c>
@@ -22684,7 +22683,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="57" spans="3:9" ht="13.2">
+    <row r="57" spans="3:9" ht="12.75">
       <c r="C57" s="1">
         <v>53</v>
       </c>
@@ -22698,7 +22697,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="58" spans="3:9" ht="13.2">
+    <row r="58" spans="3:9" ht="12.75">
       <c r="C58" s="1">
         <v>54</v>
       </c>
@@ -22712,7 +22711,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="59" spans="3:9" ht="13.2">
+    <row r="59" spans="3:9" ht="12.75">
       <c r="C59" s="1">
         <v>55</v>
       </c>
@@ -22726,7 +22725,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="60" spans="3:9" ht="13.2">
+    <row r="60" spans="3:9" ht="12.75">
       <c r="C60" s="1">
         <v>56</v>
       </c>
@@ -22740,7 +22739,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="61" spans="3:9" ht="13.2">
+    <row r="61" spans="3:9" ht="12.75">
       <c r="C61" s="1">
         <v>57</v>
       </c>
@@ -22754,7 +22753,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="3:9" ht="13.2">
+    <row r="62" spans="3:9" ht="12.75">
       <c r="C62" s="1">
         <v>58</v>
       </c>
@@ -22765,7 +22764,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="63" spans="3:9" ht="13.2">
+    <row r="63" spans="3:9" ht="12.75">
       <c r="C63" s="1">
         <v>59</v>
       </c>
@@ -22776,7 +22775,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="64" spans="3:9" ht="13.2">
+    <row r="64" spans="3:9" ht="12.75">
       <c r="C64" s="1">
         <v>60</v>
       </c>
@@ -22787,7 +22786,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="3:6" ht="13.2">
+    <row r="65" spans="3:6" ht="12.75">
       <c r="C65" s="1">
         <v>61</v>
       </c>
@@ -22954,10 +22953,10 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="7" max="7" width="18.44140625" customWidth="1"/>
-    <col min="9" max="9" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:9">
@@ -23402,20 +23401,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A4:J72"/>
+  <dimension ref="A4:J74"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C16" sqref="A12:C16"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:10" ht="13.2">
+    <row r="4" spans="1:10" ht="12.75">
       <c r="A4" t="s">
         <v>1160</v>
       </c>
@@ -23423,7 +23422,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.2">
+    <row r="6" spans="1:10" ht="12.75">
       <c r="C6" s="1" t="s">
         <v>52</v>
       </c>
@@ -23443,7 +23442,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13.2">
+    <row r="7" spans="1:10" ht="12.75">
       <c r="A7">
         <v>1</v>
       </c>
@@ -23463,15 +23462,15 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.2">
-      <c r="C8" s="1">
-        <v>2</v>
+    <row r="8" spans="1:10" ht="12.75">
+      <c r="C8" s="1" t="s">
+        <v>1525</v>
       </c>
       <c r="D8" t="s">
-        <v>1169</v>
+        <v>1523</v>
       </c>
       <c r="G8" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I8" t="s">
         <v>1165</v>
@@ -23480,15 +23479,15 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13.2">
-      <c r="C9" s="1">
-        <v>3</v>
+    <row r="9" spans="1:10" ht="12.75">
+      <c r="C9" s="1" t="s">
+        <v>1526</v>
       </c>
       <c r="D9" t="s">
-        <v>1170</v>
+        <v>1524</v>
       </c>
       <c r="G9" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I9" t="s">
         <v>1166</v>
@@ -23497,15 +23496,15 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.2">
+    <row r="10" spans="1:10" ht="12.75">
       <c r="C10" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>1178</v>
+        <v>1169</v>
       </c>
       <c r="G10" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I10" t="s">
         <v>1167</v>
@@ -23514,667 +23513,689 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.2">
+    <row r="11" spans="1:10" ht="12.75">
       <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1170</v>
+      </c>
+      <c r="G11" s="1">
         <v>5</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:10" ht="12.75">
+      <c r="C12" s="1">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1178</v>
+      </c>
+      <c r="G12" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="12.75">
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>1179</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G13" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.2">
-      <c r="C12" s="1">
+    <row r="14" spans="1:10" ht="12.75">
+      <c r="C14" s="1">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D14" t="s">
         <v>1168</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G14" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13.2">
-      <c r="C13" s="1">
+    <row r="15" spans="1:10" ht="12.75">
+      <c r="C15" s="1">
         <v>7</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>412</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G15" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.2">
-      <c r="C14" s="1">
+    <row r="16" spans="1:10" ht="12.75">
+      <c r="C16" s="1">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D16" t="s">
         <v>1193</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G16" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13.2">
-      <c r="C15" s="1">
+    <row r="17" spans="2:7" ht="12.75">
+      <c r="C17" s="1">
         <v>9</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>1176</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G17" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="13.2">
-      <c r="C16" s="1">
+    <row r="18" spans="2:7" ht="12.75">
+      <c r="C18" s="1">
         <v>10</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D18" t="s">
         <v>138</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G18" s="1">
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="13.2">
-      <c r="C17" s="1">
+    <row r="19" spans="2:7" ht="12.75">
+      <c r="C19" s="1">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D19" t="s">
         <v>1177</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G19" s="1">
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="13.2">
-      <c r="C18" s="1">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>716</v>
-      </c>
-      <c r="G18" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="13.2">
-      <c r="C19" s="1">
-        <v>13</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1227</v>
-      </c>
-      <c r="G19" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="13.2">
+    <row r="20" spans="2:7" ht="12.75">
       <c r="B20" s="65"/>
       <c r="C20" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>1180</v>
+        <v>716</v>
       </c>
       <c r="G20" s="1">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="13.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="12.75">
       <c r="B21" s="74"/>
       <c r="C21" s="1">
-        <v>15</v>
-      </c>
-      <c r="D21" s="100" t="s">
-        <v>1181</v>
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1227</v>
       </c>
       <c r="G21" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="13.2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="12.75">
       <c r="B22" s="75"/>
       <c r="C22" s="1">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G22" s="1">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="12.75">
+      <c r="C23" s="1">
+        <v>15</v>
+      </c>
+      <c r="D23" s="100" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="12.75">
+      <c r="C24" s="1">
         <v>16</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" t="s">
         <v>167</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G24" s="1">
         <v>1300</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="13.2">
-      <c r="C23" s="1">
+    <row r="25" spans="2:7" ht="12.75">
+      <c r="C25" s="1">
         <v>17</v>
       </c>
-      <c r="D23" s="105" t="s">
+      <c r="D25" s="105" t="s">
         <v>1216</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G25" s="1">
         <v>1750</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="13.2">
-      <c r="C24" s="1">
-        <v>18</v>
-      </c>
-      <c r="D24" t="s">
-        <v>715</v>
-      </c>
-      <c r="G24" s="1">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="13.2">
-      <c r="C25" s="1">
-        <v>19</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1182</v>
-      </c>
-      <c r="G25" s="1">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="13.2">
+    <row r="26" spans="2:7" ht="12.75">
       <c r="B26" s="75"/>
       <c r="C26" s="1">
-        <v>20</v>
-      </c>
-      <c r="D26" s="97" t="s">
-        <v>1217</v>
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>715</v>
       </c>
       <c r="G26" s="1">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="13.2">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="12.75">
       <c r="C27" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D27" t="s">
-        <v>1218</v>
+        <v>1182</v>
       </c>
       <c r="G27" s="1">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="13.2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="12.75">
       <c r="B28" s="74"/>
       <c r="C28" s="1">
-        <v>22</v>
-      </c>
-      <c r="D28" t="s">
-        <v>1194</v>
+        <v>20</v>
+      </c>
+      <c r="D28" s="97" t="s">
+        <v>1217</v>
       </c>
       <c r="G28" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="13.2">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="12.75">
       <c r="B29" s="74"/>
       <c r="C29" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D29" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="G29" s="1">
-        <v>6100</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="13.2">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="12.75">
       <c r="B30" s="100"/>
       <c r="C30" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D30" t="s">
-        <v>1220</v>
+        <v>1194</v>
       </c>
       <c r="G30" s="1">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="13.2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="12.75">
       <c r="B31" s="103"/>
       <c r="C31" s="1">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D31" t="s">
-        <v>1161</v>
-      </c>
-      <c r="G31" s="28" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="13.2">
+        <v>1219</v>
+      </c>
+      <c r="G31" s="1">
+        <v>6100</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="12.75">
       <c r="B32" s="75"/>
       <c r="C32" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>1183</v>
-      </c>
-      <c r="G32" s="28" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="13.2">
+        <v>1220</v>
+      </c>
+      <c r="G32" s="1">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="12.75">
       <c r="B33" s="65"/>
       <c r="C33" s="1">
-        <v>27</v>
-      </c>
-      <c r="D33" s="65" t="s">
-        <v>1221</v>
+        <v>25</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1161</v>
       </c>
       <c r="G33" s="28" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="13.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="12.75">
       <c r="C34" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="G34" s="28" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="13.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="12.75">
       <c r="B35" s="105"/>
       <c r="C35" s="1">
-        <v>29</v>
-      </c>
-      <c r="D35" t="s">
-        <v>1222</v>
+        <v>27</v>
+      </c>
+      <c r="D35" s="65" t="s">
+        <v>1221</v>
       </c>
       <c r="G35" s="28" t="s">
-        <v>1199</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="13.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="12.75">
       <c r="B36" s="74"/>
       <c r="C36" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D36" t="s">
-        <v>1223</v>
+        <v>1187</v>
       </c>
       <c r="G36" s="28" t="s">
-        <v>1200</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="15.75" customHeight="1">
       <c r="C37" s="1">
-        <v>31</v>
-      </c>
-      <c r="D37" s="100" t="s">
-        <v>1224</v>
+        <v>29</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1222</v>
       </c>
       <c r="G37" s="28" t="s">
-        <v>201</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="15.75" customHeight="1">
       <c r="B38" s="100"/>
       <c r="C38" s="1">
-        <v>32</v>
-      </c>
-      <c r="D38" s="105" t="s">
-        <v>1225</v>
+        <v>30</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1223</v>
       </c>
       <c r="G38" s="28" t="s">
-        <v>212</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="15.75" customHeight="1">
       <c r="B39" s="100"/>
       <c r="C39" s="1">
-        <v>33</v>
-      </c>
-      <c r="D39" t="s">
-        <v>1226</v>
+        <v>31</v>
+      </c>
+      <c r="D39" s="100" t="s">
+        <v>1224</v>
       </c>
       <c r="G39" s="28" t="s">
-        <v>1201</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="15.75" customHeight="1">
       <c r="B40" s="103"/>
       <c r="C40" s="1">
-        <v>34</v>
-      </c>
-      <c r="D40" t="s">
-        <v>1228</v>
+        <v>32</v>
+      </c>
+      <c r="D40" s="105" t="s">
+        <v>1225</v>
       </c>
       <c r="G40" s="28" t="s">
-        <v>1202</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="15.75" customHeight="1">
       <c r="B41" s="101"/>
       <c r="C41" s="1">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D41" t="s">
-        <v>1195</v>
+        <v>1226</v>
       </c>
       <c r="G41" s="28" t="s">
-        <v>213</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="15.75" customHeight="1">
       <c r="B42" s="74"/>
       <c r="C42" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D42" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="G42" s="28" t="s">
-        <v>214</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="15.75" customHeight="1">
       <c r="B43" s="74"/>
       <c r="C43" s="1">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D43" t="s">
-        <v>1187</v>
+        <v>1195</v>
       </c>
       <c r="G43" s="28" t="s">
-        <v>1203</v>
+        <v>213</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="15.75" customHeight="1">
       <c r="B44" s="74"/>
       <c r="C44" s="1">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D44" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="G44" s="28" t="s">
-        <v>1204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="15.75" customHeight="1">
       <c r="B45" s="105"/>
       <c r="C45" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D45" t="s">
-        <v>1231</v>
+        <v>1187</v>
       </c>
       <c r="G45" s="28" t="s">
-        <v>215</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="15.75" customHeight="1">
       <c r="B46" s="75"/>
       <c r="C46" s="1">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D46" t="s">
-        <v>140</v>
+        <v>1230</v>
       </c>
       <c r="G46" s="28" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="47" spans="2:7" ht="15.75" customHeight="1">
       <c r="B47" s="75"/>
       <c r="C47" s="1">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D47" t="s">
-        <v>1184</v>
+        <v>1231</v>
       </c>
       <c r="G47" s="28" t="s">
-        <v>275</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="15.75" customHeight="1">
       <c r="B48" s="105"/>
       <c r="C48" s="1">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D48" t="s">
-        <v>1185</v>
+        <v>140</v>
       </c>
       <c r="G48" s="28" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="49" spans="2:7" ht="15.75" customHeight="1">
       <c r="B49" s="102"/>
       <c r="C49" s="1">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D49" t="s">
-        <v>1162</v>
+        <v>1184</v>
       </c>
       <c r="G49" s="28" t="s">
-        <v>216</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="15.75" customHeight="1">
       <c r="B50" s="101"/>
       <c r="C50" s="1">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D50" t="s">
-        <v>1196</v>
+        <v>1185</v>
       </c>
       <c r="G50" s="28" t="s">
-        <v>217</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="15.75" customHeight="1">
       <c r="B51" s="100"/>
       <c r="C51" s="1">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D51" t="s">
-        <v>977</v>
+        <v>1162</v>
       </c>
       <c r="G51" s="28" t="s">
-        <v>1207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="2:7" ht="15.75" customHeight="1">
       <c r="C52" s="1">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D52" t="s">
-        <v>1192</v>
+        <v>1196</v>
       </c>
       <c r="G52" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53" spans="2:7" ht="15.75" customHeight="1">
       <c r="B53" s="105"/>
       <c r="C53" s="1">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D53" t="s">
-        <v>1188</v>
+        <v>977</v>
       </c>
       <c r="G53" s="28" t="s">
-        <v>207</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="54" spans="2:7" ht="15.75" customHeight="1">
       <c r="B54" s="65"/>
       <c r="C54" s="1">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D54" t="s">
-        <v>1189</v>
+        <v>1192</v>
       </c>
       <c r="G54" s="28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="15.75" customHeight="1">
       <c r="B55" s="97"/>
       <c r="C55" s="1">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D55" t="s">
-        <v>410</v>
+        <v>1188</v>
       </c>
       <c r="G55" s="28" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="15.75" customHeight="1">
       <c r="B56" s="105"/>
       <c r="C56" s="1">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D56" t="s">
-        <v>1186</v>
+        <v>1189</v>
       </c>
       <c r="G56" s="28" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="57" spans="2:7" ht="15.75" customHeight="1">
       <c r="B57" s="99"/>
       <c r="C57" s="1">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D57" t="s">
-        <v>715</v>
+        <v>410</v>
       </c>
       <c r="G57" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="58" spans="2:7" ht="15.75" customHeight="1">
       <c r="B58" s="97"/>
       <c r="C58" s="1">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D58" t="s">
-        <v>1197</v>
+        <v>1186</v>
       </c>
       <c r="G58" s="28" t="s">
-        <v>1208</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="2:7" ht="15.75" customHeight="1">
       <c r="C59" s="1">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D59" t="s">
-        <v>1198</v>
+        <v>715</v>
       </c>
       <c r="G59" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="60" spans="2:7" ht="15.75" customHeight="1">
       <c r="C60" s="1">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D60" t="s">
-        <v>1191</v>
+        <v>1197</v>
       </c>
       <c r="G60" s="28" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="61" spans="2:7" ht="15.75" customHeight="1">
       <c r="C61" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D61" t="s">
-        <v>414</v>
+        <v>1198</v>
       </c>
       <c r="G61" s="28" t="s">
-        <v>1210</v>
+        <v>223</v>
       </c>
     </row>
     <row r="62" spans="2:7" ht="15.75" customHeight="1">
       <c r="C62" s="1">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D62" t="s">
-        <v>1232</v>
+        <v>1191</v>
       </c>
       <c r="G62" s="28" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="63" spans="2:7" ht="15.75" customHeight="1">
       <c r="C63" s="1">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D63" t="s">
-        <v>714</v>
+        <v>414</v>
       </c>
       <c r="G63" s="28" t="s">
-        <v>1215</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="64" spans="2:7" ht="15.75" customHeight="1">
       <c r="C64" s="1">
-        <v>58</v>
-      </c>
-      <c r="D64" s="103" t="s">
-        <v>1233</v>
+        <v>56</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1232</v>
       </c>
       <c r="G64" s="28" t="s">
-        <v>1214</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="65" spans="3:7" ht="15.75" customHeight="1">
       <c r="C65" s="1">
-        <v>59</v>
-      </c>
-      <c r="D65" s="116" t="s">
-        <v>1190</v>
+        <v>57</v>
+      </c>
+      <c r="D65" t="s">
+        <v>714</v>
       </c>
       <c r="G65" s="28" t="s">
-        <v>1213</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="66" spans="3:7" ht="15.75" customHeight="1">
       <c r="C66" s="1">
-        <v>60</v>
-      </c>
-      <c r="D66" t="s">
-        <v>413</v>
-      </c>
-      <c r="G66" s="117" t="s">
-        <v>1212</v>
+        <v>58</v>
+      </c>
+      <c r="D66" s="103" t="s">
+        <v>1233</v>
+      </c>
+      <c r="G66" s="28" t="s">
+        <v>1214</v>
       </c>
     </row>
     <row r="67" spans="3:7" ht="15.75" customHeight="1">
       <c r="C67" s="1">
+        <v>59</v>
+      </c>
+      <c r="D67" s="116" t="s">
+        <v>1190</v>
+      </c>
+      <c r="G67" s="28" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7" ht="15.75" customHeight="1">
+      <c r="C68" s="1">
+        <v>60</v>
+      </c>
+      <c r="D68" t="s">
+        <v>413</v>
+      </c>
+      <c r="G68" s="117" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="69" spans="3:7" ht="15.75" customHeight="1">
+      <c r="C69" s="1">
         <v>61</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D69" t="s">
         <v>411</v>
       </c>
-      <c r="G67" s="28" t="s">
+      <c r="G69" s="28" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="72" spans="3:7" ht="15.75" customHeight="1">
-      <c r="D72" t="s">
+    <row r="74" spans="3:7" ht="15.75" customHeight="1">
+      <c r="D74" t="s">
         <v>969</v>
       </c>
     </row>
@@ -24194,23 +24215,23 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.88671875" customWidth="1"/>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
-    <col min="8" max="8" width="39.44140625" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.5546875" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="39.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:20" ht="13.2">
+    <row r="3" spans="3:20" ht="12.75">
       <c r="C3" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="5" spans="3:20" ht="13.2">
+    <row r="5" spans="3:20" ht="12.75">
       <c r="C5" s="1" t="s">
         <v>52</v>
       </c>
@@ -24266,7 +24287,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="6" spans="3:20" ht="13.2">
+    <row r="6" spans="3:20" ht="12.75">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -24292,7 +24313,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="7" spans="3:20" ht="13.2">
+    <row r="7" spans="3:20" ht="12.75">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -24312,7 +24333,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="8" spans="3:20" ht="13.2">
+    <row r="8" spans="3:20" ht="12.75">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -24332,7 +24353,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="9" spans="3:20" ht="13.2">
+    <row r="9" spans="3:20" ht="12.75">
       <c r="C9" s="1">
         <v>4</v>
       </c>
@@ -24394,21 +24415,21 @@
   </sheetPr>
   <dimension ref="C3:V305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="26.88671875" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
-    <col min="9" max="9" width="33.6640625" customWidth="1"/>
-    <col min="11" max="11" width="34.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1"/>
+    <col min="11" max="11" width="34.5703125" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:22" ht="13.2">
+    <row r="3" spans="3:22" ht="12.75">
       <c r="C3" s="1" t="s">
         <v>232</v>
       </c>
@@ -24416,7 +24437,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="3:22" ht="13.2">
+    <row r="4" spans="3:22" ht="12.75">
       <c r="K4" t="s">
         <v>1248</v>
       </c>
@@ -24430,7 +24451,7 @@
       <c r="T4" s="120"/>
       <c r="U4" s="120"/>
     </row>
-    <row r="5" spans="3:22" ht="13.2">
+    <row r="5" spans="3:22" ht="12.75">
       <c r="C5" s="1" t="s">
         <v>52</v>
       </c>
@@ -24489,7 +24510,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="3:22" ht="13.2">
+    <row r="6" spans="3:22" ht="12.75">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -24509,7 +24530,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="7" spans="3:22" ht="13.2">
+    <row r="7" spans="3:22" ht="12.75">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -24529,7 +24550,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="8" spans="3:22" ht="13.2">
+    <row r="8" spans="3:22" ht="12.75">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -24549,7 +24570,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="9" spans="3:22" ht="13.2">
+    <row r="9" spans="3:22" ht="12.75">
       <c r="C9" s="1">
         <v>4</v>
       </c>
@@ -24590,7 +24611,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="10" spans="3:22" ht="13.2">
+    <row r="10" spans="3:22" ht="12.75">
       <c r="C10" s="1">
         <v>5</v>
       </c>
@@ -24613,7 +24634,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="11" spans="3:22" ht="13.2">
+    <row r="11" spans="3:22" ht="12.75">
       <c r="C11" s="1">
         <v>6</v>
       </c>
@@ -24633,7 +24654,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="12" spans="3:22" ht="13.2">
+    <row r="12" spans="3:22" ht="12.75">
       <c r="C12" s="1">
         <v>7</v>
       </c>
@@ -24653,7 +24674,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="13" spans="3:22" ht="13.2">
+    <row r="13" spans="3:22" ht="12.75">
       <c r="C13" s="1">
         <v>8</v>
       </c>
@@ -24676,7 +24697,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="14" spans="3:22" ht="13.2">
+    <row r="14" spans="3:22" ht="12.75">
       <c r="C14" s="1">
         <v>9</v>
       </c>
@@ -24699,7 +24720,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="15" spans="3:22" ht="13.2">
+    <row r="15" spans="3:22" ht="12.75">
       <c r="C15" s="1">
         <v>10</v>
       </c>
@@ -24719,7 +24740,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="16" spans="3:22" ht="13.2">
+    <row r="16" spans="3:22" ht="12.75">
       <c r="C16" s="1">
         <v>11</v>
       </c>
@@ -24739,7 +24760,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="17" spans="3:16" ht="13.2">
+    <row r="17" spans="3:16" ht="12.75">
       <c r="C17" s="1">
         <v>12</v>
       </c>
@@ -24759,7 +24780,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="18" spans="3:16" ht="13.2">
+    <row r="18" spans="3:16" ht="12.75">
       <c r="C18" s="1">
         <v>13</v>
       </c>
@@ -24782,7 +24803,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="19" spans="3:16" ht="13.2">
+    <row r="19" spans="3:16" ht="12.75">
       <c r="C19" s="1">
         <v>14</v>
       </c>
@@ -24805,7 +24826,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="20" spans="3:16" ht="13.2">
+    <row r="20" spans="3:16" ht="12.75">
       <c r="C20" s="1">
         <v>15</v>
       </c>
@@ -24828,7 +24849,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="3:16" ht="13.2">
+    <row r="21" spans="3:16" ht="12.75">
       <c r="C21" s="1">
         <v>16</v>
       </c>
@@ -24851,7 +24872,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="22" spans="3:16" ht="13.2">
+    <row r="22" spans="3:16" ht="12.75">
       <c r="C22" s="1">
         <v>17</v>
       </c>
@@ -24874,7 +24895,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="23" spans="3:16" ht="13.2">
+    <row r="23" spans="3:16" ht="12.75">
       <c r="C23" s="1">
         <v>18</v>
       </c>
@@ -24900,7 +24921,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="3:16" ht="13.2">
+    <row r="24" spans="3:16" ht="12.75">
       <c r="C24" s="1">
         <v>19</v>
       </c>
@@ -24921,7 +24942,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="25" spans="3:16" ht="13.2">
+    <row r="25" spans="3:16" ht="12.75">
       <c r="C25" s="1">
         <v>20</v>
       </c>
@@ -24939,7 +24960,7 @@
       </c>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="3:16" ht="13.2">
+    <row r="26" spans="3:16" ht="12.75">
       <c r="C26" s="1">
         <v>21</v>
       </c>
@@ -24956,7 +24977,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="27" spans="3:16" ht="13.2">
+    <row r="27" spans="3:16" ht="12.75">
       <c r="C27" s="1">
         <v>22</v>
       </c>
@@ -24976,7 +24997,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="28" spans="3:16" ht="13.2">
+    <row r="28" spans="3:16" ht="12.75">
       <c r="C28" s="1">
         <v>23</v>
       </c>
@@ -24996,7 +25017,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="29" spans="3:16" ht="13.2">
+    <row r="29" spans="3:16" ht="12.75">
       <c r="C29" s="1">
         <v>24</v>
       </c>
@@ -25013,7 +25034,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="30" spans="3:16" ht="13.2">
+    <row r="30" spans="3:16" ht="12.75">
       <c r="C30" s="1">
         <v>25</v>
       </c>
@@ -25030,7 +25051,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="31" spans="3:16" ht="13.2">
+    <row r="31" spans="3:16" ht="12.75">
       <c r="C31" s="1">
         <v>26</v>
       </c>
@@ -25050,7 +25071,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="32" spans="3:16" ht="13.2">
+    <row r="32" spans="3:16" ht="12.75">
       <c r="C32" s="1">
         <v>27</v>
       </c>
@@ -25067,7 +25088,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="33" spans="3:12" ht="13.2">
+    <row r="33" spans="3:12" ht="12.75">
       <c r="C33" s="1">
         <v>28</v>
       </c>
@@ -25081,7 +25102,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="34" spans="3:12" ht="13.2">
+    <row r="34" spans="3:12" ht="12.75">
       <c r="C34" s="1">
         <v>29</v>
       </c>
@@ -25095,7 +25116,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="35" spans="3:12" ht="13.2">
+    <row r="35" spans="3:12" ht="12.75">
       <c r="C35" s="1">
         <v>30</v>
       </c>
@@ -25109,7 +25130,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="36" spans="3:12" ht="13.2">
+    <row r="36" spans="3:12" ht="12.75">
       <c r="C36" s="1">
         <v>31</v>
       </c>
@@ -25126,7 +25147,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="37" spans="3:12" ht="13.2">
+    <row r="37" spans="3:12" ht="12.75">
       <c r="C37" s="1">
         <v>32</v>
       </c>
@@ -25143,7 +25164,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="38" spans="3:12" ht="13.2">
+    <row r="38" spans="3:12" ht="12.75">
       <c r="C38" s="1">
         <v>33</v>
       </c>
@@ -25154,7 +25175,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="39" spans="3:12" ht="13.2">
+    <row r="39" spans="3:12" ht="12.75">
       <c r="C39" s="1">
         <v>34</v>
       </c>
@@ -25171,7 +25192,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="40" spans="3:12" ht="13.2">
+    <row r="40" spans="3:12" ht="12.75">
       <c r="C40" s="1">
         <v>35</v>
       </c>
@@ -25182,7 +25203,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="41" spans="3:12" ht="13.2">
+    <row r="41" spans="3:12" ht="12.75">
       <c r="C41" s="1">
         <v>36</v>
       </c>
@@ -25193,7 +25214,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="42" spans="3:12" ht="13.2">
+    <row r="42" spans="3:12" ht="12.75">
       <c r="C42" s="1">
         <v>37</v>
       </c>
@@ -25204,7 +25225,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="43" spans="3:12" ht="13.2">
+    <row r="43" spans="3:12" ht="12.75">
       <c r="C43" s="1">
         <v>38</v>
       </c>
@@ -25215,7 +25236,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="44" spans="3:12" ht="13.2">
+    <row r="44" spans="3:12" ht="12.75">
       <c r="C44" s="1">
         <v>39</v>
       </c>
@@ -25226,7 +25247,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="45" spans="3:12" ht="13.2">
+    <row r="45" spans="3:12" ht="12.75">
       <c r="C45" s="1">
         <v>40</v>
       </c>
@@ -25237,7 +25258,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="46" spans="3:12" ht="13.2">
+    <row r="46" spans="3:12" ht="12.75">
       <c r="C46" s="1">
         <v>41</v>
       </c>
@@ -25248,7 +25269,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="47" spans="3:12" ht="13.2">
+    <row r="47" spans="3:12" ht="12.75">
       <c r="C47" s="1">
         <v>42</v>
       </c>
@@ -25259,7 +25280,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="48" spans="3:12" ht="13.2">
+    <row r="48" spans="3:12" ht="12.75">
       <c r="C48" s="1">
         <v>43</v>
       </c>
@@ -25270,7 +25291,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="49" spans="3:13" ht="13.2">
+    <row r="49" spans="3:13" ht="12.75">
       <c r="C49" s="1">
         <v>44</v>
       </c>
@@ -25281,7 +25302,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="50" spans="3:13" ht="13.2">
+    <row r="50" spans="3:13" ht="12.75">
       <c r="C50" s="1">
         <v>45</v>
       </c>
@@ -25292,7 +25313,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="51" spans="3:13" ht="13.2">
+    <row r="51" spans="3:13" ht="12.75">
       <c r="C51" s="1">
         <v>46</v>
       </c>
@@ -25303,7 +25324,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="52" spans="3:13" ht="13.2">
+    <row r="52" spans="3:13" ht="12.75">
       <c r="C52" s="1">
         <v>47</v>
       </c>
@@ -25314,7 +25335,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="53" spans="3:13" ht="13.2">
+    <row r="53" spans="3:13" ht="12.75">
       <c r="C53" s="1">
         <v>48</v>
       </c>
@@ -25325,7 +25346,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="54" spans="3:13" ht="13.2">
+    <row r="54" spans="3:13" ht="12.75">
       <c r="C54" s="1">
         <v>49</v>
       </c>
@@ -25339,7 +25360,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="55" spans="3:13" ht="13.2">
+    <row r="55" spans="3:13" ht="12.75">
       <c r="C55" s="1">
         <v>50</v>
       </c>
@@ -25350,7 +25371,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="56" spans="3:13" ht="13.2">
+    <row r="56" spans="3:13" ht="12.75">
       <c r="C56" s="1">
         <v>51</v>
       </c>
@@ -25361,7 +25382,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="57" spans="3:13" ht="13.2">
+    <row r="57" spans="3:13" ht="12.75">
       <c r="C57" s="1">
         <v>52</v>
       </c>
@@ -25372,7 +25393,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="58" spans="3:13" ht="13.2">
+    <row r="58" spans="3:13" ht="12.75">
       <c r="C58" s="1">
         <v>53</v>
       </c>
@@ -25383,7 +25404,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="59" spans="3:13" ht="13.2">
+    <row r="59" spans="3:13" ht="12.75">
       <c r="C59" s="1">
         <v>54</v>
       </c>
@@ -25394,7 +25415,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="60" spans="3:13" ht="13.2">
+    <row r="60" spans="3:13" ht="12.75">
       <c r="C60" s="1">
         <v>55</v>
       </c>
@@ -25405,7 +25426,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="61" spans="3:13" ht="13.2">
+    <row r="61" spans="3:13" ht="12.75">
       <c r="C61" s="1">
         <v>56</v>
       </c>
@@ -25416,7 +25437,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="62" spans="3:13" ht="13.2">
+    <row r="62" spans="3:13" ht="12.75">
       <c r="C62" s="1">
         <v>57</v>
       </c>
@@ -25427,7 +25448,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="63" spans="3:13" ht="13.2">
+    <row r="63" spans="3:13" ht="12.75">
       <c r="C63" s="1">
         <v>58</v>
       </c>
@@ -25438,7 +25459,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="64" spans="3:13" ht="13.2">
+    <row r="64" spans="3:13" ht="12.75">
       <c r="C64" s="1">
         <v>59</v>
       </c>
@@ -25449,7 +25470,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="65" spans="3:11" ht="13.2">
+    <row r="65" spans="3:11" ht="12.75">
       <c r="C65" s="1">
         <v>60</v>
       </c>
@@ -25460,7 +25481,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="66" spans="3:11" ht="13.2">
+    <row r="66" spans="3:11" ht="12.75">
       <c r="C66" s="1">
         <v>61</v>
       </c>
@@ -25471,7 +25492,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="67" spans="3:11" ht="13.2">
+    <row r="67" spans="3:11" ht="12.75">
       <c r="C67" s="1">
         <v>62</v>
       </c>
@@ -25482,7 +25503,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="68" spans="3:11" ht="13.2">
+    <row r="68" spans="3:11" ht="12.75">
       <c r="C68" s="1">
         <v>63</v>
       </c>
@@ -25493,7 +25514,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="69" spans="3:11" ht="13.2">
+    <row r="69" spans="3:11" ht="12.75">
       <c r="C69" s="1">
         <v>64</v>
       </c>
@@ -25504,7 +25525,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="70" spans="3:11" ht="13.2">
+    <row r="70" spans="3:11" ht="12.75">
       <c r="C70" s="1">
         <v>65</v>
       </c>
@@ -25515,7 +25536,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="71" spans="3:11" ht="13.2">
+    <row r="71" spans="3:11" ht="12.75">
       <c r="C71" s="1">
         <v>66</v>
       </c>
@@ -25526,7 +25547,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="72" spans="3:11" ht="13.2">
+    <row r="72" spans="3:11" ht="12.75">
       <c r="C72" s="1">
         <v>67</v>
       </c>
@@ -25537,7 +25558,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="73" spans="3:11" ht="13.2">
+    <row r="73" spans="3:11" ht="12.75">
       <c r="C73" s="1">
         <v>68</v>
       </c>
@@ -25548,7 +25569,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="74" spans="3:11" ht="13.2">
+    <row r="74" spans="3:11" ht="12.75">
       <c r="C74" s="1">
         <v>69</v>
       </c>
@@ -25559,7 +25580,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="75" spans="3:11" ht="13.2">
+    <row r="75" spans="3:11" ht="12.75">
       <c r="C75" s="1">
         <v>70</v>
       </c>
@@ -25570,7 +25591,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="76" spans="3:11" ht="13.2">
+    <row r="76" spans="3:11" ht="12.75">
       <c r="C76" s="1">
         <v>71</v>
       </c>
@@ -25581,7 +25602,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="77" spans="3:11" ht="13.2">
+    <row r="77" spans="3:11" ht="12.75">
       <c r="C77" s="1">
         <v>72</v>
       </c>
@@ -25592,7 +25613,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="78" spans="3:11" ht="13.2">
+    <row r="78" spans="3:11" ht="12.75">
       <c r="C78" s="1">
         <v>73</v>
       </c>
@@ -25603,7 +25624,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="79" spans="3:11" ht="13.2">
+    <row r="79" spans="3:11" ht="12.75">
       <c r="C79" s="1">
         <v>74</v>
       </c>
@@ -25614,7 +25635,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="80" spans="3:11" ht="13.2">
+    <row r="80" spans="3:11" ht="12.75">
       <c r="C80" s="1">
         <v>75</v>
       </c>
@@ -25625,7 +25646,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="81" spans="3:11" ht="13.2">
+    <row r="81" spans="3:11" ht="12.75">
       <c r="C81" s="1">
         <v>76</v>
       </c>
@@ -25636,7 +25657,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="82" spans="3:11" ht="13.2">
+    <row r="82" spans="3:11" ht="12.75">
       <c r="C82" s="1">
         <v>77</v>
       </c>
@@ -25647,7 +25668,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="83" spans="3:11" ht="13.2">
+    <row r="83" spans="3:11" ht="12.75">
       <c r="C83" s="1">
         <v>78</v>
       </c>
@@ -25658,7 +25679,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="84" spans="3:11" ht="13.2">
+    <row r="84" spans="3:11" ht="12.75">
       <c r="C84" s="1">
         <v>79</v>
       </c>
@@ -25669,7 +25690,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="85" spans="3:11" ht="13.2">
+    <row r="85" spans="3:11" ht="12.75">
       <c r="C85" s="1">
         <v>80</v>
       </c>
@@ -25680,7 +25701,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="86" spans="3:11" ht="13.2">
+    <row r="86" spans="3:11" ht="12.75">
       <c r="C86" s="1">
         <v>81</v>
       </c>
@@ -25691,7 +25712,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="87" spans="3:11" ht="13.2">
+    <row r="87" spans="3:11" ht="12.75">
       <c r="C87" s="1">
         <v>82</v>
       </c>
@@ -25702,7 +25723,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="88" spans="3:11" ht="13.2">
+    <row r="88" spans="3:11" ht="12.75">
       <c r="C88" s="1">
         <v>83</v>
       </c>
@@ -25713,7 +25734,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="89" spans="3:11" ht="13.2">
+    <row r="89" spans="3:11" ht="12.75">
       <c r="C89" s="1">
         <v>84</v>
       </c>
@@ -25724,7 +25745,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="90" spans="3:11" ht="13.2">
+    <row r="90" spans="3:11" ht="12.75">
       <c r="C90" s="1">
         <v>85</v>
       </c>
@@ -25735,7 +25756,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="91" spans="3:11" ht="13.2">
+    <row r="91" spans="3:11" ht="12.75">
       <c r="C91" s="1">
         <v>86</v>
       </c>
@@ -25746,7 +25767,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="92" spans="3:11" ht="13.2">
+    <row r="92" spans="3:11" ht="12.75">
       <c r="C92" s="1">
         <v>87</v>
       </c>
@@ -25757,7 +25778,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="93" spans="3:11" ht="13.2">
+    <row r="93" spans="3:11" ht="12.75">
       <c r="C93" s="1">
         <v>88</v>
       </c>
@@ -25768,7 +25789,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="94" spans="3:11" ht="13.2">
+    <row r="94" spans="3:11" ht="12.75">
       <c r="C94" s="1">
         <v>89</v>
       </c>
@@ -25779,7 +25800,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="95" spans="3:11" ht="13.2">
+    <row r="95" spans="3:11" ht="12.75">
       <c r="C95" s="1">
         <v>90</v>
       </c>
@@ -25790,7 +25811,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="96" spans="3:11" ht="13.2">
+    <row r="96" spans="3:11" ht="12.75">
       <c r="C96" s="1">
         <v>91</v>
       </c>
@@ -25801,7 +25822,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="97" spans="3:11" ht="13.2">
+    <row r="97" spans="3:11" ht="12.75">
       <c r="C97" s="1">
         <v>92</v>
       </c>
@@ -25812,7 +25833,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="98" spans="3:11" ht="13.2">
+    <row r="98" spans="3:11" ht="12.75">
       <c r="C98" s="1">
         <v>93</v>
       </c>
@@ -25823,7 +25844,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="99" spans="3:11" ht="13.2">
+    <row r="99" spans="3:11" ht="12.75">
       <c r="C99" s="1">
         <v>94</v>
       </c>
@@ -25834,7 +25855,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="100" spans="3:11" ht="13.2">
+    <row r="100" spans="3:11" ht="12.75">
       <c r="C100" s="1">
         <v>95</v>
       </c>
@@ -25845,7 +25866,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="101" spans="3:11" ht="13.2">
+    <row r="101" spans="3:11" ht="12.75">
       <c r="C101" s="1">
         <v>96</v>
       </c>
@@ -25856,7 +25877,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="102" spans="3:11" ht="13.2">
+    <row r="102" spans="3:11" ht="12.75">
       <c r="C102" s="1">
         <v>97</v>
       </c>
@@ -25867,7 +25888,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="103" spans="3:11" ht="13.2">
+    <row r="103" spans="3:11" ht="12.75">
       <c r="C103" s="1">
         <v>98</v>
       </c>
@@ -25878,7 +25899,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="104" spans="3:11" ht="13.2">
+    <row r="104" spans="3:11" ht="12.75">
       <c r="C104" s="1">
         <v>99</v>
       </c>
@@ -25889,7 +25910,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="105" spans="3:11" ht="13.2">
+    <row r="105" spans="3:11" ht="12.75">
       <c r="C105" s="1">
         <v>100</v>
       </c>
@@ -27525,22 +27546,22 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
-    <col min="10" max="10" width="19.109375" customWidth="1"/>
-    <col min="11" max="11" width="51.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="51.85546875" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
-    <col min="16" max="16" width="24.33203125" customWidth="1"/>
-    <col min="17" max="17" width="19.109375" customWidth="1"/>
-    <col min="18" max="18" width="29.44140625" customWidth="1"/>
+    <col min="16" max="16" width="24.28515625" customWidth="1"/>
+    <col min="17" max="17" width="19.140625" customWidth="1"/>
+    <col min="18" max="18" width="29.42578125" customWidth="1"/>
     <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="20" width="10.88671875" customWidth="1"/>
-    <col min="21" max="21" width="3.5546875" customWidth="1"/>
-    <col min="22" max="22" width="2.109375" customWidth="1"/>
-    <col min="25" max="25" width="14.6640625" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" customWidth="1"/>
+    <col min="21" max="21" width="3.5703125" customWidth="1"/>
+    <col min="22" max="22" width="2.140625" customWidth="1"/>
+    <col min="25" max="25" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:20">

</xml_diff>

<commit_message>
UI Unlock system, debug mode, bug fixes
Implemented game unlock system for almost all of the game
Added debug mode where everything is unlocked
Fixed Research History
Moved some of the calculations to timers, for improved performance
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DCD27B-E2BF-4C8F-BA38-9ACDB1B0A6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A904DFE-983D-484A-BAC8-18CD88F70750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21570" yWindow="8010" windowWidth="20145" windowHeight="11550" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15750" yWindow="8790" windowWidth="20145" windowHeight="11550" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -23418,7 +23418,7 @@
   </sheetPr>
   <dimension ref="A4:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A60" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
@@ -24615,8 +24615,8 @@
   </sheetPr>
   <dimension ref="C3:V305"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" topLeftCell="I295" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L303" sqref="L303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Magic Locks, Achievements, Unlock Triggers, Bugs
Added Magic Lock for rarer upgrades
Added achievement count bonus, change Magic count bonus to be logarithmic
Fixed some game system unlocks, triggers for research, upgrades and achievements
Added more achievement triggers
Fixed some other bugs
Balancing
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A3929F-77FA-485A-95AC-927A8210D4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BF0516-AFC9-4981-8F9E-BFE81794CA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22770" yWindow="8220" windowWidth="20145" windowHeight="11550" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3017" uniqueCount="1532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3018" uniqueCount="1532">
   <si>
     <t xml:space="preserve">Tier </t>
   </si>
@@ -23416,10 +23416,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A4:J76"/>
+  <dimension ref="A4:Q76"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -23429,7 +23429,7 @@
     <col min="5" max="5" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:10" ht="12.75">
+    <row r="4" spans="1:17" ht="12.75">
       <c r="A4" t="s">
         <v>1155</v>
       </c>
@@ -23437,7 +23437,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="12.75">
+    <row r="6" spans="1:17" ht="12.75">
       <c r="C6" s="1" t="s">
         <v>52</v>
       </c>
@@ -23456,8 +23456,11 @@
       <c r="I6" s="1" t="s">
         <v>1159</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="12.75">
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="12.75">
       <c r="A7">
         <v>1</v>
       </c>
@@ -23479,8 +23482,31 @@
       <c r="J7" t="s">
         <v>1170</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="12.75">
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <f>LOG(L7,2)</f>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f>LOG10(L7)</f>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>LOG(L7,22)</f>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <f>LOG(L7,35)</f>
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <f>LOG(L7,7) / 2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="12.75">
       <c r="B8">
         <v>2</v>
       </c>
@@ -23499,8 +23525,31 @@
       <c r="J8" t="s">
         <v>1167</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="12.75">
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ref="M8:M71" si="0">LOG(L8,2)</f>
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ref="N8:N72" si="1">LOG10(L8)</f>
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8:O71" si="2">LOG(L8,22)</f>
+        <v>0.22424382421757541</v>
+      </c>
+      <c r="P8">
+        <f>LOG(L8,35)</f>
+        <v>0.19495902189378631</v>
+      </c>
+      <c r="Q8">
+        <f>LOG(L8,6) / 2</f>
+        <v>0.19342640361727079</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="12.75">
       <c r="B9">
         <v>3</v>
       </c>
@@ -23519,8 +23568,31 @@
       <c r="J9" t="s">
         <v>1168</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="12.75">
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>1.5849625007211563</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>0.47712125471966244</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="2"/>
+        <v>0.35541805240316376</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P9:P41" si="3">LOG(L9,35)</f>
+        <v>0.30900273887892621</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" ref="Q9:Q72" si="4">LOG(L9,6) / 2</f>
+        <v>0.30657359638272924</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="12.75">
       <c r="B10">
         <v>4</v>
       </c>
@@ -23539,8 +23611,31 @@
       <c r="J10" t="s">
         <v>1169</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="12.75">
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="2"/>
+        <v>0.44848764843515082</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="3"/>
+        <v>0.38991804378757261</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="4"/>
+        <v>0.38685280723454157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="12.75">
       <c r="B11">
         <v>5</v>
       </c>
@@ -23553,8 +23648,31 @@
       <c r="G11" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="12.75">
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>2.3219280948873622</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>0.52067803555577141</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="3"/>
+        <v>0.45268083028694278</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="4"/>
+        <v>0.44912220085196358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="12.75">
       <c r="B12">
         <v>6</v>
       </c>
@@ -23567,8 +23685,31 @@
       <c r="G12" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="12.75">
+      <c r="L12">
+        <v>6</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>2.5849625007211561</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>0.77815125038364363</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="2"/>
+        <v>0.57966187662073909</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="3"/>
+        <v>0.50396176077271249</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="12.75">
       <c r="B13">
         <v>7</v>
       </c>
@@ -23581,8 +23722,31 @@
       <c r="G13" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="12.75">
+      <c r="L13">
+        <v>7</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>2.8073549220576042</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>0.84509804001425681</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="2"/>
+        <v>0.62953200365823048</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="3"/>
+        <v>0.54731916971305716</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="4"/>
+        <v>0.54301656625084593</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="12.75">
       <c r="B14">
         <v>8</v>
       </c>
@@ -23595,8 +23759,31 @@
       <c r="G14" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="12.75">
+      <c r="L14">
+        <v>8</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="2"/>
+        <v>0.67273147265272626</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="3"/>
+        <v>0.58487706568135889</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="4"/>
+        <v>0.58027921085181233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="12.75">
       <c r="B15">
         <v>9</v>
       </c>
@@ -23609,8 +23796,31 @@
       <c r="G15" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="12.75">
+      <c r="L15">
+        <v>9</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>3.1699250014423126</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>0.95424250943932487</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="2"/>
+        <v>0.71083610480632753</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="3"/>
+        <v>0.61800547775785242</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="4"/>
+        <v>0.61314719276545848</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="12.75">
       <c r="B16">
         <v>10</v>
       </c>
@@ -23623,8 +23833,31 @@
       <c r="G16" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" ht="12.75">
+      <c r="L16">
+        <v>10</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>3.3219280948873626</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="2"/>
+        <v>0.74492185977334702</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="3"/>
+        <v>0.64763985218072917</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="4"/>
+        <v>0.64254860446923445</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" ht="12.75">
       <c r="B17">
         <v>11</v>
       </c>
@@ -23637,8 +23870,31 @@
       <c r="G17" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" ht="12.75">
+      <c r="L17">
+        <v>11</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>3.4594316186372978</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>1.0413926851582251</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="2"/>
+        <v>0.77575617578242451</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="3"/>
+        <v>0.67444740467796549</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="4"/>
+        <v>0.66914541655288629</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" ht="12.75">
       <c r="B18">
         <v>12</v>
       </c>
@@ -23651,8 +23907,31 @@
       <c r="G18" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="12.75">
+      <c r="L18">
+        <v>12</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>3.5849625007211565</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="1"/>
+        <v>1.0791812460476249</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="2"/>
+        <v>0.80390570083831459</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="3"/>
+        <v>0.69892078266649882</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="4"/>
+        <v>0.69342640361727081</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" ht="12.75">
       <c r="B19">
         <v>13</v>
       </c>
@@ -23665,8 +23944,31 @@
       <c r="G19" s="1">
         <v>130</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" ht="12.75">
+      <c r="L19">
+        <v>13</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>3.7004397181410922</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>1.1139433523068367</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="2"/>
+        <v>0.82980075368256545</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="3"/>
+        <v>0.72143410802570562</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="4"/>
+        <v>0.71576274648253868</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" ht="12.75">
       <c r="B20">
         <v>14</v>
       </c>
@@ -23679,8 +23981,31 @@
       <c r="G20" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" ht="12.75">
+      <c r="L20">
+        <v>14</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>3.8073549220576037</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>1.146128035678238</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="2"/>
+        <v>0.85377582787580586</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="3"/>
+        <v>0.7422781916068435</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="4"/>
+        <v>0.73644296986811664</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" ht="12.75">
       <c r="B21">
         <v>15</v>
       </c>
@@ -23693,8 +24018,31 @@
       <c r="G21" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" ht="12.75">
+      <c r="L21">
+        <v>15</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>3.9068905956085187</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="1"/>
+        <v>1.1760912590556813</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="2"/>
+        <v>0.87609608795893523</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="3"/>
+        <v>0.76168356916586899</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="4"/>
+        <v>0.75569579723469282</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" ht="12.75">
       <c r="B22">
         <v>16</v>
       </c>
@@ -23707,8 +24055,31 @@
       <c r="G22" s="1">
         <v>500</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" ht="12.75">
+      <c r="L22">
+        <v>16</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="1"/>
+        <v>1.2041199826559248</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="2"/>
+        <v>0.89697529687030164</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="3"/>
+        <v>0.77983608757514522</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="4"/>
+        <v>0.77370561446908315</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" ht="12.75">
       <c r="B23">
         <v>17</v>
       </c>
@@ -23721,8 +24092,31 @@
       <c r="G23" s="1">
         <v>600</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" ht="12.75">
+      <c r="L23">
+        <v>17</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>4.08746284125034</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>1.2304489213782739</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="2"/>
+        <v>0.91658829886921256</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="3"/>
+        <v>0.79688775755736296</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="4"/>
+        <v>0.79062323730228468</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" ht="12.75">
       <c r="B24">
         <v>18</v>
       </c>
@@ -23735,8 +24129,31 @@
       <c r="G24" s="1">
         <v>750</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" ht="12.75">
+      <c r="L24">
+        <v>18</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="0"/>
+        <v>4.1699250014423122</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>1.255272505103306</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="2"/>
+        <v>0.9350799290239028</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="3"/>
+        <v>0.81296449965163864</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="4"/>
+        <v>0.80657359638272919</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" ht="12.75">
       <c r="B25">
         <v>19</v>
       </c>
@@ -23749,8 +24166,31 @@
       <c r="G25" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" ht="12.75">
+      <c r="L25">
+        <v>19</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>4.2479275134435852</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="1"/>
+        <v>1.2787536009528289</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="2"/>
+        <v>0.95257151061364553</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="3"/>
+        <v>0.82817179309666522</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="4"/>
+        <v>0.82166134175224848</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" ht="12.75">
       <c r="B26">
         <v>20</v>
       </c>
@@ -23763,8 +24203,31 @@
       <c r="G26" s="1">
         <v>1300</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" ht="12.75">
+      <c r="L26">
+        <v>20</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>4.3219280948873626</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="1"/>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="2"/>
+        <v>0.96916568399092229</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="3"/>
+        <v>0.84259887407451539</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="4"/>
+        <v>0.83597500808650516</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" ht="12.75">
       <c r="B27">
         <v>21</v>
       </c>
@@ -23777,8 +24240,31 @@
       <c r="G27" s="1">
         <v>1750</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" ht="12.75">
+      <c r="L27">
+        <v>30</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="0"/>
+        <v>4.9068905956085187</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>1.4771212547196624</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="2"/>
+        <v>1.1003399121765107</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="3"/>
+        <v>0.95664259105965532</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="4"/>
+        <v>0.94912220085196364</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" ht="12.75">
       <c r="B28">
         <v>22</v>
       </c>
@@ -23791,8 +24277,31 @@
       <c r="G28" s="1">
         <v>2500</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" ht="12.75">
+      <c r="L28">
+        <v>40</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>5.3219280948873626</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>1.6020599913279623</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="2"/>
+        <v>1.1934095082084977</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="3"/>
+        <v>1.0375578959683018</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="4"/>
+        <v>1.029401411703776</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" ht="12.75">
       <c r="B29">
         <v>23</v>
       </c>
@@ -23805,8 +24314,31 @@
       <c r="G29" s="1">
         <v>3000</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" ht="12.75">
+      <c r="L29">
+        <v>50</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="0"/>
+        <v>5.6438561897747244</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>1.6989700043360187</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="2"/>
+        <v>1.2655998953291183</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="3"/>
+        <v>1.1003206824676719</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="4"/>
+        <v>1.0916708053211979</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" ht="12.75">
       <c r="B30">
         <v>24</v>
       </c>
@@ -23819,8 +24351,31 @@
       <c r="G30" s="1">
         <v>3500</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" ht="12.75">
+      <c r="L30">
+        <v>60</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>5.9068905956085187</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>1.7781512503836436</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="2"/>
+        <v>1.324583736394086</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="3"/>
+        <v>1.1516016129534417</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="4"/>
+        <v>1.1425486044692343</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" ht="12.75">
       <c r="B31">
         <v>25</v>
       </c>
@@ -23833,8 +24388,31 @@
       <c r="G31" s="1">
         <v>4200</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" ht="12.75">
+      <c r="L31">
+        <v>70</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>6.1292830169449672</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>1.8450980400142569</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="2"/>
+        <v>1.3744538634315775</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="3"/>
+        <v>1.1949590218937864</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="4"/>
+        <v>1.1855651707200805</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" ht="12.75">
       <c r="B32">
         <v>26</v>
       </c>
@@ -23847,8 +24425,31 @@
       <c r="G32" s="1">
         <v>5000</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" ht="12.75">
+      <c r="L32">
+        <v>80</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>6.3219280948873617</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>1.9030899869919435</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="2"/>
+        <v>1.4176533324260729</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="3"/>
+        <v>1.2325169178620881</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="4"/>
+        <v>1.2228278153210468</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" ht="12.75">
       <c r="B33">
         <v>27</v>
       </c>
@@ -23861,8 +24462,31 @@
       <c r="G33" s="1">
         <v>6100</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" ht="12.75">
+      <c r="L33">
+        <v>90</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="0"/>
+        <v>6.4918530963296748</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>1.954242509439325</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="2"/>
+        <v>1.4557579645796743</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="3"/>
+        <v>1.2656453299385815</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="4"/>
+        <v>1.2556957972346927</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" ht="12.75">
       <c r="B34">
         <v>28</v>
       </c>
@@ -23875,8 +24499,31 @@
       <c r="G34" s="1">
         <v>7500</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" ht="12.75">
+      <c r="L34">
+        <v>100</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="0"/>
+        <v>6.6438561897747253</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="2"/>
+        <v>1.489843719546694</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="3"/>
+        <v>1.2952797043614583</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="4"/>
+        <v>1.2850972089384689</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" ht="12.75">
       <c r="B35">
         <v>29</v>
       </c>
@@ -23889,8 +24536,31 @@
       <c r="G35" s="28" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" ht="12.75">
+      <c r="L35">
+        <v>110</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="0"/>
+        <v>6.7813597135246599</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="1"/>
+        <v>2.0413926851582249</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="2"/>
+        <v>1.5206780355557714</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="3"/>
+        <v>1.3220872568586948</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="4"/>
+        <v>1.3116940210221208</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" ht="12.75">
       <c r="B36">
         <v>30</v>
       </c>
@@ -23903,8 +24573,31 @@
       <c r="G36" s="28" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L36">
+        <v>120</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="0"/>
+        <v>6.9068905956085187</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="1"/>
+        <v>2.0791812460476247</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="2"/>
+        <v>1.5488275606116615</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="3"/>
+        <v>1.3465606348472279</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="4"/>
+        <v>1.3359750080865052</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" ht="15.75" customHeight="1">
       <c r="B37">
         <v>31</v>
       </c>
@@ -23917,8 +24610,31 @@
       <c r="G37" s="28" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L37">
+        <v>130</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="0"/>
+        <v>7.0223678130284544</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="1"/>
+        <v>2.1139433523068369</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="2"/>
+        <v>1.5747226134559122</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="3"/>
+        <v>1.3690739602064348</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="4"/>
+        <v>1.358311350951773</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" ht="15.75" customHeight="1">
       <c r="B38">
         <v>32</v>
       </c>
@@ -23931,8 +24647,31 @@
       <c r="G38" s="28" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L38">
+        <v>140</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="0"/>
+        <v>7.1292830169449664</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="1"/>
+        <v>2.1461280356782382</v>
+      </c>
+      <c r="O38">
+        <f>LOG(L38,22)</f>
+        <v>1.5986976876491528</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="3"/>
+        <v>1.3899180437875727</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="4"/>
+        <v>1.3789915743373511</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" ht="15.75" customHeight="1">
       <c r="B39">
         <v>33</v>
       </c>
@@ -23945,8 +24684,31 @@
       <c r="G39" s="28" t="s">
         <v>1194</v>
       </c>
-    </row>
-    <row r="40" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L39">
+        <v>150</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="0"/>
+        <v>7.2288186904958804</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="1"/>
+        <v>2.1760912590556813</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="2"/>
+        <v>1.6210179477322819</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="3"/>
+        <v>1.4093234213465982</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="4"/>
+        <v>1.3982444017039271</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" ht="15.75" customHeight="1">
       <c r="B40">
         <v>34</v>
       </c>
@@ -23959,8 +24721,31 @@
       <c r="G40" s="28" t="s">
         <v>1195</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L40">
+        <v>160</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="0"/>
+        <v>7.3219280948873617</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="1"/>
+        <v>2.2041199826559246</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="2"/>
+        <v>1.6418971566436484</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="3"/>
+        <v>1.4274759397558743</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="4"/>
+        <v>1.4162542189383176</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" ht="15.75" customHeight="1">
       <c r="B41">
         <v>35</v>
       </c>
@@ -23973,8 +24758,31 @@
       <c r="G41" s="28" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L41">
+        <v>170</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="0"/>
+        <v>7.4093909361377026</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="1"/>
+        <v>2.2304489213782741</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="2"/>
+        <v>1.6615101586425596</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="3"/>
+        <v>1.4445276097380921</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="4"/>
+        <v>1.4331718417715191</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" ht="15.75" customHeight="1">
       <c r="B42">
         <v>36</v>
       </c>
@@ -23987,8 +24795,31 @@
       <c r="G42" s="28" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="43" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L42">
+        <v>180</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="0"/>
+        <v>7.4918530963296748</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="1"/>
+        <v>2.255272505103306</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="2"/>
+        <v>1.6800017887972498</v>
+      </c>
+      <c r="P42">
+        <f>LOG(L42,35)</f>
+        <v>1.4606043518323679</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="4"/>
+        <v>1.4491222008519635</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" ht="15.75" customHeight="1">
       <c r="B43">
         <v>37</v>
       </c>
@@ -24001,8 +24832,31 @@
       <c r="G43" s="28" t="s">
         <v>1196</v>
       </c>
-    </row>
-    <row r="44" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L43">
+        <v>190</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="0"/>
+        <v>7.5698556083309478</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="1"/>
+        <v>2.2787536009528289</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="2"/>
+        <v>1.6974933703869926</v>
+      </c>
+      <c r="P43">
+        <f>LOG(L43,35)</f>
+        <v>1.4758116452773944</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="4"/>
+        <v>1.4642099462214828</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" ht="15.75" customHeight="1">
       <c r="B44">
         <v>38</v>
       </c>
@@ -24015,8 +24869,31 @@
       <c r="G44" s="28" t="s">
         <v>1197</v>
       </c>
-    </row>
-    <row r="45" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L44">
+        <v>200</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="0"/>
+        <v>7.6438561897747244</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="1"/>
+        <v>2.3010299956639813</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="2"/>
+        <v>1.7140875437642691</v>
+      </c>
+      <c r="P44">
+        <f t="shared" ref="P44:P57" si="5">LOG(L44,35)</f>
+        <v>1.4902387262552446</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="4"/>
+        <v>1.4785236125557395</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" ht="15.75" customHeight="1">
       <c r="B45">
         <v>39</v>
       </c>
@@ -24029,8 +24906,31 @@
       <c r="G45" s="28" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L45">
+        <v>210</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="0"/>
+        <v>7.7142455176661224</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="1"/>
+        <v>2.3222192947339191</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="2"/>
+        <v>1.7298719158347411</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="5"/>
+        <v>1.5039617607727125</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="4"/>
+        <v>1.4921387671028095</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" ht="15.75" customHeight="1">
       <c r="B46">
         <v>40</v>
       </c>
@@ -24043,8 +24943,31 @@
       <c r="G46" s="28" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L46">
+        <v>220</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="0"/>
+        <v>7.7813597135246608</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="1"/>
+        <v>2.3424226808222062</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="2"/>
+        <v>1.7449218597733469</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="5"/>
+        <v>1.517046278752481</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="4"/>
+        <v>1.5051204246393917</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" ht="15.75" customHeight="1">
       <c r="B47">
         <v>41</v>
       </c>
@@ -24057,8 +24980,31 @@
       <c r="G47" s="28" t="s">
         <v>1198</v>
       </c>
-    </row>
-    <row r="48" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L47">
+        <v>230</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="0"/>
+        <v>7.8454900509443757</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="1"/>
+        <v>2.3617278360175931</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="2"/>
+        <v>1.7593026918847074</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="5"/>
+        <v>1.5295490666095473</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="4"/>
+        <v>1.5175249251692493</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" ht="15.75" customHeight="1">
       <c r="B48">
         <v>42</v>
       </c>
@@ -24071,8 +25017,31 @@
       <c r="G48" s="28" t="s">
         <v>1199</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L48">
+        <v>240</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="0"/>
+        <v>7.9068905956085187</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="1"/>
+        <v>2.3802112417116059</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="2"/>
+        <v>1.7730713848292368</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="5"/>
+        <v>1.5415196567410143</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="4"/>
+        <v>1.529401411703776</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" ht="15.75" customHeight="1">
       <c r="B49">
         <v>43</v>
       </c>
@@ -24085,8 +25054,31 @@
       <c r="G49" s="28" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L49">
+        <v>250</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="0"/>
+        <v>7.965784284662087</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="1"/>
+        <v>2.3979400086720375</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="2"/>
+        <v>1.7862779308848897</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="5"/>
+        <v>1.5530015127546146</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="4"/>
+        <v>1.5407930061731614</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" ht="15.75" customHeight="1">
       <c r="B50">
         <v>44</v>
       </c>
@@ -24099,8 +25091,31 @@
       <c r="G50" s="28" t="s">
         <v>1200</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L50">
+        <v>300</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="0"/>
+        <v>8.2288186904958813</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="1"/>
+        <v>2.4771212547196626</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="2"/>
+        <v>1.8452617719498574</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="5"/>
+        <v>1.6042824432403844</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="4"/>
+        <v>1.5916708053211979</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" ht="15.75" customHeight="1">
       <c r="B51">
         <v>45</v>
       </c>
@@ -24113,8 +25128,31 @@
       <c r="G51" s="28" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L51">
+        <v>350</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="0"/>
+        <v>8.451211111832329</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="1"/>
+        <v>2.5440680443502757</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="2"/>
+        <v>1.8951318989873487</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="5"/>
+        <v>1.6476398521807292</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="4"/>
+        <v>1.6346873715720438</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" ht="15.75" customHeight="1">
       <c r="B52">
         <v>46</v>
       </c>
@@ -24127,8 +25165,31 @@
       <c r="G52" s="28" t="s">
         <v>1201</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L52">
+        <v>400</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="0"/>
+        <v>8.6438561897747253</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="1"/>
+        <v>2.6020599913279625</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="2"/>
+        <v>1.9383313679818446</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="5"/>
+        <v>1.6851977481490308</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="4"/>
+        <v>1.6719500161730103</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17" ht="15.75" customHeight="1">
       <c r="B53">
         <v>47</v>
       </c>
@@ -24141,8 +25202,31 @@
       <c r="G53" s="28" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L53">
+        <v>450</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="0"/>
+        <v>8.8137811912170374</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="1"/>
+        <v>2.6532125137753435</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="2"/>
+        <v>1.9764360001354457</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="5"/>
+        <v>1.7183261602255244</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="4"/>
+        <v>1.7048179980866565</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" ht="15.75" customHeight="1">
       <c r="B54">
         <v>48</v>
       </c>
@@ -24155,8 +25239,31 @@
       <c r="G54" s="28" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L54">
+        <v>500</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="0"/>
+        <v>8.965784284662087</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="1"/>
+        <v>2.6989700043360187</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="2"/>
+        <v>2.0105217551024652</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="5"/>
+        <v>1.7479605346484011</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="4"/>
+        <v>1.7342194097904322</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" ht="15.75" customHeight="1">
       <c r="B55">
         <v>49</v>
       </c>
@@ -24169,8 +25276,31 @@
       <c r="G55" s="28" t="s">
         <v>1202</v>
       </c>
-    </row>
-    <row r="56" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L55">
+        <v>550</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="0"/>
+        <v>9.1032878084120217</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="1"/>
+        <v>2.7403626894942437</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="2"/>
+        <v>2.0413560711115428</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="5"/>
+        <v>1.7747680871456373</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="4"/>
+        <v>1.7608162218740842</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" ht="15.75" customHeight="1">
       <c r="B56">
         <v>50</v>
       </c>
@@ -24183,8 +25313,31 @@
       <c r="G56" s="28" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="57" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L56">
+        <v>600</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="0"/>
+        <v>9.2288186904958813</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="1"/>
+        <v>2.7781512503836434</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="2"/>
+        <v>2.0695055961674331</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="5"/>
+        <v>1.7992414651341708</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="4"/>
+        <v>1.7850972089384687</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" ht="15.75" customHeight="1">
       <c r="B57">
         <v>51</v>
       </c>
@@ -24197,8 +25350,31 @@
       <c r="G57" s="28" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="58" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L57">
+        <v>650</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="0"/>
+        <v>9.3442959079158179</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="1"/>
+        <v>2.8129133566428557</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="2"/>
+        <v>2.0954006490116837</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="5"/>
+        <v>1.8217547904933775</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="4"/>
+        <v>1.8074335518037365</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" ht="15.75" customHeight="1">
       <c r="B58">
         <v>52</v>
       </c>
@@ -24211,8 +25387,31 @@
       <c r="G58" s="28" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="59" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L58">
+        <v>700</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="0"/>
+        <v>9.451211111832329</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="1"/>
+        <v>2.8450980400142569</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="2"/>
+        <v>2.1193757232049242</v>
+      </c>
+      <c r="P58">
+        <f>LOG(L58,35)</f>
+        <v>1.8425988740745154</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="4"/>
+        <v>1.8281137751893146</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17" ht="15.75" customHeight="1">
       <c r="B59">
         <v>53</v>
       </c>
@@ -24225,8 +25424,31 @@
       <c r="G59" s="28" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="60" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L59">
+        <v>750</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="0"/>
+        <v>9.5507467853832431</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="1"/>
+        <v>2.8750612633917001</v>
+      </c>
+      <c r="O59">
+        <f>LOG(L59,22)</f>
+        <v>2.1416959832880536</v>
+      </c>
+      <c r="P59">
+        <f>LOG(L59,35)</f>
+        <v>1.8620042516335409</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="4"/>
+        <v>1.8473666025558908</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17" ht="15.75" customHeight="1">
       <c r="B60">
         <v>54</v>
       </c>
@@ -24239,8 +25461,31 @@
       <c r="G60" s="28" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="61" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L60">
+        <v>800</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="0"/>
+        <v>9.6438561897747253</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="1"/>
+        <v>2.9030899869919438</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="2"/>
+        <v>2.1625751921994198</v>
+      </c>
+      <c r="P60">
+        <f t="shared" ref="P60:P72" si="6">LOG(L60,35)</f>
+        <v>1.8801567700428172</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="4"/>
+        <v>1.8653764197902811</v>
+      </c>
+    </row>
+    <row r="61" spans="2:17" ht="15.75" customHeight="1">
       <c r="B61">
         <v>55</v>
       </c>
@@ -24253,8 +25498,31 @@
       <c r="G61" s="28" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="62" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L61">
+        <v>850</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="0"/>
+        <v>9.7313190310250643</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="1"/>
+        <v>2.9294189257142929</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="2"/>
+        <v>2.1821881941983312</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="6"/>
+        <v>1.8972084400250351</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="4"/>
+        <v>1.8822940426234827</v>
+      </c>
+    </row>
+    <row r="62" spans="2:17" ht="15.75" customHeight="1">
       <c r="B62">
         <v>56</v>
       </c>
@@ -24267,8 +25535,31 @@
       <c r="G62" s="28" t="s">
         <v>1203</v>
       </c>
-    </row>
-    <row r="63" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L62">
+        <v>900</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="0"/>
+        <v>9.8137811912170374</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="1"/>
+        <v>2.9542425094393248</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="2"/>
+        <v>2.2006798243530215</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="6"/>
+        <v>1.9132851821193106</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="4"/>
+        <v>1.8982444017039273</v>
+      </c>
+    </row>
+    <row r="63" spans="2:17" ht="15.75" customHeight="1">
       <c r="B63">
         <v>57</v>
       </c>
@@ -24281,8 +25572,31 @@
       <c r="G63" s="28" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="64" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L63">
+        <v>950</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="0"/>
+        <v>9.8917837032183105</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="1"/>
+        <v>2.9777236052888476</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="2"/>
+        <v>2.2181714059427642</v>
+      </c>
+      <c r="P63">
+        <f t="shared" si="6"/>
+        <v>1.9284924755643373</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="4"/>
+        <v>1.9133321470734466</v>
+      </c>
+    </row>
+    <row r="64" spans="2:17" ht="15.75" customHeight="1">
       <c r="B64">
         <v>58</v>
       </c>
@@ -24295,8 +25609,31 @@
       <c r="G64" s="28" t="s">
         <v>1204</v>
       </c>
-    </row>
-    <row r="65" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L64">
+        <v>1000</v>
+      </c>
+      <c r="M64">
+        <f t="shared" si="0"/>
+        <v>9.965784284662087</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="2"/>
+        <v>2.2347655793200407</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="6"/>
+        <v>1.9429195565421873</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="4"/>
+        <v>1.927645813407703</v>
+      </c>
+    </row>
+    <row r="65" spans="2:17" ht="15.75" customHeight="1">
       <c r="B65">
         <v>59</v>
       </c>
@@ -24309,8 +25646,31 @@
       <c r="G65" s="28" t="s">
         <v>1205</v>
       </c>
-    </row>
-    <row r="66" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L65">
+        <v>5000</v>
+      </c>
+      <c r="M65">
+        <f t="shared" si="0"/>
+        <v>12.287712379549451</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="1"/>
+        <v>3.6989700043360187</v>
+      </c>
+      <c r="O65">
+        <f>LOG(L65,22)</f>
+        <v>2.7554436148758126</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="6"/>
+        <v>2.3956003868291305</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="4"/>
+        <v>2.376768014259667</v>
+      </c>
+    </row>
+    <row r="66" spans="2:17" ht="15.75" customHeight="1">
       <c r="B66">
         <v>60</v>
       </c>
@@ -24323,8 +25683,31 @@
       <c r="G66" s="28" t="s">
         <v>1206</v>
       </c>
-    </row>
-    <row r="67" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L66">
+        <v>10000</v>
+      </c>
+      <c r="M66">
+        <f t="shared" si="0"/>
+        <v>13.287712379549451</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="2"/>
+        <v>2.9796874390933881</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="6"/>
+        <v>2.5905594087229167</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="4"/>
+        <v>2.5701944178769378</v>
+      </c>
+    </row>
+    <row r="67" spans="2:17" ht="15.75" customHeight="1">
       <c r="B67">
         <v>61</v>
       </c>
@@ -24337,8 +25720,31 @@
       <c r="G67" s="28" t="s">
         <v>1210</v>
       </c>
-    </row>
-    <row r="68" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L67">
+        <v>50000</v>
+      </c>
+      <c r="M67">
+        <f t="shared" si="0"/>
+        <v>15.609640474436812</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="1"/>
+        <v>4.6989700043360187</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="2"/>
+        <v>3.500365474649159</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="6"/>
+        <v>3.0432402390098594</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="4"/>
+        <v>3.0193166187289013</v>
+      </c>
+    </row>
+    <row r="68" spans="2:17" ht="15.75" customHeight="1">
       <c r="B68">
         <v>62</v>
       </c>
@@ -24351,8 +25757,31 @@
       <c r="G68" s="28" t="s">
         <v>1209</v>
       </c>
-    </row>
-    <row r="69" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L68">
+        <v>100000</v>
+      </c>
+      <c r="M68">
+        <f t="shared" si="0"/>
+        <v>16.609640474436812</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="2"/>
+        <v>3.7246092988667345</v>
+      </c>
+      <c r="P68">
+        <f t="shared" si="6"/>
+        <v>3.2381992609036456</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" si="4"/>
+        <v>3.2127430223461722</v>
+      </c>
+    </row>
+    <row r="69" spans="2:17" ht="15.75" customHeight="1">
       <c r="B69">
         <v>63</v>
       </c>
@@ -24365,8 +25794,31 @@
       <c r="G69" s="28" t="s">
         <v>1208</v>
       </c>
-    </row>
-    <row r="70" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L69">
+        <v>250000</v>
+      </c>
+      <c r="M69">
+        <f t="shared" si="0"/>
+        <v>17.931568569324174</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="1"/>
+        <v>5.3979400086720375</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="2"/>
+        <v>4.0210435102049304</v>
+      </c>
+      <c r="P69">
+        <f t="shared" si="6"/>
+        <v>3.4959210692968021</v>
+      </c>
+      <c r="Q69">
+        <f t="shared" si="4"/>
+        <v>3.4684388195808644</v>
+      </c>
+    </row>
+    <row r="70" spans="2:17" ht="15.75" customHeight="1">
       <c r="B70">
         <v>64</v>
       </c>
@@ -24379,8 +25831,31 @@
       <c r="G70" s="117" t="s">
         <v>1207</v>
       </c>
-    </row>
-    <row r="71" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L70">
+        <v>5000000</v>
+      </c>
+      <c r="M70">
+        <f t="shared" si="0"/>
+        <v>22.253496664211539</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="1"/>
+        <v>6.6989700043360187</v>
+      </c>
+      <c r="O70">
+        <f>LOG(L70,22)</f>
+        <v>4.9902091941958533</v>
+      </c>
+      <c r="P70">
+        <f t="shared" si="6"/>
+        <v>4.3385199433713177</v>
+      </c>
+      <c r="Q70">
+        <f t="shared" si="4"/>
+        <v>4.3044138276673705</v>
+      </c>
+    </row>
+    <row r="71" spans="2:17" ht="15.75" customHeight="1">
       <c r="B71">
         <v>65</v>
       </c>
@@ -24393,8 +25868,56 @@
       <c r="G71" s="28" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="76" spans="2:7" ht="15.75" customHeight="1">
+      <c r="L71">
+        <v>50000000</v>
+      </c>
+      <c r="M71">
+        <f t="shared" si="0"/>
+        <v>25.575424759098901</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="1"/>
+        <v>7.6989700043360187</v>
+      </c>
+      <c r="O71">
+        <f t="shared" si="2"/>
+        <v>5.7351310539691998</v>
+      </c>
+      <c r="P71">
+        <f t="shared" si="6"/>
+        <v>4.9861597955520471</v>
+      </c>
+      <c r="Q71">
+        <f t="shared" si="4"/>
+        <v>4.9469624321366039</v>
+      </c>
+    </row>
+    <row r="72" spans="2:17" ht="15.75" customHeight="1">
+      <c r="L72">
+        <v>500000000</v>
+      </c>
+      <c r="M72">
+        <f t="shared" ref="M72" si="7">LOG(L72,2)</f>
+        <v>28.897352853986263</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="1"/>
+        <v>8.6989700043360187</v>
+      </c>
+      <c r="O72">
+        <f t="shared" ref="O72" si="8">LOG(L72,22)</f>
+        <v>6.4800529137425471</v>
+      </c>
+      <c r="P72">
+        <f t="shared" si="6"/>
+        <v>5.6337996477327765</v>
+      </c>
+      <c r="Q72">
+        <f t="shared" si="4"/>
+        <v>5.5895110366058391</v>
+      </c>
+    </row>
+    <row r="76" spans="2:17" ht="15.75" customHeight="1">
       <c r="D76" t="s">
         <v>964</v>
       </c>
@@ -24615,8 +26138,8 @@
   </sheetPr>
   <dimension ref="C3:V305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H297" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K303" sqref="K303"/>
+    <sheetView topLeftCell="H197" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J266" sqref="J266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Research, Save Detector, Bugs and Balance
Implemented Research up to Nr. 50, Started adding research for up to 140.
Added Save Detector
Fixed refresh and scroll log bugs
Some balancing, new research and magic upgrades
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8FA7FF-63F0-4A82-9D22-561856A694AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B8B8B0-FB42-44F2-A409-69A8612E3605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,6 @@
     <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -4597,9 +4596,6 @@
     <t>Oak Woodcamps 60% Cheaper</t>
   </si>
   <si>
-    <t>Each achievement gives 0.45% WPS</t>
-  </si>
-  <si>
     <t>1 WC per 7 Beavers</t>
   </si>
   <si>
@@ -4612,9 +4608,6 @@
     <t>50% Maple Storage</t>
   </si>
   <si>
-    <t>10% Magic WPS and Storage Boost</t>
-  </si>
-  <si>
     <t>Unlock Ash</t>
   </si>
   <si>
@@ -4636,9 +4629,6 @@
     <t>10% Magic Gain</t>
   </si>
   <si>
-    <t>Wood per click +199</t>
-  </si>
-  <si>
     <t>Woodcamps 35% cheaper</t>
   </si>
   <si>
@@ -4744,9 +4734,6 @@
     <t>woodcamps use 6% less wood</t>
   </si>
   <si>
-    <t>Oak and Apple WPS 10%</t>
-  </si>
-  <si>
     <t>Maple and Spruce WPS 22%</t>
   </si>
   <si>
@@ -4840,9 +4827,6 @@
     <t>WC Effects 11.5%</t>
   </si>
   <si>
-    <t>1 Beaver Per 29 WC</t>
-  </si>
-  <si>
     <t>WC +1 Per 22 Beavers</t>
   </si>
   <si>
@@ -4925,6 +4909,21 @@
   </si>
   <si>
     <t>Improve wood price 33%</t>
+  </si>
+  <si>
+    <t>Each achievement gives +0.45% WPS</t>
+  </si>
+  <si>
+    <t>10% Magic WPS</t>
+  </si>
+  <si>
+    <t>Oak and Apple WPS 12%</t>
+  </si>
+  <si>
+    <t>Classic and Chestnut WPC +199</t>
+  </si>
+  <si>
+    <t>1 Beaver Per 11 WC</t>
   </si>
 </sst>
 </file>
@@ -22129,8 +22128,8 @@
   </sheetPr>
   <dimension ref="C2:P157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -22516,7 +22515,7 @@
         <v>20</v>
       </c>
       <c r="F24" s="115" t="s">
-        <v>1551</v>
+        <v>1548</v>
       </c>
       <c r="P24" s="27" t="s">
         <v>288</v>
@@ -22533,7 +22532,7 @@
         <v>21</v>
       </c>
       <c r="F25" t="s">
-        <v>1623</v>
+        <v>1618</v>
       </c>
       <c r="P25" s="41" t="s">
         <v>294</v>
@@ -22570,7 +22569,7 @@
         <v>23</v>
       </c>
       <c r="F27" t="s">
-        <v>1552</v>
+        <v>1549</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>140</v>
@@ -22627,7 +22626,7 @@
         <v>26</v>
       </c>
       <c r="F30" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>411</v>
@@ -22647,7 +22646,7 @@
         <v>27</v>
       </c>
       <c r="F31" t="s">
-        <v>1544</v>
+        <v>1541</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>171</v>
@@ -22667,7 +22666,7 @@
         <v>28</v>
       </c>
       <c r="F32" s="45" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>409</v>
@@ -22687,7 +22686,7 @@
         <v>29</v>
       </c>
       <c r="F33" s="35" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="H33" s="45" t="s">
         <v>678</v>
@@ -22707,7 +22706,7 @@
         <v>30</v>
       </c>
       <c r="F34" s="45" t="s">
-        <v>1546</v>
+        <v>1543</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>175</v>
@@ -22747,7 +22746,7 @@
         <v>32</v>
       </c>
       <c r="F36" s="46" t="s">
-        <v>1624</v>
+        <v>1619</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>168</v>
@@ -22767,7 +22766,7 @@
         <v>33</v>
       </c>
       <c r="F37" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="H37" s="45" t="s">
         <v>681</v>
@@ -22787,7 +22786,7 @@
         <v>34</v>
       </c>
       <c r="F38" s="46" t="s">
-        <v>1515</v>
+        <v>1620</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>178</v>
@@ -22821,7 +22820,7 @@
         <v>36</v>
       </c>
       <c r="F40" s="46" t="s">
-        <v>1566</v>
+        <v>1562</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>166</v>
@@ -22844,7 +22843,7 @@
         <v>37</v>
       </c>
       <c r="F41" s="46" t="s">
-        <v>1538</v>
+        <v>1535</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>176</v>
@@ -22867,7 +22866,7 @@
         <v>38</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>1545</v>
+        <v>1542</v>
       </c>
       <c r="H42" s="45" t="s">
         <v>682</v>
@@ -22913,7 +22912,7 @@
         <v>40</v>
       </c>
       <c r="F44" t="s">
-        <v>1520</v>
+        <v>1621</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>177</v>
@@ -22939,7 +22938,7 @@
         <v>41</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>1564</v>
+        <v>1622</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>167</v>
@@ -22965,7 +22964,7 @@
         <v>42</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>1547</v>
+        <v>1544</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>169</v>
@@ -22991,7 +22990,7 @@
         <v>43</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>1563</v>
+        <v>1560</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>170</v>
@@ -23017,7 +23016,7 @@
         <v>44</v>
       </c>
       <c r="F48" s="46" t="s">
-        <v>1567</v>
+        <v>1563</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>693</v>
@@ -23043,7 +23042,7 @@
         <v>45</v>
       </c>
       <c r="F49" s="45" t="s">
-        <v>1530</v>
+        <v>1527</v>
       </c>
       <c r="H49" s="45" t="s">
         <v>683</v>
@@ -23092,7 +23091,7 @@
         <v>47</v>
       </c>
       <c r="F51" t="s">
-        <v>1557</v>
+        <v>1554</v>
       </c>
       <c r="H51" s="45" t="s">
         <v>686</v>
@@ -23118,7 +23117,7 @@
         <v>48</v>
       </c>
       <c r="F52" s="46" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="H52" s="45" t="s">
         <v>687</v>
@@ -23168,7 +23167,7 @@
         <v>50</v>
       </c>
       <c r="F54" s="46" t="s">
-        <v>1528</v>
+        <v>1623</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>410</v>
@@ -23194,7 +23193,7 @@
         <v>51</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>1565</v>
+        <v>1561</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>164</v>
@@ -23220,7 +23219,7 @@
         <v>52</v>
       </c>
       <c r="F56" t="s">
-        <v>1549</v>
+        <v>1546</v>
       </c>
       <c r="H56" s="45" t="s">
         <v>685</v>
@@ -23246,7 +23245,7 @@
         <v>53</v>
       </c>
       <c r="F57" s="46" t="s">
-        <v>1541</v>
+        <v>1538</v>
       </c>
       <c r="M57" t="s">
         <v>1041</v>
@@ -23269,7 +23268,7 @@
         <v>54</v>
       </c>
       <c r="F58" s="46" t="s">
-        <v>1568</v>
+        <v>1564</v>
       </c>
       <c r="M58" t="s">
         <v>1036</v>
@@ -23292,7 +23291,7 @@
         <v>55</v>
       </c>
       <c r="F59" s="45" t="s">
-        <v>1529</v>
+        <v>1526</v>
       </c>
       <c r="M59" t="s">
         <v>1064</v>
@@ -23315,7 +23314,7 @@
         <v>56</v>
       </c>
       <c r="F60" s="46" t="s">
-        <v>1534</v>
+        <v>1531</v>
       </c>
       <c r="M60" t="s">
         <v>1065</v>
@@ -23338,7 +23337,7 @@
         <v>57</v>
       </c>
       <c r="F61" s="46" t="s">
-        <v>1531</v>
+        <v>1528</v>
       </c>
       <c r="M61" t="s">
         <v>1035</v>
@@ -23358,7 +23357,7 @@
         <v>58</v>
       </c>
       <c r="F62" s="46" t="s">
-        <v>1569</v>
+        <v>1565</v>
       </c>
       <c r="M62" t="s">
         <v>1043</v>
@@ -23378,7 +23377,7 @@
         <v>59</v>
       </c>
       <c r="F63" s="35" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="M63" t="s">
         <v>1030</v>
@@ -23398,7 +23397,7 @@
         <v>60</v>
       </c>
       <c r="F64" s="46" t="s">
-        <v>1532</v>
+        <v>1529</v>
       </c>
       <c r="M64" t="s">
         <v>1047</v>
@@ -23418,7 +23417,7 @@
         <v>61</v>
       </c>
       <c r="F65" s="47" t="s">
-        <v>1570</v>
+        <v>1566</v>
       </c>
       <c r="M65" t="s">
         <v>1044</v>
@@ -23438,7 +23437,7 @@
         <v>62</v>
       </c>
       <c r="F66" s="46" t="s">
-        <v>1571</v>
+        <v>1567</v>
       </c>
       <c r="M66" t="s">
         <v>1063</v>
@@ -23458,7 +23457,7 @@
         <v>63</v>
       </c>
       <c r="F67" s="45" t="s">
-        <v>1533</v>
+        <v>1530</v>
       </c>
       <c r="M67" t="s">
         <v>1048</v>
@@ -23475,7 +23474,7 @@
         <v>64</v>
       </c>
       <c r="F68" t="s">
-        <v>1560</v>
+        <v>1557</v>
       </c>
       <c r="M68" t="s">
         <v>1049</v>
@@ -23492,7 +23491,7 @@
         <v>65</v>
       </c>
       <c r="F69" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="M69" t="s">
         <v>1031</v>
@@ -23512,7 +23511,7 @@
         <v>66</v>
       </c>
       <c r="F70" s="45" t="s">
-        <v>1537</v>
+        <v>1534</v>
       </c>
       <c r="M70" t="s">
         <v>1057</v>
@@ -23526,7 +23525,7 @@
         <v>67</v>
       </c>
       <c r="F71" s="45" t="s">
-        <v>1562</v>
+        <v>1559</v>
       </c>
       <c r="M71" t="s">
         <v>1040</v>
@@ -23543,7 +23542,7 @@
         <v>68</v>
       </c>
       <c r="F72" s="45" t="s">
-        <v>1582</v>
+        <v>1578</v>
       </c>
       <c r="M72" t="s">
         <v>1062</v>
@@ -23560,7 +23559,7 @@
         <v>69</v>
       </c>
       <c r="F73" s="35" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="M73" t="s">
         <v>1050</v>
@@ -23580,7 +23579,7 @@
         <v>70</v>
       </c>
       <c r="F74" s="45" t="s">
-        <v>1587</v>
+        <v>1583</v>
       </c>
       <c r="M74" t="s">
         <v>1052</v>
@@ -23597,7 +23596,7 @@
         <v>71</v>
       </c>
       <c r="F75" s="45" t="s">
-        <v>1535</v>
+        <v>1532</v>
       </c>
       <c r="M75" t="s">
         <v>1058</v>
@@ -23614,7 +23613,7 @@
         <v>72</v>
       </c>
       <c r="F76" s="47" t="s">
-        <v>1574</v>
+        <v>1570</v>
       </c>
       <c r="M76" t="s">
         <v>1061</v>
@@ -23628,7 +23627,7 @@
         <v>73</v>
       </c>
       <c r="F77" s="45" t="s">
-        <v>1590</v>
+        <v>1586</v>
       </c>
       <c r="M77" t="s">
         <v>94</v>
@@ -23642,7 +23641,7 @@
         <v>74</v>
       </c>
       <c r="F78" s="45" t="s">
-        <v>1542</v>
+        <v>1539</v>
       </c>
       <c r="M78" t="s">
         <v>1070</v>
@@ -23656,7 +23655,7 @@
         <v>75</v>
       </c>
       <c r="F79" s="45" t="s">
-        <v>1584</v>
+        <v>1580</v>
       </c>
       <c r="M79" t="s">
         <v>1073</v>
@@ -23670,7 +23669,7 @@
         <v>76</v>
       </c>
       <c r="F80" t="s">
-        <v>1550</v>
+        <v>1547</v>
       </c>
       <c r="M80" t="s">
         <v>1075</v>
@@ -23684,7 +23683,7 @@
         <v>77</v>
       </c>
       <c r="F81" t="s">
-        <v>1588</v>
+        <v>1584</v>
       </c>
       <c r="M81" s="114" t="s">
         <v>1077</v>
@@ -23698,7 +23697,7 @@
         <v>78</v>
       </c>
       <c r="F82" t="s">
-        <v>1593</v>
+        <v>1589</v>
       </c>
       <c r="M82" t="s">
         <v>1079</v>
@@ -23723,7 +23722,7 @@
         <v>80</v>
       </c>
       <c r="F84" t="s">
-        <v>1612</v>
+        <v>1607</v>
       </c>
       <c r="M84" t="s">
         <v>1082</v>
@@ -23734,7 +23733,7 @@
         <v>81</v>
       </c>
       <c r="F85" s="45" t="s">
-        <v>1543</v>
+        <v>1540</v>
       </c>
       <c r="M85" t="s">
         <v>1083</v>
@@ -23748,7 +23747,7 @@
         <v>82</v>
       </c>
       <c r="F86" t="s">
-        <v>1561</v>
+        <v>1558</v>
       </c>
       <c r="M86" t="s">
         <v>1087</v>
@@ -23759,7 +23758,7 @@
         <v>83</v>
       </c>
       <c r="F87" t="s">
-        <v>1591</v>
+        <v>1587</v>
       </c>
       <c r="M87" t="s">
         <v>1092</v>
@@ -23770,7 +23769,7 @@
         <v>84</v>
       </c>
       <c r="F88" s="46" t="s">
-        <v>1539</v>
+        <v>1536</v>
       </c>
       <c r="M88" t="s">
         <v>1098</v>
@@ -23781,7 +23780,7 @@
         <v>85</v>
       </c>
       <c r="F89" t="s">
-        <v>1600</v>
+        <v>1595</v>
       </c>
       <c r="M89" t="s">
         <v>1102</v>
@@ -23792,7 +23791,7 @@
         <v>86</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="M90" t="s">
         <v>1109</v>
@@ -23803,7 +23802,7 @@
         <v>87</v>
       </c>
       <c r="F91" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
       <c r="M91" t="s">
         <v>1110</v>
@@ -23814,7 +23813,7 @@
         <v>88</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>1596</v>
+        <v>1624</v>
       </c>
       <c r="M92" t="s">
         <v>1118</v>
@@ -23825,7 +23824,7 @@
         <v>89</v>
       </c>
       <c r="F93" s="35" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="M93" t="s">
         <v>1113</v>
@@ -23836,7 +23835,7 @@
         <v>90</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>1604</v>
+        <v>1599</v>
       </c>
       <c r="M94" t="s">
         <v>1119</v>
@@ -23847,7 +23846,7 @@
         <v>91</v>
       </c>
       <c r="F95" t="s">
-        <v>1558</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="96" spans="5:16" ht="15.75" customHeight="1">
@@ -23855,7 +23854,7 @@
         <v>92</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>1606</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="97" spans="5:6" ht="15.75" customHeight="1">
@@ -23863,7 +23862,7 @@
         <v>93</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>1613</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="98" spans="5:6" ht="15.75" customHeight="1">
@@ -23871,7 +23870,7 @@
         <v>94</v>
       </c>
       <c r="F98" s="45" t="s">
-        <v>1592</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="99" spans="5:6" ht="15.75" customHeight="1">
@@ -23879,7 +23878,7 @@
         <v>95</v>
       </c>
       <c r="F99" s="47" t="s">
-        <v>1575</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="100" spans="5:6" ht="15.75" customHeight="1">
@@ -23887,7 +23886,7 @@
         <v>96</v>
       </c>
       <c r="F100" s="122" t="s">
-        <v>1548</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="101" spans="5:6" ht="15.75" customHeight="1">
@@ -23895,7 +23894,7 @@
         <v>97</v>
       </c>
       <c r="F101" s="45" t="s">
-        <v>1607</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="102" spans="5:6" ht="15.75" customHeight="1">
@@ -23903,7 +23902,7 @@
         <v>98</v>
       </c>
       <c r="F102" s="45" t="s">
-        <v>1610</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="103" spans="5:6" ht="15.75" customHeight="1">
@@ -23919,7 +23918,7 @@
         <v>100</v>
       </c>
       <c r="F104" t="s">
-        <v>1579</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="105" spans="5:6" ht="15.75" customHeight="1">
@@ -23927,7 +23926,7 @@
         <v>101</v>
       </c>
       <c r="F105" t="s">
-        <v>1603</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="106" spans="5:6" ht="15.75" customHeight="1">
@@ -23935,7 +23934,7 @@
         <v>102</v>
       </c>
       <c r="F106" t="s">
-        <v>1594</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="107" spans="5:6" ht="15.75" customHeight="1">
@@ -23943,7 +23942,7 @@
         <v>103</v>
       </c>
       <c r="F107" t="s">
-        <v>1589</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="108" spans="5:6" ht="15.75" customHeight="1">
@@ -23951,7 +23950,7 @@
         <v>104</v>
       </c>
       <c r="F108" t="s">
-        <v>1598</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="109" spans="5:6" ht="15.75" customHeight="1">
@@ -23959,7 +23958,7 @@
         <v>105</v>
       </c>
       <c r="F109" t="s">
-        <v>1583</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="110" spans="5:6" ht="15.75" customHeight="1">
@@ -23967,7 +23966,7 @@
         <v>106</v>
       </c>
       <c r="F110" t="s">
-        <v>1601</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="111" spans="5:6" ht="15.75" customHeight="1">
@@ -23975,7 +23974,7 @@
         <v>107</v>
       </c>
       <c r="F111" t="s">
-        <v>1597</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="112" spans="5:6" ht="15.75" customHeight="1">
@@ -23983,7 +23982,7 @@
         <v>108</v>
       </c>
       <c r="F112" t="s">
-        <v>1611</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="113" spans="5:6" ht="15.75" customHeight="1">
@@ -23991,7 +23990,7 @@
         <v>109</v>
       </c>
       <c r="F113" s="35" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="114" spans="5:6" ht="15.75" customHeight="1">
@@ -23999,7 +23998,7 @@
         <v>110</v>
       </c>
       <c r="F114" s="45" t="s">
-        <v>1536</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="115" spans="5:6" ht="15.75" customHeight="1">
@@ -24007,7 +24006,7 @@
         <v>111</v>
       </c>
       <c r="F115" t="s">
-        <v>1608</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="116" spans="5:6" ht="15.75" customHeight="1">
@@ -24015,7 +24014,7 @@
         <v>112</v>
       </c>
       <c r="F116" t="s">
-        <v>1614</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="117" spans="5:6" ht="15.75" customHeight="1">
@@ -24023,7 +24022,7 @@
         <v>113</v>
       </c>
       <c r="F117" t="s">
-        <v>1602</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="118" spans="5:6" ht="15.75" customHeight="1">
@@ -24031,7 +24030,7 @@
         <v>114</v>
       </c>
       <c r="F118" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="119" spans="5:6" ht="15.75" customHeight="1">
@@ -24039,7 +24038,7 @@
         <v>115</v>
       </c>
       <c r="F119" t="s">
-        <v>1585</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="120" spans="5:6" ht="15.75" customHeight="1">
@@ -24047,7 +24046,7 @@
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>1615</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="121" spans="5:6" ht="15.75" customHeight="1">
@@ -24055,7 +24054,7 @@
         <v>117</v>
       </c>
       <c r="F121" s="46" t="s">
-        <v>1540</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="122" spans="5:6" ht="15.75" customHeight="1">
@@ -24063,7 +24062,7 @@
         <v>118</v>
       </c>
       <c r="F122" t="s">
-        <v>1609</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="123" spans="5:6" ht="15.75" customHeight="1">
@@ -24071,7 +24070,7 @@
         <v>119</v>
       </c>
       <c r="F123" s="35" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="124" spans="5:6" ht="15.75" customHeight="1">
@@ -24079,7 +24078,7 @@
         <v>120</v>
       </c>
       <c r="F124" t="s">
-        <v>1580</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="125" spans="5:6" ht="15.75" customHeight="1">
@@ -24087,7 +24086,7 @@
         <v>121</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>1616</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="126" spans="5:6" ht="15.75" customHeight="1">
@@ -24095,7 +24094,7 @@
         <v>122</v>
       </c>
       <c r="F126" t="s">
-        <v>1578</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="127" spans="5:6" ht="15.75" customHeight="1">
@@ -24103,7 +24102,7 @@
         <v>123</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>1618</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="128" spans="5:6" ht="15.75" customHeight="1">
@@ -24111,7 +24110,7 @@
         <v>124</v>
       </c>
       <c r="F128" t="s">
-        <v>1559</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="129" spans="5:6" ht="15.75" customHeight="1">
@@ -24119,7 +24118,7 @@
         <v>125</v>
       </c>
       <c r="F129" t="s">
-        <v>1599</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="130" spans="5:6" ht="15.75" customHeight="1">
@@ -24127,7 +24126,7 @@
         <v>126</v>
       </c>
       <c r="F130" s="47" t="s">
-        <v>1576</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="131" spans="5:6" ht="15.75" customHeight="1">
@@ -24135,7 +24134,7 @@
         <v>127</v>
       </c>
       <c r="F131" t="s">
-        <v>1617</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="132" spans="5:6" ht="15.75" customHeight="1">
@@ -24143,7 +24142,7 @@
         <v>128</v>
       </c>
       <c r="F132" t="s">
-        <v>1586</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="133" spans="5:6" ht="15.75" customHeight="1">
@@ -24151,7 +24150,7 @@
         <v>129</v>
       </c>
       <c r="F133" s="35" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="134" spans="5:6" ht="15.75" customHeight="1">
@@ -24159,7 +24158,7 @@
         <v>130</v>
       </c>
       <c r="F134" t="s">
-        <v>1619</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="135" spans="5:6" ht="15.75" customHeight="1">
@@ -24167,7 +24166,7 @@
         <v>131</v>
       </c>
       <c r="F135" t="s">
-        <v>1555</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="136" spans="5:6" ht="15.75" customHeight="1">
@@ -24175,7 +24174,7 @@
         <v>132</v>
       </c>
       <c r="F136" t="s">
-        <v>1620</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="137" spans="5:6" ht="15.75" customHeight="1">
@@ -24183,7 +24182,7 @@
         <v>133</v>
       </c>
       <c r="F137" t="s">
-        <v>1573</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="138" spans="5:6" ht="15.75" customHeight="1">
@@ -24199,7 +24198,7 @@
         <v>135</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>1554</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="140" spans="5:6" ht="15.75" customHeight="1">
@@ -24207,7 +24206,7 @@
         <v>136</v>
       </c>
       <c r="F140" t="s">
-        <v>1621</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="141" spans="5:6" ht="15.75" customHeight="1">
@@ -24215,7 +24214,7 @@
         <v>137</v>
       </c>
       <c r="F141" t="s">
-        <v>1605</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="142" spans="5:6" ht="15.75" customHeight="1">
@@ -24223,7 +24222,7 @@
         <v>138</v>
       </c>
       <c r="F142" t="s">
-        <v>1572</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="143" spans="5:6" ht="15.75" customHeight="1">
@@ -24231,7 +24230,7 @@
         <v>139</v>
       </c>
       <c r="F143" t="s">
-        <v>1622</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="144" spans="5:6" ht="15.75" customHeight="1">
@@ -24239,7 +24238,7 @@
         <v>140</v>
       </c>
       <c r="F144" t="s">
-        <v>1556</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="145" spans="5:5" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Bug fixes and balancing
Fixed component and value updates not happening / being slow.
Added a new research item.
Balancing
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B8B8B0-FB42-44F2-A409-69A8612E3605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2208E698-0890-4EBD-92CD-D8F10A33BC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -22128,7 +22128,7 @@
   </sheetPr>
   <dimension ref="C2:P157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A134" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
@@ -24744,10 +24744,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A4:Q76"/>
+  <dimension ref="A4:S76"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -24757,7 +24757,7 @@
     <col min="5" max="5" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:17" ht="12.75">
+    <row r="4" spans="1:19" ht="12.75">
       <c r="A4" t="s">
         <v>1136</v>
       </c>
@@ -24765,7 +24765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="12.75">
+    <row r="6" spans="1:19" ht="12.75">
       <c r="C6" s="1" t="s">
         <v>52</v>
       </c>
@@ -24788,7 +24788,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="12.75">
+    <row r="7" spans="1:19" ht="12.75">
       <c r="A7">
         <v>1</v>
       </c>
@@ -24833,8 +24833,12 @@
         <f>LOG(L7,7) / 2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="12.75">
+      <c r="R7">
+        <f>ROUND(LOG(L7,20),3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="12.75">
       <c r="B8">
         <v>2</v>
       </c>
@@ -24876,8 +24880,16 @@
         <f>LOG(L8,6) / 2</f>
         <v>0.19342640361727079</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" ht="12.75">
+      <c r="R8">
+        <f t="shared" ref="R8:R71" si="3">ROUND(LOG(L8,20),3)</f>
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="S8">
+        <f>ROUND(LOG(L8,17),3)</f>
+        <v>0.245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="12.75">
       <c r="B9">
         <v>3</v>
       </c>
@@ -24912,15 +24924,23 @@
         <v>0.35541805240316376</v>
       </c>
       <c r="P9">
-        <f t="shared" ref="P9:P41" si="3">LOG(L9,35)</f>
+        <f t="shared" ref="P9:P41" si="4">LOG(L9,35)</f>
         <v>0.30900273887892621</v>
       </c>
       <c r="Q9">
-        <f t="shared" ref="Q9:Q72" si="4">LOG(L9,6) / 2</f>
+        <f t="shared" ref="Q9:Q72" si="5">LOG(L9,6) / 2</f>
         <v>0.30657359638272924</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" ht="12.75">
+      <c r="R9">
+        <f t="shared" si="3"/>
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="S9">
+        <f t="shared" ref="S9:S72" si="6">ROUND(LOG(L9,17),3)</f>
+        <v>0.38800000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="12.75">
       <c r="B10">
         <v>4</v>
       </c>
@@ -24955,15 +24975,23 @@
         <v>0.44848764843515082</v>
       </c>
       <c r="P10">
+        <f t="shared" si="4"/>
+        <v>0.38991804378757261</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="5"/>
+        <v>0.38685280723454157</v>
+      </c>
+      <c r="R10">
         <f t="shared" si="3"/>
-        <v>0.38991804378757261</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="4"/>
-        <v>0.38685280723454157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="12.75">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="6"/>
+        <v>0.48899999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="12.75">
       <c r="B11">
         <v>5</v>
       </c>
@@ -24992,15 +25020,23 @@
         <v>0.52067803555577141</v>
       </c>
       <c r="P11">
+        <f t="shared" si="4"/>
+        <v>0.45268083028694278</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="5"/>
+        <v>0.44912220085196358</v>
+      </c>
+      <c r="R11">
         <f t="shared" si="3"/>
-        <v>0.45268083028694278</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="4"/>
-        <v>0.44912220085196358</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="12.75">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="6"/>
+        <v>0.56799999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="12.75">
       <c r="B12">
         <v>6</v>
       </c>
@@ -25029,15 +25065,23 @@
         <v>0.57966187662073909</v>
       </c>
       <c r="P12">
+        <f t="shared" si="4"/>
+        <v>0.50396176077271249</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="R12">
         <f t="shared" si="3"/>
-        <v>0.50396176077271249</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="12.75">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="6"/>
+        <v>0.63200000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="12.75">
       <c r="B13">
         <v>7</v>
       </c>
@@ -25066,15 +25110,23 @@
         <v>0.62953200365823048</v>
       </c>
       <c r="P13">
+        <f t="shared" si="4"/>
+        <v>0.54731916971305716</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="5"/>
+        <v>0.54301656625084593</v>
+      </c>
+      <c r="R13">
         <f t="shared" si="3"/>
-        <v>0.54731916971305716</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="4"/>
-        <v>0.54301656625084593</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="12.75">
+        <v>0.65</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="6"/>
+        <v>0.68700000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="12.75">
       <c r="B14">
         <v>8</v>
       </c>
@@ -25103,15 +25155,23 @@
         <v>0.67273147265272626</v>
       </c>
       <c r="P14">
+        <f t="shared" si="4"/>
+        <v>0.58487706568135889</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="5"/>
+        <v>0.58027921085181233</v>
+      </c>
+      <c r="R14">
         <f t="shared" si="3"/>
-        <v>0.58487706568135889</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="4"/>
-        <v>0.58027921085181233</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="12.75">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="6"/>
+        <v>0.73399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="12.75">
       <c r="B15">
         <v>9</v>
       </c>
@@ -25140,15 +25200,23 @@
         <v>0.71083610480632753</v>
       </c>
       <c r="P15">
+        <f t="shared" si="4"/>
+        <v>0.61800547775785242</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="5"/>
+        <v>0.61314719276545848</v>
+      </c>
+      <c r="R15">
         <f t="shared" si="3"/>
-        <v>0.61800547775785242</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="4"/>
-        <v>0.61314719276545848</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="12.75">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="6"/>
+        <v>0.77600000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="12.75">
       <c r="B16">
         <v>10</v>
       </c>
@@ -25177,15 +25245,23 @@
         <v>0.74492185977334702</v>
       </c>
       <c r="P16">
+        <f t="shared" si="4"/>
+        <v>0.64763985218072917</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="5"/>
+        <v>0.64254860446923445</v>
+      </c>
+      <c r="R16">
         <f t="shared" si="3"/>
-        <v>0.64763985218072917</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="4"/>
-        <v>0.64254860446923445</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" ht="12.75">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="6"/>
+        <v>0.81299999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" ht="12.75">
       <c r="B17">
         <v>11</v>
       </c>
@@ -25214,15 +25290,23 @@
         <v>0.77575617578242451</v>
       </c>
       <c r="P17">
+        <f t="shared" si="4"/>
+        <v>0.67444740467796549</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="5"/>
+        <v>0.66914541655288629</v>
+      </c>
+      <c r="R17">
         <f t="shared" si="3"/>
-        <v>0.67444740467796549</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="4"/>
-        <v>0.66914541655288629</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" ht="12.75">
+        <v>0.8</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="6"/>
+        <v>0.84599999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" ht="12.75">
       <c r="B18">
         <v>12</v>
       </c>
@@ -25251,15 +25335,23 @@
         <v>0.80390570083831459</v>
       </c>
       <c r="P18">
+        <f t="shared" si="4"/>
+        <v>0.69892078266649882</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="5"/>
+        <v>0.69342640361727081</v>
+      </c>
+      <c r="R18">
         <f t="shared" si="3"/>
-        <v>0.69892078266649882</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="4"/>
-        <v>0.69342640361727081</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17" ht="12.75">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="6"/>
+        <v>0.877</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" ht="12.75">
       <c r="B19">
         <v>13</v>
       </c>
@@ -25288,15 +25380,23 @@
         <v>0.82980075368256545</v>
       </c>
       <c r="P19">
+        <f t="shared" si="4"/>
+        <v>0.72143410802570562</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="5"/>
+        <v>0.71576274648253868</v>
+      </c>
+      <c r="R19">
         <f t="shared" si="3"/>
-        <v>0.72143410802570562</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="4"/>
-        <v>0.71576274648253868</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" ht="12.75">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="6"/>
+        <v>0.90500000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" ht="12.75">
       <c r="B20">
         <v>14</v>
       </c>
@@ -25325,15 +25425,23 @@
         <v>0.85377582787580586</v>
       </c>
       <c r="P20">
+        <f t="shared" si="4"/>
+        <v>0.7422781916068435</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="5"/>
+        <v>0.73644296986811664</v>
+      </c>
+      <c r="R20">
         <f t="shared" si="3"/>
-        <v>0.7422781916068435</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="4"/>
-        <v>0.73644296986811664</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" ht="12.75">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="6"/>
+        <v>0.93100000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" ht="12.75">
       <c r="B21">
         <v>15</v>
       </c>
@@ -25362,15 +25470,23 @@
         <v>0.87609608795893523</v>
       </c>
       <c r="P21">
+        <f t="shared" si="4"/>
+        <v>0.76168356916586899</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="5"/>
+        <v>0.75569579723469282</v>
+      </c>
+      <c r="R21">
         <f t="shared" si="3"/>
-        <v>0.76168356916586899</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="4"/>
-        <v>0.75569579723469282</v>
-      </c>
-    </row>
-    <row r="22" spans="2:17" ht="12.75">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="6"/>
+        <v>0.95599999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" ht="12.75">
       <c r="B22">
         <v>16</v>
       </c>
@@ -25399,15 +25515,23 @@
         <v>0.89697529687030164</v>
       </c>
       <c r="P22">
+        <f t="shared" si="4"/>
+        <v>0.77983608757514522</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="5"/>
+        <v>0.77370561446908315</v>
+      </c>
+      <c r="R22">
         <f t="shared" si="3"/>
-        <v>0.77983608757514522</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="4"/>
-        <v>0.77370561446908315</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17" ht="12.75">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="6"/>
+        <v>0.97899999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" ht="12.75">
       <c r="B23">
         <v>17</v>
       </c>
@@ -25436,15 +25560,23 @@
         <v>0.91658829886921256</v>
       </c>
       <c r="P23">
+        <f t="shared" si="4"/>
+        <v>0.79688775755736296</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="5"/>
+        <v>0.79062323730228468</v>
+      </c>
+      <c r="R23">
         <f t="shared" si="3"/>
-        <v>0.79688775755736296</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="4"/>
-        <v>0.79062323730228468</v>
-      </c>
-    </row>
-    <row r="24" spans="2:17" ht="12.75">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" ht="12.75">
       <c r="B24">
         <v>18</v>
       </c>
@@ -25473,15 +25605,23 @@
         <v>0.9350799290239028</v>
       </c>
       <c r="P24">
+        <f t="shared" si="4"/>
+        <v>0.81296449965163864</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="5"/>
+        <v>0.80657359638272919</v>
+      </c>
+      <c r="R24">
         <f t="shared" si="3"/>
-        <v>0.81296449965163864</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="4"/>
-        <v>0.80657359638272919</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17" ht="12.75">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="6"/>
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" ht="12.75">
       <c r="B25">
         <v>19</v>
       </c>
@@ -25510,15 +25650,23 @@
         <v>0.95257151061364553</v>
       </c>
       <c r="P25">
+        <f t="shared" si="4"/>
+        <v>0.82817179309666522</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="5"/>
+        <v>0.82166134175224848</v>
+      </c>
+      <c r="R25">
         <f t="shared" si="3"/>
-        <v>0.82817179309666522</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="4"/>
-        <v>0.82166134175224848</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17" ht="12.75">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="6"/>
+        <v>1.0389999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" ht="12.75">
       <c r="B26">
         <v>20</v>
       </c>
@@ -25547,15 +25695,23 @@
         <v>0.96916568399092229</v>
       </c>
       <c r="P26">
+        <f t="shared" si="4"/>
+        <v>0.84259887407451539</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="5"/>
+        <v>0.83597500808650516</v>
+      </c>
+      <c r="R26">
         <f t="shared" si="3"/>
-        <v>0.84259887407451539</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="4"/>
-        <v>0.83597500808650516</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17" ht="12.75">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="6"/>
+        <v>1.0569999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" ht="12.75">
       <c r="B27">
         <v>21</v>
       </c>
@@ -25584,15 +25740,23 @@
         <v>1.1003399121765107</v>
       </c>
       <c r="P27">
+        <f t="shared" si="4"/>
+        <v>0.95664259105965532</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="5"/>
+        <v>0.94912220085196364</v>
+      </c>
+      <c r="R27">
         <f t="shared" si="3"/>
-        <v>0.95664259105965532</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="4"/>
-        <v>0.94912220085196364</v>
-      </c>
-    </row>
-    <row r="28" spans="2:17" ht="12.75">
+        <v>1.135</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="6"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" ht="12.75">
       <c r="B28">
         <v>22</v>
       </c>
@@ -25621,15 +25785,23 @@
         <v>1.1934095082084977</v>
       </c>
       <c r="P28">
+        <f t="shared" si="4"/>
+        <v>1.0375578959683018</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="5"/>
+        <v>1.029401411703776</v>
+      </c>
+      <c r="R28">
         <f t="shared" si="3"/>
-        <v>1.0375578959683018</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="4"/>
-        <v>1.029401411703776</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17" ht="12.75">
+        <v>1.2310000000000001</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="6"/>
+        <v>1.302</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" ht="12.75">
       <c r="B29">
         <v>23</v>
       </c>
@@ -25658,15 +25830,23 @@
         <v>1.2655998953291183</v>
       </c>
       <c r="P29">
+        <f t="shared" si="4"/>
+        <v>1.1003206824676719</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="5"/>
+        <v>1.0916708053211979</v>
+      </c>
+      <c r="R29">
         <f t="shared" si="3"/>
-        <v>1.1003206824676719</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="4"/>
-        <v>1.0916708053211979</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17" ht="12.75">
+        <v>1.306</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="6"/>
+        <v>1.381</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" ht="12.75">
       <c r="B30">
         <v>24</v>
       </c>
@@ -25695,15 +25875,23 @@
         <v>1.324583736394086</v>
       </c>
       <c r="P30">
+        <f t="shared" si="4"/>
+        <v>1.1516016129534417</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="5"/>
+        <v>1.1425486044692343</v>
+      </c>
+      <c r="R30">
         <f t="shared" si="3"/>
-        <v>1.1516016129534417</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" si="4"/>
-        <v>1.1425486044692343</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17" ht="12.75">
+        <v>1.367</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="6"/>
+        <v>1.4450000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" ht="12.75">
       <c r="B31">
         <v>25</v>
       </c>
@@ -25732,15 +25920,23 @@
         <v>1.3744538634315775</v>
       </c>
       <c r="P31">
+        <f t="shared" si="4"/>
+        <v>1.1949590218937864</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="5"/>
+        <v>1.1855651707200805</v>
+      </c>
+      <c r="R31">
         <f t="shared" si="3"/>
-        <v>1.1949590218937864</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="4"/>
-        <v>1.1855651707200805</v>
-      </c>
-    </row>
-    <row r="32" spans="2:17" ht="12.75">
+        <v>1.4179999999999999</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="6"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" ht="12.75">
       <c r="B32">
         <v>26</v>
       </c>
@@ -25769,15 +25965,23 @@
         <v>1.4176533324260729</v>
       </c>
       <c r="P32">
+        <f t="shared" si="4"/>
+        <v>1.2325169178620881</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="5"/>
+        <v>1.2228278153210468</v>
+      </c>
+      <c r="R32">
         <f t="shared" si="3"/>
-        <v>1.2325169178620881</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="4"/>
-        <v>1.2228278153210468</v>
-      </c>
-    </row>
-    <row r="33" spans="2:17" ht="12.75">
+        <v>1.4630000000000001</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="6"/>
+        <v>1.5469999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:19" ht="12.75">
       <c r="B33">
         <v>27</v>
       </c>
@@ -25806,15 +26010,23 @@
         <v>1.4557579645796743</v>
       </c>
       <c r="P33">
+        <f t="shared" si="4"/>
+        <v>1.2656453299385815</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="5"/>
+        <v>1.2556957972346927</v>
+      </c>
+      <c r="R33">
         <f t="shared" si="3"/>
-        <v>1.2656453299385815</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="4"/>
-        <v>1.2556957972346927</v>
-      </c>
-    </row>
-    <row r="34" spans="2:17" ht="12.75">
+        <v>1.502</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="6"/>
+        <v>1.5880000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" ht="12.75">
       <c r="B34">
         <v>28</v>
       </c>
@@ -25843,15 +26055,23 @@
         <v>1.489843719546694</v>
       </c>
       <c r="P34">
+        <f t="shared" si="4"/>
+        <v>1.2952797043614583</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="5"/>
+        <v>1.2850972089384689</v>
+      </c>
+      <c r="R34">
         <f t="shared" si="3"/>
-        <v>1.2952797043614583</v>
-      </c>
-      <c r="Q34">
-        <f t="shared" si="4"/>
-        <v>1.2850972089384689</v>
-      </c>
-    </row>
-    <row r="35" spans="2:17" ht="12.75">
+        <v>1.5369999999999999</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="6"/>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19" ht="12.75">
       <c r="B35">
         <v>29</v>
       </c>
@@ -25880,15 +26100,23 @@
         <v>1.5206780355557714</v>
       </c>
       <c r="P35">
+        <f t="shared" si="4"/>
+        <v>1.3220872568586948</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="5"/>
+        <v>1.3116940210221208</v>
+      </c>
+      <c r="R35">
         <f t="shared" si="3"/>
-        <v>1.3220872568586948</v>
-      </c>
-      <c r="Q35">
-        <f t="shared" si="4"/>
-        <v>1.3116940210221208</v>
-      </c>
-    </row>
-    <row r="36" spans="2:17" ht="12.75">
+        <v>1.569</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="6"/>
+        <v>1.659</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" ht="12.75">
       <c r="B36">
         <v>30</v>
       </c>
@@ -25917,15 +26145,23 @@
         <v>1.5488275606116615</v>
       </c>
       <c r="P36">
+        <f t="shared" si="4"/>
+        <v>1.3465606348472279</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="5"/>
+        <v>1.3359750080865052</v>
+      </c>
+      <c r="R36">
         <f t="shared" si="3"/>
-        <v>1.3465606348472279</v>
-      </c>
-      <c r="Q36">
-        <f t="shared" si="4"/>
-        <v>1.3359750080865052</v>
-      </c>
-    </row>
-    <row r="37" spans="2:17" ht="15.75" customHeight="1">
+        <v>1.5980000000000001</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="6"/>
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" ht="15.75" customHeight="1">
       <c r="B37">
         <v>31</v>
       </c>
@@ -25954,15 +26190,23 @@
         <v>1.5747226134559122</v>
       </c>
       <c r="P37">
+        <f t="shared" si="4"/>
+        <v>1.3690739602064348</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="5"/>
+        <v>1.358311350951773</v>
+      </c>
+      <c r="R37">
         <f t="shared" si="3"/>
-        <v>1.3690739602064348</v>
-      </c>
-      <c r="Q37">
-        <f t="shared" si="4"/>
-        <v>1.358311350951773</v>
-      </c>
-    </row>
-    <row r="38" spans="2:17" ht="15.75" customHeight="1">
+        <v>1.625</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="6"/>
+        <v>1.718</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19" ht="15.75" customHeight="1">
       <c r="B38">
         <v>32</v>
       </c>
@@ -25991,15 +26235,23 @@
         <v>1.5986976876491528</v>
       </c>
       <c r="P38">
+        <f t="shared" si="4"/>
+        <v>1.3899180437875727</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="5"/>
+        <v>1.3789915743373511</v>
+      </c>
+      <c r="R38">
         <f t="shared" si="3"/>
-        <v>1.3899180437875727</v>
-      </c>
-      <c r="Q38">
-        <f t="shared" si="4"/>
-        <v>1.3789915743373511</v>
-      </c>
-    </row>
-    <row r="39" spans="2:17" ht="15.75" customHeight="1">
+        <v>1.65</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="6"/>
+        <v>1.744</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19" ht="15.75" customHeight="1">
       <c r="B39">
         <v>33</v>
       </c>
@@ -26028,15 +26280,23 @@
         <v>1.6210179477322819</v>
       </c>
       <c r="P39">
+        <f t="shared" si="4"/>
+        <v>1.4093234213465982</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="5"/>
+        <v>1.3982444017039271</v>
+      </c>
+      <c r="R39">
         <f t="shared" si="3"/>
-        <v>1.4093234213465982</v>
-      </c>
-      <c r="Q39">
-        <f t="shared" si="4"/>
-        <v>1.3982444017039271</v>
-      </c>
-    </row>
-    <row r="40" spans="2:17" ht="15.75" customHeight="1">
+        <v>1.673</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="6"/>
+        <v>1.7689999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19" ht="15.75" customHeight="1">
       <c r="B40">
         <v>34</v>
       </c>
@@ -26065,15 +26325,23 @@
         <v>1.6418971566436484</v>
       </c>
       <c r="P40">
+        <f t="shared" si="4"/>
+        <v>1.4274759397558743</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="5"/>
+        <v>1.4162542189383176</v>
+      </c>
+      <c r="R40">
         <f t="shared" si="3"/>
-        <v>1.4274759397558743</v>
-      </c>
-      <c r="Q40">
-        <f t="shared" si="4"/>
-        <v>1.4162542189383176</v>
-      </c>
-    </row>
-    <row r="41" spans="2:17" ht="15.75" customHeight="1">
+        <v>1.694</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="6"/>
+        <v>1.7909999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19" ht="15.75" customHeight="1">
       <c r="B41">
         <v>35</v>
       </c>
@@ -26102,15 +26370,23 @@
         <v>1.6615101586425596</v>
       </c>
       <c r="P41">
+        <f t="shared" si="4"/>
+        <v>1.4445276097380921</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="5"/>
+        <v>1.4331718417715191</v>
+      </c>
+      <c r="R41">
         <f t="shared" si="3"/>
-        <v>1.4445276097380921</v>
-      </c>
-      <c r="Q41">
-        <f t="shared" si="4"/>
-        <v>1.4331718417715191</v>
-      </c>
-    </row>
-    <row r="42" spans="2:17" ht="15.75" customHeight="1">
+        <v>1.714</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="6"/>
+        <v>1.8129999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19" ht="15.75" customHeight="1">
       <c r="B42">
         <v>36</v>
       </c>
@@ -26143,11 +26419,19 @@
         <v>1.4606043518323679</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.4491222008519635</v>
       </c>
-    </row>
-    <row r="43" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R42">
+        <f>ROUND(LOG(L42,20),3)</f>
+        <v>1.7330000000000001</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="6"/>
+        <v>1.833</v>
+      </c>
+    </row>
+    <row r="43" spans="2:19" ht="15.75" customHeight="1">
       <c r="B43">
         <v>37</v>
       </c>
@@ -26180,11 +26464,19 @@
         <v>1.4758116452773944</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.4642099462214828</v>
       </c>
-    </row>
-    <row r="44" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R43">
+        <f t="shared" si="3"/>
+        <v>1.7509999999999999</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="6"/>
+        <v>1.8520000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="2:19" ht="15.75" customHeight="1">
       <c r="B44">
         <v>38</v>
       </c>
@@ -26213,15 +26505,23 @@
         <v>1.7140875437642691</v>
       </c>
       <c r="P44">
-        <f t="shared" ref="P44:P57" si="5">LOG(L44,35)</f>
+        <f t="shared" ref="P44:P57" si="7">LOG(L44,35)</f>
         <v>1.4902387262552446</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.4785236125557395</v>
       </c>
-    </row>
-    <row r="45" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R44">
+        <f t="shared" si="3"/>
+        <v>1.7689999999999999</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="6"/>
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="45" spans="2:19" ht="15.75" customHeight="1">
       <c r="B45">
         <v>39</v>
       </c>
@@ -26250,15 +26550,23 @@
         <v>1.7298719158347411</v>
       </c>
       <c r="P45">
+        <f t="shared" si="7"/>
+        <v>1.5039617607727125</v>
+      </c>
+      <c r="Q45">
         <f t="shared" si="5"/>
-        <v>1.5039617607727125</v>
-      </c>
-      <c r="Q45">
-        <f t="shared" si="4"/>
         <v>1.4921387671028095</v>
       </c>
-    </row>
-    <row r="46" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R45">
+        <f t="shared" si="3"/>
+        <v>1.7849999999999999</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="6"/>
+        <v>1.887</v>
+      </c>
+    </row>
+    <row r="46" spans="2:19" ht="15.75" customHeight="1">
       <c r="B46">
         <v>40</v>
       </c>
@@ -26287,15 +26595,23 @@
         <v>1.7449218597733469</v>
       </c>
       <c r="P46">
+        <f t="shared" si="7"/>
+        <v>1.517046278752481</v>
+      </c>
+      <c r="Q46">
         <f t="shared" si="5"/>
-        <v>1.517046278752481</v>
-      </c>
-      <c r="Q46">
-        <f t="shared" si="4"/>
         <v>1.5051204246393917</v>
       </c>
-    </row>
-    <row r="47" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R46">
+        <f t="shared" si="3"/>
+        <v>1.8</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="6"/>
+        <v>1.9039999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="2:19" ht="15.75" customHeight="1">
       <c r="B47">
         <v>41</v>
       </c>
@@ -26324,15 +26640,23 @@
         <v>1.7593026918847074</v>
       </c>
       <c r="P47">
+        <f t="shared" si="7"/>
+        <v>1.5295490666095473</v>
+      </c>
+      <c r="Q47">
         <f t="shared" si="5"/>
-        <v>1.5295490666095473</v>
-      </c>
-      <c r="Q47">
-        <f t="shared" si="4"/>
         <v>1.5175249251692493</v>
       </c>
-    </row>
-    <row r="48" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R47">
+        <f t="shared" si="3"/>
+        <v>1.8149999999999999</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="6"/>
+        <v>1.919</v>
+      </c>
+    </row>
+    <row r="48" spans="2:19" ht="15.75" customHeight="1">
       <c r="B48">
         <v>42</v>
       </c>
@@ -26361,15 +26685,23 @@
         <v>1.7730713848292368</v>
       </c>
       <c r="P48">
+        <f t="shared" si="7"/>
+        <v>1.5415196567410143</v>
+      </c>
+      <c r="Q48">
         <f t="shared" si="5"/>
-        <v>1.5415196567410143</v>
-      </c>
-      <c r="Q48">
-        <f t="shared" si="4"/>
         <v>1.529401411703776</v>
       </c>
-    </row>
-    <row r="49" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R48">
+        <f t="shared" si="3"/>
+        <v>1.829</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="6"/>
+        <v>1.9339999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="2:19" ht="15.75" customHeight="1">
       <c r="B49">
         <v>43</v>
       </c>
@@ -26398,15 +26730,23 @@
         <v>1.7862779308848897</v>
       </c>
       <c r="P49">
+        <f t="shared" si="7"/>
+        <v>1.5530015127546146</v>
+      </c>
+      <c r="Q49">
         <f t="shared" si="5"/>
-        <v>1.5530015127546146</v>
-      </c>
-      <c r="Q49">
-        <f t="shared" si="4"/>
         <v>1.5407930061731614</v>
       </c>
-    </row>
-    <row r="50" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R49">
+        <f t="shared" si="3"/>
+        <v>1.843</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="6"/>
+        <v>1.9490000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="2:19" ht="15.75" customHeight="1">
       <c r="B50">
         <v>44</v>
       </c>
@@ -26435,15 +26775,23 @@
         <v>1.8452617719498574</v>
       </c>
       <c r="P50">
+        <f t="shared" si="7"/>
+        <v>1.6042824432403844</v>
+      </c>
+      <c r="Q50">
         <f t="shared" si="5"/>
-        <v>1.6042824432403844</v>
-      </c>
-      <c r="Q50">
-        <f t="shared" si="4"/>
         <v>1.5916708053211979</v>
       </c>
-    </row>
-    <row r="51" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R50">
+        <f t="shared" si="3"/>
+        <v>1.9039999999999999</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="6"/>
+        <v>2.0129999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="2:19" ht="15.75" customHeight="1">
       <c r="B51">
         <v>45</v>
       </c>
@@ -26472,15 +26820,23 @@
         <v>1.8951318989873487</v>
       </c>
       <c r="P51">
+        <f t="shared" si="7"/>
+        <v>1.6476398521807292</v>
+      </c>
+      <c r="Q51">
         <f t="shared" si="5"/>
-        <v>1.6476398521807292</v>
-      </c>
-      <c r="Q51">
-        <f t="shared" si="4"/>
         <v>1.6346873715720438</v>
       </c>
-    </row>
-    <row r="52" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R51">
+        <f t="shared" si="3"/>
+        <v>1.9550000000000001</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="6"/>
+        <v>2.0680000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="2:19" ht="15.75" customHeight="1">
       <c r="B52">
         <v>46</v>
       </c>
@@ -26509,15 +26865,23 @@
         <v>1.9383313679818446</v>
       </c>
       <c r="P52">
+        <f t="shared" si="7"/>
+        <v>1.6851977481490308</v>
+      </c>
+      <c r="Q52">
         <f t="shared" si="5"/>
-        <v>1.6851977481490308</v>
-      </c>
-      <c r="Q52">
-        <f t="shared" si="4"/>
         <v>1.6719500161730103</v>
       </c>
-    </row>
-    <row r="53" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R52">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="S52">
+        <f t="shared" si="6"/>
+        <v>2.1150000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="2:19" ht="15.75" customHeight="1">
       <c r="B53">
         <v>47</v>
       </c>
@@ -26546,15 +26910,23 @@
         <v>1.9764360001354457</v>
       </c>
       <c r="P53">
+        <f t="shared" si="7"/>
+        <v>1.7183261602255244</v>
+      </c>
+      <c r="Q53">
         <f t="shared" si="5"/>
-        <v>1.7183261602255244</v>
-      </c>
-      <c r="Q53">
-        <f t="shared" si="4"/>
         <v>1.7048179980866565</v>
       </c>
-    </row>
-    <row r="54" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R53">
+        <f t="shared" si="3"/>
+        <v>2.0390000000000001</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="6"/>
+        <v>2.1560000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="2:19" ht="15.75" customHeight="1">
       <c r="B54">
         <v>48</v>
       </c>
@@ -26583,15 +26955,23 @@
         <v>2.0105217551024652</v>
       </c>
       <c r="P54">
+        <f t="shared" si="7"/>
+        <v>1.7479605346484011</v>
+      </c>
+      <c r="Q54">
         <f t="shared" si="5"/>
-        <v>1.7479605346484011</v>
-      </c>
-      <c r="Q54">
-        <f t="shared" si="4"/>
         <v>1.7342194097904322</v>
       </c>
-    </row>
-    <row r="55" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R54">
+        <f t="shared" si="3"/>
+        <v>2.0739999999999998</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="6"/>
+        <v>2.1930000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="2:19" ht="15.75" customHeight="1">
       <c r="B55">
         <v>49</v>
       </c>
@@ -26620,15 +27000,23 @@
         <v>2.0413560711115428</v>
       </c>
       <c r="P55">
+        <f t="shared" si="7"/>
+        <v>1.7747680871456373</v>
+      </c>
+      <c r="Q55">
         <f t="shared" si="5"/>
-        <v>1.7747680871456373</v>
-      </c>
-      <c r="Q55">
-        <f t="shared" si="4"/>
         <v>1.7608162218740842</v>
       </c>
-    </row>
-    <row r="56" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R55">
+        <f t="shared" si="3"/>
+        <v>2.1059999999999999</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="6"/>
+        <v>2.2269999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="2:19" ht="15.75" customHeight="1">
       <c r="B56">
         <v>50</v>
       </c>
@@ -26657,15 +27045,23 @@
         <v>2.0695055961674331</v>
       </c>
       <c r="P56">
+        <f t="shared" si="7"/>
+        <v>1.7992414651341708</v>
+      </c>
+      <c r="Q56">
         <f t="shared" si="5"/>
-        <v>1.7992414651341708</v>
-      </c>
-      <c r="Q56">
-        <f t="shared" si="4"/>
         <v>1.7850972089384687</v>
       </c>
-    </row>
-    <row r="57" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R56">
+        <f t="shared" si="3"/>
+        <v>2.1349999999999998</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="6"/>
+        <v>2.258</v>
+      </c>
+    </row>
+    <row r="57" spans="2:19" ht="15.75" customHeight="1">
       <c r="B57">
         <v>51</v>
       </c>
@@ -26694,15 +27090,23 @@
         <v>2.0954006490116837</v>
       </c>
       <c r="P57">
+        <f t="shared" si="7"/>
+        <v>1.8217547904933775</v>
+      </c>
+      <c r="Q57">
         <f t="shared" si="5"/>
-        <v>1.8217547904933775</v>
-      </c>
-      <c r="Q57">
-        <f t="shared" si="4"/>
         <v>1.8074335518037365</v>
       </c>
-    </row>
-    <row r="58" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R57">
+        <f t="shared" si="3"/>
+        <v>2.1619999999999999</v>
+      </c>
+      <c r="S57">
+        <f t="shared" si="6"/>
+        <v>2.286</v>
+      </c>
+    </row>
+    <row r="58" spans="2:19" ht="15.75" customHeight="1">
       <c r="B58">
         <v>52</v>
       </c>
@@ -26735,11 +27139,19 @@
         <v>1.8425988740745154</v>
       </c>
       <c r="Q58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.8281137751893146</v>
       </c>
-    </row>
-    <row r="59" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R58">
+        <f t="shared" si="3"/>
+        <v>2.1869999999999998</v>
+      </c>
+      <c r="S58">
+        <f t="shared" si="6"/>
+        <v>2.3119999999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="2:19" ht="15.75" customHeight="1">
       <c r="B59">
         <v>53</v>
       </c>
@@ -26772,11 +27184,19 @@
         <v>1.8620042516335409</v>
       </c>
       <c r="Q59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.8473666025558908</v>
       </c>
-    </row>
-    <row r="60" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R59">
+        <f t="shared" si="3"/>
+        <v>2.21</v>
+      </c>
+      <c r="S59">
+        <f t="shared" si="6"/>
+        <v>2.3370000000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="2:19" ht="15.75" customHeight="1">
       <c r="B60">
         <v>54</v>
       </c>
@@ -26805,15 +27225,23 @@
         <v>2.1625751921994198</v>
       </c>
       <c r="P60">
-        <f t="shared" ref="P60:P72" si="6">LOG(L60,35)</f>
+        <f t="shared" ref="P60:P72" si="8">LOG(L60,35)</f>
         <v>1.8801567700428172</v>
       </c>
       <c r="Q60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.8653764197902811</v>
       </c>
-    </row>
-    <row r="61" spans="2:17" ht="15.75" customHeight="1">
+      <c r="R60">
+        <f t="shared" si="3"/>
+        <v>2.2309999999999999</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="6"/>
+        <v>2.359</v>
+      </c>
+    </row>
+    <row r="61" spans="2:19" ht="15.75" customHeight="1">
       <c r="B61">
         <v>55</v>
       </c>
@@ -26842,15 +27270,23 @@
         <v>2.1821881941983312</v>
       </c>
       <c r="P61">
+        <f t="shared" si="8"/>
+        <v>1.8972084400250351</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="5"/>
+        <v>1.8822940426234827</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="3"/>
+        <v>2.2519999999999998</v>
+      </c>
+      <c r="S61">
         <f t="shared" si="6"/>
-        <v>1.8972084400250351</v>
-      </c>
-      <c r="Q61">
-        <f t="shared" si="4"/>
-        <v>1.8822940426234827</v>
-      </c>
-    </row>
-    <row r="62" spans="2:17" ht="15.75" customHeight="1">
+        <v>2.3809999999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="2:19" ht="15.75" customHeight="1">
       <c r="B62">
         <v>56</v>
       </c>
@@ -26879,15 +27315,23 @@
         <v>2.2006798243530215</v>
       </c>
       <c r="P62">
+        <f t="shared" si="8"/>
+        <v>1.9132851821193106</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="5"/>
+        <v>1.8982444017039273</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="3"/>
+        <v>2.2709999999999999</v>
+      </c>
+      <c r="S62">
         <f t="shared" si="6"/>
-        <v>1.9132851821193106</v>
-      </c>
-      <c r="Q62">
-        <f t="shared" si="4"/>
-        <v>1.8982444017039273</v>
-      </c>
-    </row>
-    <row r="63" spans="2:17" ht="15.75" customHeight="1">
+        <v>2.4009999999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="2:19" ht="15.75" customHeight="1">
       <c r="B63">
         <v>57</v>
       </c>
@@ -26916,15 +27360,23 @@
         <v>2.2181714059427642</v>
       </c>
       <c r="P63">
+        <f t="shared" si="8"/>
+        <v>1.9284924755643373</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="5"/>
+        <v>1.9133321470734466</v>
+      </c>
+      <c r="R63">
+        <f t="shared" si="3"/>
+        <v>2.2890000000000001</v>
+      </c>
+      <c r="S63">
         <f t="shared" si="6"/>
-        <v>1.9284924755643373</v>
-      </c>
-      <c r="Q63">
-        <f t="shared" si="4"/>
-        <v>1.9133321470734466</v>
-      </c>
-    </row>
-    <row r="64" spans="2:17" ht="15.75" customHeight="1">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="64" spans="2:19" ht="15.75" customHeight="1">
       <c r="B64">
         <v>58</v>
       </c>
@@ -26953,15 +27405,23 @@
         <v>2.2347655793200407</v>
       </c>
       <c r="P64">
+        <f t="shared" si="8"/>
+        <v>1.9429195565421873</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="5"/>
+        <v>1.927645813407703</v>
+      </c>
+      <c r="R64">
+        <f t="shared" si="3"/>
+        <v>2.306</v>
+      </c>
+      <c r="S64">
         <f t="shared" si="6"/>
-        <v>1.9429195565421873</v>
-      </c>
-      <c r="Q64">
-        <f t="shared" si="4"/>
-        <v>1.927645813407703</v>
-      </c>
-    </row>
-    <row r="65" spans="2:17" ht="15.75" customHeight="1">
+        <v>2.4380000000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="2:19" ht="15.75" customHeight="1">
       <c r="B65">
         <v>59</v>
       </c>
@@ -26990,15 +27450,23 @@
         <v>2.7554436148758126</v>
       </c>
       <c r="P65">
+        <f t="shared" si="8"/>
+        <v>2.3956003868291305</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="5"/>
+        <v>2.376768014259667</v>
+      </c>
+      <c r="R65">
+        <f t="shared" si="3"/>
+        <v>2.843</v>
+      </c>
+      <c r="S65">
         <f t="shared" si="6"/>
-        <v>2.3956003868291305</v>
-      </c>
-      <c r="Q65">
-        <f t="shared" si="4"/>
-        <v>2.376768014259667</v>
-      </c>
-    </row>
-    <row r="66" spans="2:17" ht="15.75" customHeight="1">
+        <v>3.0059999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="2:19" ht="15.75" customHeight="1">
       <c r="B66">
         <v>60</v>
       </c>
@@ -27027,15 +27495,23 @@
         <v>2.9796874390933881</v>
       </c>
       <c r="P66">
+        <f t="shared" si="8"/>
+        <v>2.5905594087229167</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="5"/>
+        <v>2.5701944178769378</v>
+      </c>
+      <c r="R66">
+        <f t="shared" si="3"/>
+        <v>3.0739999999999998</v>
+      </c>
+      <c r="S66">
         <f t="shared" si="6"/>
-        <v>2.5905594087229167</v>
-      </c>
-      <c r="Q66">
-        <f t="shared" si="4"/>
-        <v>2.5701944178769378</v>
-      </c>
-    </row>
-    <row r="67" spans="2:17" ht="15.75" customHeight="1">
+        <v>3.2509999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="2:19" ht="15.75" customHeight="1">
       <c r="B67">
         <v>61</v>
       </c>
@@ -27064,15 +27540,23 @@
         <v>3.500365474649159</v>
       </c>
       <c r="P67">
+        <f t="shared" si="8"/>
+        <v>3.0432402390098594</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="5"/>
+        <v>3.0193166187289013</v>
+      </c>
+      <c r="R67">
+        <f t="shared" si="3"/>
+        <v>3.6120000000000001</v>
+      </c>
+      <c r="S67">
         <f t="shared" si="6"/>
-        <v>3.0432402390098594</v>
-      </c>
-      <c r="Q67">
-        <f t="shared" si="4"/>
-        <v>3.0193166187289013</v>
-      </c>
-    </row>
-    <row r="68" spans="2:17" ht="15.75" customHeight="1">
+        <v>3.819</v>
+      </c>
+    </row>
+    <row r="68" spans="2:19" ht="15.75" customHeight="1">
       <c r="B68">
         <v>62</v>
       </c>
@@ -27101,15 +27585,23 @@
         <v>3.7246092988667345</v>
       </c>
       <c r="P68">
+        <f t="shared" si="8"/>
+        <v>3.2381992609036456</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" si="5"/>
+        <v>3.2127430223461722</v>
+      </c>
+      <c r="R68">
+        <f t="shared" si="3"/>
+        <v>3.843</v>
+      </c>
+      <c r="S68">
         <f t="shared" si="6"/>
-        <v>3.2381992609036456</v>
-      </c>
-      <c r="Q68">
-        <f t="shared" si="4"/>
-        <v>3.2127430223461722</v>
-      </c>
-    </row>
-    <row r="69" spans="2:17" ht="15.75" customHeight="1">
+        <v>4.0640000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="2:19" ht="15.75" customHeight="1">
       <c r="B69">
         <v>63</v>
       </c>
@@ -27138,15 +27630,23 @@
         <v>4.0210435102049304</v>
       </c>
       <c r="P69">
+        <f t="shared" si="8"/>
+        <v>3.4959210692968021</v>
+      </c>
+      <c r="Q69">
+        <f t="shared" si="5"/>
+        <v>3.4684388195808644</v>
+      </c>
+      <c r="R69">
+        <f t="shared" si="3"/>
+        <v>4.149</v>
+      </c>
+      <c r="S69">
         <f t="shared" si="6"/>
-        <v>3.4959210692968021</v>
-      </c>
-      <c r="Q69">
-        <f t="shared" si="4"/>
-        <v>3.4684388195808644</v>
-      </c>
-    </row>
-    <row r="70" spans="2:17" ht="15.75" customHeight="1">
+        <v>4.3869999999999996</v>
+      </c>
+    </row>
+    <row r="70" spans="2:19" ht="15.75" customHeight="1">
       <c r="B70">
         <v>64</v>
       </c>
@@ -27175,15 +27675,23 @@
         <v>4.9902091941958533</v>
       </c>
       <c r="P70">
+        <f t="shared" si="8"/>
+        <v>4.3385199433713177</v>
+      </c>
+      <c r="Q70">
+        <f t="shared" si="5"/>
+        <v>4.3044138276673705</v>
+      </c>
+      <c r="R70">
+        <f t="shared" si="3"/>
+        <v>5.149</v>
+      </c>
+      <c r="S70">
         <f t="shared" si="6"/>
-        <v>4.3385199433713177</v>
-      </c>
-      <c r="Q70">
-        <f t="shared" si="4"/>
-        <v>4.3044138276673705</v>
-      </c>
-    </row>
-    <row r="71" spans="2:17" ht="15.75" customHeight="1">
+        <v>5.444</v>
+      </c>
+    </row>
+    <row r="71" spans="2:19" ht="15.75" customHeight="1">
       <c r="B71">
         <v>65</v>
       </c>
@@ -27212,20 +27720,28 @@
         <v>5.7351310539691998</v>
       </c>
       <c r="P71">
+        <f t="shared" si="8"/>
+        <v>4.9861597955520471</v>
+      </c>
+      <c r="Q71">
+        <f t="shared" si="5"/>
+        <v>4.9469624321366039</v>
+      </c>
+      <c r="R71">
+        <f t="shared" si="3"/>
+        <v>5.9180000000000001</v>
+      </c>
+      <c r="S71">
         <f t="shared" si="6"/>
-        <v>4.9861597955520471</v>
-      </c>
-      <c r="Q71">
-        <f t="shared" si="4"/>
-        <v>4.9469624321366039</v>
-      </c>
-    </row>
-    <row r="72" spans="2:17" ht="15.75" customHeight="1">
+        <v>6.2569999999999997</v>
+      </c>
+    </row>
+    <row r="72" spans="2:19" ht="15.75" customHeight="1">
       <c r="L72">
         <v>500000000</v>
       </c>
       <c r="M72">
-        <f t="shared" ref="M72" si="7">LOG(L72,2)</f>
+        <f t="shared" ref="M72" si="9">LOG(L72,2)</f>
         <v>28.897352853986263</v>
       </c>
       <c r="N72">
@@ -27233,19 +27749,27 @@
         <v>8.6989700043360187</v>
       </c>
       <c r="O72">
-        <f t="shared" ref="O72" si="8">LOG(L72,22)</f>
+        <f t="shared" ref="O72" si="10">LOG(L72,22)</f>
         <v>6.4800529137425471</v>
       </c>
       <c r="P72">
+        <f t="shared" si="8"/>
+        <v>5.6337996477327765</v>
+      </c>
+      <c r="Q72">
+        <f t="shared" si="5"/>
+        <v>5.5895110366058391</v>
+      </c>
+      <c r="R72">
+        <f t="shared" ref="R72" si="11">ROUND(LOG(L72,20),3)</f>
+        <v>6.6859999999999999</v>
+      </c>
+      <c r="S72">
         <f t="shared" si="6"/>
-        <v>5.6337996477327765</v>
-      </c>
-      <c r="Q72">
-        <f t="shared" si="4"/>
-        <v>5.5895110366058391</v>
-      </c>
-    </row>
-    <row r="76" spans="2:17" ht="15.75" customHeight="1">
+        <v>7.07</v>
+      </c>
+    </row>
+    <row r="76" spans="2:19" ht="15.75" customHeight="1">
       <c r="D76" t="s">
         <v>945</v>
       </c>

</xml_diff>

<commit_message>
Achievement rewards, game balance and bugs
Updated Achievement reward logic
Game Balancing
Fixed production slider not working, Auto Clicker bugs and other bugs
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2208E698-0890-4EBD-92CD-D8F10A33BC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BE9EF4-CF9D-4A7F-A06F-2440BD92AF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13785" yWindow="0" windowWidth="20145" windowHeight="12150" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -24744,10 +24744,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A4:S76"/>
+  <dimension ref="A4:Z76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -24757,7 +24757,7 @@
     <col min="5" max="5" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:19" ht="12.75">
+    <row r="4" spans="1:26" ht="12.75">
       <c r="A4" t="s">
         <v>1136</v>
       </c>
@@ -24765,7 +24765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="12.75">
+    <row r="6" spans="1:26" ht="12.75">
       <c r="C6" s="1" t="s">
         <v>52</v>
       </c>
@@ -24787,8 +24787,14 @@
       <c r="L6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="12.75">
+      <c r="V6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Y6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="12.75">
       <c r="A7">
         <v>1</v>
       </c>
@@ -24837,8 +24843,26 @@
         <f>ROUND(LOG(L7,20),3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" ht="12.75">
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>35000</v>
+      </c>
+      <c r="W7">
+        <v>35000</v>
+      </c>
+      <c r="X7">
+        <v>35000</v>
+      </c>
+      <c r="Y7">
+        <v>35000</v>
+      </c>
+      <c r="Z7">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="12.75">
       <c r="B8">
         <v>2</v>
       </c>
@@ -24888,8 +24912,30 @@
         <f>ROUND(LOG(L8,17),3)</f>
         <v>0.245</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" ht="12.75">
+      <c r="T8">
+        <v>2</v>
+      </c>
+      <c r="U8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="V8">
+        <f>ROUND(V7*$U$8, 0)</f>
+        <v>38500</v>
+      </c>
+      <c r="W8">
+        <f>ROUND(W7*$U$9, 0)</f>
+        <v>40250</v>
+      </c>
+      <c r="X8">
+        <f>ROUND(X7*$U$12, 0)</f>
+        <v>36750</v>
+      </c>
+      <c r="Y8">
+        <f>ROUND(Y7*$U$13, 0)</f>
+        <v>36400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="12.75">
       <c r="B9">
         <v>3</v>
       </c>
@@ -24939,8 +24985,30 @@
         <f t="shared" ref="S9:S72" si="6">ROUND(LOG(L9,17),3)</f>
         <v>0.38800000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" ht="12.75">
+      <c r="T9">
+        <v>3</v>
+      </c>
+      <c r="U9">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="V9">
+        <f t="shared" ref="V9:V71" si="7">ROUND(V8*$U$8, 0)</f>
+        <v>42350</v>
+      </c>
+      <c r="W9">
+        <f t="shared" ref="W9:W71" si="8">ROUND(W8*$U$9, 0)</f>
+        <v>46288</v>
+      </c>
+      <c r="X9">
+        <f t="shared" ref="X9:X71" si="9">ROUND(X8*$U$12, 0)</f>
+        <v>38588</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" ref="Y9:Y71" si="10">ROUND(Y8*$U$13, 0)</f>
+        <v>37856</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="12.75">
       <c r="B10">
         <v>4</v>
       </c>
@@ -24990,8 +25058,30 @@
         <f t="shared" si="6"/>
         <v>0.48899999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" ht="12.75">
+      <c r="T10">
+        <v>4</v>
+      </c>
+      <c r="U10">
+        <v>1.2</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="7"/>
+        <v>46585</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="8"/>
+        <v>53231</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="9"/>
+        <v>40517</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="10"/>
+        <v>39370</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="12.75">
       <c r="B11">
         <v>5</v>
       </c>
@@ -25035,8 +25125,30 @@
         <f t="shared" si="6"/>
         <v>0.56799999999999995</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" ht="12.75">
+      <c r="T11">
+        <v>5</v>
+      </c>
+      <c r="U11">
+        <v>1.25</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="7"/>
+        <v>51244</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="8"/>
+        <v>61216</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="9"/>
+        <v>42543</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="10"/>
+        <v>40945</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="12.75">
       <c r="B12">
         <v>6</v>
       </c>
@@ -25080,8 +25192,30 @@
         <f t="shared" si="6"/>
         <v>0.63200000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" ht="12.75">
+      <c r="T12">
+        <v>6</v>
+      </c>
+      <c r="U12">
+        <v>1.05</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="7"/>
+        <v>56368</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="8"/>
+        <v>70398</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="9"/>
+        <v>44670</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="10"/>
+        <v>42583</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="12.75">
       <c r="B13">
         <v>7</v>
       </c>
@@ -25125,8 +25259,30 @@
         <f t="shared" si="6"/>
         <v>0.68700000000000006</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" ht="12.75">
+      <c r="T13">
+        <v>7</v>
+      </c>
+      <c r="U13">
+        <v>1.04</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="7"/>
+        <v>62005</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="8"/>
+        <v>80958</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="9"/>
+        <v>46904</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="10"/>
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="12.75">
       <c r="B14">
         <v>8</v>
       </c>
@@ -25170,8 +25326,30 @@
         <f t="shared" si="6"/>
         <v>0.73399999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" ht="12.75">
+      <c r="T14">
+        <v>8</v>
+      </c>
+      <c r="U14">
+        <v>1.03</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="7"/>
+        <v>68206</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="8"/>
+        <v>93102</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="9"/>
+        <v>49249</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="10"/>
+        <v>46057</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="12.75">
       <c r="B15">
         <v>9</v>
       </c>
@@ -25215,8 +25393,30 @@
         <f t="shared" si="6"/>
         <v>0.77600000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" ht="12.75">
+      <c r="T15">
+        <v>9</v>
+      </c>
+      <c r="U15">
+        <v>1.02</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="7"/>
+        <v>75027</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="8"/>
+        <v>107067</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="9"/>
+        <v>51711</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="10"/>
+        <v>47899</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="12.75">
       <c r="B16">
         <v>10</v>
       </c>
@@ -25260,8 +25460,30 @@
         <f t="shared" si="6"/>
         <v>0.81299999999999994</v>
       </c>
-    </row>
-    <row r="17" spans="2:19" ht="12.75">
+      <c r="T16">
+        <v>10</v>
+      </c>
+      <c r="U16">
+        <v>1.01</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="7"/>
+        <v>82530</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="8"/>
+        <v>123127</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="9"/>
+        <v>54297</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="10"/>
+        <v>49815</v>
+      </c>
+    </row>
+    <row r="17" spans="2:25" ht="12.75">
       <c r="B17">
         <v>11</v>
       </c>
@@ -25305,8 +25527,27 @@
         <f t="shared" si="6"/>
         <v>0.84599999999999997</v>
       </c>
-    </row>
-    <row r="18" spans="2:19" ht="12.75">
+      <c r="T17">
+        <v>11</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="7"/>
+        <v>90783</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="8"/>
+        <v>141596</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="9"/>
+        <v>57012</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="10"/>
+        <v>51808</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25" ht="12.75">
       <c r="B18">
         <v>12</v>
       </c>
@@ -25350,8 +25591,27 @@
         <f t="shared" si="6"/>
         <v>0.877</v>
       </c>
-    </row>
-    <row r="19" spans="2:19" ht="12.75">
+      <c r="T18">
+        <v>12</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="7"/>
+        <v>99861</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="8"/>
+        <v>162835</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="9"/>
+        <v>59863</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="10"/>
+        <v>53880</v>
+      </c>
+    </row>
+    <row r="19" spans="2:25" ht="12.75">
       <c r="B19">
         <v>13</v>
       </c>
@@ -25395,8 +25655,27 @@
         <f t="shared" si="6"/>
         <v>0.90500000000000003</v>
       </c>
-    </row>
-    <row r="20" spans="2:19" ht="12.75">
+      <c r="T19">
+        <v>13</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="7"/>
+        <v>109847</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="8"/>
+        <v>187260</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="9"/>
+        <v>62856</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" si="10"/>
+        <v>56035</v>
+      </c>
+    </row>
+    <row r="20" spans="2:25" ht="12.75">
       <c r="B20">
         <v>14</v>
       </c>
@@ -25440,8 +25719,27 @@
         <f t="shared" si="6"/>
         <v>0.93100000000000005</v>
       </c>
-    </row>
-    <row r="21" spans="2:19" ht="12.75">
+      <c r="T20">
+        <v>14</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="7"/>
+        <v>120832</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="8"/>
+        <v>215349</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="9"/>
+        <v>65999</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="10"/>
+        <v>58276</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" ht="12.75">
       <c r="B21">
         <v>15</v>
       </c>
@@ -25485,8 +25783,27 @@
         <f t="shared" si="6"/>
         <v>0.95599999999999996</v>
       </c>
-    </row>
-    <row r="22" spans="2:19" ht="12.75">
+      <c r="T21">
+        <v>15</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="7"/>
+        <v>132915</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="8"/>
+        <v>247651</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="9"/>
+        <v>69299</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="10"/>
+        <v>60607</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25" ht="12.75">
       <c r="B22">
         <v>16</v>
       </c>
@@ -25530,8 +25847,27 @@
         <f t="shared" si="6"/>
         <v>0.97899999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="2:19" ht="12.75">
+      <c r="T22">
+        <v>16</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="7"/>
+        <v>146207</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="8"/>
+        <v>284799</v>
+      </c>
+      <c r="X22">
+        <f t="shared" si="9"/>
+        <v>72764</v>
+      </c>
+      <c r="Y22">
+        <f t="shared" si="10"/>
+        <v>63031</v>
+      </c>
+    </row>
+    <row r="23" spans="2:25" ht="12.75">
       <c r="B23">
         <v>17</v>
       </c>
@@ -25575,8 +25911,27 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:19" ht="12.75">
+      <c r="T23">
+        <v>17</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="7"/>
+        <v>160828</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="8"/>
+        <v>327519</v>
+      </c>
+      <c r="X23">
+        <f t="shared" si="9"/>
+        <v>76402</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" si="10"/>
+        <v>65552</v>
+      </c>
+    </row>
+    <row r="24" spans="2:25" ht="12.75">
       <c r="B24">
         <v>18</v>
       </c>
@@ -25620,8 +25975,27 @@
         <f t="shared" si="6"/>
         <v>1.02</v>
       </c>
-    </row>
-    <row r="25" spans="2:19" ht="12.75">
+      <c r="T24">
+        <v>18</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="7"/>
+        <v>176911</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="8"/>
+        <v>376647</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="9"/>
+        <v>80222</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="10"/>
+        <v>68174</v>
+      </c>
+    </row>
+    <row r="25" spans="2:25" ht="12.75">
       <c r="B25">
         <v>19</v>
       </c>
@@ -25665,8 +26039,27 @@
         <f t="shared" si="6"/>
         <v>1.0389999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="2:19" ht="12.75">
+      <c r="T25">
+        <v>19</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="7"/>
+        <v>194602</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="8"/>
+        <v>433144</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="9"/>
+        <v>84233</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" si="10"/>
+        <v>70901</v>
+      </c>
+    </row>
+    <row r="26" spans="2:25" ht="12.75">
       <c r="B26">
         <v>20</v>
       </c>
@@ -25710,8 +26103,27 @@
         <f t="shared" si="6"/>
         <v>1.0569999999999999</v>
       </c>
-    </row>
-    <row r="27" spans="2:19" ht="12.75">
+      <c r="T26">
+        <v>20</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="7"/>
+        <v>214062</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="8"/>
+        <v>498116</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="9"/>
+        <v>88445</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" si="10"/>
+        <v>73737</v>
+      </c>
+    </row>
+    <row r="27" spans="2:25" ht="12.75">
       <c r="B27">
         <v>21</v>
       </c>
@@ -25755,8 +26167,27 @@
         <f t="shared" si="6"/>
         <v>1.2</v>
       </c>
-    </row>
-    <row r="28" spans="2:19" ht="12.75">
+      <c r="T27">
+        <v>21</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="7"/>
+        <v>235468</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="8"/>
+        <v>572833</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="9"/>
+        <v>92867</v>
+      </c>
+      <c r="Y27">
+        <f t="shared" si="10"/>
+        <v>76686</v>
+      </c>
+    </row>
+    <row r="28" spans="2:25" ht="12.75">
       <c r="B28">
         <v>22</v>
       </c>
@@ -25800,8 +26231,27 @@
         <f t="shared" si="6"/>
         <v>1.302</v>
       </c>
-    </row>
-    <row r="29" spans="2:19" ht="12.75">
+      <c r="T28">
+        <v>22</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="7"/>
+        <v>259015</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="8"/>
+        <v>658758</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="9"/>
+        <v>97510</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" si="10"/>
+        <v>79753</v>
+      </c>
+    </row>
+    <row r="29" spans="2:25" ht="12.75">
       <c r="B29">
         <v>23</v>
       </c>
@@ -25845,8 +26295,27 @@
         <f t="shared" si="6"/>
         <v>1.381</v>
       </c>
-    </row>
-    <row r="30" spans="2:19" ht="12.75">
+      <c r="T29">
+        <v>23</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="7"/>
+        <v>284917</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="8"/>
+        <v>757572</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="9"/>
+        <v>102386</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" si="10"/>
+        <v>82943</v>
+      </c>
+    </row>
+    <row r="30" spans="2:25" ht="12.75">
       <c r="B30">
         <v>24</v>
       </c>
@@ -25890,8 +26359,27 @@
         <f t="shared" si="6"/>
         <v>1.4450000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="2:19" ht="12.75">
+      <c r="T30">
+        <v>24</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="7"/>
+        <v>313409</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="8"/>
+        <v>871208</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="9"/>
+        <v>107505</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="10"/>
+        <v>86261</v>
+      </c>
+    </row>
+    <row r="31" spans="2:25" ht="12.75">
       <c r="B31">
         <v>25</v>
       </c>
@@ -25935,8 +26423,27 @@
         <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="32" spans="2:19" ht="12.75">
+      <c r="T31">
+        <v>25</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="7"/>
+        <v>344750</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="8"/>
+        <v>1001889</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="9"/>
+        <v>112880</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="10"/>
+        <v>89711</v>
+      </c>
+    </row>
+    <row r="32" spans="2:25" ht="12.75">
       <c r="B32">
         <v>26</v>
       </c>
@@ -25980,8 +26487,27 @@
         <f t="shared" si="6"/>
         <v>1.5469999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="2:19" ht="12.75">
+      <c r="T32">
+        <v>26</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="7"/>
+        <v>379225</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="8"/>
+        <v>1152172</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="9"/>
+        <v>118524</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="10"/>
+        <v>93299</v>
+      </c>
+    </row>
+    <row r="33" spans="2:25" ht="12.75">
       <c r="B33">
         <v>27</v>
       </c>
@@ -26025,8 +26551,27 @@
         <f t="shared" si="6"/>
         <v>1.5880000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="2:19" ht="12.75">
+      <c r="T33">
+        <v>27</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="7"/>
+        <v>417148</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="8"/>
+        <v>1324998</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="9"/>
+        <v>124450</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="10"/>
+        <v>97031</v>
+      </c>
+    </row>
+    <row r="34" spans="2:25" ht="12.75">
       <c r="B34">
         <v>28</v>
       </c>
@@ -26070,8 +26615,27 @@
         <f t="shared" si="6"/>
         <v>1.625</v>
       </c>
-    </row>
-    <row r="35" spans="2:19" ht="12.75">
+      <c r="T34">
+        <v>28</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="7"/>
+        <v>458863</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="8"/>
+        <v>1523748</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="9"/>
+        <v>130673</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="10"/>
+        <v>100912</v>
+      </c>
+    </row>
+    <row r="35" spans="2:25" ht="12.75">
       <c r="B35">
         <v>29</v>
       </c>
@@ -26115,8 +26679,27 @@
         <f t="shared" si="6"/>
         <v>1.659</v>
       </c>
-    </row>
-    <row r="36" spans="2:19" ht="12.75">
+      <c r="T35">
+        <v>29</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="7"/>
+        <v>504749</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="8"/>
+        <v>1752310</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="9"/>
+        <v>137207</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="10"/>
+        <v>104948</v>
+      </c>
+    </row>
+    <row r="36" spans="2:25" ht="12.75">
       <c r="B36">
         <v>30</v>
       </c>
@@ -26160,8 +26743,27 @@
         <f t="shared" si="6"/>
         <v>1.69</v>
       </c>
-    </row>
-    <row r="37" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T36">
+        <v>30</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="7"/>
+        <v>555224</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="8"/>
+        <v>2015157</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="9"/>
+        <v>144067</v>
+      </c>
+      <c r="Y36">
+        <f t="shared" si="10"/>
+        <v>109146</v>
+      </c>
+    </row>
+    <row r="37" spans="2:25" ht="15.75" customHeight="1">
       <c r="B37">
         <v>31</v>
       </c>
@@ -26205,8 +26807,27 @@
         <f t="shared" si="6"/>
         <v>1.718</v>
       </c>
-    </row>
-    <row r="38" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T37">
+        <v>31</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="7"/>
+        <v>610746</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="8"/>
+        <v>2317431</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="9"/>
+        <v>151270</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" si="10"/>
+        <v>113512</v>
+      </c>
+    </row>
+    <row r="38" spans="2:25" ht="15.75" customHeight="1">
       <c r="B38">
         <v>32</v>
       </c>
@@ -26250,8 +26871,27 @@
         <f t="shared" si="6"/>
         <v>1.744</v>
       </c>
-    </row>
-    <row r="39" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T38">
+        <v>32</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="7"/>
+        <v>671821</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="8"/>
+        <v>2665046</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="9"/>
+        <v>158834</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" si="10"/>
+        <v>118052</v>
+      </c>
+    </row>
+    <row r="39" spans="2:25" ht="15.75" customHeight="1">
       <c r="B39">
         <v>33</v>
       </c>
@@ -26295,8 +26935,27 @@
         <f t="shared" si="6"/>
         <v>1.7689999999999999</v>
       </c>
-    </row>
-    <row r="40" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T39">
+        <v>33</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="7"/>
+        <v>739003</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="8"/>
+        <v>3064803</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="9"/>
+        <v>166776</v>
+      </c>
+      <c r="Y39">
+        <f t="shared" si="10"/>
+        <v>122774</v>
+      </c>
+    </row>
+    <row r="40" spans="2:25" ht="15.75" customHeight="1">
       <c r="B40">
         <v>34</v>
       </c>
@@ -26340,8 +26999,27 @@
         <f t="shared" si="6"/>
         <v>1.7909999999999999</v>
       </c>
-    </row>
-    <row r="41" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T40">
+        <v>34</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="7"/>
+        <v>812903</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="8"/>
+        <v>3524523</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="9"/>
+        <v>175115</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" si="10"/>
+        <v>127685</v>
+      </c>
+    </row>
+    <row r="41" spans="2:25" ht="15.75" customHeight="1">
       <c r="B41">
         <v>35</v>
       </c>
@@ -26385,8 +27063,27 @@
         <f t="shared" si="6"/>
         <v>1.8129999999999999</v>
       </c>
-    </row>
-    <row r="42" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T41">
+        <v>35</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="7"/>
+        <v>894193</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="8"/>
+        <v>4053201</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="9"/>
+        <v>183871</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" si="10"/>
+        <v>132792</v>
+      </c>
+    </row>
+    <row r="42" spans="2:25" ht="15.75" customHeight="1">
       <c r="B42">
         <v>36</v>
       </c>
@@ -26430,8 +27127,27 @@
         <f t="shared" si="6"/>
         <v>1.833</v>
       </c>
-    </row>
-    <row r="43" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T42">
+        <v>36</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="7"/>
+        <v>983612</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="8"/>
+        <v>4661181</v>
+      </c>
+      <c r="X42">
+        <f t="shared" si="9"/>
+        <v>193065</v>
+      </c>
+      <c r="Y42">
+        <f t="shared" si="10"/>
+        <v>138104</v>
+      </c>
+    </row>
+    <row r="43" spans="2:25" ht="15.75" customHeight="1">
       <c r="B43">
         <v>37</v>
       </c>
@@ -26475,8 +27191,27 @@
         <f t="shared" si="6"/>
         <v>1.8520000000000001</v>
       </c>
-    </row>
-    <row r="44" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T43">
+        <v>37</v>
+      </c>
+      <c r="V43">
+        <f t="shared" si="7"/>
+        <v>1081973</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="8"/>
+        <v>5360358</v>
+      </c>
+      <c r="X43">
+        <f t="shared" si="9"/>
+        <v>202718</v>
+      </c>
+      <c r="Y43">
+        <f t="shared" si="10"/>
+        <v>143628</v>
+      </c>
+    </row>
+    <row r="44" spans="2:25" ht="15.75" customHeight="1">
       <c r="B44">
         <v>38</v>
       </c>
@@ -26505,7 +27240,7 @@
         <v>1.7140875437642691</v>
       </c>
       <c r="P44">
-        <f t="shared" ref="P44:P57" si="7">LOG(L44,35)</f>
+        <f t="shared" ref="P44:P57" si="11">LOG(L44,35)</f>
         <v>1.4902387262552446</v>
       </c>
       <c r="Q44">
@@ -26520,8 +27255,27 @@
         <f t="shared" si="6"/>
         <v>1.87</v>
       </c>
-    </row>
-    <row r="45" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T44">
+        <v>38</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="7"/>
+        <v>1190170</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="8"/>
+        <v>6164412</v>
+      </c>
+      <c r="X44">
+        <f t="shared" si="9"/>
+        <v>212854</v>
+      </c>
+      <c r="Y44">
+        <f t="shared" si="10"/>
+        <v>149373</v>
+      </c>
+    </row>
+    <row r="45" spans="2:25" ht="15.75" customHeight="1">
       <c r="B45">
         <v>39</v>
       </c>
@@ -26550,7 +27304,7 @@
         <v>1.7298719158347411</v>
       </c>
       <c r="P45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.5039617607727125</v>
       </c>
       <c r="Q45">
@@ -26565,8 +27319,27 @@
         <f t="shared" si="6"/>
         <v>1.887</v>
       </c>
-    </row>
-    <row r="46" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T45">
+        <v>39</v>
+      </c>
+      <c r="V45">
+        <f t="shared" si="7"/>
+        <v>1309187</v>
+      </c>
+      <c r="W45">
+        <f t="shared" si="8"/>
+        <v>7089074</v>
+      </c>
+      <c r="X45">
+        <f t="shared" si="9"/>
+        <v>223497</v>
+      </c>
+      <c r="Y45">
+        <f t="shared" si="10"/>
+        <v>155348</v>
+      </c>
+    </row>
+    <row r="46" spans="2:25" ht="15.75" customHeight="1">
       <c r="B46">
         <v>40</v>
       </c>
@@ -26595,7 +27368,7 @@
         <v>1.7449218597733469</v>
       </c>
       <c r="P46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.517046278752481</v>
       </c>
       <c r="Q46">
@@ -26610,8 +27383,27 @@
         <f t="shared" si="6"/>
         <v>1.9039999999999999</v>
       </c>
-    </row>
-    <row r="47" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T46">
+        <v>40</v>
+      </c>
+      <c r="V46">
+        <f t="shared" si="7"/>
+        <v>1440106</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="8"/>
+        <v>8152435</v>
+      </c>
+      <c r="X46">
+        <f t="shared" si="9"/>
+        <v>234672</v>
+      </c>
+      <c r="Y46">
+        <f t="shared" si="10"/>
+        <v>161562</v>
+      </c>
+    </row>
+    <row r="47" spans="2:25" ht="15.75" customHeight="1">
       <c r="B47">
         <v>41</v>
       </c>
@@ -26640,7 +27432,7 @@
         <v>1.7593026918847074</v>
       </c>
       <c r="P47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.5295490666095473</v>
       </c>
       <c r="Q47">
@@ -26655,8 +27447,27 @@
         <f t="shared" si="6"/>
         <v>1.919</v>
       </c>
-    </row>
-    <row r="48" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T47">
+        <v>41</v>
+      </c>
+      <c r="V47">
+        <f t="shared" si="7"/>
+        <v>1584117</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="8"/>
+        <v>9375300</v>
+      </c>
+      <c r="X47">
+        <f t="shared" si="9"/>
+        <v>246406</v>
+      </c>
+      <c r="Y47">
+        <f t="shared" si="10"/>
+        <v>168024</v>
+      </c>
+    </row>
+    <row r="48" spans="2:25" ht="15.75" customHeight="1">
       <c r="B48">
         <v>42</v>
       </c>
@@ -26685,7 +27496,7 @@
         <v>1.7730713848292368</v>
       </c>
       <c r="P48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.5415196567410143</v>
       </c>
       <c r="Q48">
@@ -26700,8 +27511,27 @@
         <f t="shared" si="6"/>
         <v>1.9339999999999999</v>
       </c>
-    </row>
-    <row r="49" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T48">
+        <v>42</v>
+      </c>
+      <c r="V48">
+        <f t="shared" si="7"/>
+        <v>1742529</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="8"/>
+        <v>10781595</v>
+      </c>
+      <c r="X48">
+        <f t="shared" si="9"/>
+        <v>258726</v>
+      </c>
+      <c r="Y48">
+        <f t="shared" si="10"/>
+        <v>174745</v>
+      </c>
+    </row>
+    <row r="49" spans="2:25" ht="15.75" customHeight="1">
       <c r="B49">
         <v>43</v>
       </c>
@@ -26730,7 +27560,7 @@
         <v>1.7862779308848897</v>
       </c>
       <c r="P49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.5530015127546146</v>
       </c>
       <c r="Q49">
@@ -26745,8 +27575,27 @@
         <f t="shared" si="6"/>
         <v>1.9490000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T49">
+        <v>43</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="7"/>
+        <v>1916782</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="8"/>
+        <v>12398834</v>
+      </c>
+      <c r="X49">
+        <f t="shared" si="9"/>
+        <v>271662</v>
+      </c>
+      <c r="Y49">
+        <f t="shared" si="10"/>
+        <v>181735</v>
+      </c>
+    </row>
+    <row r="50" spans="2:25" ht="15.75" customHeight="1">
       <c r="B50">
         <v>44</v>
       </c>
@@ -26775,7 +27624,7 @@
         <v>1.8452617719498574</v>
       </c>
       <c r="P50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.6042824432403844</v>
       </c>
       <c r="Q50">
@@ -26790,8 +27639,27 @@
         <f t="shared" si="6"/>
         <v>2.0129999999999999</v>
       </c>
-    </row>
-    <row r="51" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T50">
+        <v>44</v>
+      </c>
+      <c r="V50">
+        <f t="shared" si="7"/>
+        <v>2108460</v>
+      </c>
+      <c r="W50">
+        <f t="shared" si="8"/>
+        <v>14258659</v>
+      </c>
+      <c r="X50">
+        <f t="shared" si="9"/>
+        <v>285245</v>
+      </c>
+      <c r="Y50">
+        <f t="shared" si="10"/>
+        <v>189004</v>
+      </c>
+    </row>
+    <row r="51" spans="2:25" ht="15.75" customHeight="1">
       <c r="B51">
         <v>45</v>
       </c>
@@ -26820,7 +27688,7 @@
         <v>1.8951318989873487</v>
       </c>
       <c r="P51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.6476398521807292</v>
       </c>
       <c r="Q51">
@@ -26835,8 +27703,27 @@
         <f t="shared" si="6"/>
         <v>2.0680000000000001</v>
       </c>
-    </row>
-    <row r="52" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T51">
+        <v>45</v>
+      </c>
+      <c r="V51">
+        <f t="shared" si="7"/>
+        <v>2319306</v>
+      </c>
+      <c r="W51">
+        <f t="shared" si="8"/>
+        <v>16397458</v>
+      </c>
+      <c r="X51">
+        <f t="shared" si="9"/>
+        <v>299507</v>
+      </c>
+      <c r="Y51">
+        <f t="shared" si="10"/>
+        <v>196564</v>
+      </c>
+    </row>
+    <row r="52" spans="2:25" ht="15.75" customHeight="1">
       <c r="B52">
         <v>46</v>
       </c>
@@ -26865,7 +27752,7 @@
         <v>1.9383313679818446</v>
       </c>
       <c r="P52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.6851977481490308</v>
       </c>
       <c r="Q52">
@@ -26880,8 +27767,27 @@
         <f t="shared" si="6"/>
         <v>2.1150000000000002</v>
       </c>
-    </row>
-    <row r="53" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T52">
+        <v>46</v>
+      </c>
+      <c r="V52">
+        <f t="shared" si="7"/>
+        <v>2551237</v>
+      </c>
+      <c r="W52">
+        <f t="shared" si="8"/>
+        <v>18857077</v>
+      </c>
+      <c r="X52">
+        <f t="shared" si="9"/>
+        <v>314482</v>
+      </c>
+      <c r="Y52">
+        <f t="shared" si="10"/>
+        <v>204427</v>
+      </c>
+    </row>
+    <row r="53" spans="2:25" ht="15.75" customHeight="1">
       <c r="B53">
         <v>47</v>
       </c>
@@ -26910,7 +27816,7 @@
         <v>1.9764360001354457</v>
       </c>
       <c r="P53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.7183261602255244</v>
       </c>
       <c r="Q53">
@@ -26925,8 +27831,27 @@
         <f t="shared" si="6"/>
         <v>2.1560000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T53">
+        <v>47</v>
+      </c>
+      <c r="V53">
+        <f t="shared" si="7"/>
+        <v>2806361</v>
+      </c>
+      <c r="W53">
+        <f t="shared" si="8"/>
+        <v>21685639</v>
+      </c>
+      <c r="X53">
+        <f t="shared" si="9"/>
+        <v>330206</v>
+      </c>
+      <c r="Y53">
+        <f t="shared" si="10"/>
+        <v>212604</v>
+      </c>
+    </row>
+    <row r="54" spans="2:25" ht="15.75" customHeight="1">
       <c r="B54">
         <v>48</v>
       </c>
@@ -26955,7 +27880,7 @@
         <v>2.0105217551024652</v>
       </c>
       <c r="P54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.7479605346484011</v>
       </c>
       <c r="Q54">
@@ -26970,8 +27895,27 @@
         <f t="shared" si="6"/>
         <v>2.1930000000000001</v>
       </c>
-    </row>
-    <row r="55" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T54">
+        <v>48</v>
+      </c>
+      <c r="V54">
+        <f t="shared" si="7"/>
+        <v>3086997</v>
+      </c>
+      <c r="W54">
+        <f t="shared" si="8"/>
+        <v>24938485</v>
+      </c>
+      <c r="X54">
+        <f t="shared" si="9"/>
+        <v>346716</v>
+      </c>
+      <c r="Y54">
+        <f t="shared" si="10"/>
+        <v>221108</v>
+      </c>
+    </row>
+    <row r="55" spans="2:25" ht="15.75" customHeight="1">
       <c r="B55">
         <v>49</v>
       </c>
@@ -27000,7 +27944,7 @@
         <v>2.0413560711115428</v>
       </c>
       <c r="P55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.7747680871456373</v>
       </c>
       <c r="Q55">
@@ -27015,8 +27959,27 @@
         <f t="shared" si="6"/>
         <v>2.2269999999999999</v>
       </c>
-    </row>
-    <row r="56" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T55">
+        <v>49</v>
+      </c>
+      <c r="V55">
+        <f t="shared" si="7"/>
+        <v>3395697</v>
+      </c>
+      <c r="W55">
+        <f t="shared" si="8"/>
+        <v>28679258</v>
+      </c>
+      <c r="X55">
+        <f t="shared" si="9"/>
+        <v>364052</v>
+      </c>
+      <c r="Y55">
+        <f t="shared" si="10"/>
+        <v>229952</v>
+      </c>
+    </row>
+    <row r="56" spans="2:25" ht="15.75" customHeight="1">
       <c r="B56">
         <v>50</v>
       </c>
@@ -27045,7 +28008,7 @@
         <v>2.0695055961674331</v>
       </c>
       <c r="P56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.7992414651341708</v>
       </c>
       <c r="Q56">
@@ -27060,8 +28023,27 @@
         <f t="shared" si="6"/>
         <v>2.258</v>
       </c>
-    </row>
-    <row r="57" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T56">
+        <v>50</v>
+      </c>
+      <c r="V56">
+        <f t="shared" si="7"/>
+        <v>3735267</v>
+      </c>
+      <c r="W56">
+        <f t="shared" si="8"/>
+        <v>32981147</v>
+      </c>
+      <c r="X56">
+        <f t="shared" si="9"/>
+        <v>382255</v>
+      </c>
+      <c r="Y56">
+        <f t="shared" si="10"/>
+        <v>239150</v>
+      </c>
+    </row>
+    <row r="57" spans="2:25" ht="15.75" customHeight="1">
       <c r="B57">
         <v>51</v>
       </c>
@@ -27090,7 +28072,7 @@
         <v>2.0954006490116837</v>
       </c>
       <c r="P57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.8217547904933775</v>
       </c>
       <c r="Q57">
@@ -27105,8 +28087,27 @@
         <f t="shared" si="6"/>
         <v>2.286</v>
       </c>
-    </row>
-    <row r="58" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T57">
+        <v>51</v>
+      </c>
+      <c r="V57">
+        <f t="shared" si="7"/>
+        <v>4108794</v>
+      </c>
+      <c r="W57">
+        <f t="shared" si="8"/>
+        <v>37928319</v>
+      </c>
+      <c r="X57">
+        <f t="shared" si="9"/>
+        <v>401368</v>
+      </c>
+      <c r="Y57">
+        <f t="shared" si="10"/>
+        <v>248716</v>
+      </c>
+    </row>
+    <row r="58" spans="2:25" ht="15.75" customHeight="1">
       <c r="B58">
         <v>52</v>
       </c>
@@ -27150,8 +28151,27 @@
         <f t="shared" si="6"/>
         <v>2.3119999999999998</v>
       </c>
-    </row>
-    <row r="59" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T58">
+        <v>52</v>
+      </c>
+      <c r="V58">
+        <f t="shared" si="7"/>
+        <v>4519673</v>
+      </c>
+      <c r="W58">
+        <f t="shared" si="8"/>
+        <v>43617567</v>
+      </c>
+      <c r="X58">
+        <f t="shared" si="9"/>
+        <v>421436</v>
+      </c>
+      <c r="Y58">
+        <f t="shared" si="10"/>
+        <v>258665</v>
+      </c>
+    </row>
+    <row r="59" spans="2:25" ht="15.75" customHeight="1">
       <c r="B59">
         <v>53</v>
       </c>
@@ -27195,8 +28215,27 @@
         <f t="shared" si="6"/>
         <v>2.3370000000000002</v>
       </c>
-    </row>
-    <row r="60" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T59">
+        <v>53</v>
+      </c>
+      <c r="V59">
+        <f t="shared" si="7"/>
+        <v>4971640</v>
+      </c>
+      <c r="W59">
+        <f t="shared" si="8"/>
+        <v>50160202</v>
+      </c>
+      <c r="X59">
+        <f t="shared" si="9"/>
+        <v>442508</v>
+      </c>
+      <c r="Y59">
+        <f t="shared" si="10"/>
+        <v>269012</v>
+      </c>
+    </row>
+    <row r="60" spans="2:25" ht="15.75" customHeight="1">
       <c r="B60">
         <v>54</v>
       </c>
@@ -27225,7 +28264,7 @@
         <v>2.1625751921994198</v>
       </c>
       <c r="P60">
-        <f t="shared" ref="P60:P72" si="8">LOG(L60,35)</f>
+        <f t="shared" ref="P60:P72" si="12">LOG(L60,35)</f>
         <v>1.8801567700428172</v>
       </c>
       <c r="Q60">
@@ -27240,8 +28279,27 @@
         <f t="shared" si="6"/>
         <v>2.359</v>
       </c>
-    </row>
-    <row r="61" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T60">
+        <v>54</v>
+      </c>
+      <c r="V60">
+        <f t="shared" si="7"/>
+        <v>5468804</v>
+      </c>
+      <c r="W60">
+        <f t="shared" si="8"/>
+        <v>57684232</v>
+      </c>
+      <c r="X60">
+        <f t="shared" si="9"/>
+        <v>464633</v>
+      </c>
+      <c r="Y60">
+        <f t="shared" si="10"/>
+        <v>279772</v>
+      </c>
+    </row>
+    <row r="61" spans="2:25" ht="15.75" customHeight="1">
       <c r="B61">
         <v>55</v>
       </c>
@@ -27270,7 +28328,7 @@
         <v>2.1821881941983312</v>
       </c>
       <c r="P61">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1.8972084400250351</v>
       </c>
       <c r="Q61">
@@ -27285,8 +28343,27 @@
         <f t="shared" si="6"/>
         <v>2.3809999999999998</v>
       </c>
-    </row>
-    <row r="62" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T61">
+        <v>55</v>
+      </c>
+      <c r="V61">
+        <f t="shared" si="7"/>
+        <v>6015684</v>
+      </c>
+      <c r="W61">
+        <f t="shared" si="8"/>
+        <v>66336867</v>
+      </c>
+      <c r="X61">
+        <f t="shared" si="9"/>
+        <v>487865</v>
+      </c>
+      <c r="Y61">
+        <f t="shared" si="10"/>
+        <v>290963</v>
+      </c>
+    </row>
+    <row r="62" spans="2:25" ht="15.75" customHeight="1">
       <c r="B62">
         <v>56</v>
       </c>
@@ -27315,7 +28392,7 @@
         <v>2.2006798243530215</v>
       </c>
       <c r="P62">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1.9132851821193106</v>
       </c>
       <c r="Q62">
@@ -27330,8 +28407,27 @@
         <f t="shared" si="6"/>
         <v>2.4009999999999998</v>
       </c>
-    </row>
-    <row r="63" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T62">
+        <v>56</v>
+      </c>
+      <c r="V62">
+        <f t="shared" si="7"/>
+        <v>6617252</v>
+      </c>
+      <c r="W62">
+        <f t="shared" si="8"/>
+        <v>76287397</v>
+      </c>
+      <c r="X62">
+        <f t="shared" si="9"/>
+        <v>512258</v>
+      </c>
+      <c r="Y62">
+        <f t="shared" si="10"/>
+        <v>302602</v>
+      </c>
+    </row>
+    <row r="63" spans="2:25" ht="15.75" customHeight="1">
       <c r="B63">
         <v>57</v>
       </c>
@@ -27360,7 +28456,7 @@
         <v>2.2181714059427642</v>
       </c>
       <c r="P63">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1.9284924755643373</v>
       </c>
       <c r="Q63">
@@ -27375,8 +28471,27 @@
         <f t="shared" si="6"/>
         <v>2.42</v>
       </c>
-    </row>
-    <row r="64" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T63">
+        <v>57</v>
+      </c>
+      <c r="V63">
+        <f t="shared" si="7"/>
+        <v>7278977</v>
+      </c>
+      <c r="W63">
+        <f t="shared" si="8"/>
+        <v>87730507</v>
+      </c>
+      <c r="X63">
+        <f t="shared" si="9"/>
+        <v>537871</v>
+      </c>
+      <c r="Y63">
+        <f t="shared" si="10"/>
+        <v>314706</v>
+      </c>
+    </row>
+    <row r="64" spans="2:25" ht="15.75" customHeight="1">
       <c r="B64">
         <v>58</v>
       </c>
@@ -27405,7 +28520,7 @@
         <v>2.2347655793200407</v>
       </c>
       <c r="P64">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1.9429195565421873</v>
       </c>
       <c r="Q64">
@@ -27420,8 +28535,27 @@
         <f t="shared" si="6"/>
         <v>2.4380000000000002</v>
       </c>
-    </row>
-    <row r="65" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T64">
+        <v>58</v>
+      </c>
+      <c r="V64">
+        <f t="shared" si="7"/>
+        <v>8006875</v>
+      </c>
+      <c r="W64">
+        <f t="shared" si="8"/>
+        <v>100890083</v>
+      </c>
+      <c r="X64">
+        <f t="shared" si="9"/>
+        <v>564765</v>
+      </c>
+      <c r="Y64">
+        <f t="shared" si="10"/>
+        <v>327294</v>
+      </c>
+    </row>
+    <row r="65" spans="2:25" ht="15.75" customHeight="1">
       <c r="B65">
         <v>59</v>
       </c>
@@ -27450,7 +28584,7 @@
         <v>2.7554436148758126</v>
       </c>
       <c r="P65">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2.3956003868291305</v>
       </c>
       <c r="Q65">
@@ -27465,8 +28599,27 @@
         <f t="shared" si="6"/>
         <v>3.0059999999999998</v>
       </c>
-    </row>
-    <row r="66" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T65">
+        <v>59</v>
+      </c>
+      <c r="V65">
+        <f t="shared" si="7"/>
+        <v>8807563</v>
+      </c>
+      <c r="W65">
+        <f t="shared" si="8"/>
+        <v>116023595</v>
+      </c>
+      <c r="X65">
+        <f t="shared" si="9"/>
+        <v>593003</v>
+      </c>
+      <c r="Y65">
+        <f t="shared" si="10"/>
+        <v>340386</v>
+      </c>
+    </row>
+    <row r="66" spans="2:25" ht="15.75" customHeight="1">
       <c r="B66">
         <v>60</v>
       </c>
@@ -27495,7 +28648,7 @@
         <v>2.9796874390933881</v>
       </c>
       <c r="P66">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2.5905594087229167</v>
       </c>
       <c r="Q66">
@@ -27510,8 +28663,27 @@
         <f t="shared" si="6"/>
         <v>3.2509999999999999</v>
       </c>
-    </row>
-    <row r="67" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T66">
+        <v>60</v>
+      </c>
+      <c r="V66">
+        <f t="shared" si="7"/>
+        <v>9688319</v>
+      </c>
+      <c r="W66">
+        <f t="shared" si="8"/>
+        <v>133427134</v>
+      </c>
+      <c r="X66">
+        <f t="shared" si="9"/>
+        <v>622653</v>
+      </c>
+      <c r="Y66">
+        <f t="shared" si="10"/>
+        <v>354001</v>
+      </c>
+    </row>
+    <row r="67" spans="2:25" ht="15.75" customHeight="1">
       <c r="B67">
         <v>61</v>
       </c>
@@ -27540,7 +28712,7 @@
         <v>3.500365474649159</v>
       </c>
       <c r="P67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3.0432402390098594</v>
       </c>
       <c r="Q67">
@@ -27555,8 +28727,27 @@
         <f t="shared" si="6"/>
         <v>3.819</v>
       </c>
-    </row>
-    <row r="68" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T67">
+        <v>61</v>
+      </c>
+      <c r="V67">
+        <f t="shared" si="7"/>
+        <v>10657151</v>
+      </c>
+      <c r="W67">
+        <f t="shared" si="8"/>
+        <v>153441204</v>
+      </c>
+      <c r="X67">
+        <f t="shared" si="9"/>
+        <v>653786</v>
+      </c>
+      <c r="Y67">
+        <f t="shared" si="10"/>
+        <v>368161</v>
+      </c>
+    </row>
+    <row r="68" spans="2:25" ht="15.75" customHeight="1">
       <c r="B68">
         <v>62</v>
       </c>
@@ -27585,7 +28776,7 @@
         <v>3.7246092988667345</v>
       </c>
       <c r="P68">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3.2381992609036456</v>
       </c>
       <c r="Q68">
@@ -27600,8 +28791,27 @@
         <f t="shared" si="6"/>
         <v>4.0640000000000001</v>
       </c>
-    </row>
-    <row r="69" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T68">
+        <v>62</v>
+      </c>
+      <c r="V68">
+        <f t="shared" si="7"/>
+        <v>11722866</v>
+      </c>
+      <c r="W68">
+        <f t="shared" si="8"/>
+        <v>176457385</v>
+      </c>
+      <c r="X68">
+        <f t="shared" si="9"/>
+        <v>686475</v>
+      </c>
+      <c r="Y68">
+        <f t="shared" si="10"/>
+        <v>382887</v>
+      </c>
+    </row>
+    <row r="69" spans="2:25" ht="15.75" customHeight="1">
       <c r="B69">
         <v>63</v>
       </c>
@@ -27630,7 +28840,7 @@
         <v>4.0210435102049304</v>
       </c>
       <c r="P69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3.4959210692968021</v>
       </c>
       <c r="Q69">
@@ -27645,8 +28855,27 @@
         <f t="shared" si="6"/>
         <v>4.3869999999999996</v>
       </c>
-    </row>
-    <row r="70" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T69">
+        <v>63</v>
+      </c>
+      <c r="V69">
+        <f t="shared" si="7"/>
+        <v>12895153</v>
+      </c>
+      <c r="W69">
+        <f t="shared" si="8"/>
+        <v>202925993</v>
+      </c>
+      <c r="X69">
+        <f t="shared" si="9"/>
+        <v>720799</v>
+      </c>
+      <c r="Y69">
+        <f t="shared" si="10"/>
+        <v>398202</v>
+      </c>
+    </row>
+    <row r="70" spans="2:25" ht="15.75" customHeight="1">
       <c r="B70">
         <v>64</v>
       </c>
@@ -27675,7 +28904,7 @@
         <v>4.9902091941958533</v>
       </c>
       <c r="P70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.3385199433713177</v>
       </c>
       <c r="Q70">
@@ -27690,8 +28919,27 @@
         <f t="shared" si="6"/>
         <v>5.444</v>
       </c>
-    </row>
-    <row r="71" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T70">
+        <v>64</v>
+      </c>
+      <c r="V70">
+        <f t="shared" si="7"/>
+        <v>14184668</v>
+      </c>
+      <c r="W70">
+        <f t="shared" si="8"/>
+        <v>233364892</v>
+      </c>
+      <c r="X70">
+        <f t="shared" si="9"/>
+        <v>756839</v>
+      </c>
+      <c r="Y70">
+        <f t="shared" si="10"/>
+        <v>414130</v>
+      </c>
+    </row>
+    <row r="71" spans="2:25" ht="15.75" customHeight="1">
       <c r="B71">
         <v>65</v>
       </c>
@@ -27720,7 +28968,7 @@
         <v>5.7351310539691998</v>
       </c>
       <c r="P71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.9861597955520471</v>
       </c>
       <c r="Q71">
@@ -27735,13 +28983,32 @@
         <f t="shared" si="6"/>
         <v>6.2569999999999997</v>
       </c>
-    </row>
-    <row r="72" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T71">
+        <v>65</v>
+      </c>
+      <c r="V71">
+        <f t="shared" si="7"/>
+        <v>15603135</v>
+      </c>
+      <c r="W71">
+        <f t="shared" si="8"/>
+        <v>268369626</v>
+      </c>
+      <c r="X71">
+        <f t="shared" si="9"/>
+        <v>794681</v>
+      </c>
+      <c r="Y71">
+        <f t="shared" si="10"/>
+        <v>430695</v>
+      </c>
+    </row>
+    <row r="72" spans="2:25" ht="15.75" customHeight="1">
       <c r="L72">
         <v>500000000</v>
       </c>
       <c r="M72">
-        <f t="shared" ref="M72" si="9">LOG(L72,2)</f>
+        <f t="shared" ref="M72" si="13">LOG(L72,2)</f>
         <v>28.897352853986263</v>
       </c>
       <c r="N72">
@@ -27749,11 +29016,11 @@
         <v>8.6989700043360187</v>
       </c>
       <c r="O72">
-        <f t="shared" ref="O72" si="10">LOG(L72,22)</f>
+        <f t="shared" ref="O72" si="14">LOG(L72,22)</f>
         <v>6.4800529137425471</v>
       </c>
       <c r="P72">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>5.6337996477327765</v>
       </c>
       <c r="Q72">
@@ -27761,15 +29028,18 @@
         <v>5.5895110366058391</v>
       </c>
       <c r="R72">
-        <f t="shared" ref="R72" si="11">ROUND(LOG(L72,20),3)</f>
+        <f t="shared" ref="R72" si="15">ROUND(LOG(L72,20),3)</f>
         <v>6.6859999999999999</v>
       </c>
       <c r="S72">
         <f t="shared" si="6"/>
         <v>7.07</v>
       </c>
-    </row>
-    <row r="76" spans="2:19" ht="15.75" customHeight="1">
+      <c r="T72">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="2:25" ht="15.75" customHeight="1">
       <c r="D76" t="s">
         <v>945</v>
       </c>

</xml_diff>

<commit_message>
Magic upgrades and History, Research, Fishing
Added Magic Upgrade History
Changed how magic gain works
Added 2 more Magic Upgrades
Implemented research items up to 70
Balancing chestnut and cherry
Started reimplementing fishing and other fishing mechanics
Some formatting
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917E9079-EAAB-4160-A8AD-BDAB0B96C176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2711332C-8A42-460E-ACE9-694CF1E4A584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3218" uniqueCount="1626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3234" uniqueCount="1627">
   <si>
     <t xml:space="preserve">Tier </t>
   </si>
@@ -4800,9 +4800,6 @@
     <t>10% WPS</t>
   </si>
   <si>
-    <t>Ash Beavers 13%</t>
-  </si>
-  <si>
     <t>Oak gives 25% More Magic</t>
   </si>
   <si>
@@ -4927,6 +4924,12 @@
   </si>
   <si>
     <t>Here</t>
+  </si>
+  <si>
+    <t>at 60 research</t>
+  </si>
+  <si>
+    <t>Ash Beaver 13% Better</t>
   </si>
 </sst>
 </file>
@@ -8399,7 +8402,7 @@
   <dimension ref="A2:O53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F18" sqref="F4:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -22131,8 +22134,8 @@
   </sheetPr>
   <dimension ref="C2:P157"/>
   <sheetViews>
-    <sheetView topLeftCell="A134" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F141" sqref="F141"/>
+    <sheetView topLeftCell="A125" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -22535,7 +22538,7 @@
         <v>21</v>
       </c>
       <c r="F25" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="P25" s="41" t="s">
         <v>294</v>
@@ -22749,7 +22752,7 @@
         <v>32</v>
       </c>
       <c r="F36" s="46" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>168</v>
@@ -22789,7 +22792,7 @@
         <v>34</v>
       </c>
       <c r="F38" s="46" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>178</v>
@@ -22915,7 +22918,7 @@
         <v>40</v>
       </c>
       <c r="F44" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>177</v>
@@ -22941,7 +22944,7 @@
         <v>41</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>167</v>
@@ -23170,7 +23173,7 @@
         <v>50</v>
       </c>
       <c r="F54" s="46" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>410</v>
@@ -23582,7 +23585,7 @@
         <v>70</v>
       </c>
       <c r="F74" s="45" t="s">
-        <v>1583</v>
+        <v>1626</v>
       </c>
       <c r="M74" t="s">
         <v>1052</v>
@@ -23630,7 +23633,7 @@
         <v>73</v>
       </c>
       <c r="F77" s="45" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="M77" t="s">
         <v>94</v>
@@ -23686,7 +23689,7 @@
         <v>77</v>
       </c>
       <c r="F81" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="M81" s="114" t="s">
         <v>1077</v>
@@ -23700,7 +23703,7 @@
         <v>78</v>
       </c>
       <c r="F82" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="M82" t="s">
         <v>1079</v>
@@ -23725,7 +23728,7 @@
         <v>80</v>
       </c>
       <c r="F84" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="M84" t="s">
         <v>1082</v>
@@ -23761,7 +23764,7 @@
         <v>83</v>
       </c>
       <c r="F87" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="M87" t="s">
         <v>1092</v>
@@ -23783,7 +23786,7 @@
         <v>85</v>
       </c>
       <c r="F89" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="M89" t="s">
         <v>1102</v>
@@ -23816,7 +23819,7 @@
         <v>88</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="M92" t="s">
         <v>1118</v>
@@ -23838,7 +23841,7 @@
         <v>90</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="M94" t="s">
         <v>1119</v>
@@ -23857,146 +23860,223 @@
         <v>92</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>1601</v>
-      </c>
-    </row>
-    <row r="97" spans="5:6" ht="15.75" customHeight="1">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="97" spans="5:14" ht="15.75" customHeight="1">
       <c r="E97" s="1">
         <v>93</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="98" spans="5:6" ht="15.75" customHeight="1">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="98" spans="5:14" ht="15.75" customHeight="1">
       <c r="E98" s="1">
         <v>94</v>
       </c>
       <c r="F98" s="45" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="99" spans="5:6" ht="15.75" customHeight="1">
+        <v>1587</v>
+      </c>
+      <c r="M98" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="99" spans="5:14" ht="15.75" customHeight="1">
       <c r="E99" s="1">
         <v>95</v>
       </c>
       <c r="F99" s="47" t="s">
         <v>1571</v>
       </c>
-    </row>
-    <row r="100" spans="5:6" ht="15.75" customHeight="1">
+      <c r="M99" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="N99" s="40">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="100" spans="5:14" ht="15.75" customHeight="1">
       <c r="E100" s="1">
         <v>96</v>
       </c>
       <c r="F100" s="122" t="s">
         <v>1545</v>
       </c>
-    </row>
-    <row r="101" spans="5:6" ht="15.75" customHeight="1">
+      <c r="M100" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="N100" s="40">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="101" spans="5:14" ht="15.75" customHeight="1">
       <c r="E101" s="1">
         <v>97</v>
       </c>
       <c r="F101" s="45" t="s">
-        <v>1602</v>
-      </c>
-    </row>
-    <row r="102" spans="5:6" ht="15.75" customHeight="1">
+        <v>1601</v>
+      </c>
+      <c r="M101" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="N101" s="40">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="102" spans="5:14" ht="15.75" customHeight="1">
       <c r="E102" s="1">
         <v>98</v>
       </c>
       <c r="F102" s="45" t="s">
-        <v>1605</v>
-      </c>
-    </row>
-    <row r="103" spans="5:6" ht="15.75" customHeight="1">
+        <v>1604</v>
+      </c>
+      <c r="M102" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="N102" s="40">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="103" spans="5:14" ht="15.75" customHeight="1">
       <c r="E103" s="1">
         <v>99</v>
       </c>
       <c r="F103" s="35" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="104" spans="5:6" ht="15.75" customHeight="1">
+      <c r="M103" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="N103" s="40">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104" spans="5:14" ht="15.75" customHeight="1">
       <c r="E104" s="1">
         <v>100</v>
       </c>
       <c r="F104" t="s">
         <v>1575</v>
       </c>
-    </row>
-    <row r="105" spans="5:6" ht="15.75" customHeight="1">
+      <c r="M104" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="N104" s="40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="105" spans="5:14" ht="15.75" customHeight="1">
       <c r="E105" s="1">
         <v>101</v>
       </c>
       <c r="F105" t="s">
-        <v>1598</v>
-      </c>
-    </row>
-    <row r="106" spans="5:6" ht="15.75" customHeight="1">
+        <v>1597</v>
+      </c>
+      <c r="M105" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="N105" s="40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="5:14" ht="15.75" customHeight="1">
       <c r="E106" s="1">
         <v>102</v>
       </c>
       <c r="F106" t="s">
-        <v>1590</v>
-      </c>
-    </row>
-    <row r="107" spans="5:6" ht="15.75" customHeight="1">
+        <v>1589</v>
+      </c>
+      <c r="M106" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="N106" s="40"/>
+    </row>
+    <row r="107" spans="5:14" ht="15.75" customHeight="1">
       <c r="E107" s="1">
         <v>103</v>
       </c>
       <c r="F107" t="s">
-        <v>1585</v>
-      </c>
-    </row>
-    <row r="108" spans="5:6" ht="15.75" customHeight="1">
+        <v>1584</v>
+      </c>
+      <c r="M107" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="N107" s="40"/>
+    </row>
+    <row r="108" spans="5:14" ht="15.75" customHeight="1">
       <c r="E108" s="1">
         <v>104</v>
       </c>
       <c r="F108" t="s">
-        <v>1593</v>
-      </c>
-    </row>
-    <row r="109" spans="5:6" ht="15.75" customHeight="1">
+        <v>1592</v>
+      </c>
+      <c r="M108" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="N108" s="40"/>
+    </row>
+    <row r="109" spans="5:14" ht="15.75" customHeight="1">
       <c r="E109" s="1">
         <v>105</v>
       </c>
       <c r="F109" t="s">
         <v>1579</v>
       </c>
-    </row>
-    <row r="110" spans="5:6" ht="15.75" customHeight="1">
+      <c r="M109" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="N109" s="40"/>
+    </row>
+    <row r="110" spans="5:14" ht="15.75" customHeight="1">
       <c r="E110" s="1">
         <v>106</v>
       </c>
       <c r="F110" t="s">
-        <v>1596</v>
-      </c>
-    </row>
-    <row r="111" spans="5:6" ht="15.75" customHeight="1">
+        <v>1595</v>
+      </c>
+      <c r="M110" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="N110" s="40"/>
+    </row>
+    <row r="111" spans="5:14" ht="15.75" customHeight="1">
       <c r="E111" s="1">
         <v>107</v>
       </c>
       <c r="F111" t="s">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="112" spans="5:6" ht="15.75" customHeight="1">
+        <v>1591</v>
+      </c>
+      <c r="M111" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="N111" s="40"/>
+    </row>
+    <row r="112" spans="5:14" ht="15.75" customHeight="1">
       <c r="E112" s="1">
         <v>108</v>
       </c>
       <c r="F112" t="s">
-        <v>1606</v>
-      </c>
-    </row>
-    <row r="113" spans="5:6" ht="15.75" customHeight="1">
+        <v>1605</v>
+      </c>
+      <c r="M112" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="N112" s="40"/>
+    </row>
+    <row r="113" spans="5:14" ht="15.75" customHeight="1">
       <c r="E113" s="1">
         <v>109</v>
       </c>
       <c r="F113" s="35" t="s">
         <v>1522</v>
       </c>
-    </row>
-    <row r="114" spans="5:6" ht="15.75" customHeight="1">
+      <c r="M113" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="N113" s="40"/>
+    </row>
+    <row r="114" spans="5:14" ht="15.75" customHeight="1">
       <c r="E114" s="1">
         <v>110</v>
       </c>
@@ -24004,39 +24084,39 @@
         <v>1533</v>
       </c>
     </row>
-    <row r="115" spans="5:6" ht="15.75" customHeight="1">
+    <row r="115" spans="5:14" ht="15.75" customHeight="1">
       <c r="E115" s="1">
         <v>111</v>
       </c>
       <c r="F115" t="s">
-        <v>1603</v>
-      </c>
-    </row>
-    <row r="116" spans="5:6" ht="15.75" customHeight="1">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="116" spans="5:14" ht="15.75" customHeight="1">
       <c r="E116" s="1">
         <v>112</v>
       </c>
       <c r="F116" t="s">
-        <v>1609</v>
-      </c>
-    </row>
-    <row r="117" spans="5:6" ht="15.75" customHeight="1">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="117" spans="5:14" ht="15.75" customHeight="1">
       <c r="E117" s="1">
         <v>113</v>
       </c>
       <c r="F117" t="s">
-        <v>1597</v>
-      </c>
-    </row>
-    <row r="118" spans="5:6" ht="15.75" customHeight="1">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="118" spans="5:14" ht="15.75" customHeight="1">
       <c r="E118" s="1">
         <v>114</v>
       </c>
       <c r="F118" t="s">
-        <v>1591</v>
-      </c>
-    </row>
-    <row r="119" spans="5:6" ht="15.75" customHeight="1">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="119" spans="5:14" ht="15.75" customHeight="1">
       <c r="E119" s="1">
         <v>115</v>
       </c>
@@ -24044,15 +24124,15 @@
         <v>1581</v>
       </c>
     </row>
-    <row r="120" spans="5:6" ht="15.75" customHeight="1">
+    <row r="120" spans="5:14" ht="15.75" customHeight="1">
       <c r="E120" s="1">
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>1610</v>
-      </c>
-    </row>
-    <row r="121" spans="5:6" ht="15.75" customHeight="1">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="121" spans="5:14" ht="15.75" customHeight="1">
       <c r="E121" s="1">
         <v>117</v>
       </c>
@@ -24060,15 +24140,15 @@
         <v>1537</v>
       </c>
     </row>
-    <row r="122" spans="5:6" ht="15.75" customHeight="1">
+    <row r="122" spans="5:14" ht="15.75" customHeight="1">
       <c r="E122" s="1">
         <v>118</v>
       </c>
       <c r="F122" t="s">
-        <v>1604</v>
-      </c>
-    </row>
-    <row r="123" spans="5:6" ht="15.75" customHeight="1">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="123" spans="5:14" ht="15.75" customHeight="1">
       <c r="E123" s="1">
         <v>119</v>
       </c>
@@ -24076,7 +24156,7 @@
         <v>1523</v>
       </c>
     </row>
-    <row r="124" spans="5:6" ht="15.75" customHeight="1">
+    <row r="124" spans="5:14" ht="15.75" customHeight="1">
       <c r="E124" s="1">
         <v>120</v>
       </c>
@@ -24084,15 +24164,15 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="125" spans="5:6" ht="15.75" customHeight="1">
+    <row r="125" spans="5:14" ht="15.75" customHeight="1">
       <c r="E125" s="1">
         <v>121</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>1611</v>
-      </c>
-    </row>
-    <row r="126" spans="5:6" ht="15.75" customHeight="1">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="126" spans="5:14" ht="15.75" customHeight="1">
       <c r="E126" s="1">
         <v>122</v>
       </c>
@@ -24100,15 +24180,15 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="127" spans="5:6" ht="15.75" customHeight="1">
+    <row r="127" spans="5:14" ht="15.75" customHeight="1">
       <c r="E127" s="1">
         <v>123</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>1613</v>
-      </c>
-    </row>
-    <row r="128" spans="5:6" ht="15.75" customHeight="1">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="128" spans="5:14" ht="15.75" customHeight="1">
       <c r="E128" s="1">
         <v>124</v>
       </c>
@@ -24121,7 +24201,7 @@
         <v>125</v>
       </c>
       <c r="F129" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="130" spans="5:6" ht="15.75" customHeight="1">
@@ -24137,7 +24217,7 @@
         <v>127</v>
       </c>
       <c r="F131" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="132" spans="5:6" ht="15.75" customHeight="1">
@@ -24161,7 +24241,7 @@
         <v>130</v>
       </c>
       <c r="F134" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="135" spans="5:6" ht="15.75" customHeight="1">
@@ -24177,7 +24257,7 @@
         <v>132</v>
       </c>
       <c r="F136" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="137" spans="5:6" ht="15.75" customHeight="1">
@@ -24209,7 +24289,7 @@
         <v>136</v>
       </c>
       <c r="F140" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="141" spans="5:6" ht="15.75" customHeight="1">
@@ -24217,7 +24297,7 @@
         <v>137</v>
       </c>
       <c r="F141" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="142" spans="5:6" ht="15.75" customHeight="1">
@@ -24233,7 +24313,7 @@
         <v>139</v>
       </c>
       <c r="F143" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="144" spans="5:6" ht="15.75" customHeight="1">
@@ -24749,8 +24829,8 @@
   </sheetPr>
   <dimension ref="A3:AB114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N57" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AB74" sqref="AB74"/>
+    <sheetView tabSelected="1" topLeftCell="N64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="X90" sqref="X90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -25045,7 +25125,7 @@
         <v>37276</v>
       </c>
       <c r="AA9">
-        <f t="shared" ref="AA9:AA71" si="13">AA8+Z9</f>
+        <f t="shared" ref="AA9:AA70" si="13">AA8+Z9</f>
         <v>108396</v>
       </c>
     </row>
@@ -29679,7 +29759,7 @@
         <v>9553102</v>
       </c>
       <c r="AB76" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="77" spans="2:28" ht="15.75" customHeight="1">
@@ -29695,7 +29775,7 @@
         <v>33703033</v>
       </c>
       <c r="Z77">
-        <f t="shared" ref="Z77:Z114" si="23">ROUND($Z$75*POWER(1.0003,T77-1),0)</f>
+        <f t="shared" ref="Z77:Z105" si="23">ROUND($Z$75*POWER(1.0003,T77-1),0)</f>
         <v>596706</v>
       </c>
       <c r="AA77">
@@ -30312,7 +30392,7 @@
         <v>29236980</v>
       </c>
       <c r="AB106" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="107" spans="20:28" ht="15.75" customHeight="1">
@@ -30328,7 +30408,7 @@
         <v>2.9469590085807801E+110</v>
       </c>
       <c r="Z107">
-        <f t="shared" ref="Z107:Z114" si="24">ROUND($Z$105*POWER(1.00001,T107-1),0)</f>
+        <f t="shared" ref="Z107:Z108" si="24">ROUND($Z$105*POWER(1.00001,T107-1),0)</f>
         <v>807042</v>
       </c>
       <c r="AA107">
@@ -30378,7 +30458,7 @@
         <v>31784361</v>
       </c>
       <c r="AB109" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="110" spans="20:28" ht="15.75" customHeight="1">
@@ -30394,7 +30474,7 @@
         <v>#NUM!</v>
       </c>
       <c r="Z110">
-        <f t="shared" ref="Z110:Z114" si="25">ROUND($Z$108*POWER(1.000001,T110-1),0)</f>
+        <f t="shared" ref="Z110" si="25">ROUND($Z$108*POWER(1.000001,T110-1),0)</f>
         <v>937648</v>
       </c>
       <c r="AA110">
@@ -30423,7 +30503,7 @@
         <v>33683394</v>
       </c>
       <c r="AB111" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="112" spans="20:28" ht="15.75" customHeight="1">
@@ -30447,7 +30527,7 @@
         <v>34694070</v>
       </c>
       <c r="AB112" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="113" spans="20:28" ht="15.75" customHeight="1">
@@ -30471,7 +30551,7 @@
         <v>35756564</v>
       </c>
       <c r="AB113" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="114" spans="20:28" ht="15.75" customHeight="1">
@@ -30495,7 +30575,7 @@
         <v>36873533</v>
       </c>
       <c r="AB114" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fishing Store, Removed Spots and Other Fishing Logic
Remade the bait store to a fishing store with less baits to more upgrades
Removed fishing spots
Added FishBiscuts to saves, changed bait to shop items in saves
Made older saves playable
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777573DC-D925-4559-B669-2F877AE27470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738F7297-2C2D-4715-ACC1-14F4DE4D6252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,11 @@
     <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3265" uniqueCount="1654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3267" uniqueCount="1650">
   <si>
     <t xml:space="preserve">Tier </t>
   </si>
@@ -4924,36 +4923,6 @@
     <t>Gem Shop</t>
   </si>
   <si>
-    <t>Bait 1</t>
-  </si>
-  <si>
-    <t>Bait 2</t>
-  </si>
-  <si>
-    <t>Bait 3</t>
-  </si>
-  <si>
-    <t>Bait 4</t>
-  </si>
-  <si>
-    <t>Bait 5</t>
-  </si>
-  <si>
-    <t>Bait 6</t>
-  </si>
-  <si>
-    <t>Bait 7</t>
-  </si>
-  <si>
-    <t>Bait 8</t>
-  </si>
-  <si>
-    <t>Bait 9</t>
-  </si>
-  <si>
-    <t>Bait 10</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
@@ -5012,6 +4981,24 @@
   </si>
   <si>
     <t>1+ beaver</t>
+  </si>
+  <si>
+    <t>Unlock</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>New Fishing Level</t>
+  </si>
+  <si>
+    <t>Fishing Chance +1</t>
+  </si>
+  <si>
+    <t>Chance To Not Use Bait 10%</t>
+  </si>
+  <si>
+    <t>100 * n</t>
   </si>
 </sst>
 </file>
@@ -34001,20 +33988,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="C3:T62"/>
+  <dimension ref="B3:U62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q32:Q33"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="19.140625" customWidth="1"/>
-    <col min="11" max="11" width="51.85546875" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
     <col min="16" max="16" width="24.28515625" customWidth="1"/>
     <col min="17" max="17" width="19.140625" customWidth="1"/>
@@ -34026,7 +34013,7 @@
     <col min="25" max="25" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:20">
+    <row r="3" spans="3:21">
       <c r="C3" s="1" t="s">
         <v>258</v>
       </c>
@@ -34037,12 +34024,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="3:20">
+    <row r="4" spans="3:21">
       <c r="E4" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="3:20">
+    <row r="5" spans="3:21">
       <c r="C5" s="1" t="s">
         <v>52</v>
       </c>
@@ -34077,13 +34064,16 @@
         <v>823</v>
       </c>
       <c r="O5" s="46" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P5" s="46" t="s">
         <v>824</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="3:20">
+    <row r="6" spans="3:21">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -34103,19 +34093,22 @@
         <v>716</v>
       </c>
       <c r="K6" t="s">
-        <v>1651</v>
+        <v>1641</v>
       </c>
       <c r="M6" t="s">
-        <v>1648</v>
+        <v>1638</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
-      <c r="O6" s="45" t="s">
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6" s="45" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="7" spans="3:20">
+    <row r="7" spans="3:21">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -34135,31 +34128,34 @@
         <v>715</v>
       </c>
       <c r="K7" t="s">
-        <v>1652</v>
+        <v>1642</v>
       </c>
       <c r="M7" t="s">
-        <v>1649</v>
+        <v>1639</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="3:20">
+    <row r="8" spans="3:21">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -34182,23 +34178,26 @@
         <v>1139</v>
       </c>
       <c r="M8" t="s">
-        <v>1650</v>
+        <v>1640</v>
       </c>
       <c r="N8">
         <v>5</v>
       </c>
-      <c r="P8" s="1">
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
         <v>1</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="S8" s="29"/>
-    </row>
-    <row r="9" spans="3:20">
+      <c r="T8" s="29"/>
+    </row>
+    <row r="9" spans="3:21">
       <c r="C9" s="1">
         <v>4</v>
       </c>
@@ -34218,7 +34217,7 @@
         <v>742</v>
       </c>
       <c r="K9" t="s">
-        <v>1653</v>
+        <v>1643</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -34226,18 +34225,21 @@
       <c r="N9">
         <v>0</v>
       </c>
-      <c r="P9" s="1">
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
         <v>2</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="R9" s="50" t="s">
+      <c r="S9" s="50" t="s">
         <v>806</v>
       </c>
-      <c r="S9" s="30"/>
-    </row>
-    <row r="10" spans="3:20">
+      <c r="T9" s="30"/>
+    </row>
+    <row r="10" spans="3:21">
       <c r="C10" s="1">
         <v>5</v>
       </c>
@@ -34265,18 +34267,21 @@
       <c r="N10">
         <v>0</v>
       </c>
-      <c r="P10" s="1">
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
         <v>3</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="S10" s="32"/>
-    </row>
-    <row r="11" spans="3:20">
+      <c r="T10" s="32"/>
+    </row>
+    <row r="11" spans="3:21">
       <c r="C11" s="1">
         <v>6</v>
       </c>
@@ -34304,18 +34309,21 @@
       <c r="N11">
         <v>10</v>
       </c>
-      <c r="P11" s="1">
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="1">
         <v>4</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="S11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="S11" s="33"/>
-    </row>
-    <row r="12" spans="3:20">
+      <c r="T11" s="33"/>
+    </row>
+    <row r="12" spans="3:21">
       <c r="C12" s="1">
         <v>7</v>
       </c>
@@ -34346,18 +34354,21 @@
       <c r="N12">
         <v>20</v>
       </c>
-      <c r="P12" s="1">
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="1">
         <v>5</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="S12" s="34"/>
-    </row>
-    <row r="13" spans="3:20">
+      <c r="T12" s="34"/>
+    </row>
+    <row r="13" spans="3:21">
       <c r="C13" s="1">
         <v>8</v>
       </c>
@@ -34385,8 +34396,11 @@
       <c r="N13">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="3:20">
+      <c r="O13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:21">
       <c r="C14" s="1">
         <v>9</v>
       </c>
@@ -34414,8 +34428,11 @@
       <c r="N14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="3:20">
+      <c r="O14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:21">
       <c r="C15" s="1">
         <v>10</v>
       </c>
@@ -34443,8 +34460,11 @@
       <c r="N15">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="3:20">
+      <c r="O15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="3:21">
       <c r="C16" s="1">
         <v>11</v>
       </c>
@@ -34472,8 +34492,11 @@
       <c r="N16">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="3:14">
+      <c r="O16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15">
       <c r="C17" s="1">
         <v>12</v>
       </c>
@@ -34495,8 +34518,11 @@
       <c r="N17">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="3:14">
+      <c r="O17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15">
       <c r="C18" s="1">
         <v>13</v>
       </c>
@@ -34518,8 +34544,11 @@
       <c r="N18">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="3:14">
+      <c r="O18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15">
       <c r="C19" s="1">
         <v>14</v>
       </c>
@@ -34541,8 +34570,11 @@
       <c r="N19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="3:14">
+      <c r="O19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15">
       <c r="C20" s="1">
         <v>15</v>
       </c>
@@ -34564,8 +34596,11 @@
       <c r="N20">
         <v>185</v>
       </c>
-    </row>
-    <row r="21" spans="3:14">
+      <c r="O20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15">
       <c r="C21" s="1">
         <v>16</v>
       </c>
@@ -34587,8 +34622,11 @@
       <c r="N21">
         <v>110</v>
       </c>
-    </row>
-    <row r="22" spans="3:14">
+      <c r="O21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15">
       <c r="C22" s="1">
         <v>17</v>
       </c>
@@ -34610,8 +34648,11 @@
       <c r="N22">
         <v>230</v>
       </c>
-    </row>
-    <row r="23" spans="3:14">
+      <c r="O22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15">
       <c r="C23" s="1">
         <v>18</v>
       </c>
@@ -34633,8 +34674,11 @@
       <c r="N23">
         <v>55</v>
       </c>
-    </row>
-    <row r="24" spans="3:14">
+      <c r="O23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15">
       <c r="C24" s="1">
         <v>19</v>
       </c>
@@ -34656,8 +34700,11 @@
       <c r="N24">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="3:14">
+      <c r="O24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15">
       <c r="C25" s="1">
         <v>20</v>
       </c>
@@ -34679,8 +34726,11 @@
       <c r="N25">
         <v>110</v>
       </c>
-    </row>
-    <row r="26" spans="3:14">
+      <c r="O25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15">
       <c r="C26" s="1">
         <v>21</v>
       </c>
@@ -34702,8 +34752,11 @@
       <c r="N26">
         <v>145</v>
       </c>
-    </row>
-    <row r="27" spans="3:14">
+      <c r="O26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15">
       <c r="I27" s="1">
         <v>22</v>
       </c>
@@ -34719,8 +34772,11 @@
       <c r="N27">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="3:14">
+      <c r="O27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15">
       <c r="C28" t="s">
         <v>1623</v>
       </c>
@@ -34739,10 +34795,19 @@
       <c r="N28">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="3:14">
+      <c r="O28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15">
       <c r="E29" t="s">
-        <v>1634</v>
+        <v>1624</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1644</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1645</v>
       </c>
       <c r="I29" s="1">
         <v>24</v>
@@ -34759,10 +34824,13 @@
       <c r="N29">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="3:14">
-      <c r="C30" t="s">
-        <v>1624</v>
+      <c r="O29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15">
+      <c r="C30" s="46" t="s">
+        <v>812</v>
       </c>
       <c r="D30">
         <v>5</v>
@@ -34770,6 +34838,12 @@
       <c r="E30">
         <v>10</v>
       </c>
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
       <c r="I30" s="1">
         <v>25</v>
       </c>
@@ -34785,17 +34859,26 @@
       <c r="N30">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="3:14">
-      <c r="C31" t="s">
-        <v>1625</v>
+      <c r="O30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15">
+      <c r="C31" s="46" t="s">
+        <v>817</v>
       </c>
       <c r="D31">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E31">
         <v>10</v>
       </c>
+      <c r="F31">
+        <v>350</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
       <c r="I31" s="1">
         <v>26</v>
       </c>
@@ -34811,17 +34894,26 @@
       <c r="N31">
         <v>80</v>
       </c>
-    </row>
-    <row r="32" spans="3:14">
-      <c r="C32" t="s">
-        <v>1626</v>
+      <c r="O31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15">
+      <c r="C32" s="46" t="s">
+        <v>818</v>
       </c>
       <c r="D32">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="E32">
         <v>10</v>
       </c>
+      <c r="F32">
+        <v>1500</v>
+      </c>
+      <c r="G32">
+        <v>3</v>
+      </c>
       <c r="I32" s="1">
         <v>27</v>
       </c>
@@ -34837,17 +34929,26 @@
       <c r="N32">
         <v>185</v>
       </c>
-    </row>
-    <row r="33" spans="3:14">
-      <c r="C33" t="s">
-        <v>1627</v>
+      <c r="O32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15">
+      <c r="C33" s="46" t="s">
+        <v>819</v>
       </c>
       <c r="D33">
-        <v>200</v>
+        <v>650</v>
       </c>
       <c r="E33">
         <v>10</v>
       </c>
+      <c r="F33">
+        <v>6500</v>
+      </c>
+      <c r="G33">
+        <v>4</v>
+      </c>
       <c r="I33" s="1">
         <v>28</v>
       </c>
@@ -34863,17 +34964,26 @@
       <c r="N33">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="3:14">
-      <c r="C34" t="s">
-        <v>1628</v>
+      <c r="O33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15">
+      <c r="C34" s="46" t="s">
+        <v>816</v>
       </c>
       <c r="D34">
-        <v>450</v>
+        <v>3000</v>
       </c>
       <c r="E34">
         <v>10</v>
       </c>
+      <c r="F34">
+        <v>30000</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
       <c r="I34" s="1">
         <v>29</v>
       </c>
@@ -34889,17 +34999,20 @@
       <c r="N34">
         <v>145</v>
       </c>
-    </row>
-    <row r="35" spans="3:14">
+      <c r="O34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15">
+      <c r="B35">
+        <v>1</v>
+      </c>
       <c r="C35" t="s">
-        <v>1629</v>
+        <v>1625</v>
       </c>
       <c r="D35">
         <v>1000</v>
       </c>
-      <c r="E35">
-        <v>10</v>
-      </c>
       <c r="I35" s="1">
         <v>30</v>
       </c>
@@ -34915,16 +35028,19 @@
       <c r="N35">
         <v>80</v>
       </c>
-    </row>
-    <row r="36" spans="3:14">
+      <c r="O35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15">
+      <c r="B36">
+        <v>2</v>
+      </c>
       <c r="C36" t="s">
-        <v>1630</v>
+        <v>1626</v>
       </c>
       <c r="D36">
-        <v>2500</v>
-      </c>
-      <c r="E36">
-        <v>10</v>
+        <v>50000</v>
       </c>
       <c r="I36" s="1">
         <v>31</v>
@@ -34941,16 +35057,19 @@
       <c r="N36">
         <v>230</v>
       </c>
-    </row>
-    <row r="37" spans="3:14">
+      <c r="O36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15">
+      <c r="B37">
+        <v>3</v>
+      </c>
       <c r="C37" t="s">
-        <v>1631</v>
+        <v>1627</v>
       </c>
       <c r="D37">
-        <v>3500</v>
-      </c>
-      <c r="E37">
-        <v>5</v>
+        <v>250000</v>
       </c>
       <c r="I37" s="1">
         <v>32</v>
@@ -34967,16 +35086,19 @@
       <c r="N37">
         <v>100</v>
       </c>
-    </row>
-    <row r="38" spans="3:14">
+      <c r="O37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15">
+      <c r="B38">
+        <v>4</v>
+      </c>
       <c r="C38" t="s">
-        <v>1632</v>
+        <v>1628</v>
       </c>
       <c r="D38">
-        <v>5000</v>
-      </c>
-      <c r="E38">
-        <v>5</v>
+        <v>300</v>
       </c>
       <c r="I38" s="1">
         <v>33</v>
@@ -34993,16 +35115,19 @@
       <c r="N38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="3:14">
+      <c r="O38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15">
+      <c r="B39">
+        <v>5</v>
+      </c>
       <c r="C39" t="s">
-        <v>1633</v>
+        <v>1629</v>
       </c>
       <c r="D39">
-        <v>10000</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
+        <v>6000</v>
       </c>
       <c r="I39" s="1">
         <v>34</v>
@@ -35019,13 +35144,19 @@
       <c r="N39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="3:14">
+      <c r="O39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15">
+      <c r="B40">
+        <v>6</v>
+      </c>
       <c r="C40" t="s">
-        <v>1635</v>
+        <v>1630</v>
       </c>
       <c r="D40">
-        <v>1000</v>
+        <v>90000</v>
       </c>
       <c r="I40" s="1">
         <v>35</v>
@@ -35042,13 +35173,19 @@
       <c r="N40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="3:14">
+      <c r="O40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15">
+      <c r="B41">
+        <v>7</v>
+      </c>
       <c r="C41" t="s">
-        <v>1636</v>
+        <v>1631</v>
       </c>
       <c r="D41">
-        <v>50000</v>
+        <v>300</v>
       </c>
       <c r="I41" s="1">
         <v>36</v>
@@ -35065,13 +35202,19 @@
       <c r="N41">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="3:14">
+      <c r="O41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15">
+      <c r="B42">
+        <v>8</v>
+      </c>
       <c r="C42" t="s">
-        <v>1637</v>
+        <v>1632</v>
       </c>
       <c r="D42">
-        <v>250000</v>
+        <v>6000</v>
       </c>
       <c r="I42" s="1">
         <v>37</v>
@@ -35088,13 +35231,19 @@
       <c r="N42">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="3:14">
+      <c r="O42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15">
+      <c r="B43">
+        <v>9</v>
+      </c>
       <c r="C43" t="s">
-        <v>1638</v>
+        <v>1633</v>
       </c>
       <c r="D43">
-        <v>300</v>
+        <v>90000</v>
       </c>
       <c r="I43" s="1">
         <v>38</v>
@@ -35111,13 +35260,19 @@
       <c r="N43">
         <v>20</v>
       </c>
-    </row>
-    <row r="44" spans="3:14">
+      <c r="O43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15">
+      <c r="B44">
+        <v>10</v>
+      </c>
       <c r="C44" t="s">
-        <v>1639</v>
-      </c>
-      <c r="D44">
-        <v>6000</v>
+        <v>1137</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1636</v>
       </c>
       <c r="I44" s="1">
         <v>39</v>
@@ -35134,13 +35289,19 @@
       <c r="N44">
         <v>20</v>
       </c>
-    </row>
-    <row r="45" spans="3:14">
+      <c r="O44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15">
+      <c r="B45">
+        <v>11</v>
+      </c>
       <c r="C45" t="s">
-        <v>1640</v>
-      </c>
-      <c r="D45">
-        <v>90000</v>
+        <v>1138</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1634</v>
       </c>
       <c r="I45" s="1">
         <v>40</v>
@@ -35157,13 +35318,19 @@
       <c r="N45">
         <v>35</v>
       </c>
-    </row>
-    <row r="46" spans="3:14">
+      <c r="O45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15">
+      <c r="B46">
+        <v>12</v>
+      </c>
       <c r="C46" t="s">
-        <v>1641</v>
-      </c>
-      <c r="D46">
-        <v>300</v>
+        <v>1139</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1635</v>
       </c>
       <c r="I46" s="1">
         <v>41</v>
@@ -35180,13 +35347,19 @@
       <c r="N46">
         <v>55</v>
       </c>
-    </row>
-    <row r="47" spans="3:14">
+      <c r="O46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15">
+      <c r="B47">
+        <v>13</v>
+      </c>
       <c r="C47" t="s">
-        <v>1642</v>
+        <v>1637</v>
       </c>
       <c r="D47">
-        <v>6000</v>
+        <v>7500</v>
       </c>
       <c r="I47" s="1">
         <v>42</v>
@@ -35203,13 +35376,19 @@
       <c r="N47">
         <v>80</v>
       </c>
-    </row>
-    <row r="48" spans="3:14">
+      <c r="O47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15">
+      <c r="B48">
+        <v>14</v>
+      </c>
       <c r="C48" t="s">
-        <v>1643</v>
+        <v>1647</v>
       </c>
       <c r="D48">
-        <v>90000</v>
+        <v>1000</v>
       </c>
       <c r="I48" s="1">
         <v>43</v>
@@ -35226,13 +35405,19 @@
       <c r="N48">
         <v>100</v>
       </c>
-    </row>
-    <row r="49" spans="3:14">
+      <c r="O48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15">
+      <c r="B49">
+        <v>15</v>
+      </c>
       <c r="C49" t="s">
-        <v>1137</v>
-      </c>
-      <c r="D49" t="s">
-        <v>1646</v>
+        <v>1647</v>
+      </c>
+      <c r="D49">
+        <v>7000</v>
       </c>
       <c r="I49" s="1">
         <v>44</v>
@@ -35249,13 +35434,19 @@
       <c r="N49">
         <v>110</v>
       </c>
-    </row>
-    <row r="50" spans="3:14">
+      <c r="O49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15">
+      <c r="B50">
+        <v>16</v>
+      </c>
       <c r="C50" t="s">
-        <v>1138</v>
+        <v>1648</v>
       </c>
       <c r="D50" t="s">
-        <v>1644</v>
+        <v>1649</v>
       </c>
       <c r="I50" s="1">
         <v>45</v>
@@ -35272,14 +35463,11 @@
       <c r="N50">
         <v>145</v>
       </c>
-    </row>
-    <row r="51" spans="3:14">
-      <c r="C51" t="s">
-        <v>1139</v>
-      </c>
-      <c r="D51" t="s">
-        <v>1645</v>
-      </c>
+      <c r="O50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15">
       <c r="I51" s="1">
         <v>46</v>
       </c>
@@ -35295,14 +35483,11 @@
       <c r="N51">
         <v>185</v>
       </c>
-    </row>
-    <row r="52" spans="3:14">
-      <c r="C52" t="s">
-        <v>1647</v>
-      </c>
-      <c r="D52">
-        <v>7500</v>
-      </c>
+      <c r="O51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15">
       <c r="I52" s="1">
         <v>47</v>
       </c>
@@ -35318,8 +35503,11 @@
       <c r="N52">
         <v>230</v>
       </c>
-    </row>
-    <row r="53" spans="3:14">
+      <c r="O52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15">
       <c r="I53" s="1">
         <v>48</v>
       </c>
@@ -35335,8 +35523,11 @@
       <c r="N53">
         <v>230</v>
       </c>
-    </row>
-    <row r="54" spans="3:14">
+      <c r="O53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15">
       <c r="I54" s="1">
         <v>49</v>
       </c>
@@ -35352,50 +35543,53 @@
       <c r="N54">
         <v>145</v>
       </c>
-    </row>
-    <row r="55" spans="3:14">
+      <c r="O54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15">
       <c r="I55" s="1">
         <v>50</v>
       </c>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="3:14">
+    <row r="56" spans="2:15">
       <c r="I56" s="1">
         <v>51</v>
       </c>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="3:14">
+    <row r="57" spans="2:15">
       <c r="I57" s="1">
         <v>52</v>
       </c>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="3:14">
+    <row r="58" spans="2:15">
       <c r="I58" s="1">
         <v>53</v>
       </c>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="3:14">
+    <row r="59" spans="2:15">
       <c r="I59" s="1">
         <v>54</v>
       </c>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="3:14">
+    <row r="60" spans="2:15">
       <c r="I60" s="1">
         <v>55</v>
       </c>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="3:14">
+    <row r="61" spans="2:15">
       <c r="I61" s="1">
         <v>56</v>
       </c>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="3:14">
+    <row r="62" spans="2:15">
       <c r="I62" s="1">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
Big Fishing Fixes Research, Magic, Achievements
Fix Add Fishing Value Application for fishing and normal game
Use Bait When Fishing
Fix a lot of Fishing Bugs
Redo some of The Achievements
Add New Research and Magic Upgrades
Added Temporary Fishing Bonuses for WPS and WPC
Implemented Keep Research Magic Upgrades
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EC1F28-3B47-453E-9F88-5C104E3BABBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2109E3B-481E-4024-91EA-38A2A1E0F1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5857,6 +5857,7 @@
     <xf numFmtId="0" fontId="7" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="47" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5864,7 +5865,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9528,19 +9528,19 @@
       <c r="K5" s="45" t="s">
         <v>358</v>
       </c>
-      <c r="M5" s="123" t="s">
+      <c r="M5" s="124" t="s">
         <v>78</v>
       </c>
-      <c r="N5" s="123"/>
-      <c r="O5" s="123"/>
-      <c r="P5" s="123"/>
-      <c r="Q5" s="123"/>
-      <c r="R5" s="123"/>
-      <c r="S5" s="123"/>
-      <c r="T5" s="123"/>
-      <c r="U5" s="123"/>
-      <c r="V5" s="123"/>
-      <c r="W5" s="123"/>
+      <c r="N5" s="124"/>
+      <c r="O5" s="124"/>
+      <c r="P5" s="124"/>
+      <c r="Q5" s="124"/>
+      <c r="R5" s="124"/>
+      <c r="S5" s="124"/>
+      <c r="T5" s="124"/>
+      <c r="U5" s="124"/>
+      <c r="V5" s="124"/>
+      <c r="W5" s="124"/>
       <c r="AA5" s="1" t="s">
         <v>52</v>
       </c>
@@ -30973,15 +30973,15 @@
       <c r="K4" t="s">
         <v>1178</v>
       </c>
-      <c r="O4" s="124" t="s">
+      <c r="O4" s="125" t="s">
         <v>227</v>
       </c>
-      <c r="P4" s="125"/>
-      <c r="Q4" s="125"/>
-      <c r="R4" s="125"/>
-      <c r="S4" s="125"/>
-      <c r="T4" s="125"/>
-      <c r="U4" s="125"/>
+      <c r="P4" s="126"/>
+      <c r="Q4" s="126"/>
+      <c r="R4" s="126"/>
+      <c r="S4" s="126"/>
+      <c r="T4" s="126"/>
+      <c r="U4" s="126"/>
     </row>
     <row r="5" spans="3:22" ht="12.75">
       <c r="C5" s="1" t="s">
@@ -34074,8 +34074,8 @@
   </sheetPr>
   <dimension ref="B3:U82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N74" sqref="N74"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -34101,7 +34101,7 @@
     <col min="25" max="25" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:21">
+    <row r="3" spans="3:21" ht="12.75">
       <c r="C3" s="1" t="s">
         <v>258</v>
       </c>
@@ -34112,12 +34112,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="3:21">
+    <row r="4" spans="3:21" ht="12.75">
       <c r="E4" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="3:21">
+    <row r="5" spans="3:21" ht="12.75">
       <c r="C5" s="1" t="s">
         <v>52</v>
       </c>
@@ -34161,7 +34161,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="3:21">
+    <row r="6" spans="3:21" ht="12.75">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -34196,7 +34196,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="7" spans="3:21">
+    <row r="7" spans="3:21" ht="12.75">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -34243,7 +34243,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="3:21">
+    <row r="8" spans="3:21" ht="12.75">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -34285,7 +34285,7 @@
       </c>
       <c r="T8" s="29"/>
     </row>
-    <row r="9" spans="3:21">
+    <row r="9" spans="3:21" ht="12.75">
       <c r="C9" s="1">
         <v>4</v>
       </c>
@@ -34327,7 +34327,7 @@
       </c>
       <c r="T9" s="30"/>
     </row>
-    <row r="10" spans="3:21">
+    <row r="10" spans="3:21" ht="12.75">
       <c r="C10" s="1">
         <v>5</v>
       </c>
@@ -34369,7 +34369,7 @@
       </c>
       <c r="T10" s="32"/>
     </row>
-    <row r="11" spans="3:21">
+    <row r="11" spans="3:21" ht="12.75">
       <c r="C11" s="1">
         <v>6</v>
       </c>
@@ -34411,7 +34411,7 @@
       </c>
       <c r="T11" s="33"/>
     </row>
-    <row r="12" spans="3:21">
+    <row r="12" spans="3:21" ht="12.75">
       <c r="C12" s="1">
         <v>7</v>
       </c>
@@ -34456,7 +34456,7 @@
       </c>
       <c r="T12" s="34"/>
     </row>
-    <row r="13" spans="3:21">
+    <row r="13" spans="3:21" ht="12.75">
       <c r="C13" s="1">
         <v>8</v>
       </c>
@@ -34488,7 +34488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="3:21">
+    <row r="14" spans="3:21" ht="12.75">
       <c r="C14" s="1">
         <v>9</v>
       </c>
@@ -34520,7 +34520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:21">
+    <row r="15" spans="3:21" ht="12.75">
       <c r="C15" s="1">
         <v>10</v>
       </c>
@@ -34552,7 +34552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="3:21">
+    <row r="16" spans="3:21" ht="12.75">
       <c r="C16" s="1">
         <v>11</v>
       </c>
@@ -34584,7 +34584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:15">
+    <row r="17" spans="3:15" ht="12.75">
       <c r="C17" s="1">
         <v>12</v>
       </c>
@@ -34610,7 +34610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="3:15">
+    <row r="18" spans="3:15" ht="12.75">
       <c r="C18" s="1">
         <v>13</v>
       </c>
@@ -34636,7 +34636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="3:15">
+    <row r="19" spans="3:15" ht="12.75">
       <c r="C19" s="1">
         <v>14</v>
       </c>
@@ -34662,7 +34662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:15">
+    <row r="20" spans="3:15" ht="12.75">
       <c r="C20" s="1">
         <v>15</v>
       </c>
@@ -34688,7 +34688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="3:15">
+    <row r="21" spans="3:15" ht="12.75">
       <c r="C21" s="1">
         <v>16</v>
       </c>
@@ -34714,7 +34714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="3:15">
+    <row r="22" spans="3:15" ht="12.75">
       <c r="C22" s="1">
         <v>17</v>
       </c>
@@ -34740,7 +34740,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="3:15">
+    <row r="23" spans="3:15" ht="12.75">
       <c r="C23" s="1">
         <v>18</v>
       </c>
@@ -34766,7 +34766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="3:15">
+    <row r="24" spans="3:15" ht="12.75">
       <c r="C24" s="1">
         <v>19</v>
       </c>
@@ -34792,7 +34792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="3:15">
+    <row r="25" spans="3:15" ht="12.75">
       <c r="C25" s="1">
         <v>20</v>
       </c>
@@ -34818,7 +34818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="3:15">
+    <row r="26" spans="3:15" ht="12.75">
       <c r="C26" s="1">
         <v>21</v>
       </c>
@@ -34844,7 +34844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="3:15">
+    <row r="27" spans="3:15" ht="12.75">
       <c r="I27" s="1">
         <v>22</v>
       </c>
@@ -34864,7 +34864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="3:15">
+    <row r="28" spans="3:15" ht="12.75">
       <c r="C28" t="s">
         <v>1583</v>
       </c>
@@ -34887,7 +34887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="3:15">
+    <row r="29" spans="3:15" ht="12.75">
       <c r="E29" t="s">
         <v>1584</v>
       </c>
@@ -34916,7 +34916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="3:15">
+    <row r="30" spans="3:15" ht="12.75">
       <c r="C30" s="46" t="s">
         <v>774</v>
       </c>
@@ -34951,7 +34951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="3:15">
+    <row r="31" spans="3:15" ht="12.75">
       <c r="C31" s="46" t="s">
         <v>779</v>
       </c>
@@ -34986,7 +34986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="3:15">
+    <row r="32" spans="3:15" ht="12.75">
       <c r="C32" s="46" t="s">
         <v>780</v>
       </c>
@@ -35021,7 +35021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:15">
+    <row r="33" spans="2:15" ht="12.75">
       <c r="C33" s="46" t="s">
         <v>781</v>
       </c>
@@ -35056,7 +35056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:15">
+    <row r="34" spans="2:15" ht="12.75">
       <c r="C34" s="46" t="s">
         <v>778</v>
       </c>
@@ -35091,7 +35091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:15">
+    <row r="35" spans="2:15" ht="12.75">
       <c r="B35">
         <v>1</v>
       </c>
@@ -35120,7 +35120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:15">
+    <row r="36" spans="2:15" ht="12.75">
       <c r="B36">
         <v>2</v>
       </c>
@@ -35149,7 +35149,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="2:15">
+    <row r="37" spans="2:15" ht="12.75">
       <c r="B37">
         <v>3</v>
       </c>
@@ -35178,7 +35178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="2:15">
+    <row r="38" spans="2:15" ht="12.75">
       <c r="B38">
         <v>4</v>
       </c>
@@ -35207,7 +35207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:15">
+    <row r="39" spans="2:15" ht="12.75">
       <c r="B39">
         <v>5</v>
       </c>
@@ -35236,7 +35236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:15">
+    <row r="40" spans="2:15" ht="12.75">
       <c r="B40">
         <v>6</v>
       </c>
@@ -35265,7 +35265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:15">
+    <row r="41" spans="2:15" ht="12.75">
       <c r="B41">
         <v>7</v>
       </c>
@@ -35294,7 +35294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:15">
+    <row r="42" spans="2:15" ht="12.75">
       <c r="B42">
         <v>8</v>
       </c>
@@ -35323,7 +35323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:15">
+    <row r="43" spans="2:15" ht="12.75">
       <c r="B43">
         <v>9</v>
       </c>
@@ -35352,7 +35352,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="2:15">
+    <row r="44" spans="2:15" ht="12.75">
       <c r="B44">
         <v>10</v>
       </c>
@@ -35381,7 +35381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="2:15">
+    <row r="45" spans="2:15" ht="12.75">
       <c r="B45">
         <v>11</v>
       </c>
@@ -35410,7 +35410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="2:15">
+    <row r="46" spans="2:15" ht="12.75">
       <c r="B46">
         <v>12</v>
       </c>
@@ -35439,7 +35439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="2:15">
+    <row r="47" spans="2:15" ht="12.75">
       <c r="B47">
         <v>13</v>
       </c>
@@ -35468,7 +35468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="2:15">
+    <row r="48" spans="2:15" ht="12.75">
       <c r="B48">
         <v>14</v>
       </c>
@@ -35497,7 +35497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="2:15">
+    <row r="49" spans="2:15" ht="12.75">
       <c r="B49">
         <v>15</v>
       </c>
@@ -35526,7 +35526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="2:15">
+    <row r="50" spans="2:15" ht="12.75">
       <c r="B50">
         <v>16</v>
       </c>
@@ -35555,7 +35555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="2:15">
+    <row r="51" spans="2:15" ht="12.75">
       <c r="I51" s="1">
         <v>46</v>
       </c>
@@ -35575,7 +35575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="2:15">
+    <row r="52" spans="2:15" ht="12.75">
       <c r="I52" s="1">
         <v>47</v>
       </c>
@@ -35595,7 +35595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="2:15">
+    <row r="53" spans="2:15" ht="12.75">
       <c r="I53" s="1">
         <v>48</v>
       </c>
@@ -35615,7 +35615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:15">
+    <row r="54" spans="2:15" ht="12.75">
       <c r="I54" s="1">
         <v>49</v>
       </c>
@@ -35635,56 +35635,56 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:15">
+    <row r="55" spans="2:15" ht="12.75">
       <c r="I55" s="1">
         <v>50</v>
       </c>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="2:15">
+    <row r="56" spans="2:15" ht="12.75">
       <c r="I56" s="1">
         <v>51</v>
       </c>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="2:15">
+    <row r="57" spans="2:15" ht="12.75">
       <c r="I57" s="1">
         <v>52</v>
       </c>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="2:15">
+    <row r="58" spans="2:15" ht="12.75">
       <c r="I58" s="1">
         <v>53</v>
       </c>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="2:15">
+    <row r="59" spans="2:15" ht="12.75">
       <c r="I59" s="1">
         <v>54</v>
       </c>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="2:15">
+    <row r="60" spans="2:15" ht="12.75">
       <c r="I60" s="1">
         <v>55</v>
       </c>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="2:15">
+    <row r="61" spans="2:15" ht="12.75">
       <c r="I61" s="1">
         <v>56</v>
       </c>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="2:15">
+    <row r="62" spans="2:15" ht="12.75">
       <c r="I62" s="1">
         <v>57</v>
       </c>
       <c r="K62" s="1"/>
     </row>
     <row r="65" spans="8:15" ht="15.75" customHeight="1">
-      <c r="J65" s="126" t="s">
+      <c r="J65" s="123" t="s">
         <v>1651</v>
       </c>
       <c r="K65" s="45" t="s">
@@ -36042,7 +36042,7 @@
       </c>
     </row>
     <row r="80" spans="8:15" ht="15.75" customHeight="1">
-      <c r="J80" s="126" t="s">
+      <c r="J80" s="123" t="s">
         <v>1653</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Performance, Text Log, Balancing and Bugs
Fixed a lot of bugs
Game and Fishing Balancing
Added 1 new Research, Changed some of the Achievements
Added text log messages for temp bonuses and caught fish
Game Performance optimization (fixed fish stutter)
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2109E3B-481E-4024-91EA-38A2A1E0F1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4929C22-4BA5-431C-84CB-8F1AAE99497F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23865" yWindow="7590" windowWidth="20145" windowHeight="12150" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -34074,8 +34074,8 @@
   </sheetPr>
   <dimension ref="B3:U82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="E8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Fish Tooltips, Balancing, Ash and Bugs
Fish Tooltips now with price and effect
Fixed visual and Fishing Bugs
Changed some of the Achievements
Scaling up/down and balancing Fishing and Game Values
Started work on Ash Wood
In the code reshuffled fish
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4929C22-4BA5-431C-84CB-8F1AAE99497F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D03011-6403-4100-8B1B-EAD97E4B9A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23865" yWindow="7590" windowWidth="20145" windowHeight="12150" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23850" yWindow="8805" windowWidth="20145" windowHeight="12150" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -34074,8 +34074,8 @@
   </sheetPr>
   <dimension ref="B3:U82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="F39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -34086,8 +34086,8 @@
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
     <col min="10" max="10" width="23.140625" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>

</xml_diff>

<commit_message>
More Research Items, Balancing and Bugs
Fixed visual Fishing and Achievement Bugs
Updated Bot and Upgrade Prices
Added 8 more Research Items, adjusted Research Timings
Game Balancing
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D03011-6403-4100-8B1B-EAD97E4B9A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85585A45-FC01-43EA-89F7-7835DB1E7969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23850" yWindow="8805" windowWidth="20145" windowHeight="12150" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23850" yWindow="8805" windowWidth="20145" windowHeight="12150" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -24982,8 +24982,8 @@
   </sheetPr>
   <dimension ref="A3:AB114"/>
   <sheetViews>
-    <sheetView topLeftCell="N64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="X90" sqref="X90"/>
+    <sheetView tabSelected="1" topLeftCell="Q92" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Z100" sqref="Z100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -34074,7 +34074,7 @@
   </sheetPr>
   <dimension ref="B3:U82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="F36" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Game Flow Balancing and Bug Fixes
Bug Fixes for features not tested before
Add more Research prices and rest of the missing bonus calculations
Couple more Magic Upgrades and Research
Balancing
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85585A45-FC01-43EA-89F7-7835DB1E7969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C836C11-0292-4CC8-BC14-C3C5EC6F8EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23850" yWindow="8805" windowWidth="20145" windowHeight="12150" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -4518,9 +4518,6 @@
     <t>Woodcamps 20% more storage</t>
   </si>
   <si>
-    <t>Woodcamps 27.5% WPS</t>
-  </si>
-  <si>
     <t>woodcamps use 10% less wood</t>
   </si>
   <si>
@@ -4536,12 +4533,6 @@
     <t>Each achievement gives +0.75% WPS</t>
   </si>
   <si>
-    <t>Each achievement gives +0.55% Storage</t>
-  </si>
-  <si>
-    <t>Each achievement gives +0.25% WPC</t>
-  </si>
-  <si>
     <t>Maple WC Storage 75%</t>
   </si>
   <si>
@@ -4554,15 +4545,9 @@
     <t>Classic Upgrades 33% Cheaper</t>
   </si>
   <si>
-    <t>1% wps per achievement</t>
-  </si>
-  <si>
     <t>Classic Wood +10 Woodcamps</t>
   </si>
   <si>
-    <t>storage from WC +27.5%</t>
-  </si>
-  <si>
     <t>Classic wood types +2 beavers</t>
   </si>
   <si>
@@ -4572,9 +4557,6 @@
     <t>Rare Upgrades 44% Cheaper</t>
   </si>
   <si>
-    <t>Mythic Upgrades 44% Cheaper</t>
-  </si>
-  <si>
     <t>Gold Upgrades 30% Cheaper</t>
   </si>
   <si>
@@ -4584,9 +4566,6 @@
     <t>7.5% WPC To WPS</t>
   </si>
   <si>
-    <t>3.5% WPC To WPS</t>
-  </si>
-  <si>
     <t>2.5% WPC To WPS</t>
   </si>
   <si>
@@ -4659,45 +4638,21 @@
     <t>Storage 4.5%</t>
   </si>
   <si>
-    <t>6% WPS</t>
-  </si>
-  <si>
     <t>8% WPS</t>
   </si>
   <si>
     <t>10% WPS</t>
   </si>
   <si>
-    <t>Oak gives 25% More Magic</t>
-  </si>
-  <si>
-    <t>Classic And Rare WPS 15.5%</t>
-  </si>
-  <si>
-    <t>Birch WPS 36%</t>
-  </si>
-  <si>
     <t>Spruce WC Price -66%</t>
   </si>
   <si>
     <t>Mahogany Price 11%</t>
   </si>
   <si>
-    <t>Classic WPC +9%</t>
-  </si>
-  <si>
-    <t>Rare WPC +8%</t>
-  </si>
-  <si>
     <t>WC Effects 11.5%</t>
   </si>
   <si>
-    <t>WC +1 Per 22 Beavers</t>
-  </si>
-  <si>
-    <t>Magic bonuses x1.2</t>
-  </si>
-  <si>
     <t>Achievement Bonuses +15%</t>
   </si>
   <si>
@@ -4710,36 +4665,12 @@
     <t>Ebony +7 Beavers</t>
   </si>
   <si>
-    <t>Mahogany WPS 11%</t>
-  </si>
-  <si>
     <t>Rare Storage +23.5%</t>
   </si>
   <si>
-    <t>Mythic Storage 28%</t>
-  </si>
-  <si>
-    <t>Upgrade price -20%</t>
-  </si>
-  <si>
     <t>Ebony storage 15%</t>
   </si>
   <si>
-    <t>Dogwood Beaver price -11%</t>
-  </si>
-  <si>
-    <t>Dogwood +1WC Per 19 Beavers</t>
-  </si>
-  <si>
-    <t>Research Time -55%</t>
-  </si>
-  <si>
-    <t>Research Time -0.2% Per Achievement</t>
-  </si>
-  <si>
-    <t>WPS +5% per Unlocked Wood Type</t>
-  </si>
-  <si>
     <t>WPC, Storage +3%  Per Unlocked Wood</t>
   </si>
   <si>
@@ -4752,9 +4683,6 @@
     <t>Rosewood Storage 13.5%</t>
   </si>
   <si>
-    <t>Rosewood WC Effect +8%</t>
-  </si>
-  <si>
     <t>Classic Upgrades 39% Cheaper</t>
   </si>
   <si>
@@ -4767,9 +4695,6 @@
     <t>WPS 1% Per Achievement</t>
   </si>
   <si>
-    <t>Mythic WPC x2</t>
-  </si>
-  <si>
     <t xml:space="preserve">reaserch time -25% </t>
   </si>
   <si>
@@ -4788,9 +4713,6 @@
     <t>Classic and Chestnut WPC +199</t>
   </si>
   <si>
-    <t>1 Beaver Per 11 WC</t>
-  </si>
-  <si>
     <t>Here</t>
   </si>
   <si>
@@ -5074,6 +4996,84 @@
   </si>
   <si>
     <t>ShopItem</t>
+  </si>
+  <si>
+    <t>Birch, Maple WPS 36%</t>
+  </si>
+  <si>
+    <t>Classic WPC 3x</t>
+  </si>
+  <si>
+    <t>Achievement give 20% More Storage</t>
+  </si>
+  <si>
+    <t>Classic and Rare WPS 15%</t>
+  </si>
+  <si>
+    <t>Storage from Beavers +27.5%</t>
+  </si>
+  <si>
+    <t>Magic Bonuses +10%</t>
+  </si>
+  <si>
+    <t>Rare WPS +5% per Unlocked Wood Type</t>
+  </si>
+  <si>
+    <t>Achievements Give +35% WPC</t>
+  </si>
+  <si>
+    <t>Classic, Rare +15 Beavers</t>
+  </si>
+  <si>
+    <t>33% WPC</t>
+  </si>
+  <si>
+    <t>Classic and Rare Upgrade price -20%</t>
+  </si>
+  <si>
+    <t>Achievements Give +10% WPS</t>
+  </si>
+  <si>
+    <t>Research Time -15%</t>
+  </si>
+  <si>
+    <t>Mahogany WPS 22%</t>
+  </si>
+  <si>
+    <t>Rare and Mythic WPC +25%</t>
+  </si>
+  <si>
+    <t>Classic And Rare WPS 17.5%</t>
+  </si>
+  <si>
+    <t>Magic Effects 20%</t>
+  </si>
+  <si>
+    <t>Mythic WC Price -45%</t>
+  </si>
+  <si>
+    <t>Research Time -20%</t>
+  </si>
+  <si>
+    <t>WPS +27.5%</t>
+  </si>
+  <si>
+    <t>Mythic Beaver price -25%</t>
+  </si>
+  <si>
+    <t>Dogwood +9 Woodcamps and Beavers</t>
+  </si>
+  <si>
+    <t>Rosewood WC Effect +20%</t>
+  </si>
+  <si>
+    <t>Mythic Upgrades 80% Cheaper</t>
+  </si>
+  <si>
+    <t>Mythic Storage 33%</t>
+  </si>
+  <si>
+    <t>WPC x5</t>
   </si>
 </sst>
 </file>
@@ -22287,8 +22287,8 @@
   </sheetPr>
   <dimension ref="C2:P157"/>
   <sheetViews>
-    <sheetView topLeftCell="A125" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -22674,7 +22674,7 @@
         <v>20</v>
       </c>
       <c r="F24" s="115" t="s">
-        <v>1504</v>
+        <v>1499</v>
       </c>
       <c r="P24" s="27" t="s">
         <v>288</v>
@@ -22691,7 +22691,7 @@
         <v>21</v>
       </c>
       <c r="F25" t="s">
-        <v>1573</v>
+        <v>1548</v>
       </c>
       <c r="P25" s="41" t="s">
         <v>294</v>
@@ -22728,7 +22728,7 @@
         <v>23</v>
       </c>
       <c r="F27" t="s">
-        <v>1505</v>
+        <v>1500</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>140</v>
@@ -22805,7 +22805,7 @@
         <v>27</v>
       </c>
       <c r="F31" t="s">
-        <v>1497</v>
+        <v>1494</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>171</v>
@@ -22865,7 +22865,7 @@
         <v>30</v>
       </c>
       <c r="F34" s="45" t="s">
-        <v>1499</v>
+        <v>1496</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>175</v>
@@ -22905,7 +22905,7 @@
         <v>32</v>
       </c>
       <c r="F36" s="46" t="s">
-        <v>1574</v>
+        <v>1549</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>168</v>
@@ -22945,7 +22945,7 @@
         <v>34</v>
       </c>
       <c r="F38" s="46" t="s">
-        <v>1575</v>
+        <v>1550</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>178</v>
@@ -22979,7 +22979,7 @@
         <v>36</v>
       </c>
       <c r="F40" s="46" t="s">
-        <v>1518</v>
+        <v>1511</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>166</v>
@@ -23002,7 +23002,7 @@
         <v>37</v>
       </c>
       <c r="F41" s="46" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>176</v>
@@ -23025,7 +23025,7 @@
         <v>38</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>1498</v>
+        <v>1495</v>
       </c>
       <c r="H42" s="45" t="s">
         <v>682</v>
@@ -23071,7 +23071,7 @@
         <v>40</v>
       </c>
       <c r="F44" t="s">
-        <v>1576</v>
+        <v>1551</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>177</v>
@@ -23097,7 +23097,7 @@
         <v>41</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>1577</v>
+        <v>1552</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>167</v>
@@ -23123,7 +23123,7 @@
         <v>42</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>1500</v>
+        <v>1497</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>169</v>
@@ -23149,7 +23149,7 @@
         <v>43</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>1516</v>
+        <v>1509</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>170</v>
@@ -23175,7 +23175,7 @@
         <v>44</v>
       </c>
       <c r="F48" s="46" t="s">
-        <v>1519</v>
+        <v>1512</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>693</v>
@@ -23250,7 +23250,7 @@
         <v>47</v>
       </c>
       <c r="F51" t="s">
-        <v>1510</v>
+        <v>1504</v>
       </c>
       <c r="H51" s="45" t="s">
         <v>686</v>
@@ -23326,7 +23326,7 @@
         <v>50</v>
       </c>
       <c r="F54" s="46" t="s">
-        <v>1578</v>
+        <v>1553</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>410</v>
@@ -23352,7 +23352,7 @@
         <v>51</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>1517</v>
+        <v>1510</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>164</v>
@@ -23378,7 +23378,7 @@
         <v>52</v>
       </c>
       <c r="F56" t="s">
-        <v>1502</v>
+        <v>1498</v>
       </c>
       <c r="H56" s="45" t="s">
         <v>685</v>
@@ -23404,7 +23404,7 @@
         <v>53</v>
       </c>
       <c r="F57" s="46" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="M57" t="s">
         <v>997</v>
@@ -23427,7 +23427,7 @@
         <v>54</v>
       </c>
       <c r="F58" s="46" t="s">
-        <v>1520</v>
+        <v>1513</v>
       </c>
       <c r="M58" t="s">
         <v>992</v>
@@ -23516,7 +23516,7 @@
         <v>58</v>
       </c>
       <c r="F62" s="46" t="s">
-        <v>1521</v>
+        <v>1514</v>
       </c>
       <c r="M62" t="s">
         <v>999</v>
@@ -23576,7 +23576,7 @@
         <v>61</v>
       </c>
       <c r="F65" s="47" t="s">
-        <v>1522</v>
+        <v>1515</v>
       </c>
       <c r="M65" t="s">
         <v>1000</v>
@@ -23596,7 +23596,7 @@
         <v>62</v>
       </c>
       <c r="F66" s="46" t="s">
-        <v>1523</v>
+        <v>1516</v>
       </c>
       <c r="M66" t="s">
         <v>1019</v>
@@ -23633,7 +23633,7 @@
         <v>64</v>
       </c>
       <c r="F68" t="s">
-        <v>1513</v>
+        <v>1506</v>
       </c>
       <c r="M68" t="s">
         <v>1005</v>
@@ -23650,7 +23650,7 @@
         <v>65</v>
       </c>
       <c r="F69" t="s">
-        <v>1533</v>
+        <v>1526</v>
       </c>
       <c r="M69" t="s">
         <v>987</v>
@@ -23670,7 +23670,7 @@
         <v>66</v>
       </c>
       <c r="F70" s="45" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="M70" t="s">
         <v>1013</v>
@@ -23684,7 +23684,7 @@
         <v>67</v>
       </c>
       <c r="F71" s="45" t="s">
-        <v>1515</v>
+        <v>1508</v>
       </c>
       <c r="M71" t="s">
         <v>996</v>
@@ -23701,7 +23701,7 @@
         <v>68</v>
       </c>
       <c r="F72" s="45" t="s">
-        <v>1534</v>
+        <v>1527</v>
       </c>
       <c r="M72" t="s">
         <v>1018</v>
@@ -23738,7 +23738,7 @@
         <v>70</v>
       </c>
       <c r="F74" s="45" t="s">
-        <v>1582</v>
+        <v>1556</v>
       </c>
       <c r="M74" t="s">
         <v>1008</v>
@@ -23772,7 +23772,7 @@
         <v>72</v>
       </c>
       <c r="F76" s="47" t="s">
-        <v>1526</v>
+        <v>1519</v>
       </c>
       <c r="M76" t="s">
         <v>1017</v>
@@ -23786,7 +23786,7 @@
         <v>73</v>
       </c>
       <c r="F77" s="45" t="s">
-        <v>1541</v>
+        <v>1649</v>
       </c>
       <c r="M77" t="s">
         <v>94</v>
@@ -23800,7 +23800,7 @@
         <v>74</v>
       </c>
       <c r="F78" s="45" t="s">
-        <v>1495</v>
+        <v>1651</v>
       </c>
       <c r="M78" t="s">
         <v>1026</v>
@@ -23814,7 +23814,7 @@
         <v>75</v>
       </c>
       <c r="F79" s="45" t="s">
-        <v>1536</v>
+        <v>1652</v>
       </c>
       <c r="M79" t="s">
         <v>1029</v>
@@ -23828,7 +23828,7 @@
         <v>76</v>
       </c>
       <c r="F80" t="s">
-        <v>1503</v>
+        <v>1653</v>
       </c>
       <c r="M80" t="s">
         <v>1031</v>
@@ -23842,7 +23842,7 @@
         <v>77</v>
       </c>
       <c r="F81" t="s">
-        <v>1539</v>
+        <v>1654</v>
       </c>
       <c r="M81" s="114" t="s">
         <v>1033</v>
@@ -23856,7 +23856,7 @@
         <v>78</v>
       </c>
       <c r="F82" t="s">
-        <v>1544</v>
+        <v>1650</v>
       </c>
       <c r="M82" t="s">
         <v>1035</v>
@@ -23881,7 +23881,7 @@
         <v>80</v>
       </c>
       <c r="F84" t="s">
-        <v>1562</v>
+        <v>1655</v>
       </c>
       <c r="M84" t="s">
         <v>1038</v>
@@ -23892,7 +23892,7 @@
         <v>81</v>
       </c>
       <c r="F85" s="45" t="s">
-        <v>1496</v>
+        <v>1656</v>
       </c>
       <c r="M85" t="s">
         <v>1039</v>
@@ -23906,7 +23906,7 @@
         <v>82</v>
       </c>
       <c r="F86" t="s">
-        <v>1514</v>
+        <v>1507</v>
       </c>
       <c r="M86" t="s">
         <v>1043</v>
@@ -23917,7 +23917,7 @@
         <v>83</v>
       </c>
       <c r="F87" t="s">
-        <v>1542</v>
+        <v>1531</v>
       </c>
       <c r="M87" t="s">
         <v>1048</v>
@@ -23928,7 +23928,7 @@
         <v>84</v>
       </c>
       <c r="F88" s="46" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="M88" t="s">
         <v>1054</v>
@@ -23939,7 +23939,7 @@
         <v>85</v>
       </c>
       <c r="F89" t="s">
-        <v>1550</v>
+        <v>1535</v>
       </c>
       <c r="M89" t="s">
         <v>1058</v>
@@ -23950,7 +23950,7 @@
         <v>86</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>1506</v>
+        <v>1501</v>
       </c>
       <c r="M90" t="s">
         <v>1065</v>
@@ -23961,7 +23961,7 @@
         <v>87</v>
       </c>
       <c r="F91" t="s">
-        <v>1529</v>
+        <v>1522</v>
       </c>
       <c r="M91" t="s">
         <v>1066</v>
@@ -23972,7 +23972,7 @@
         <v>88</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>1579</v>
+        <v>1657</v>
       </c>
       <c r="M92" t="s">
         <v>1074</v>
@@ -23994,7 +23994,7 @@
         <v>90</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>1554</v>
+        <v>1538</v>
       </c>
       <c r="M94" t="s">
         <v>1075</v>
@@ -24005,7 +24005,7 @@
         <v>91</v>
       </c>
       <c r="F95" t="s">
-        <v>1511</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="96" spans="5:16" ht="15.75" customHeight="1">
@@ -24013,7 +24013,7 @@
         <v>92</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>1556</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="97" spans="5:14" ht="15.75" customHeight="1">
@@ -24021,7 +24021,7 @@
         <v>93</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>1563</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="98" spans="5:14" ht="15.75" customHeight="1">
@@ -24029,10 +24029,10 @@
         <v>94</v>
       </c>
       <c r="F98" s="45" t="s">
-        <v>1543</v>
+        <v>1532</v>
       </c>
       <c r="M98" t="s">
-        <v>1581</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="99" spans="5:14" ht="15.75" customHeight="1">
@@ -24040,7 +24040,7 @@
         <v>95</v>
       </c>
       <c r="F99" s="47" t="s">
-        <v>1527</v>
+        <v>1520</v>
       </c>
       <c r="M99" s="35" t="s">
         <v>3</v>
@@ -24054,7 +24054,7 @@
         <v>96</v>
       </c>
       <c r="F100" s="122" t="s">
-        <v>1501</v>
+        <v>1660</v>
       </c>
       <c r="M100" s="35" t="s">
         <v>18</v>
@@ -24068,7 +24068,7 @@
         <v>97</v>
       </c>
       <c r="F101" s="45" t="s">
-        <v>1557</v>
+        <v>1539</v>
       </c>
       <c r="M101" s="35" t="s">
         <v>9</v>
@@ -24082,7 +24082,7 @@
         <v>98</v>
       </c>
       <c r="F102" s="45" t="s">
-        <v>1560</v>
+        <v>1661</v>
       </c>
       <c r="M102" s="35" t="s">
         <v>14</v>
@@ -24110,7 +24110,7 @@
         <v>100</v>
       </c>
       <c r="F104" t="s">
-        <v>1531</v>
+        <v>1524</v>
       </c>
       <c r="M104" s="35" t="s">
         <v>16</v>
@@ -24124,7 +24124,7 @@
         <v>101</v>
       </c>
       <c r="F105" t="s">
-        <v>1553</v>
+        <v>1662</v>
       </c>
       <c r="M105" s="47" t="s">
         <v>26</v>
@@ -24138,7 +24138,7 @@
         <v>102</v>
       </c>
       <c r="F106" t="s">
-        <v>1545</v>
+        <v>1663</v>
       </c>
       <c r="M106" s="35" t="s">
         <v>29</v>
@@ -24150,7 +24150,7 @@
         <v>103</v>
       </c>
       <c r="F107" t="s">
-        <v>1540</v>
+        <v>1664</v>
       </c>
       <c r="M107" s="35" t="s">
         <v>31</v>
@@ -24162,7 +24162,7 @@
         <v>104</v>
       </c>
       <c r="F108" t="s">
-        <v>1548</v>
+        <v>1665</v>
       </c>
       <c r="M108" s="35" t="s">
         <v>33</v>
@@ -24174,7 +24174,7 @@
         <v>105</v>
       </c>
       <c r="F109" t="s">
-        <v>1535</v>
+        <v>1528</v>
       </c>
       <c r="M109" s="35" t="s">
         <v>37</v>
@@ -24186,7 +24186,7 @@
         <v>106</v>
       </c>
       <c r="F110" t="s">
-        <v>1551</v>
+        <v>1536</v>
       </c>
       <c r="M110" s="35" t="s">
         <v>39</v>
@@ -24198,7 +24198,7 @@
         <v>107</v>
       </c>
       <c r="F111" t="s">
-        <v>1547</v>
+        <v>1666</v>
       </c>
       <c r="M111" s="35" t="s">
         <v>41</v>
@@ -24210,7 +24210,7 @@
         <v>108</v>
       </c>
       <c r="F112" t="s">
-        <v>1561</v>
+        <v>1667</v>
       </c>
       <c r="M112" s="35" t="s">
         <v>45</v>
@@ -24234,7 +24234,7 @@
         <v>110</v>
       </c>
       <c r="F114" s="45" t="s">
-        <v>1489</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="115" spans="5:14" ht="15.75" customHeight="1">
@@ -24242,7 +24242,7 @@
         <v>111</v>
       </c>
       <c r="F115" t="s">
-        <v>1558</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="116" spans="5:14" ht="15.75" customHeight="1">
@@ -24250,7 +24250,7 @@
         <v>112</v>
       </c>
       <c r="F116" t="s">
-        <v>1564</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="117" spans="5:14" ht="15.75" customHeight="1">
@@ -24258,7 +24258,7 @@
         <v>113</v>
       </c>
       <c r="F117" t="s">
-        <v>1552</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="118" spans="5:14" ht="15.75" customHeight="1">
@@ -24266,7 +24266,7 @@
         <v>114</v>
       </c>
       <c r="F118" t="s">
-        <v>1546</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="119" spans="5:14" ht="15.75" customHeight="1">
@@ -24274,7 +24274,7 @@
         <v>115</v>
       </c>
       <c r="F119" t="s">
-        <v>1537</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="120" spans="5:14" ht="15.75" customHeight="1">
@@ -24282,7 +24282,7 @@
         <v>116</v>
       </c>
       <c r="F120" t="s">
-        <v>1565</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="121" spans="5:14" ht="15.75" customHeight="1">
@@ -24290,7 +24290,7 @@
         <v>117</v>
       </c>
       <c r="F121" s="46" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="122" spans="5:14" ht="15.75" customHeight="1">
@@ -24298,7 +24298,7 @@
         <v>118</v>
       </c>
       <c r="F122" t="s">
-        <v>1559</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="123" spans="5:14" ht="15.75" customHeight="1">
@@ -24314,7 +24314,7 @@
         <v>120</v>
       </c>
       <c r="F124" t="s">
-        <v>1532</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="125" spans="5:14" ht="15.75" customHeight="1">
@@ -24322,7 +24322,7 @@
         <v>121</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>1566</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="126" spans="5:14" ht="15.75" customHeight="1">
@@ -24330,7 +24330,7 @@
         <v>122</v>
       </c>
       <c r="F126" t="s">
-        <v>1530</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="127" spans="5:14" ht="15.75" customHeight="1">
@@ -24338,7 +24338,7 @@
         <v>123</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>1568</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="128" spans="5:14" ht="15.75" customHeight="1">
@@ -24346,7 +24346,7 @@
         <v>124</v>
       </c>
       <c r="F128" t="s">
-        <v>1512</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="129" spans="5:6" ht="15.75" customHeight="1">
@@ -24354,7 +24354,7 @@
         <v>125</v>
       </c>
       <c r="F129" t="s">
-        <v>1549</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="130" spans="5:6" ht="15.75" customHeight="1">
@@ -24362,7 +24362,7 @@
         <v>126</v>
       </c>
       <c r="F130" s="47" t="s">
-        <v>1528</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="131" spans="5:6" ht="15.75" customHeight="1">
@@ -24370,7 +24370,7 @@
         <v>127</v>
       </c>
       <c r="F131" t="s">
-        <v>1567</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="132" spans="5:6" ht="15.75" customHeight="1">
@@ -24378,7 +24378,7 @@
         <v>128</v>
       </c>
       <c r="F132" t="s">
-        <v>1538</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="133" spans="5:6" ht="15.75" customHeight="1">
@@ -24394,7 +24394,7 @@
         <v>130</v>
       </c>
       <c r="F134" t="s">
-        <v>1569</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="135" spans="5:6" ht="15.75" customHeight="1">
@@ -24402,7 +24402,7 @@
         <v>131</v>
       </c>
       <c r="F135" t="s">
-        <v>1508</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="136" spans="5:6" ht="15.75" customHeight="1">
@@ -24410,7 +24410,7 @@
         <v>132</v>
       </c>
       <c r="F136" t="s">
-        <v>1570</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="137" spans="5:6" ht="15.75" customHeight="1">
@@ -24418,7 +24418,7 @@
         <v>133</v>
       </c>
       <c r="F137" t="s">
-        <v>1525</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="138" spans="5:6" ht="15.75" customHeight="1">
@@ -24434,7 +24434,7 @@
         <v>135</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>1507</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="140" spans="5:6" ht="15.75" customHeight="1">
@@ -24442,7 +24442,7 @@
         <v>136</v>
       </c>
       <c r="F140" t="s">
-        <v>1571</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="141" spans="5:6" ht="15.75" customHeight="1">
@@ -24450,7 +24450,7 @@
         <v>137</v>
       </c>
       <c r="F141" t="s">
-        <v>1555</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="142" spans="5:6" ht="15.75" customHeight="1">
@@ -24458,7 +24458,7 @@
         <v>138</v>
       </c>
       <c r="F142" t="s">
-        <v>1524</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="143" spans="5:6" ht="15.75" customHeight="1">
@@ -24466,7 +24466,7 @@
         <v>139</v>
       </c>
       <c r="F143" t="s">
-        <v>1572</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="144" spans="5:6" ht="15.75" customHeight="1">
@@ -24474,7 +24474,7 @@
         <v>140</v>
       </c>
       <c r="F144" t="s">
-        <v>1509</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="145" spans="5:5" ht="15.75" customHeight="1">
@@ -24982,8 +24982,8 @@
   </sheetPr>
   <dimension ref="A3:AB114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q92" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Z100" sqref="Z100"/>
+    <sheetView topLeftCell="Q92" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V107" sqref="V107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -29912,7 +29912,7 @@
         <v>9553102</v>
       </c>
       <c r="AB76" t="s">
-        <v>1580</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="77" spans="2:28" ht="15.75" customHeight="1">
@@ -30545,7 +30545,7 @@
         <v>29236980</v>
       </c>
       <c r="AB106" t="s">
-        <v>1580</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="107" spans="20:28" ht="15.75" customHeight="1">
@@ -30611,7 +30611,7 @@
         <v>31784361</v>
       </c>
       <c r="AB109" t="s">
-        <v>1580</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="110" spans="20:28" ht="15.75" customHeight="1">
@@ -30656,7 +30656,7 @@
         <v>33683394</v>
       </c>
       <c r="AB111" t="s">
-        <v>1580</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="112" spans="20:28" ht="15.75" customHeight="1">
@@ -30680,7 +30680,7 @@
         <v>34694070</v>
       </c>
       <c r="AB112" t="s">
-        <v>1580</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="113" spans="20:28" ht="15.75" customHeight="1">
@@ -30704,7 +30704,7 @@
         <v>35756564</v>
       </c>
       <c r="AB113" t="s">
-        <v>1580</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="114" spans="20:28" ht="15.75" customHeight="1">
@@ -30728,7 +30728,7 @@
         <v>36873533</v>
       </c>
       <c r="AB114" t="s">
-        <v>1580</v>
+        <v>1554</v>
       </c>
     </row>
   </sheetData>
@@ -34152,7 +34152,7 @@
         <v>785</v>
       </c>
       <c r="O5" s="46" t="s">
-        <v>1606</v>
+        <v>1580</v>
       </c>
       <c r="P5" s="46" t="s">
         <v>786</v>
@@ -34181,10 +34181,10 @@
         <v>716</v>
       </c>
       <c r="K6" t="s">
-        <v>1601</v>
+        <v>1575</v>
       </c>
       <c r="M6" t="s">
-        <v>1598</v>
+        <v>1572</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -34216,10 +34216,10 @@
         <v>715</v>
       </c>
       <c r="K7" t="s">
-        <v>1602</v>
+        <v>1576</v>
       </c>
       <c r="M7" t="s">
-        <v>1599</v>
+        <v>1573</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -34266,7 +34266,7 @@
         <v>1099</v>
       </c>
       <c r="M8" t="s">
-        <v>1600</v>
+        <v>1574</v>
       </c>
       <c r="N8">
         <v>5</v>
@@ -34305,7 +34305,7 @@
         <v>731</v>
       </c>
       <c r="K9" t="s">
-        <v>1603</v>
+        <v>1577</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -34347,7 +34347,7 @@
         <v>720</v>
       </c>
       <c r="K10" t="s">
-        <v>1610</v>
+        <v>1584</v>
       </c>
       <c r="M10">
         <v>3</v>
@@ -34389,7 +34389,7 @@
         <v>725</v>
       </c>
       <c r="K11" t="s">
-        <v>1611</v>
+        <v>1585</v>
       </c>
       <c r="M11">
         <v>18</v>
@@ -34434,7 +34434,7 @@
         <v>726</v>
       </c>
       <c r="K12" t="s">
-        <v>1612</v>
+        <v>1586</v>
       </c>
       <c r="M12">
         <v>60</v>
@@ -34476,7 +34476,7 @@
         <v>717</v>
       </c>
       <c r="K13" t="s">
-        <v>1613</v>
+        <v>1587</v>
       </c>
       <c r="M13">
         <v>230</v>
@@ -34508,7 +34508,7 @@
         <v>719</v>
       </c>
       <c r="K14" t="s">
-        <v>1614</v>
+        <v>1588</v>
       </c>
       <c r="M14">
         <v>5</v>
@@ -34540,7 +34540,7 @@
         <v>723</v>
       </c>
       <c r="K15" t="s">
-        <v>1647</v>
+        <v>1621</v>
       </c>
       <c r="M15">
         <v>75</v>
@@ -34572,7 +34572,7 @@
         <v>724</v>
       </c>
       <c r="K16" t="s">
-        <v>1617</v>
+        <v>1591</v>
       </c>
       <c r="M16">
         <v>300</v>
@@ -34598,7 +34598,7 @@
         <v>718</v>
       </c>
       <c r="K17" t="s">
-        <v>1615</v>
+        <v>1589</v>
       </c>
       <c r="M17">
         <v>800</v>
@@ -34624,7 +34624,7 @@
         <v>721</v>
       </c>
       <c r="K18" t="s">
-        <v>1616</v>
+        <v>1590</v>
       </c>
       <c r="M18">
         <v>660</v>
@@ -34650,7 +34650,7 @@
         <v>722</v>
       </c>
       <c r="K19" t="s">
-        <v>1618</v>
+        <v>1592</v>
       </c>
       <c r="M19">
         <v>2</v>
@@ -34702,7 +34702,7 @@
         <v>737</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>1619</v>
+        <v>1593</v>
       </c>
       <c r="M21">
         <v>730</v>
@@ -34754,7 +34754,7 @@
         <v>732</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>1648</v>
+        <v>1622</v>
       </c>
       <c r="M23">
         <v>260</v>
@@ -34780,7 +34780,7 @@
         <v>733</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>1620</v>
+        <v>1594</v>
       </c>
       <c r="M24">
         <v>125</v>
@@ -34806,7 +34806,7 @@
         <v>734</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>1621</v>
+        <v>1595</v>
       </c>
       <c r="M25">
         <v>1200</v>
@@ -34852,7 +34852,7 @@
         <v>738</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>1622</v>
+        <v>1596</v>
       </c>
       <c r="M27">
         <v>160</v>
@@ -34866,7 +34866,7 @@
     </row>
     <row r="28" spans="3:15" ht="12.75">
       <c r="C28" t="s">
-        <v>1583</v>
+        <v>1557</v>
       </c>
       <c r="I28" s="1">
         <v>23</v>
@@ -34875,7 +34875,7 @@
         <v>741</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>1623</v>
+        <v>1597</v>
       </c>
       <c r="M28">
         <v>20</v>
@@ -34889,13 +34889,13 @@
     </row>
     <row r="29" spans="3:15" ht="12.75">
       <c r="E29" t="s">
-        <v>1584</v>
+        <v>1558</v>
       </c>
       <c r="F29" t="s">
-        <v>1604</v>
+        <v>1578</v>
       </c>
       <c r="G29" t="s">
-        <v>1605</v>
+        <v>1579</v>
       </c>
       <c r="I29" s="1">
         <v>24</v>
@@ -34904,7 +34904,7 @@
         <v>743</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>1624</v>
+        <v>1598</v>
       </c>
       <c r="M29">
         <v>40</v>
@@ -34939,7 +34939,7 @@
         <v>744</v>
       </c>
       <c r="K30" s="46" t="s">
-        <v>1669</v>
+        <v>1643</v>
       </c>
       <c r="M30">
         <v>90</v>
@@ -35044,7 +35044,7 @@
         <v>747</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>1625</v>
+        <v>1599</v>
       </c>
       <c r="M33">
         <v>25</v>
@@ -35079,7 +35079,7 @@
         <v>748</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>1626</v>
+        <v>1600</v>
       </c>
       <c r="M34">
         <v>2230</v>
@@ -35096,7 +35096,7 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>1585</v>
+        <v>1559</v>
       </c>
       <c r="D35">
         <v>1000</v>
@@ -35108,7 +35108,7 @@
         <v>749</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>1627</v>
+        <v>1601</v>
       </c>
       <c r="M35">
         <v>89</v>
@@ -35125,7 +35125,7 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>1586</v>
+        <v>1560</v>
       </c>
       <c r="D36">
         <v>50000</v>
@@ -35137,7 +35137,7 @@
         <v>750</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>1628</v>
+        <v>1602</v>
       </c>
       <c r="M36">
         <v>4400</v>
@@ -35154,7 +35154,7 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>1587</v>
+        <v>1561</v>
       </c>
       <c r="D37">
         <v>250000</v>
@@ -35166,7 +35166,7 @@
         <v>751</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>1629</v>
+        <v>1603</v>
       </c>
       <c r="M37">
         <v>555</v>
@@ -35183,7 +35183,7 @@
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>1588</v>
+        <v>1562</v>
       </c>
       <c r="D38">
         <v>300</v>
@@ -35195,7 +35195,7 @@
         <v>752</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>1630</v>
+        <v>1604</v>
       </c>
       <c r="M38">
         <v>1</v>
@@ -35212,7 +35212,7 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>1589</v>
+        <v>1563</v>
       </c>
       <c r="D39">
         <v>6000</v>
@@ -35224,7 +35224,7 @@
         <v>753</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>1631</v>
+        <v>1605</v>
       </c>
       <c r="M39">
         <v>3</v>
@@ -35241,7 +35241,7 @@
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>1590</v>
+        <v>1564</v>
       </c>
       <c r="D40">
         <v>90000</v>
@@ -35253,7 +35253,7 @@
         <v>754</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>1632</v>
+        <v>1606</v>
       </c>
       <c r="M40">
         <v>6</v>
@@ -35270,7 +35270,7 @@
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>1591</v>
+        <v>1565</v>
       </c>
       <c r="D41">
         <v>300</v>
@@ -35282,7 +35282,7 @@
         <v>755</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>1633</v>
+        <v>1607</v>
       </c>
       <c r="M41">
         <v>10</v>
@@ -35299,7 +35299,7 @@
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>1592</v>
+        <v>1566</v>
       </c>
       <c r="D42">
         <v>6000</v>
@@ -35311,7 +35311,7 @@
         <v>756</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>1634</v>
+        <v>1608</v>
       </c>
       <c r="M42">
         <v>14</v>
@@ -35328,7 +35328,7 @@
         <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>1593</v>
+        <v>1567</v>
       </c>
       <c r="D43">
         <v>90000</v>
@@ -35340,7 +35340,7 @@
         <v>757</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>1635</v>
+        <v>1609</v>
       </c>
       <c r="M43">
         <v>19</v>
@@ -35360,7 +35360,7 @@
         <v>1097</v>
       </c>
       <c r="D44" t="s">
-        <v>1596</v>
+        <v>1570</v>
       </c>
       <c r="I44" s="1">
         <v>39</v>
@@ -35369,7 +35369,7 @@
         <v>758</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>1636</v>
+        <v>1610</v>
       </c>
       <c r="M44">
         <v>24</v>
@@ -35389,7 +35389,7 @@
         <v>1098</v>
       </c>
       <c r="D45" t="s">
-        <v>1594</v>
+        <v>1568</v>
       </c>
       <c r="I45" s="1">
         <v>40</v>
@@ -35398,7 +35398,7 @@
         <v>759</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>1637</v>
+        <v>1611</v>
       </c>
       <c r="M45">
         <v>30</v>
@@ -35418,7 +35418,7 @@
         <v>1099</v>
       </c>
       <c r="D46" t="s">
-        <v>1595</v>
+        <v>1569</v>
       </c>
       <c r="I46" s="1">
         <v>41</v>
@@ -35427,7 +35427,7 @@
         <v>760</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>1638</v>
+        <v>1612</v>
       </c>
       <c r="M46">
         <v>36</v>
@@ -35444,7 +35444,7 @@
         <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>1597</v>
+        <v>1571</v>
       </c>
       <c r="D47">
         <v>7500</v>
@@ -35456,7 +35456,7 @@
         <v>761</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>1639</v>
+        <v>1613</v>
       </c>
       <c r="M47">
         <v>43</v>
@@ -35473,7 +35473,7 @@
         <v>14</v>
       </c>
       <c r="C48" t="s">
-        <v>1607</v>
+        <v>1581</v>
       </c>
       <c r="D48">
         <v>1000</v>
@@ -35485,7 +35485,7 @@
         <v>762</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>1640</v>
+        <v>1614</v>
       </c>
       <c r="M48">
         <v>55</v>
@@ -35502,7 +35502,7 @@
         <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>1607</v>
+        <v>1581</v>
       </c>
       <c r="D49">
         <v>7000</v>
@@ -35514,7 +35514,7 @@
         <v>763</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>1641</v>
+        <v>1615</v>
       </c>
       <c r="M49">
         <v>70</v>
@@ -35531,10 +35531,10 @@
         <v>16</v>
       </c>
       <c r="C50" t="s">
-        <v>1608</v>
+        <v>1582</v>
       </c>
       <c r="D50" t="s">
-        <v>1609</v>
+        <v>1583</v>
       </c>
       <c r="I50" s="1">
         <v>45</v>
@@ -35543,7 +35543,7 @@
         <v>764</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>1642</v>
+        <v>1616</v>
       </c>
       <c r="M50">
         <v>90</v>
@@ -35563,7 +35563,7 @@
         <v>765</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>1643</v>
+        <v>1617</v>
       </c>
       <c r="M51">
         <v>120</v>
@@ -35583,7 +35583,7 @@
         <v>766</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>1644</v>
+        <v>1618</v>
       </c>
       <c r="M52">
         <v>200</v>
@@ -35603,7 +35603,7 @@
         <v>787</v>
       </c>
       <c r="K53" s="46" t="s">
-        <v>1645</v>
+        <v>1619</v>
       </c>
       <c r="M53">
         <v>1100</v>
@@ -35623,7 +35623,7 @@
         <v>788</v>
       </c>
       <c r="K54" s="46" t="s">
-        <v>1646</v>
+        <v>1620</v>
       </c>
       <c r="M54">
         <v>600</v>
@@ -35685,7 +35685,7 @@
     </row>
     <row r="65" spans="8:15" ht="15.75" customHeight="1">
       <c r="J65" s="123" t="s">
-        <v>1651</v>
+        <v>1625</v>
       </c>
       <c r="K65" s="45" t="s">
         <v>75</v>
@@ -35694,24 +35694,24 @@
         <v>11</v>
       </c>
       <c r="M65" s="45" t="s">
-        <v>1662</v>
+        <v>1636</v>
       </c>
       <c r="N65" s="45" t="s">
-        <v>1663</v>
+        <v>1637</v>
       </c>
       <c r="O65" s="45" t="s">
-        <v>1664</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="66" spans="8:15" ht="15.75" customHeight="1">
       <c r="H66" s="45" t="s">
-        <v>1670</v>
+        <v>1644</v>
       </c>
       <c r="I66">
         <v>1</v>
       </c>
       <c r="J66" s="45" t="s">
-        <v>1649</v>
+        <v>1623</v>
       </c>
       <c r="K66">
         <v>1</v>
@@ -35731,13 +35731,13 @@
     </row>
     <row r="67" spans="8:15" ht="15.75" customHeight="1">
       <c r="H67" s="45" t="s">
-        <v>1671</v>
+        <v>1645</v>
       </c>
       <c r="I67">
         <v>2</v>
       </c>
       <c r="J67" s="45" t="s">
-        <v>1668</v>
+        <v>1642</v>
       </c>
       <c r="K67">
         <v>1</v>
@@ -35757,13 +35757,13 @@
     </row>
     <row r="68" spans="8:15" ht="15.75" customHeight="1">
       <c r="H68" s="45" t="s">
-        <v>1670</v>
+        <v>1644</v>
       </c>
       <c r="I68">
         <v>3</v>
       </c>
       <c r="J68" s="45" t="s">
-        <v>1661</v>
+        <v>1635</v>
       </c>
       <c r="K68" s="45">
         <v>0</v>
@@ -35783,13 +35783,13 @@
     </row>
     <row r="69" spans="8:15" ht="15.75" customHeight="1">
       <c r="H69" s="45" t="s">
-        <v>1672</v>
+        <v>1646</v>
       </c>
       <c r="I69">
         <v>4</v>
       </c>
       <c r="J69" s="45" t="s">
-        <v>1660</v>
+        <v>1634</v>
       </c>
       <c r="K69">
         <v>1</v>
@@ -35809,13 +35809,13 @@
     </row>
     <row r="70" spans="8:15" ht="15.75" customHeight="1">
       <c r="H70" s="45" t="s">
-        <v>1671</v>
+        <v>1645</v>
       </c>
       <c r="I70">
         <v>5</v>
       </c>
       <c r="J70" s="45" t="s">
-        <v>1665</v>
+        <v>1639</v>
       </c>
       <c r="K70">
         <v>1</v>
@@ -35835,13 +35835,13 @@
     </row>
     <row r="71" spans="8:15" ht="15.75" customHeight="1">
       <c r="H71" s="45" t="s">
-        <v>1673</v>
+        <v>1647</v>
       </c>
       <c r="I71">
         <v>6</v>
       </c>
       <c r="J71" s="45" t="s">
-        <v>1650</v>
+        <v>1624</v>
       </c>
       <c r="K71">
         <v>2</v>
@@ -35861,13 +35861,13 @@
     </row>
     <row r="72" spans="8:15" ht="15.75" customHeight="1">
       <c r="H72" s="45" t="s">
-        <v>1670</v>
+        <v>1644</v>
       </c>
       <c r="I72">
         <v>7</v>
       </c>
       <c r="J72" s="45" t="s">
-        <v>1659</v>
+        <v>1633</v>
       </c>
       <c r="K72">
         <v>1</v>
@@ -35887,13 +35887,13 @@
     </row>
     <row r="73" spans="8:15" ht="15.75" customHeight="1">
       <c r="H73" s="45" t="s">
-        <v>1671</v>
+        <v>1645</v>
       </c>
       <c r="I73">
         <v>8</v>
       </c>
       <c r="J73" s="45" t="s">
-        <v>1658</v>
+        <v>1632</v>
       </c>
       <c r="K73">
         <v>0</v>
@@ -35913,13 +35913,13 @@
     </row>
     <row r="74" spans="8:15" ht="15.75" customHeight="1">
       <c r="H74" s="45" t="s">
-        <v>1670</v>
+        <v>1644</v>
       </c>
       <c r="I74">
         <v>9</v>
       </c>
       <c r="J74" s="45" t="s">
-        <v>1657</v>
+        <v>1631</v>
       </c>
       <c r="K74">
         <v>0</v>
@@ -35939,13 +35939,13 @@
     </row>
     <row r="75" spans="8:15" ht="15.75" customHeight="1">
       <c r="H75" s="45" t="s">
-        <v>1670</v>
+        <v>1644</v>
       </c>
       <c r="I75">
         <v>10</v>
       </c>
       <c r="J75" s="45" t="s">
-        <v>1656</v>
+        <v>1630</v>
       </c>
       <c r="K75">
         <v>0</v>
@@ -35965,13 +35965,13 @@
     </row>
     <row r="76" spans="8:15" ht="15.75" customHeight="1">
       <c r="H76" s="45" t="s">
-        <v>1672</v>
+        <v>1646</v>
       </c>
       <c r="I76">
         <v>11</v>
       </c>
       <c r="J76" s="45" t="s">
-        <v>1655</v>
+        <v>1629</v>
       </c>
       <c r="K76">
         <v>0</v>
@@ -35991,13 +35991,13 @@
     </row>
     <row r="77" spans="8:15" ht="15.75" customHeight="1">
       <c r="H77" s="45" t="s">
-        <v>1670</v>
+        <v>1644</v>
       </c>
       <c r="I77">
         <v>12</v>
       </c>
       <c r="J77" s="45" t="s">
-        <v>1654</v>
+        <v>1628</v>
       </c>
       <c r="K77">
         <v>1</v>
@@ -36017,13 +36017,13 @@
     </row>
     <row r="78" spans="8:15" ht="15.75" customHeight="1">
       <c r="H78" s="45" t="s">
-        <v>1674</v>
+        <v>1648</v>
       </c>
       <c r="I78">
         <v>13</v>
       </c>
       <c r="J78" s="45" t="s">
-        <v>1652</v>
+        <v>1626</v>
       </c>
       <c r="K78">
         <v>0</v>
@@ -36043,12 +36043,12 @@
     </row>
     <row r="80" spans="8:15" ht="15.75" customHeight="1">
       <c r="J80" s="123" t="s">
-        <v>1653</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="81" spans="10:13" ht="15.75" customHeight="1">
       <c r="J81" s="45" t="s">
-        <v>1666</v>
+        <v>1640</v>
       </c>
       <c r="M81">
         <v>0</v>
@@ -36056,7 +36056,7 @@
     </row>
     <row r="82" spans="10:13" ht="15.75" customHeight="1">
       <c r="J82" s="45" t="s">
-        <v>1667</v>
+        <v>1641</v>
       </c>
       <c r="M82">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed Broken Save issue, added README
other minor fixes
</commit_message>
<xml_diff>
--- a/Beavers incremental mega sheet.xlsx
+++ b/Beavers incremental mega sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\godot\BeaverIncremental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C836C11-0292-4CC8-BC14-C3C5EC6F8EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D5C636-0555-4FDE-8F42-90092FE6C843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="7890" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralValues" sheetId="1" r:id="rId1"/>
@@ -22287,7 +22287,7 @@
   </sheetPr>
   <dimension ref="C2:P157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A131" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
@@ -24982,8 +24982,8 @@
   </sheetPr>
   <dimension ref="A3:AB114"/>
   <sheetViews>
-    <sheetView topLeftCell="Q92" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V107" sqref="V107"/>
+    <sheetView topLeftCell="Q86" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V94" sqref="V94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -30741,10 +30741,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="C3:T16"/>
+  <dimension ref="C3:T39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -30933,6 +30933,141 @@
     <row r="16" spans="3:20" ht="15.75" customHeight="1">
       <c r="D16" t="s">
         <v>900</v>
+      </c>
+    </row>
+    <row r="25" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <f>ROUND(L25*L25/2.65+L25,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L26">
+        <v>2</v>
+      </c>
+      <c r="M26">
+        <f t="shared" ref="M26:M39" si="0">ROUND(L26*L26/2.65+L26,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L27">
+        <v>3</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L28">
+        <v>4</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L29">
+        <v>5</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L30">
+        <v>6</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L31">
+        <v>7</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L32">
+        <v>8</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L33">
+        <v>9</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L34">
+        <v>10</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L35">
+        <v>11</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L36">
+        <v>12</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L37">
+        <v>13</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L38">
+        <v>14</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="12:13" ht="15.75" customHeight="1">
+      <c r="L39">
+        <v>15</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>